<commit_message>
print more organized infos
</commit_message>
<xml_diff>
--- a/templates/template_risk_indicators.xlsx
+++ b/templates/template_risk_indicators.xlsx
@@ -4371,7 +4371,7 @@
         <v>1</v>
       </c>
       <c r="N48" t="n">
-        <v>1</v>
+        <v>0.9444444444444444</v>
       </c>
       <c r="O48" t="n">
         <v>1</v>
@@ -5438,7 +5438,7 @@
         <v/>
       </c>
       <c r="M62" s="14" t="n">
-        <v>0.9444444444444444</v>
+        <v>1</v>
       </c>
       <c r="N62" s="5" t="n">
         <v>1</v>
@@ -5744,7 +5744,7 @@
         <v/>
       </c>
       <c r="M66" s="14" t="n">
-        <v>0.7222222222222222</v>
+        <v>1</v>
       </c>
       <c r="N66" s="5" t="n">
         <v>1</v>
@@ -5960,7 +5960,7 @@
         <v>1</v>
       </c>
       <c r="I69" t="n">
-        <v>0.4482758620689655</v>
+        <v>0.2380952380952381</v>
       </c>
       <c r="J69" t="n">
         <v>1</v>
@@ -5974,7 +5974,7 @@
         <v/>
       </c>
       <c r="M69" t="n">
-        <v>0.9444444444444444</v>
+        <v>1</v>
       </c>
       <c r="N69" t="n">
         <v>1</v>
@@ -5994,10 +5994,10 @@
         <v>0</v>
       </c>
       <c r="S69" t="n">
-        <v>1</v>
+        <v>0.7619047619047619</v>
       </c>
       <c r="T69" t="n">
-        <v>1</v>
+        <v>0.7619047619047619</v>
       </c>
       <c r="U69" s="8">
         <f>(T69-S69)/S69</f>
@@ -6050,7 +6050,7 @@
         <v/>
       </c>
       <c r="M70" s="14" t="n">
-        <v>0.8888888888888888</v>
+        <v>1</v>
       </c>
       <c r="N70" s="5" t="n">
         <v>1</v>
@@ -6280,7 +6280,7 @@
         <v/>
       </c>
       <c r="M73" t="n">
-        <v>0.9444444444444444</v>
+        <v>1</v>
       </c>
       <c r="N73" t="n">
         <v>1</v>
@@ -6297,7 +6297,7 @@
         <v/>
       </c>
       <c r="R73" t="n">
-        <v>0</v>
+        <v>0.8432203389830508</v>
       </c>
       <c r="S73" t="n">
         <v>0</v>
@@ -6356,13 +6356,13 @@
         <v/>
       </c>
       <c r="M74" s="14" t="n">
-        <v>0.9444444444444444</v>
+        <v>1</v>
       </c>
       <c r="N74" s="5" t="n">
-        <v>0.7777777777777778</v>
+        <v>1</v>
       </c>
       <c r="O74" s="6" t="n">
-        <v>0.7777777777777778</v>
+        <v>1</v>
       </c>
       <c r="P74" s="8">
         <f>(O74-N74)/N74</f>
@@ -6572,7 +6572,7 @@
         <v>1</v>
       </c>
       <c r="I77" t="n">
-        <v>0.425</v>
+        <v>1</v>
       </c>
       <c r="J77" t="n">
         <v>1</v>
@@ -6586,7 +6586,7 @@
         <v/>
       </c>
       <c r="M77" t="n">
-        <v>0.8888888888888888</v>
+        <v>1</v>
       </c>
       <c r="N77" t="n">
         <v>1</v>
@@ -6606,10 +6606,10 @@
         <v>0</v>
       </c>
       <c r="S77" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="T77" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="U77" s="8">
         <f>(T77-S77)/S77</f>
@@ -6665,10 +6665,10 @@
         <v>1</v>
       </c>
       <c r="N78" s="5" t="n">
-        <v>0.8888888888888888</v>
+        <v>1</v>
       </c>
       <c r="O78" s="6" t="n">
-        <v>0.8888888888888888</v>
+        <v>1</v>
       </c>
       <c r="P78" s="8">
         <f>(O78-N78)/N78</f>
@@ -6878,7 +6878,7 @@
         <v>1</v>
       </c>
       <c r="I81" t="n">
-        <v>0.4865900383141762</v>
+        <v>0.4621212121212122</v>
       </c>
       <c r="J81" t="n">
         <v>1</v>
@@ -6892,7 +6892,7 @@
         <v/>
       </c>
       <c r="M81" t="n">
-        <v>0.9444444444444444</v>
+        <v>1</v>
       </c>
       <c r="N81" t="n">
         <v>1</v>
@@ -6968,13 +6968,13 @@
         <v/>
       </c>
       <c r="M82" s="14" t="n">
-        <v>0.9444444444444444</v>
+        <v>1</v>
       </c>
       <c r="N82" s="5" t="n">
-        <v>0.8333333333333334</v>
+        <v>0.8888888888888888</v>
       </c>
       <c r="O82" s="6" t="n">
-        <v>0.8333333333333334</v>
+        <v>0.8888888888888888</v>
       </c>
       <c r="P82" s="8">
         <f>(O82-N82)/N82</f>
@@ -7184,7 +7184,7 @@
         <v>1</v>
       </c>
       <c r="I85" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J85" t="n">
         <v>1</v>
@@ -7218,10 +7218,10 @@
         <v>0</v>
       </c>
       <c r="S85" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="T85" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="U85" s="8">
         <f>(T85-S85)/S85</f>
@@ -7274,13 +7274,13 @@
         <v/>
       </c>
       <c r="M86" s="14" t="n">
-        <v>0.8333333333333334</v>
+        <v>0.9444444444444444</v>
       </c>
       <c r="N86" s="5" t="n">
-        <v>0.7777777777777778</v>
+        <v>0.5555555555555556</v>
       </c>
       <c r="O86" s="6" t="n">
-        <v>0.7777777777777778</v>
+        <v>0.5555555555555556</v>
       </c>
       <c r="P86" s="8">
         <f>(O86-N86)/N86</f>
@@ -7580,13 +7580,13 @@
         <v/>
       </c>
       <c r="M90" s="14" t="n">
-        <v>0.8333333333333334</v>
+        <v>0.8888888888888888</v>
       </c>
       <c r="N90" s="5" t="n">
-        <v>0.8333333333333334</v>
+        <v>0.8888888888888888</v>
       </c>
       <c r="O90" s="6" t="n">
-        <v>0.8333333333333334</v>
+        <v>0.8888888888888888</v>
       </c>
       <c r="P90" s="8">
         <f>(O90-N90)/N90</f>
@@ -7886,13 +7886,13 @@
         <v/>
       </c>
       <c r="M94" s="14" t="n">
-        <v>0.8333333333333334</v>
+        <v>0.9444444444444444</v>
       </c>
       <c r="N94" s="5" t="n">
-        <v>0.8333333333333334</v>
+        <v>0.9444444444444444</v>
       </c>
       <c r="O94" s="6" t="n">
-        <v>0.8333333333333334</v>
+        <v>0.9444444444444444</v>
       </c>
       <c r="P94" s="8">
         <f>(O94-N94)/N94</f>
@@ -8192,13 +8192,13 @@
         <v/>
       </c>
       <c r="M98" s="14" t="n">
-        <v>0.8333333333333334</v>
+        <v>1</v>
       </c>
       <c r="N98" s="5" t="n">
-        <v>0.8333333333333334</v>
+        <v>1</v>
       </c>
       <c r="O98" s="6" t="n">
-        <v>0.8333333333333334</v>
+        <v>1</v>
       </c>
       <c r="P98" s="8">
         <f>(O98-N98)/N98</f>
@@ -8498,13 +8498,13 @@
         <v/>
       </c>
       <c r="M102" s="14" t="n">
-        <v>0.6111111111111112</v>
+        <v>1</v>
       </c>
       <c r="N102" s="5" t="n">
-        <v>0.6111111111111112</v>
+        <v>1</v>
       </c>
       <c r="O102" s="6" t="n">
-        <v>0.6111111111111112</v>
+        <v>1</v>
       </c>
       <c r="P102" s="8">
         <f>(O102-N102)/N102</f>
@@ -8804,13 +8804,13 @@
         <v/>
       </c>
       <c r="M106" s="14" t="n">
-        <v>0.5555555555555556</v>
+        <v>1</v>
       </c>
       <c r="N106" s="5" t="n">
-        <v>0.5555555555555556</v>
+        <v>1</v>
       </c>
       <c r="O106" s="6" t="n">
-        <v>0.5555555555555556</v>
+        <v>1</v>
       </c>
       <c r="P106" s="8">
         <f>(O106-N106)/N106</f>
@@ -9110,13 +9110,13 @@
         <v/>
       </c>
       <c r="M110" s="14" t="n">
+        <v>1</v>
+      </c>
+      <c r="N110" s="5" t="n">
         <v>0.7222222222222222</v>
       </c>
-      <c r="N110" s="5" t="n">
-        <v>0.3888888888888889</v>
-      </c>
       <c r="O110" s="6" t="n">
-        <v>0.3888888888888889</v>
+        <v>0.7222222222222222</v>
       </c>
       <c r="P110" s="8">
         <f>(O110-N110)/N110</f>
@@ -9419,10 +9419,10 @@
         <v>1</v>
       </c>
       <c r="N114" s="5" t="n">
-        <v>0.3333333333333333</v>
+        <v>0.5555555555555556</v>
       </c>
       <c r="O114" s="6" t="n">
-        <v>0.3333333333333333</v>
+        <v>0.5555555555555556</v>
       </c>
       <c r="P114" s="8">
         <f>(O114-N114)/N114</f>
@@ -9708,7 +9708,7 @@
         <v>1</v>
       </c>
       <c r="I118" s="5" t="n">
-        <v>1</v>
+        <v>0.4285714285714286</v>
       </c>
       <c r="J118" s="6" t="n">
         <v>1</v>
@@ -9722,13 +9722,13 @@
         <v/>
       </c>
       <c r="M118" s="14" t="n">
-        <v>0.8333333333333334</v>
+        <v>1</v>
       </c>
       <c r="N118" s="5" t="n">
-        <v>0.8333333333333334</v>
+        <v>1</v>
       </c>
       <c r="O118" s="6" t="n">
-        <v>0.8333333333333334</v>
+        <v>1</v>
       </c>
       <c r="P118" s="8">
         <f>(O118-N118)/N118</f>
@@ -9742,10 +9742,10 @@
         <v>0</v>
       </c>
       <c r="S118" s="5" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="T118" s="6" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="U118" s="8">
         <f>(T118-S118)/S118</f>
@@ -10028,13 +10028,13 @@
         <v/>
       </c>
       <c r="M122" s="14" t="n">
-        <v>0.5555555555555556</v>
+        <v>1</v>
       </c>
       <c r="N122" s="5" t="n">
-        <v>0.5555555555555556</v>
+        <v>0.7222222222222222</v>
       </c>
       <c r="O122" s="6" t="n">
-        <v>0.5555555555555556</v>
+        <v>0.7777777777777778</v>
       </c>
       <c r="P122" s="8">
         <f>(O122-N122)/N122</f>
@@ -10048,10 +10048,10 @@
         <v>0</v>
       </c>
       <c r="S122" s="5" t="n">
-        <v>0</v>
+        <v>0.425531914893617</v>
       </c>
       <c r="T122" s="6" t="n">
-        <v>0</v>
+        <v>0.425531914893617</v>
       </c>
       <c r="U122" s="8">
         <f>(T122-S122)/S122</f>
@@ -10334,7 +10334,7 @@
         <v/>
       </c>
       <c r="M126" s="14" t="n">
-        <v>0.8333333333333334</v>
+        <v>1</v>
       </c>
       <c r="N126" s="5" t="n">
         <v>0.8888888888888888</v>
@@ -10354,10 +10354,10 @@
         <v>0</v>
       </c>
       <c r="S126" s="5" t="n">
-        <v>0</v>
+        <v>0.5904761904761905</v>
       </c>
       <c r="T126" s="6" t="n">
-        <v>0</v>
+        <v>0.5904761904761905</v>
       </c>
       <c r="U126" s="8">
         <f>(T126-S126)/S126</f>
@@ -10398,10 +10398,10 @@
         <v>1</v>
       </c>
       <c r="I127" s="4" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J127" s="8" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K127" s="8">
         <f>(J127-I127)/I127</f>
@@ -10432,10 +10432,10 @@
         <v>0</v>
       </c>
       <c r="S127" s="4" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="T127" s="8" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="U127" s="8">
         <f>(T127-S127)/S127</f>
@@ -10640,13 +10640,13 @@
         <v/>
       </c>
       <c r="M130" s="14" t="n">
-        <v>0.5555555555555556</v>
+        <v>1</v>
       </c>
       <c r="N130" s="5" t="n">
-        <v>0.5555555555555556</v>
+        <v>0.9444444444444444</v>
       </c>
       <c r="O130" s="6" t="n">
-        <v>0.5555555555555556</v>
+        <v>0.9444444444444444</v>
       </c>
       <c r="P130" s="8">
         <f>(O130-N130)/N130</f>
@@ -10660,10 +10660,10 @@
         <v>0</v>
       </c>
       <c r="S130" s="5" t="n">
-        <v>0</v>
+        <v>0.6804123711340206</v>
       </c>
       <c r="T130" s="6" t="n">
-        <v>0</v>
+        <v>0.6804123711340206</v>
       </c>
       <c r="U130" s="8">
         <f>(T130-S130)/S130</f>
@@ -10783,7 +10783,7 @@
         <v>0</v>
       </c>
       <c r="J132" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K132" s="8">
         <f>(J132-I132)/I132</f>
@@ -10946,13 +10946,13 @@
         <v/>
       </c>
       <c r="M134" s="14" t="n">
-        <v>0.6111111111111112</v>
+        <v>1</v>
       </c>
       <c r="N134" s="5" t="n">
-        <v>0.6111111111111112</v>
+        <v>0.8888888888888888</v>
       </c>
       <c r="O134" s="6" t="n">
-        <v>0.6111111111111112</v>
+        <v>0.8333333333333334</v>
       </c>
       <c r="P134" s="8">
         <f>(O134-N134)/N134</f>
@@ -10966,10 +10966,10 @@
         <v>0</v>
       </c>
       <c r="S134" s="5" t="n">
-        <v>0.05797101449275366</v>
+        <v>0.1978021978021978</v>
       </c>
       <c r="T134" s="6" t="n">
-        <v>0.05797101449275366</v>
+        <v>0.1978021978021978</v>
       </c>
       <c r="U134" s="8">
         <f>(T134-S134)/S134</f>
@@ -11089,7 +11089,7 @@
         <v>0</v>
       </c>
       <c r="J136" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K136" s="8">
         <f>(J136-I136)/I136</f>
@@ -11238,7 +11238,7 @@
         <v>1</v>
       </c>
       <c r="I138" s="5" t="n">
-        <v>1</v>
+        <v>0.3882978723404256</v>
       </c>
       <c r="J138" s="6" t="n">
         <v>1</v>
@@ -11252,7 +11252,7 @@
         <v/>
       </c>
       <c r="M138" s="14" t="n">
-        <v>0.9444444444444444</v>
+        <v>1</v>
       </c>
       <c r="N138" s="5" t="n">
         <v>1</v>
@@ -11269,13 +11269,13 @@
         <v/>
       </c>
       <c r="R138" s="14" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="S138" s="5" t="n">
-        <v>1</v>
+        <v>0.6117021276595744</v>
       </c>
       <c r="T138" s="6" t="n">
-        <v>1</v>
+        <v>0.6117021276595744</v>
       </c>
       <c r="U138" s="8">
         <f>(T138-S138)/S138</f>
@@ -11544,7 +11544,7 @@
         <v>1</v>
       </c>
       <c r="I142" s="5" t="n">
-        <v>1</v>
+        <v>0.4545454545454546</v>
       </c>
       <c r="J142" s="6" t="n">
         <v>1</v>
@@ -11558,13 +11558,13 @@
         <v/>
       </c>
       <c r="M142" s="14" t="n">
-        <v>0.8888888888888888</v>
+        <v>1</v>
       </c>
       <c r="N142" s="5" t="n">
-        <v>0.7222222222222222</v>
+        <v>1</v>
       </c>
       <c r="O142" s="6" t="n">
-        <v>0.7222222222222222</v>
+        <v>1</v>
       </c>
       <c r="P142" s="8">
         <f>(O142-N142)/N142</f>
@@ -11578,10 +11578,10 @@
         <v>0</v>
       </c>
       <c r="S142" s="5" t="n">
-        <v>0</v>
+        <v>0.5454545454545454</v>
       </c>
       <c r="T142" s="6" t="n">
-        <v>0</v>
+        <v>0.5454545454545454</v>
       </c>
       <c r="U142" s="8">
         <f>(T142-S142)/S142</f>
@@ -11698,7 +11698,7 @@
         <v>1</v>
       </c>
       <c r="I144" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J144" t="n">
         <v>1</v>
@@ -11732,10 +11732,10 @@
         <v>0</v>
       </c>
       <c r="S144" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="T144" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="U144" s="8">
         <f>(T144-S144)/S144</f>
@@ -11774,10 +11774,10 @@
         <v>1</v>
       </c>
       <c r="I145" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J145" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K145" s="8">
         <f>(J145-I145)/I145</f>
@@ -11808,10 +11808,10 @@
         <v>0</v>
       </c>
       <c r="S145" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="T145" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="U145" s="8">
         <f>(T145-S145)/S145</f>
@@ -11867,7 +11867,7 @@
         <v>1</v>
       </c>
       <c r="N146" s="5" t="n">
-        <v>1</v>
+        <v>0.9444444444444444</v>
       </c>
       <c r="O146" s="6" t="n">
         <v>1</v>
@@ -11884,10 +11884,10 @@
         <v>0</v>
       </c>
       <c r="S146" s="5" t="n">
-        <v>0.03048780487804881</v>
+        <v>0</v>
       </c>
       <c r="T146" s="6" t="n">
-        <v>0.03048780487804881</v>
+        <v>0</v>
       </c>
       <c r="U146" s="8">
         <f>(T146-S146)/S146</f>
@@ -12004,7 +12004,7 @@
         <v>1</v>
       </c>
       <c r="I148" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J148" t="n">
         <v>1</v>
@@ -12018,7 +12018,7 @@
         <v/>
       </c>
       <c r="M148" t="n">
-        <v>0.8333333333333334</v>
+        <v>1</v>
       </c>
       <c r="N148" t="n">
         <v>1</v>
@@ -12038,10 +12038,10 @@
         <v>0</v>
       </c>
       <c r="S148" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="T148" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="U148" s="8">
         <f>(T148-S148)/S148</f>
@@ -12083,7 +12083,7 @@
         <v>0</v>
       </c>
       <c r="J149" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K149" s="8">
         <f>(J149-I149)/I149</f>
@@ -12094,7 +12094,7 @@
         <v/>
       </c>
       <c r="M149" t="n">
-        <v>1</v>
+        <v>0.9444444444444444</v>
       </c>
       <c r="N149" t="n">
         <v>1</v>
@@ -12173,10 +12173,10 @@
         <v>1</v>
       </c>
       <c r="N150" s="5" t="n">
-        <v>0.8333333333333334</v>
+        <v>0.8888888888888888</v>
       </c>
       <c r="O150" s="6" t="n">
-        <v>0.8333333333333334</v>
+        <v>0.8888888888888888</v>
       </c>
       <c r="P150" s="8">
         <f>(O150-N150)/N150</f>
@@ -12187,13 +12187,13 @@
         <v/>
       </c>
       <c r="R150" s="14" t="n">
-        <v>0</v>
+        <v>0.3529411764705883</v>
       </c>
       <c r="S150" s="5" t="n">
-        <v>0.360655737704918</v>
+        <v>0.1176470588235294</v>
       </c>
       <c r="T150" s="6" t="n">
-        <v>0.360655737704918</v>
+        <v>0.1176470588235294</v>
       </c>
       <c r="U150" s="8">
         <f>(T150-S150)/S150</f>
@@ -12310,7 +12310,7 @@
         <v>1</v>
       </c>
       <c r="I152" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J152" t="n">
         <v>1</v>
@@ -12344,10 +12344,10 @@
         <v>0</v>
       </c>
       <c r="S152" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="T152" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="U152" s="8">
         <f>(T152-S152)/S152</f>
@@ -12400,7 +12400,7 @@
         <v/>
       </c>
       <c r="M153" t="n">
-        <v>1</v>
+        <v>0.9444444444444444</v>
       </c>
       <c r="N153" t="n">
         <v>1</v>
@@ -12476,13 +12476,13 @@
         <v/>
       </c>
       <c r="M154" s="14" t="n">
+        <v>1</v>
+      </c>
+      <c r="N154" s="5" t="n">
         <v>0.8888888888888888</v>
       </c>
-      <c r="N154" s="5" t="n">
-        <v>0.9444444444444444</v>
-      </c>
       <c r="O154" s="6" t="n">
-        <v>0.9444444444444444</v>
+        <v>0.8888888888888888</v>
       </c>
       <c r="P154" s="8">
         <f>(O154-N154)/N154</f>
@@ -12493,7 +12493,7 @@
         <v/>
       </c>
       <c r="R154" s="14" t="n">
-        <v>0</v>
+        <v>0.03378378378378377</v>
       </c>
       <c r="S154" s="5" t="n">
         <v>0</v>
@@ -12540,7 +12540,7 @@
         <v>1</v>
       </c>
       <c r="I155" s="4" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J155" s="8" t="n">
         <v>1</v>
@@ -12574,10 +12574,10 @@
         <v>0</v>
       </c>
       <c r="S155" s="4" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="T155" s="8" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="U155" s="8">
         <f>(T155-S155)/S155</f>
@@ -12616,7 +12616,7 @@
         <v>1</v>
       </c>
       <c r="I156" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J156" t="n">
         <v>1</v>
@@ -12630,7 +12630,7 @@
         <v/>
       </c>
       <c r="M156" t="n">
-        <v>0.9444444444444444</v>
+        <v>1</v>
       </c>
       <c r="N156" t="n">
         <v>1</v>
@@ -12650,10 +12650,10 @@
         <v>0</v>
       </c>
       <c r="S156" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="T156" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="U156" s="8">
         <f>(T156-S156)/S156</f>
@@ -12695,7 +12695,7 @@
         <v>0</v>
       </c>
       <c r="J157" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K157" s="8">
         <f>(J157-I157)/I157</f>
@@ -12768,7 +12768,7 @@
         <v>1</v>
       </c>
       <c r="I158" s="5" t="n">
-        <v>0.03571428571428581</v>
+        <v>0.1111111111111112</v>
       </c>
       <c r="J158" s="6" t="n">
         <v>1</v>
@@ -12922,7 +12922,7 @@
         <v>1</v>
       </c>
       <c r="I160" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J160" t="n">
         <v>1</v>
@@ -12936,10 +12936,10 @@
         <v/>
       </c>
       <c r="M160" t="n">
-        <v>0.9444444444444444</v>
+        <v>1</v>
       </c>
       <c r="N160" t="n">
-        <v>1</v>
+        <v>0.8888888888888888</v>
       </c>
       <c r="O160" t="n">
         <v>1</v>
@@ -12956,10 +12956,10 @@
         <v>0</v>
       </c>
       <c r="S160" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="T160" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="U160" s="8">
         <f>(T160-S160)/S160</f>
@@ -13001,7 +13001,7 @@
         <v>0</v>
       </c>
       <c r="J161" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K161" s="8">
         <f>(J161-I161)/I161</f>
@@ -13074,7 +13074,7 @@
         <v>1</v>
       </c>
       <c r="I162" s="5" t="n">
-        <v>0.09090909090909305</v>
+        <v>0.4252873563218391</v>
       </c>
       <c r="J162" s="6" t="n">
         <v>1</v>
@@ -13108,10 +13108,10 @@
         <v>0</v>
       </c>
       <c r="S162" s="5" t="n">
-        <v>1</v>
+        <v>0.5747126436781609</v>
       </c>
       <c r="T162" s="6" t="n">
-        <v>1</v>
+        <v>0.5747126436781609</v>
       </c>
       <c r="U162" s="8">
         <f>(T162-S162)/S162</f>
@@ -13228,7 +13228,7 @@
         <v>1</v>
       </c>
       <c r="I164" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J164" t="n">
         <v>1</v>
@@ -13262,10 +13262,10 @@
         <v>0</v>
       </c>
       <c r="S164" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="T164" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="U164" s="8">
         <f>(T164-S164)/S164</f>
@@ -13304,7 +13304,7 @@
         <v>1</v>
       </c>
       <c r="I165" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J165" t="n">
         <v>1</v>
@@ -13338,10 +13338,10 @@
         <v>0</v>
       </c>
       <c r="S165" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="T165" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="U165" s="8">
         <f>(T165-S165)/S165</f>
@@ -13400,7 +13400,7 @@
         <v>1</v>
       </c>
       <c r="O166" s="6" t="n">
-        <v>0.9444444444444444</v>
+        <v>1</v>
       </c>
       <c r="P166" s="8">
         <f>(O166-N166)/N166</f>

</xml_diff>

<commit_message>
templates actualisées et last code version
</commit_message>
<xml_diff>
--- a/templates/template_risk_indicators.xlsx
+++ b/templates/template_risk_indicators.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24701"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\stiss\Nextcloud\SC_DSS_SIMU\templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{38476E2A-5CC4-46B1-A1B7-1FC5BDE4FABB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C2CE400E-8A61-475A-B3D2-ED5BDF7C83D1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="223" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="227" uniqueCount="24">
   <si>
     <t>Robustesse</t>
   </si>
@@ -94,6 +94,15 @@
   </si>
   <si>
     <t>impact S1= out S1- In S1/ In S1</t>
+  </si>
+  <si>
+    <t>Class</t>
+  </si>
+  <si>
+    <t>In</t>
+  </si>
+  <si>
+    <t>Out</t>
   </si>
 </sst>
 </file>
@@ -314,7 +323,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="24">
+  <cellXfs count="29">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
@@ -333,6 +342,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="9" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="3" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -343,12 +353,72 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Pourcentage" xfId="1" builtinId="5"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="7">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC00000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -359,6 +429,55 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>28</xdr:col>
+      <xdr:colOff>160812</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>111332</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>38</xdr:col>
+      <xdr:colOff>307005</xdr:colOff>
+      <xdr:row>25</xdr:row>
+      <xdr:rowOff>12432</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Image 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{98CA093A-D8F0-4848-A445-47354178EBE7}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="15969838" y="903020"/>
+          <a:ext cx="6207557" cy="4069834"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -624,10 +743,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AC169"/>
+  <dimension ref="A1:AB169"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="L1" zoomScale="77" zoomScaleNormal="77" workbookViewId="0">
-      <selection activeCell="AD12" sqref="AD12"/>
+    <sheetView tabSelected="1" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
+      <selection activeCell="AF35" sqref="AF35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -649,52 +768,52 @@
     <col min="20" max="21" width="8.140625" style="13" bestFit="1" customWidth="1"/>
     <col min="22" max="22" width="9.85546875" style="2" customWidth="1"/>
     <col min="25" max="25" width="10.140625" style="13" customWidth="1"/>
+    <col min="26" max="28" width="9.85546875" style="13" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:29" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:28" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="3"/>
       <c r="B1" s="3"/>
-      <c r="C1" s="21" t="s">
-        <v>0</v>
-      </c>
-      <c r="D1" s="22"/>
-      <c r="E1" s="22"/>
-      <c r="F1" s="22"/>
-      <c r="G1" s="23"/>
-      <c r="H1" s="21" t="s">
+      <c r="C1" s="22" t="s">
+        <v>0</v>
+      </c>
+      <c r="D1" s="23"/>
+      <c r="E1" s="23"/>
+      <c r="F1" s="23"/>
+      <c r="G1" s="24"/>
+      <c r="H1" s="22" t="s">
         <v>1</v>
       </c>
-      <c r="I1" s="22"/>
-      <c r="J1" s="22"/>
-      <c r="K1" s="22"/>
-      <c r="L1" s="23"/>
-      <c r="M1" s="21" t="s">
+      <c r="I1" s="23"/>
+      <c r="J1" s="23"/>
+      <c r="K1" s="23"/>
+      <c r="L1" s="24"/>
+      <c r="M1" s="22" t="s">
         <v>2</v>
       </c>
-      <c r="N1" s="22"/>
-      <c r="O1" s="22"/>
-      <c r="P1" s="22"/>
-      <c r="Q1" s="23"/>
-      <c r="R1" s="21" t="s">
+      <c r="N1" s="23"/>
+      <c r="O1" s="23"/>
+      <c r="P1" s="23"/>
+      <c r="Q1" s="24"/>
+      <c r="R1" s="22" t="s">
         <v>3</v>
       </c>
-      <c r="S1" s="22"/>
-      <c r="T1" s="22"/>
-      <c r="U1" s="22"/>
-      <c r="V1" s="23"/>
-      <c r="W1" s="18" t="s">
+      <c r="S1" s="23"/>
+      <c r="T1" s="23"/>
+      <c r="U1" s="23"/>
+      <c r="V1" s="24"/>
+      <c r="W1" s="19" t="s">
         <v>4</v>
       </c>
-      <c r="X1" s="19"/>
-      <c r="Y1" s="20"/>
-      <c r="AB1" s="8" t="s">
-        <v>5</v>
-      </c>
-      <c r="AC1" s="8" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="2" spans="1:29" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="X1" s="20"/>
+      <c r="Y1" s="21"/>
+      <c r="Z1" s="26" t="s">
+        <v>21</v>
+      </c>
+      <c r="AA1" s="27"/>
+      <c r="AB1" s="28"/>
+    </row>
+    <row r="2" spans="1:28" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="14" t="s">
         <v>7</v>
       </c>
@@ -770,8 +889,17 @@
       <c r="Y2" s="15" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="3" spans="1:29" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="Z2" s="14" t="s">
+        <v>9</v>
+      </c>
+      <c r="AA2" s="18" t="s">
+        <v>22</v>
+      </c>
+      <c r="AB2" s="18" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="3" spans="1:28" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="3">
         <v>1</v>
       </c>
@@ -832,8 +960,20 @@
         <f>IF(X3&gt;0, (W3-X3)/X3, 0)</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="4" spans="1:29" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="Z3" s="25" t="str">
+        <f>IF(AND(C3&lt;0.5, H3 &gt;= 0.5,M3&gt;=0.5, R3&lt;0.5), "F",IF(AND(C3&lt;0.5, H3 &gt;= 0.5,M3&gt;=0.5, R3&gt;=0.5), "E2",IF(AND(C3&lt;0.5, H3 &gt;= 0.5,M3&lt;0.5, R3&lt;0.5), "E1",IF(AND(C3&lt;0.5, H3 &gt;= 0.5,M3&lt;0.5, R3&gt;=0.5), "D2",IF(AND(C3&lt;0.5, H3 &lt;0.5,M3&gt;=0.5, R3&lt;0.5), "D1",IF(AND(C3&lt;0.5, H3 &lt; 0.5,M3&gt;=0.5, R3&gt;=0.5), "C2",IF(AND(C3&lt;0.5, H3 &lt; 0.5,M3&lt;0.5, R3&lt;0.5), "C1",IF(AND(C3&lt;0.5, H3 &lt; 0.5,M3&lt;0.5, R3&gt;=0.5), "B","A"))))))))</f>
+        <v>C1</v>
+      </c>
+      <c r="AA3" s="25" t="str">
+        <f>IF(AND(D3&lt;0.5, I3 &gt;= 0.5,N3&gt;=0.5, S3&lt;0.5), "F",IF(AND(D3&lt;0.5, I3 &gt;= 0.5,N3&gt;=0.5, S3&gt;=0.5), "E2",IF(AND(D3&lt;0.5, I3 &gt;= 0.5,N3&lt;0.5, S3&lt;0.5), "E1",IF(AND(D3&lt;0.5, I3 &gt;= 0.5,N3&lt;0.5, S3&gt;=0.5), "D2",IF(AND(D3&lt;0.5, I3 &lt;0.5,N3&gt;=0.5, S3&lt;0.5), "D1",IF(AND(D3&lt;0.5, I3 &lt; 0.5,N3&gt;=0.5, S3&gt;=0.5), "C2",IF(AND(D3&lt;0.5, I3 &lt; 0.5,N3&lt;0.5, S3&lt;0.5), "C1",IF(AND(D3&lt;0.5, I3 &lt; 0.5,N3&lt;0.5, S3&gt;=0.5), "B","A"))))))))</f>
+        <v>C1</v>
+      </c>
+      <c r="AB3" s="25" t="str">
+        <f>IF(AND(E3&lt;0.5, J3 &gt;= 0.5,O3&gt;=0.5, T3&lt;0.5), "F",IF(AND(E3&lt;0.5, J3 &gt;= 0.5,O3&gt;=0.5, T3&gt;=0.5), "E2",IF(AND(E3&lt;0.5, J3 &gt;= 0.5,O3&lt;0.5, T3&lt;0.5), "E1",IF(AND(E3&lt;0.5, J3 &gt;= 0.5,O3&lt;0.5, T3&gt;=0.5), "D2",IF(AND(E3&lt;0.5, J3 &lt;0.5,O3&gt;=0.5, T3&lt;0.5), "D1",IF(AND(E3&lt;0.5, J3 &lt; 0.5,O3&gt;=0.5, T3&gt;=0.5), "C2",IF(AND(E3&lt;0.5, J3 &lt; 0.5,O3&lt;0.5, T3&lt;0.5), "C1",IF(AND(E3&lt;0.5, J3 &lt; 0.5,O3&lt;0.5, T3&gt;=0.5), "B","A"))))))))</f>
+        <v>C1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:28" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="1"/>
       <c r="B4" s="1" t="s">
         <v>16</v>
@@ -889,8 +1029,20 @@
         <f>IF(X4&gt;0, (W4-X4)/X4, 0)</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="5" spans="1:29" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="Z4" s="25" t="str">
+        <f>IF(AND(C4&lt;0.5, H4 &gt;= 0.5,M4&gt;=0.5, R4&lt;0.5), "F",IF(AND(C4&lt;0.5, H4 &gt;= 0.5,M4&gt;=0.5, R4&gt;=0.5), "E2",IF(AND(C4&lt;0.5, H4 &gt;= 0.5,M4&lt;0.5, R4&lt;0.5), "E1",IF(AND(C4&lt;0.5, H4 &gt;= 0.5,M4&lt;0.5, R4&gt;=0.5), "D2",IF(AND(C4&lt;0.5, H4 &lt;0.5,M4&gt;=0.5, R4&lt;0.5), "D1",IF(AND(C4&lt;0.5, H4 &lt; 0.5,M4&gt;=0.5, R4&gt;=0.5), "C2",IF(AND(C4&lt;0.5, H4 &lt; 0.5,M4&lt;0.5, R4&lt;0.5), "C1",IF(AND(C4&lt;0.5, H4 &lt; 0.5,M4&lt;0.5, R4&gt;=0.5), "B","A"))))))))</f>
+        <v>C1</v>
+      </c>
+      <c r="AA4" s="25" t="str">
+        <f>IF(AND(D4&lt;0.5, I4 &gt;= 0.5,N4&gt;=0.5, S4&lt;0.5), "F",IF(AND(D4&lt;0.5, I4 &gt;= 0.5,N4&gt;=0.5, S4&gt;=0.5), "E2",IF(AND(D4&lt;0.5, I4 &gt;= 0.5,N4&lt;0.5, S4&lt;0.5), "E1",IF(AND(D4&lt;0.5, I4 &gt;= 0.5,N4&lt;0.5, S4&gt;=0.5), "D2",IF(AND(D4&lt;0.5, I4 &lt;0.5,N4&gt;=0.5, S4&lt;0.5), "D1",IF(AND(D4&lt;0.5, I4 &lt; 0.5,N4&gt;=0.5, S4&gt;=0.5), "C2",IF(AND(D4&lt;0.5, I4 &lt; 0.5,N4&lt;0.5, S4&lt;0.5), "C1",IF(AND(D4&lt;0.5, I4 &lt; 0.5,N4&lt;0.5, S4&gt;=0.5), "B","A"))))))))</f>
+        <v>C1</v>
+      </c>
+      <c r="AB4" s="25" t="str">
+        <f>IF(AND(E4&lt;0.5, J4 &gt;= 0.5,O4&gt;=0.5, T4&lt;0.5), "F",IF(AND(E4&lt;0.5, J4 &gt;= 0.5,O4&gt;=0.5, T4&gt;=0.5), "E2",IF(AND(E4&lt;0.5, J4 &gt;= 0.5,O4&lt;0.5, T4&lt;0.5), "E1",IF(AND(E4&lt;0.5, J4 &gt;= 0.5,O4&lt;0.5, T4&gt;=0.5), "D2",IF(AND(E4&lt;0.5, J4 &lt;0.5,O4&gt;=0.5, T4&lt;0.5), "D1",IF(AND(E4&lt;0.5, J4 &lt; 0.5,O4&gt;=0.5, T4&gt;=0.5), "C2",IF(AND(E4&lt;0.5, J4 &lt; 0.5,O4&lt;0.5, T4&lt;0.5), "C1",IF(AND(E4&lt;0.5, J4 &lt; 0.5,O4&lt;0.5, T4&gt;=0.5), "B","A"))))))))</f>
+        <v>C1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:28" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="1"/>
       <c r="B5" s="1" t="s">
         <v>17</v>
@@ -946,8 +1098,20 @@
         <f>IF(X5&gt;0, (W5-X5)/X5, 0)</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="6" spans="1:29" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="Z5" s="25" t="str">
+        <f>IF(AND(C5&lt;0.5, H5 &gt;= 0.5,M5&gt;=0.5, R5&lt;0.5), "F",IF(AND(C5&lt;0.5, H5 &gt;= 0.5,M5&gt;=0.5, R5&gt;=0.5), "E2",IF(AND(C5&lt;0.5, H5 &gt;= 0.5,M5&lt;0.5, R5&lt;0.5), "E1",IF(AND(C5&lt;0.5, H5 &gt;= 0.5,M5&lt;0.5, R5&gt;=0.5), "D2",IF(AND(C5&lt;0.5, H5 &lt;0.5,M5&gt;=0.5, R5&lt;0.5), "D1",IF(AND(C5&lt;0.5, H5 &lt; 0.5,M5&gt;=0.5, R5&gt;=0.5), "C2",IF(AND(C5&lt;0.5, H5 &lt; 0.5,M5&lt;0.5, R5&lt;0.5), "C1",IF(AND(C5&lt;0.5, H5 &lt; 0.5,M5&lt;0.5, R5&gt;=0.5), "B","A"))))))))</f>
+        <v>C1</v>
+      </c>
+      <c r="AA5" s="25" t="str">
+        <f>IF(AND(D5&lt;0.5, I5 &gt;= 0.5,N5&gt;=0.5, S5&lt;0.5), "F",IF(AND(D5&lt;0.5, I5 &gt;= 0.5,N5&gt;=0.5, S5&gt;=0.5), "E2",IF(AND(D5&lt;0.5, I5 &gt;= 0.5,N5&lt;0.5, S5&lt;0.5), "E1",IF(AND(D5&lt;0.5, I5 &gt;= 0.5,N5&lt;0.5, S5&gt;=0.5), "D2",IF(AND(D5&lt;0.5, I5 &lt;0.5,N5&gt;=0.5, S5&lt;0.5), "D1",IF(AND(D5&lt;0.5, I5 &lt; 0.5,N5&gt;=0.5, S5&gt;=0.5), "C2",IF(AND(D5&lt;0.5, I5 &lt; 0.5,N5&lt;0.5, S5&lt;0.5), "C1",IF(AND(D5&lt;0.5, I5 &lt; 0.5,N5&lt;0.5, S5&gt;=0.5), "B","A"))))))))</f>
+        <v>C1</v>
+      </c>
+      <c r="AB5" s="25" t="str">
+        <f>IF(AND(E5&lt;0.5, J5 &gt;= 0.5,O5&gt;=0.5, T5&lt;0.5), "F",IF(AND(E5&lt;0.5, J5 &gt;= 0.5,O5&gt;=0.5, T5&gt;=0.5), "E2",IF(AND(E5&lt;0.5, J5 &gt;= 0.5,O5&lt;0.5, T5&lt;0.5), "E1",IF(AND(E5&lt;0.5, J5 &gt;= 0.5,O5&lt;0.5, T5&gt;=0.5), "D2",IF(AND(E5&lt;0.5, J5 &lt;0.5,O5&gt;=0.5, T5&lt;0.5), "D1",IF(AND(E5&lt;0.5, J5 &lt; 0.5,O5&gt;=0.5, T5&gt;=0.5), "C2",IF(AND(E5&lt;0.5, J5 &lt; 0.5,O5&lt;0.5, T5&lt;0.5), "C1",IF(AND(E5&lt;0.5, J5 &lt; 0.5,O5&lt;0.5, T5&gt;=0.5), "B","A"))))))))</f>
+        <v>C1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:28" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="4"/>
       <c r="B6" s="4" t="s">
         <v>18</v>
@@ -1006,8 +1170,20 @@
         <f>IF(X6&gt;0, (W6-X6)/X6, 0)</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="7" spans="1:29" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="Z6" s="25" t="str">
+        <f>IF(AND(C6&lt;0.5, H6 &gt;= 0.5,M6&gt;=0.5, R6&lt;0.5), "F",IF(AND(C6&lt;0.5, H6 &gt;= 0.5,M6&gt;=0.5, R6&gt;=0.5), "E2",IF(AND(C6&lt;0.5, H6 &gt;= 0.5,M6&lt;0.5, R6&lt;0.5), "E1",IF(AND(C6&lt;0.5, H6 &gt;= 0.5,M6&lt;0.5, R6&gt;=0.5), "D2",IF(AND(C6&lt;0.5, H6 &lt;0.5,M6&gt;=0.5, R6&lt;0.5), "D1",IF(AND(C6&lt;0.5, H6 &lt; 0.5,M6&gt;=0.5, R6&gt;=0.5), "C2",IF(AND(C6&lt;0.5, H6 &lt; 0.5,M6&lt;0.5, R6&lt;0.5), "C1",IF(AND(C6&lt;0.5, H6 &lt; 0.5,M6&lt;0.5, R6&gt;=0.5), "B","A"))))))))</f>
+        <v>C1</v>
+      </c>
+      <c r="AA6" s="25" t="str">
+        <f>IF(AND(D6&lt;0.5, I6 &gt;= 0.5,N6&gt;=0.5, S6&lt;0.5), "F",IF(AND(D6&lt;0.5, I6 &gt;= 0.5,N6&gt;=0.5, S6&gt;=0.5), "E2",IF(AND(D6&lt;0.5, I6 &gt;= 0.5,N6&lt;0.5, S6&lt;0.5), "E1",IF(AND(D6&lt;0.5, I6 &gt;= 0.5,N6&lt;0.5, S6&gt;=0.5), "D2",IF(AND(D6&lt;0.5, I6 &lt;0.5,N6&gt;=0.5, S6&lt;0.5), "D1",IF(AND(D6&lt;0.5, I6 &lt; 0.5,N6&gt;=0.5, S6&gt;=0.5), "C2",IF(AND(D6&lt;0.5, I6 &lt; 0.5,N6&lt;0.5, S6&lt;0.5), "C1",IF(AND(D6&lt;0.5, I6 &lt; 0.5,N6&lt;0.5, S6&gt;=0.5), "B","A"))))))))</f>
+        <v>C1</v>
+      </c>
+      <c r="AB6" s="25" t="str">
+        <f>IF(AND(E6&lt;0.5, J6 &gt;= 0.5,O6&gt;=0.5, T6&lt;0.5), "F",IF(AND(E6&lt;0.5, J6 &gt;= 0.5,O6&gt;=0.5, T6&gt;=0.5), "E2",IF(AND(E6&lt;0.5, J6 &gt;= 0.5,O6&lt;0.5, T6&lt;0.5), "E1",IF(AND(E6&lt;0.5, J6 &gt;= 0.5,O6&lt;0.5, T6&gt;=0.5), "D2",IF(AND(E6&lt;0.5, J6 &lt;0.5,O6&gt;=0.5, T6&lt;0.5), "D1",IF(AND(E6&lt;0.5, J6 &lt; 0.5,O6&gt;=0.5, T6&gt;=0.5), "C2",IF(AND(E6&lt;0.5, J6 &lt; 0.5,O6&lt;0.5, T6&lt;0.5), "C1",IF(AND(E6&lt;0.5, J6 &lt; 0.5,O6&lt;0.5, T6&gt;=0.5), "B","A"))))))))</f>
+        <v>C1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:28" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="3">
         <v>2</v>
       </c>
@@ -1059,8 +1235,20 @@
         <v>0</v>
       </c>
       <c r="W7" s="6"/>
-    </row>
-    <row r="8" spans="1:29" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="Z7" s="25" t="str">
+        <f>IF(AND(C7&lt;0.5, H7 &gt;= 0.5,M7&gt;=0.5, R7&lt;0.5), "F",IF(AND(C7&lt;0.5, H7 &gt;= 0.5,M7&gt;=0.5, R7&gt;=0.5), "E2",IF(AND(C7&lt;0.5, H7 &gt;= 0.5,M7&lt;0.5, R7&lt;0.5), "E1",IF(AND(C7&lt;0.5, H7 &gt;= 0.5,M7&lt;0.5, R7&gt;=0.5), "D2",IF(AND(C7&lt;0.5, H7 &lt;0.5,M7&gt;=0.5, R7&lt;0.5), "D1",IF(AND(C7&lt;0.5, H7 &lt; 0.5,M7&gt;=0.5, R7&gt;=0.5), "C2",IF(AND(C7&lt;0.5, H7 &lt; 0.5,M7&lt;0.5, R7&lt;0.5), "C1",IF(AND(C7&lt;0.5, H7 &lt; 0.5,M7&lt;0.5, R7&gt;=0.5), "B","A"))))))))</f>
+        <v>C1</v>
+      </c>
+      <c r="AA7" s="25" t="str">
+        <f>IF(AND(D7&lt;0.5, I7 &gt;= 0.5,N7&gt;=0.5, S7&lt;0.5), "F",IF(AND(D7&lt;0.5, I7 &gt;= 0.5,N7&gt;=0.5, S7&gt;=0.5), "E2",IF(AND(D7&lt;0.5, I7 &gt;= 0.5,N7&lt;0.5, S7&lt;0.5), "E1",IF(AND(D7&lt;0.5, I7 &gt;= 0.5,N7&lt;0.5, S7&gt;=0.5), "D2",IF(AND(D7&lt;0.5, I7 &lt;0.5,N7&gt;=0.5, S7&lt;0.5), "D1",IF(AND(D7&lt;0.5, I7 &lt; 0.5,N7&gt;=0.5, S7&gt;=0.5), "C2",IF(AND(D7&lt;0.5, I7 &lt; 0.5,N7&lt;0.5, S7&lt;0.5), "C1",IF(AND(D7&lt;0.5, I7 &lt; 0.5,N7&lt;0.5, S7&gt;=0.5), "B","A"))))))))</f>
+        <v>C1</v>
+      </c>
+      <c r="AB7" s="25" t="str">
+        <f>IF(AND(E7&lt;0.5, J7 &gt;= 0.5,O7&gt;=0.5, T7&lt;0.5), "F",IF(AND(E7&lt;0.5, J7 &gt;= 0.5,O7&gt;=0.5, T7&gt;=0.5), "E2",IF(AND(E7&lt;0.5, J7 &gt;= 0.5,O7&lt;0.5, T7&lt;0.5), "E1",IF(AND(E7&lt;0.5, J7 &gt;= 0.5,O7&lt;0.5, T7&gt;=0.5), "D2",IF(AND(E7&lt;0.5, J7 &lt;0.5,O7&gt;=0.5, T7&lt;0.5), "D1",IF(AND(E7&lt;0.5, J7 &lt; 0.5,O7&gt;=0.5, T7&gt;=0.5), "C2",IF(AND(E7&lt;0.5, J7 &lt; 0.5,O7&lt;0.5, T7&lt;0.5), "C1",IF(AND(E7&lt;0.5, J7 &lt; 0.5,O7&lt;0.5, T7&gt;=0.5), "B","A"))))))))</f>
+        <v>C1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:28" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="1"/>
       <c r="B8" s="1" t="s">
         <v>16</v>
@@ -1106,8 +1294,20 @@
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="9" spans="1:29" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="Z8" s="25" t="str">
+        <f>IF(AND(C8&lt;0.5, H8 &gt;= 0.5,M8&gt;=0.5, R8&lt;0.5), "F",IF(AND(C8&lt;0.5, H8 &gt;= 0.5,M8&gt;=0.5, R8&gt;=0.5), "E2",IF(AND(C8&lt;0.5, H8 &gt;= 0.5,M8&lt;0.5, R8&lt;0.5), "E1",IF(AND(C8&lt;0.5, H8 &gt;= 0.5,M8&lt;0.5, R8&gt;=0.5), "D2",IF(AND(C8&lt;0.5, H8 &lt;0.5,M8&gt;=0.5, R8&lt;0.5), "D1",IF(AND(C8&lt;0.5, H8 &lt; 0.5,M8&gt;=0.5, R8&gt;=0.5), "C2",IF(AND(C8&lt;0.5, H8 &lt; 0.5,M8&lt;0.5, R8&lt;0.5), "C1",IF(AND(C8&lt;0.5, H8 &lt; 0.5,M8&lt;0.5, R8&gt;=0.5), "B","A"))))))))</f>
+        <v>C1</v>
+      </c>
+      <c r="AA8" s="25" t="str">
+        <f>IF(AND(D8&lt;0.5, I8 &gt;= 0.5,N8&gt;=0.5, S8&lt;0.5), "F",IF(AND(D8&lt;0.5, I8 &gt;= 0.5,N8&gt;=0.5, S8&gt;=0.5), "E2",IF(AND(D8&lt;0.5, I8 &gt;= 0.5,N8&lt;0.5, S8&lt;0.5), "E1",IF(AND(D8&lt;0.5, I8 &gt;= 0.5,N8&lt;0.5, S8&gt;=0.5), "D2",IF(AND(D8&lt;0.5, I8 &lt;0.5,N8&gt;=0.5, S8&lt;0.5), "D1",IF(AND(D8&lt;0.5, I8 &lt; 0.5,N8&gt;=0.5, S8&gt;=0.5), "C2",IF(AND(D8&lt;0.5, I8 &lt; 0.5,N8&lt;0.5, S8&lt;0.5), "C1",IF(AND(D8&lt;0.5, I8 &lt; 0.5,N8&lt;0.5, S8&gt;=0.5), "B","A"))))))))</f>
+        <v>C1</v>
+      </c>
+      <c r="AB8" s="25" t="str">
+        <f>IF(AND(E8&lt;0.5, J8 &gt;= 0.5,O8&gt;=0.5, T8&lt;0.5), "F",IF(AND(E8&lt;0.5, J8 &gt;= 0.5,O8&gt;=0.5, T8&gt;=0.5), "E2",IF(AND(E8&lt;0.5, J8 &gt;= 0.5,O8&lt;0.5, T8&lt;0.5), "E1",IF(AND(E8&lt;0.5, J8 &gt;= 0.5,O8&lt;0.5, T8&gt;=0.5), "D2",IF(AND(E8&lt;0.5, J8 &lt;0.5,O8&gt;=0.5, T8&lt;0.5), "D1",IF(AND(E8&lt;0.5, J8 &lt; 0.5,O8&gt;=0.5, T8&gt;=0.5), "C2",IF(AND(E8&lt;0.5, J8 &lt; 0.5,O8&lt;0.5, T8&lt;0.5), "C1",IF(AND(E8&lt;0.5, J8 &lt; 0.5,O8&lt;0.5, T8&gt;=0.5), "B","A"))))))))</f>
+        <v>C1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:28" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="1"/>
       <c r="B9" s="1" t="s">
         <v>17</v>
@@ -1153,14 +1353,20 @@
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
-      <c r="X9" s="8" t="s">
-        <v>9</v>
-      </c>
-      <c r="Y9" s="8" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="10" spans="1:29" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="Z9" s="25" t="str">
+        <f>IF(AND(C9&lt;0.5, H9 &gt;= 0.5,M9&gt;=0.5, R9&lt;0.5), "F",IF(AND(C9&lt;0.5, H9 &gt;= 0.5,M9&gt;=0.5, R9&gt;=0.5), "E2",IF(AND(C9&lt;0.5, H9 &gt;= 0.5,M9&lt;0.5, R9&lt;0.5), "E1",IF(AND(C9&lt;0.5, H9 &gt;= 0.5,M9&lt;0.5, R9&gt;=0.5), "D2",IF(AND(C9&lt;0.5, H9 &lt;0.5,M9&gt;=0.5, R9&lt;0.5), "D1",IF(AND(C9&lt;0.5, H9 &lt; 0.5,M9&gt;=0.5, R9&gt;=0.5), "C2",IF(AND(C9&lt;0.5, H9 &lt; 0.5,M9&lt;0.5, R9&lt;0.5), "C1",IF(AND(C9&lt;0.5, H9 &lt; 0.5,M9&lt;0.5, R9&gt;=0.5), "B","A"))))))))</f>
+        <v>C1</v>
+      </c>
+      <c r="AA9" s="25" t="str">
+        <f>IF(AND(D9&lt;0.5, I9 &gt;= 0.5,N9&gt;=0.5, S9&lt;0.5), "F",IF(AND(D9&lt;0.5, I9 &gt;= 0.5,N9&gt;=0.5, S9&gt;=0.5), "E2",IF(AND(D9&lt;0.5, I9 &gt;= 0.5,N9&lt;0.5, S9&lt;0.5), "E1",IF(AND(D9&lt;0.5, I9 &gt;= 0.5,N9&lt;0.5, S9&gt;=0.5), "D2",IF(AND(D9&lt;0.5, I9 &lt;0.5,N9&gt;=0.5, S9&lt;0.5), "D1",IF(AND(D9&lt;0.5, I9 &lt; 0.5,N9&gt;=0.5, S9&gt;=0.5), "C2",IF(AND(D9&lt;0.5, I9 &lt; 0.5,N9&lt;0.5, S9&lt;0.5), "C1",IF(AND(D9&lt;0.5, I9 &lt; 0.5,N9&lt;0.5, S9&gt;=0.5), "B","A"))))))))</f>
+        <v>C1</v>
+      </c>
+      <c r="AB9" s="25" t="str">
+        <f>IF(AND(E9&lt;0.5, J9 &gt;= 0.5,O9&gt;=0.5, T9&lt;0.5), "F",IF(AND(E9&lt;0.5, J9 &gt;= 0.5,O9&gt;=0.5, T9&gt;=0.5), "E2",IF(AND(E9&lt;0.5, J9 &gt;= 0.5,O9&lt;0.5, T9&lt;0.5), "E1",IF(AND(E9&lt;0.5, J9 &gt;= 0.5,O9&lt;0.5, T9&gt;=0.5), "D2",IF(AND(E9&lt;0.5, J9 &lt;0.5,O9&gt;=0.5, T9&lt;0.5), "D1",IF(AND(E9&lt;0.5, J9 &lt; 0.5,O9&gt;=0.5, T9&gt;=0.5), "C2",IF(AND(E9&lt;0.5, J9 &lt; 0.5,O9&lt;0.5, T9&lt;0.5), "C1",IF(AND(E9&lt;0.5, J9 &lt; 0.5,O9&lt;0.5, T9&gt;=0.5), "B","A"))))))))</f>
+        <v>C1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:28" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" s="4"/>
       <c r="B10" s="4" t="s">
         <v>18</v>
@@ -1209,8 +1415,26 @@
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="11" spans="1:29" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="W10" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="X10" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="Z10" s="25" t="str">
+        <f>IF(AND(C10&lt;0.5, H10 &gt;= 0.5,M10&gt;=0.5, R10&lt;0.5), "F",IF(AND(C10&lt;0.5, H10 &gt;= 0.5,M10&gt;=0.5, R10&gt;=0.5), "E2",IF(AND(C10&lt;0.5, H10 &gt;= 0.5,M10&lt;0.5, R10&lt;0.5), "E1",IF(AND(C10&lt;0.5, H10 &gt;= 0.5,M10&lt;0.5, R10&gt;=0.5), "D2",IF(AND(C10&lt;0.5, H10 &lt;0.5,M10&gt;=0.5, R10&lt;0.5), "D1",IF(AND(C10&lt;0.5, H10 &lt; 0.5,M10&gt;=0.5, R10&gt;=0.5), "C2",IF(AND(C10&lt;0.5, H10 &lt; 0.5,M10&lt;0.5, R10&lt;0.5), "C1",IF(AND(C10&lt;0.5, H10 &lt; 0.5,M10&lt;0.5, R10&gt;=0.5), "B","A"))))))))</f>
+        <v>C1</v>
+      </c>
+      <c r="AA10" s="25" t="str">
+        <f>IF(AND(D10&lt;0.5, I10 &gt;= 0.5,N10&gt;=0.5, S10&lt;0.5), "F",IF(AND(D10&lt;0.5, I10 &gt;= 0.5,N10&gt;=0.5, S10&gt;=0.5), "E2",IF(AND(D10&lt;0.5, I10 &gt;= 0.5,N10&lt;0.5, S10&lt;0.5), "E1",IF(AND(D10&lt;0.5, I10 &gt;= 0.5,N10&lt;0.5, S10&gt;=0.5), "D2",IF(AND(D10&lt;0.5, I10 &lt;0.5,N10&gt;=0.5, S10&lt;0.5), "D1",IF(AND(D10&lt;0.5, I10 &lt; 0.5,N10&gt;=0.5, S10&gt;=0.5), "C2",IF(AND(D10&lt;0.5, I10 &lt; 0.5,N10&lt;0.5, S10&lt;0.5), "C1",IF(AND(D10&lt;0.5, I10 &lt; 0.5,N10&lt;0.5, S10&gt;=0.5), "B","A"))))))))</f>
+        <v>C1</v>
+      </c>
+      <c r="AB10" s="25" t="str">
+        <f>IF(AND(E10&lt;0.5, J10 &gt;= 0.5,O10&gt;=0.5, T10&lt;0.5), "F",IF(AND(E10&lt;0.5, J10 &gt;= 0.5,O10&gt;=0.5, T10&gt;=0.5), "E2",IF(AND(E10&lt;0.5, J10 &gt;= 0.5,O10&lt;0.5, T10&lt;0.5), "E1",IF(AND(E10&lt;0.5, J10 &gt;= 0.5,O10&lt;0.5, T10&gt;=0.5), "D2",IF(AND(E10&lt;0.5, J10 &lt;0.5,O10&gt;=0.5, T10&lt;0.5), "D1",IF(AND(E10&lt;0.5, J10 &lt; 0.5,O10&gt;=0.5, T10&gt;=0.5), "C2",IF(AND(E10&lt;0.5, J10 &lt; 0.5,O10&lt;0.5, T10&lt;0.5), "C1",IF(AND(E10&lt;0.5, J10 &lt; 0.5,O10&lt;0.5, T10&gt;=0.5), "B","A"))))))))</f>
+        <v>C1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:28" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="3">
         <v>3</v>
       </c>
@@ -1261,11 +1485,26 @@
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
-      <c r="X11" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="12" spans="1:29" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="W11" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="X11" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="Z11" s="25" t="str">
+        <f>IF(AND(C11&lt;0.5, H11 &gt;= 0.5,M11&gt;=0.5, R11&lt;0.5), "F",IF(AND(C11&lt;0.5, H11 &gt;= 0.5,M11&gt;=0.5, R11&gt;=0.5), "E2",IF(AND(C11&lt;0.5, H11 &gt;= 0.5,M11&lt;0.5, R11&lt;0.5), "E1",IF(AND(C11&lt;0.5, H11 &gt;= 0.5,M11&lt;0.5, R11&gt;=0.5), "D2",IF(AND(C11&lt;0.5, H11 &lt;0.5,M11&gt;=0.5, R11&lt;0.5), "D1",IF(AND(C11&lt;0.5, H11 &lt; 0.5,M11&gt;=0.5, R11&gt;=0.5), "C2",IF(AND(C11&lt;0.5, H11 &lt; 0.5,M11&lt;0.5, R11&lt;0.5), "C1",IF(AND(C11&lt;0.5, H11 &lt; 0.5,M11&lt;0.5, R11&gt;=0.5), "B","A"))))))))</f>
+        <v>C1</v>
+      </c>
+      <c r="AA11" s="25" t="str">
+        <f>IF(AND(D11&lt;0.5, I11 &gt;= 0.5,N11&gt;=0.5, S11&lt;0.5), "F",IF(AND(D11&lt;0.5, I11 &gt;= 0.5,N11&gt;=0.5, S11&gt;=0.5), "E2",IF(AND(D11&lt;0.5, I11 &gt;= 0.5,N11&lt;0.5, S11&lt;0.5), "E1",IF(AND(D11&lt;0.5, I11 &gt;= 0.5,N11&lt;0.5, S11&gt;=0.5), "D2",IF(AND(D11&lt;0.5, I11 &lt;0.5,N11&gt;=0.5, S11&lt;0.5), "D1",IF(AND(D11&lt;0.5, I11 &lt; 0.5,N11&gt;=0.5, S11&gt;=0.5), "C2",IF(AND(D11&lt;0.5, I11 &lt; 0.5,N11&lt;0.5, S11&lt;0.5), "C1",IF(AND(D11&lt;0.5, I11 &lt; 0.5,N11&lt;0.5, S11&gt;=0.5), "B","A"))))))))</f>
+        <v>C1</v>
+      </c>
+      <c r="AB11" s="25" t="str">
+        <f>IF(AND(E11&lt;0.5, J11 &gt;= 0.5,O11&gt;=0.5, T11&lt;0.5), "F",IF(AND(E11&lt;0.5, J11 &gt;= 0.5,O11&gt;=0.5, T11&gt;=0.5), "E2",IF(AND(E11&lt;0.5, J11 &gt;= 0.5,O11&lt;0.5, T11&lt;0.5), "E1",IF(AND(E11&lt;0.5, J11 &gt;= 0.5,O11&lt;0.5, T11&gt;=0.5), "D2",IF(AND(E11&lt;0.5, J11 &lt;0.5,O11&gt;=0.5, T11&lt;0.5), "D1",IF(AND(E11&lt;0.5, J11 &lt; 0.5,O11&gt;=0.5, T11&gt;=0.5), "C2",IF(AND(E11&lt;0.5, J11 &lt; 0.5,O11&lt;0.5, T11&lt;0.5), "C1",IF(AND(E11&lt;0.5, J11 &lt; 0.5,O11&lt;0.5, T11&gt;=0.5), "B","A"))))))))</f>
+        <v>C1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:28" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="1"/>
       <c r="B12" s="1" t="s">
         <v>16</v>
@@ -1311,8 +1550,24 @@
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="13" spans="1:29" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="W12" t="s">
+        <v>20</v>
+      </c>
+      <c r="X12" s="13"/>
+      <c r="Z12" s="25" t="str">
+        <f>IF(AND(C12&lt;0.5, H12 &gt;= 0.5,M12&gt;=0.5, R12&lt;0.5), "F",IF(AND(C12&lt;0.5, H12 &gt;= 0.5,M12&gt;=0.5, R12&gt;=0.5), "E2",IF(AND(C12&lt;0.5, H12 &gt;= 0.5,M12&lt;0.5, R12&lt;0.5), "E1",IF(AND(C12&lt;0.5, H12 &gt;= 0.5,M12&lt;0.5, R12&gt;=0.5), "D2",IF(AND(C12&lt;0.5, H12 &lt;0.5,M12&gt;=0.5, R12&lt;0.5), "D1",IF(AND(C12&lt;0.5, H12 &lt; 0.5,M12&gt;=0.5, R12&gt;=0.5), "C2",IF(AND(C12&lt;0.5, H12 &lt; 0.5,M12&lt;0.5, R12&lt;0.5), "C1",IF(AND(C12&lt;0.5, H12 &lt; 0.5,M12&lt;0.5, R12&gt;=0.5), "B","A"))))))))</f>
+        <v>C1</v>
+      </c>
+      <c r="AA12" s="25" t="str">
+        <f>IF(AND(D12&lt;0.5, I12 &gt;= 0.5,N12&gt;=0.5, S12&lt;0.5), "F",IF(AND(D12&lt;0.5, I12 &gt;= 0.5,N12&gt;=0.5, S12&gt;=0.5), "E2",IF(AND(D12&lt;0.5, I12 &gt;= 0.5,N12&lt;0.5, S12&lt;0.5), "E1",IF(AND(D12&lt;0.5, I12 &gt;= 0.5,N12&lt;0.5, S12&gt;=0.5), "D2",IF(AND(D12&lt;0.5, I12 &lt;0.5,N12&gt;=0.5, S12&lt;0.5), "D1",IF(AND(D12&lt;0.5, I12 &lt; 0.5,N12&gt;=0.5, S12&gt;=0.5), "C2",IF(AND(D12&lt;0.5, I12 &lt; 0.5,N12&lt;0.5, S12&lt;0.5), "C1",IF(AND(D12&lt;0.5, I12 &lt; 0.5,N12&lt;0.5, S12&gt;=0.5), "B","A"))))))))</f>
+        <v>C1</v>
+      </c>
+      <c r="AB12" s="25" t="str">
+        <f>IF(AND(E12&lt;0.5, J12 &gt;= 0.5,O12&gt;=0.5, T12&lt;0.5), "F",IF(AND(E12&lt;0.5, J12 &gt;= 0.5,O12&gt;=0.5, T12&gt;=0.5), "E2",IF(AND(E12&lt;0.5, J12 &gt;= 0.5,O12&lt;0.5, T12&lt;0.5), "E1",IF(AND(E12&lt;0.5, J12 &gt;= 0.5,O12&lt;0.5, T12&gt;=0.5), "D2",IF(AND(E12&lt;0.5, J12 &lt;0.5,O12&gt;=0.5, T12&lt;0.5), "D1",IF(AND(E12&lt;0.5, J12 &lt; 0.5,O12&gt;=0.5, T12&gt;=0.5), "C2",IF(AND(E12&lt;0.5, J12 &lt; 0.5,O12&lt;0.5, T12&lt;0.5), "C1",IF(AND(E12&lt;0.5, J12 &lt; 0.5,O12&lt;0.5, T12&gt;=0.5), "B","A"))))))))</f>
+        <v>C1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:28" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A13" s="1"/>
       <c r="B13" s="1" t="s">
         <v>17</v>
@@ -1358,8 +1613,20 @@
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="14" spans="1:29" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="Z13" s="25" t="str">
+        <f>IF(AND(C13&lt;0.5, H13 &gt;= 0.5,M13&gt;=0.5, R13&lt;0.5), "F",IF(AND(C13&lt;0.5, H13 &gt;= 0.5,M13&gt;=0.5, R13&gt;=0.5), "E2",IF(AND(C13&lt;0.5, H13 &gt;= 0.5,M13&lt;0.5, R13&lt;0.5), "E1",IF(AND(C13&lt;0.5, H13 &gt;= 0.5,M13&lt;0.5, R13&gt;=0.5), "D2",IF(AND(C13&lt;0.5, H13 &lt;0.5,M13&gt;=0.5, R13&lt;0.5), "D1",IF(AND(C13&lt;0.5, H13 &lt; 0.5,M13&gt;=0.5, R13&gt;=0.5), "C2",IF(AND(C13&lt;0.5, H13 &lt; 0.5,M13&lt;0.5, R13&lt;0.5), "C1",IF(AND(C13&lt;0.5, H13 &lt; 0.5,M13&lt;0.5, R13&gt;=0.5), "B","A"))))))))</f>
+        <v>C1</v>
+      </c>
+      <c r="AA13" s="25" t="str">
+        <f>IF(AND(D13&lt;0.5, I13 &gt;= 0.5,N13&gt;=0.5, S13&lt;0.5), "F",IF(AND(D13&lt;0.5, I13 &gt;= 0.5,N13&gt;=0.5, S13&gt;=0.5), "E2",IF(AND(D13&lt;0.5, I13 &gt;= 0.5,N13&lt;0.5, S13&lt;0.5), "E1",IF(AND(D13&lt;0.5, I13 &gt;= 0.5,N13&lt;0.5, S13&gt;=0.5), "D2",IF(AND(D13&lt;0.5, I13 &lt;0.5,N13&gt;=0.5, S13&lt;0.5), "D1",IF(AND(D13&lt;0.5, I13 &lt; 0.5,N13&gt;=0.5, S13&gt;=0.5), "C2",IF(AND(D13&lt;0.5, I13 &lt; 0.5,N13&lt;0.5, S13&lt;0.5), "C1",IF(AND(D13&lt;0.5, I13 &lt; 0.5,N13&lt;0.5, S13&gt;=0.5), "B","A"))))))))</f>
+        <v>C1</v>
+      </c>
+      <c r="AB13" s="25" t="str">
+        <f>IF(AND(E13&lt;0.5, J13 &gt;= 0.5,O13&gt;=0.5, T13&lt;0.5), "F",IF(AND(E13&lt;0.5, J13 &gt;= 0.5,O13&gt;=0.5, T13&gt;=0.5), "E2",IF(AND(E13&lt;0.5, J13 &gt;= 0.5,O13&lt;0.5, T13&lt;0.5), "E1",IF(AND(E13&lt;0.5, J13 &gt;= 0.5,O13&lt;0.5, T13&gt;=0.5), "D2",IF(AND(E13&lt;0.5, J13 &lt;0.5,O13&gt;=0.5, T13&lt;0.5), "D1",IF(AND(E13&lt;0.5, J13 &lt; 0.5,O13&gt;=0.5, T13&gt;=0.5), "C2",IF(AND(E13&lt;0.5, J13 &lt; 0.5,O13&lt;0.5, T13&lt;0.5), "C1",IF(AND(E13&lt;0.5, J13 &lt; 0.5,O13&lt;0.5, T13&gt;=0.5), "B","A"))))))))</f>
+        <v>C1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:28" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A14" s="4"/>
       <c r="B14" s="4" t="s">
         <v>18</v>
@@ -1408,8 +1675,20 @@
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="15" spans="1:29" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="Z14" s="25" t="str">
+        <f>IF(AND(C14&lt;0.5, H14 &gt;= 0.5,M14&gt;=0.5, R14&lt;0.5), "F",IF(AND(C14&lt;0.5, H14 &gt;= 0.5,M14&gt;=0.5, R14&gt;=0.5), "E2",IF(AND(C14&lt;0.5, H14 &gt;= 0.5,M14&lt;0.5, R14&lt;0.5), "E1",IF(AND(C14&lt;0.5, H14 &gt;= 0.5,M14&lt;0.5, R14&gt;=0.5), "D2",IF(AND(C14&lt;0.5, H14 &lt;0.5,M14&gt;=0.5, R14&lt;0.5), "D1",IF(AND(C14&lt;0.5, H14 &lt; 0.5,M14&gt;=0.5, R14&gt;=0.5), "C2",IF(AND(C14&lt;0.5, H14 &lt; 0.5,M14&lt;0.5, R14&lt;0.5), "C1",IF(AND(C14&lt;0.5, H14 &lt; 0.5,M14&lt;0.5, R14&gt;=0.5), "B","A"))))))))</f>
+        <v>C1</v>
+      </c>
+      <c r="AA14" s="25" t="str">
+        <f>IF(AND(D14&lt;0.5, I14 &gt;= 0.5,N14&gt;=0.5, S14&lt;0.5), "F",IF(AND(D14&lt;0.5, I14 &gt;= 0.5,N14&gt;=0.5, S14&gt;=0.5), "E2",IF(AND(D14&lt;0.5, I14 &gt;= 0.5,N14&lt;0.5, S14&lt;0.5), "E1",IF(AND(D14&lt;0.5, I14 &gt;= 0.5,N14&lt;0.5, S14&gt;=0.5), "D2",IF(AND(D14&lt;0.5, I14 &lt;0.5,N14&gt;=0.5, S14&lt;0.5), "D1",IF(AND(D14&lt;0.5, I14 &lt; 0.5,N14&gt;=0.5, S14&gt;=0.5), "C2",IF(AND(D14&lt;0.5, I14 &lt; 0.5,N14&lt;0.5, S14&lt;0.5), "C1",IF(AND(D14&lt;0.5, I14 &lt; 0.5,N14&lt;0.5, S14&gt;=0.5), "B","A"))))))))</f>
+        <v>C1</v>
+      </c>
+      <c r="AB14" s="25" t="str">
+        <f>IF(AND(E14&lt;0.5, J14 &gt;= 0.5,O14&gt;=0.5, T14&lt;0.5), "F",IF(AND(E14&lt;0.5, J14 &gt;= 0.5,O14&gt;=0.5, T14&gt;=0.5), "E2",IF(AND(E14&lt;0.5, J14 &gt;= 0.5,O14&lt;0.5, T14&lt;0.5), "E1",IF(AND(E14&lt;0.5, J14 &gt;= 0.5,O14&lt;0.5, T14&gt;=0.5), "D2",IF(AND(E14&lt;0.5, J14 &lt;0.5,O14&gt;=0.5, T14&lt;0.5), "D1",IF(AND(E14&lt;0.5, J14 &lt; 0.5,O14&gt;=0.5, T14&gt;=0.5), "C2",IF(AND(E14&lt;0.5, J14 &lt; 0.5,O14&lt;0.5, T14&lt;0.5), "C1",IF(AND(E14&lt;0.5, J14 &lt; 0.5,O14&lt;0.5, T14&gt;=0.5), "B","A"))))))))</f>
+        <v>C1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:28" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A15" s="3">
         <v>4</v>
       </c>
@@ -1460,8 +1739,20 @@
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="16" spans="1:29" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="Z15" s="25" t="str">
+        <f>IF(AND(C15&lt;0.5, H15 &gt;= 0.5,M15&gt;=0.5, R15&lt;0.5), "F",IF(AND(C15&lt;0.5, H15 &gt;= 0.5,M15&gt;=0.5, R15&gt;=0.5), "E2",IF(AND(C15&lt;0.5, H15 &gt;= 0.5,M15&lt;0.5, R15&lt;0.5), "E1",IF(AND(C15&lt;0.5, H15 &gt;= 0.5,M15&lt;0.5, R15&gt;=0.5), "D2",IF(AND(C15&lt;0.5, H15 &lt;0.5,M15&gt;=0.5, R15&lt;0.5), "D1",IF(AND(C15&lt;0.5, H15 &lt; 0.5,M15&gt;=0.5, R15&gt;=0.5), "C2",IF(AND(C15&lt;0.5, H15 &lt; 0.5,M15&lt;0.5, R15&lt;0.5), "C1",IF(AND(C15&lt;0.5, H15 &lt; 0.5,M15&lt;0.5, R15&gt;=0.5), "B","A"))))))))</f>
+        <v>C1</v>
+      </c>
+      <c r="AA15" s="25" t="str">
+        <f>IF(AND(D15&lt;0.5, I15 &gt;= 0.5,N15&gt;=0.5, S15&lt;0.5), "F",IF(AND(D15&lt;0.5, I15 &gt;= 0.5,N15&gt;=0.5, S15&gt;=0.5), "E2",IF(AND(D15&lt;0.5, I15 &gt;= 0.5,N15&lt;0.5, S15&lt;0.5), "E1",IF(AND(D15&lt;0.5, I15 &gt;= 0.5,N15&lt;0.5, S15&gt;=0.5), "D2",IF(AND(D15&lt;0.5, I15 &lt;0.5,N15&gt;=0.5, S15&lt;0.5), "D1",IF(AND(D15&lt;0.5, I15 &lt; 0.5,N15&gt;=0.5, S15&gt;=0.5), "C2",IF(AND(D15&lt;0.5, I15 &lt; 0.5,N15&lt;0.5, S15&lt;0.5), "C1",IF(AND(D15&lt;0.5, I15 &lt; 0.5,N15&lt;0.5, S15&gt;=0.5), "B","A"))))))))</f>
+        <v>C1</v>
+      </c>
+      <c r="AB15" s="25" t="str">
+        <f>IF(AND(E15&lt;0.5, J15 &gt;= 0.5,O15&gt;=0.5, T15&lt;0.5), "F",IF(AND(E15&lt;0.5, J15 &gt;= 0.5,O15&gt;=0.5, T15&gt;=0.5), "E2",IF(AND(E15&lt;0.5, J15 &gt;= 0.5,O15&lt;0.5, T15&lt;0.5), "E1",IF(AND(E15&lt;0.5, J15 &gt;= 0.5,O15&lt;0.5, T15&gt;=0.5), "D2",IF(AND(E15&lt;0.5, J15 &lt;0.5,O15&gt;=0.5, T15&lt;0.5), "D1",IF(AND(E15&lt;0.5, J15 &lt; 0.5,O15&gt;=0.5, T15&gt;=0.5), "C2",IF(AND(E15&lt;0.5, J15 &lt; 0.5,O15&lt;0.5, T15&lt;0.5), "C1",IF(AND(E15&lt;0.5, J15 &lt; 0.5,O15&lt;0.5, T15&gt;=0.5), "B","A"))))))))</f>
+        <v>C1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:28" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A16" s="1"/>
       <c r="B16" s="1" t="s">
         <v>16</v>
@@ -1507,8 +1798,20 @@
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="17" spans="1:22" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="Z16" s="25" t="str">
+        <f>IF(AND(C16&lt;0.5, H16 &gt;= 0.5,M16&gt;=0.5, R16&lt;0.5), "F",IF(AND(C16&lt;0.5, H16 &gt;= 0.5,M16&gt;=0.5, R16&gt;=0.5), "E2",IF(AND(C16&lt;0.5, H16 &gt;= 0.5,M16&lt;0.5, R16&lt;0.5), "E1",IF(AND(C16&lt;0.5, H16 &gt;= 0.5,M16&lt;0.5, R16&gt;=0.5), "D2",IF(AND(C16&lt;0.5, H16 &lt;0.5,M16&gt;=0.5, R16&lt;0.5), "D1",IF(AND(C16&lt;0.5, H16 &lt; 0.5,M16&gt;=0.5, R16&gt;=0.5), "C2",IF(AND(C16&lt;0.5, H16 &lt; 0.5,M16&lt;0.5, R16&lt;0.5), "C1",IF(AND(C16&lt;0.5, H16 &lt; 0.5,M16&lt;0.5, R16&gt;=0.5), "B","A"))))))))</f>
+        <v>C1</v>
+      </c>
+      <c r="AA16" s="25" t="str">
+        <f>IF(AND(D16&lt;0.5, I16 &gt;= 0.5,N16&gt;=0.5, S16&lt;0.5), "F",IF(AND(D16&lt;0.5, I16 &gt;= 0.5,N16&gt;=0.5, S16&gt;=0.5), "E2",IF(AND(D16&lt;0.5, I16 &gt;= 0.5,N16&lt;0.5, S16&lt;0.5), "E1",IF(AND(D16&lt;0.5, I16 &gt;= 0.5,N16&lt;0.5, S16&gt;=0.5), "D2",IF(AND(D16&lt;0.5, I16 &lt;0.5,N16&gt;=0.5, S16&lt;0.5), "D1",IF(AND(D16&lt;0.5, I16 &lt; 0.5,N16&gt;=0.5, S16&gt;=0.5), "C2",IF(AND(D16&lt;0.5, I16 &lt; 0.5,N16&lt;0.5, S16&lt;0.5), "C1",IF(AND(D16&lt;0.5, I16 &lt; 0.5,N16&lt;0.5, S16&gt;=0.5), "B","A"))))))))</f>
+        <v>C1</v>
+      </c>
+      <c r="AB16" s="25" t="str">
+        <f>IF(AND(E16&lt;0.5, J16 &gt;= 0.5,O16&gt;=0.5, T16&lt;0.5), "F",IF(AND(E16&lt;0.5, J16 &gt;= 0.5,O16&gt;=0.5, T16&gt;=0.5), "E2",IF(AND(E16&lt;0.5, J16 &gt;= 0.5,O16&lt;0.5, T16&lt;0.5), "E1",IF(AND(E16&lt;0.5, J16 &gt;= 0.5,O16&lt;0.5, T16&gt;=0.5), "D2",IF(AND(E16&lt;0.5, J16 &lt;0.5,O16&gt;=0.5, T16&lt;0.5), "D1",IF(AND(E16&lt;0.5, J16 &lt; 0.5,O16&gt;=0.5, T16&gt;=0.5), "C2",IF(AND(E16&lt;0.5, J16 &lt; 0.5,O16&lt;0.5, T16&lt;0.5), "C1",IF(AND(E16&lt;0.5, J16 &lt; 0.5,O16&lt;0.5, T16&gt;=0.5), "B","A"))))))))</f>
+        <v>C1</v>
+      </c>
+    </row>
+    <row r="17" spans="1:28" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A17" s="1"/>
       <c r="B17" s="1" t="s">
         <v>17</v>
@@ -1554,8 +1857,20 @@
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="18" spans="1:22" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="Z17" s="25" t="str">
+        <f>IF(AND(C17&lt;0.5, H17 &gt;= 0.5,M17&gt;=0.5, R17&lt;0.5), "F",IF(AND(C17&lt;0.5, H17 &gt;= 0.5,M17&gt;=0.5, R17&gt;=0.5), "E2",IF(AND(C17&lt;0.5, H17 &gt;= 0.5,M17&lt;0.5, R17&lt;0.5), "E1",IF(AND(C17&lt;0.5, H17 &gt;= 0.5,M17&lt;0.5, R17&gt;=0.5), "D2",IF(AND(C17&lt;0.5, H17 &lt;0.5,M17&gt;=0.5, R17&lt;0.5), "D1",IF(AND(C17&lt;0.5, H17 &lt; 0.5,M17&gt;=0.5, R17&gt;=0.5), "C2",IF(AND(C17&lt;0.5, H17 &lt; 0.5,M17&lt;0.5, R17&lt;0.5), "C1",IF(AND(C17&lt;0.5, H17 &lt; 0.5,M17&lt;0.5, R17&gt;=0.5), "B","A"))))))))</f>
+        <v>C1</v>
+      </c>
+      <c r="AA17" s="25" t="str">
+        <f>IF(AND(D17&lt;0.5, I17 &gt;= 0.5,N17&gt;=0.5, S17&lt;0.5), "F",IF(AND(D17&lt;0.5, I17 &gt;= 0.5,N17&gt;=0.5, S17&gt;=0.5), "E2",IF(AND(D17&lt;0.5, I17 &gt;= 0.5,N17&lt;0.5, S17&lt;0.5), "E1",IF(AND(D17&lt;0.5, I17 &gt;= 0.5,N17&lt;0.5, S17&gt;=0.5), "D2",IF(AND(D17&lt;0.5, I17 &lt;0.5,N17&gt;=0.5, S17&lt;0.5), "D1",IF(AND(D17&lt;0.5, I17 &lt; 0.5,N17&gt;=0.5, S17&gt;=0.5), "C2",IF(AND(D17&lt;0.5, I17 &lt; 0.5,N17&lt;0.5, S17&lt;0.5), "C1",IF(AND(D17&lt;0.5, I17 &lt; 0.5,N17&lt;0.5, S17&gt;=0.5), "B","A"))))))))</f>
+        <v>C1</v>
+      </c>
+      <c r="AB17" s="25" t="str">
+        <f>IF(AND(E17&lt;0.5, J17 &gt;= 0.5,O17&gt;=0.5, T17&lt;0.5), "F",IF(AND(E17&lt;0.5, J17 &gt;= 0.5,O17&gt;=0.5, T17&gt;=0.5), "E2",IF(AND(E17&lt;0.5, J17 &gt;= 0.5,O17&lt;0.5, T17&lt;0.5), "E1",IF(AND(E17&lt;0.5, J17 &gt;= 0.5,O17&lt;0.5, T17&gt;=0.5), "D2",IF(AND(E17&lt;0.5, J17 &lt;0.5,O17&gt;=0.5, T17&lt;0.5), "D1",IF(AND(E17&lt;0.5, J17 &lt; 0.5,O17&gt;=0.5, T17&gt;=0.5), "C2",IF(AND(E17&lt;0.5, J17 &lt; 0.5,O17&lt;0.5, T17&lt;0.5), "C1",IF(AND(E17&lt;0.5, J17 &lt; 0.5,O17&lt;0.5, T17&gt;=0.5), "B","A"))))))))</f>
+        <v>C1</v>
+      </c>
+    </row>
+    <row r="18" spans="1:28" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A18" s="4"/>
       <c r="B18" s="4" t="s">
         <v>18</v>
@@ -1604,8 +1919,20 @@
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="19" spans="1:22" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="Z18" s="25" t="str">
+        <f>IF(AND(C18&lt;0.5, H18 &gt;= 0.5,M18&gt;=0.5, R18&lt;0.5), "F",IF(AND(C18&lt;0.5, H18 &gt;= 0.5,M18&gt;=0.5, R18&gt;=0.5), "E2",IF(AND(C18&lt;0.5, H18 &gt;= 0.5,M18&lt;0.5, R18&lt;0.5), "E1",IF(AND(C18&lt;0.5, H18 &gt;= 0.5,M18&lt;0.5, R18&gt;=0.5), "D2",IF(AND(C18&lt;0.5, H18 &lt;0.5,M18&gt;=0.5, R18&lt;0.5), "D1",IF(AND(C18&lt;0.5, H18 &lt; 0.5,M18&gt;=0.5, R18&gt;=0.5), "C2",IF(AND(C18&lt;0.5, H18 &lt; 0.5,M18&lt;0.5, R18&lt;0.5), "C1",IF(AND(C18&lt;0.5, H18 &lt; 0.5,M18&lt;0.5, R18&gt;=0.5), "B","A"))))))))</f>
+        <v>C1</v>
+      </c>
+      <c r="AA18" s="25" t="str">
+        <f>IF(AND(D18&lt;0.5, I18 &gt;= 0.5,N18&gt;=0.5, S18&lt;0.5), "F",IF(AND(D18&lt;0.5, I18 &gt;= 0.5,N18&gt;=0.5, S18&gt;=0.5), "E2",IF(AND(D18&lt;0.5, I18 &gt;= 0.5,N18&lt;0.5, S18&lt;0.5), "E1",IF(AND(D18&lt;0.5, I18 &gt;= 0.5,N18&lt;0.5, S18&gt;=0.5), "D2",IF(AND(D18&lt;0.5, I18 &lt;0.5,N18&gt;=0.5, S18&lt;0.5), "D1",IF(AND(D18&lt;0.5, I18 &lt; 0.5,N18&gt;=0.5, S18&gt;=0.5), "C2",IF(AND(D18&lt;0.5, I18 &lt; 0.5,N18&lt;0.5, S18&lt;0.5), "C1",IF(AND(D18&lt;0.5, I18 &lt; 0.5,N18&lt;0.5, S18&gt;=0.5), "B","A"))))))))</f>
+        <v>C1</v>
+      </c>
+      <c r="AB18" s="25" t="str">
+        <f>IF(AND(E18&lt;0.5, J18 &gt;= 0.5,O18&gt;=0.5, T18&lt;0.5), "F",IF(AND(E18&lt;0.5, J18 &gt;= 0.5,O18&gt;=0.5, T18&gt;=0.5), "E2",IF(AND(E18&lt;0.5, J18 &gt;= 0.5,O18&lt;0.5, T18&lt;0.5), "E1",IF(AND(E18&lt;0.5, J18 &gt;= 0.5,O18&lt;0.5, T18&gt;=0.5), "D2",IF(AND(E18&lt;0.5, J18 &lt;0.5,O18&gt;=0.5, T18&lt;0.5), "D1",IF(AND(E18&lt;0.5, J18 &lt; 0.5,O18&gt;=0.5, T18&gt;=0.5), "C2",IF(AND(E18&lt;0.5, J18 &lt; 0.5,O18&lt;0.5, T18&lt;0.5), "C1",IF(AND(E18&lt;0.5, J18 &lt; 0.5,O18&lt;0.5, T18&gt;=0.5), "B","A"))))))))</f>
+        <v>C1</v>
+      </c>
+    </row>
+    <row r="19" spans="1:28" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A19" s="3">
         <v>5</v>
       </c>
@@ -1656,8 +1983,20 @@
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="20" spans="1:22" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="Z19" s="25" t="str">
+        <f>IF(AND(C19&lt;0.5, H19 &gt;= 0.5,M19&gt;=0.5, R19&lt;0.5), "F",IF(AND(C19&lt;0.5, H19 &gt;= 0.5,M19&gt;=0.5, R19&gt;=0.5), "E2",IF(AND(C19&lt;0.5, H19 &gt;= 0.5,M19&lt;0.5, R19&lt;0.5), "E1",IF(AND(C19&lt;0.5, H19 &gt;= 0.5,M19&lt;0.5, R19&gt;=0.5), "D2",IF(AND(C19&lt;0.5, H19 &lt;0.5,M19&gt;=0.5, R19&lt;0.5), "D1",IF(AND(C19&lt;0.5, H19 &lt; 0.5,M19&gt;=0.5, R19&gt;=0.5), "C2",IF(AND(C19&lt;0.5, H19 &lt; 0.5,M19&lt;0.5, R19&lt;0.5), "C1",IF(AND(C19&lt;0.5, H19 &lt; 0.5,M19&lt;0.5, R19&gt;=0.5), "B","A"))))))))</f>
+        <v>C1</v>
+      </c>
+      <c r="AA19" s="25" t="str">
+        <f>IF(AND(D19&lt;0.5, I19 &gt;= 0.5,N19&gt;=0.5, S19&lt;0.5), "F",IF(AND(D19&lt;0.5, I19 &gt;= 0.5,N19&gt;=0.5, S19&gt;=0.5), "E2",IF(AND(D19&lt;0.5, I19 &gt;= 0.5,N19&lt;0.5, S19&lt;0.5), "E1",IF(AND(D19&lt;0.5, I19 &gt;= 0.5,N19&lt;0.5, S19&gt;=0.5), "D2",IF(AND(D19&lt;0.5, I19 &lt;0.5,N19&gt;=0.5, S19&lt;0.5), "D1",IF(AND(D19&lt;0.5, I19 &lt; 0.5,N19&gt;=0.5, S19&gt;=0.5), "C2",IF(AND(D19&lt;0.5, I19 &lt; 0.5,N19&lt;0.5, S19&lt;0.5), "C1",IF(AND(D19&lt;0.5, I19 &lt; 0.5,N19&lt;0.5, S19&gt;=0.5), "B","A"))))))))</f>
+        <v>C1</v>
+      </c>
+      <c r="AB19" s="25" t="str">
+        <f>IF(AND(E19&lt;0.5, J19 &gt;= 0.5,O19&gt;=0.5, T19&lt;0.5), "F",IF(AND(E19&lt;0.5, J19 &gt;= 0.5,O19&gt;=0.5, T19&gt;=0.5), "E2",IF(AND(E19&lt;0.5, J19 &gt;= 0.5,O19&lt;0.5, T19&lt;0.5), "E1",IF(AND(E19&lt;0.5, J19 &gt;= 0.5,O19&lt;0.5, T19&gt;=0.5), "D2",IF(AND(E19&lt;0.5, J19 &lt;0.5,O19&gt;=0.5, T19&lt;0.5), "D1",IF(AND(E19&lt;0.5, J19 &lt; 0.5,O19&gt;=0.5, T19&gt;=0.5), "C2",IF(AND(E19&lt;0.5, J19 &lt; 0.5,O19&lt;0.5, T19&lt;0.5), "C1",IF(AND(E19&lt;0.5, J19 &lt; 0.5,O19&lt;0.5, T19&gt;=0.5), "B","A"))))))))</f>
+        <v>C1</v>
+      </c>
+    </row>
+    <row r="20" spans="1:28" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A20" s="1"/>
       <c r="B20" s="1" t="s">
         <v>16</v>
@@ -1703,8 +2042,20 @@
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="21" spans="1:22" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="Z20" s="25" t="str">
+        <f>IF(AND(C20&lt;0.5, H20 &gt;= 0.5,M20&gt;=0.5, R20&lt;0.5), "F",IF(AND(C20&lt;0.5, H20 &gt;= 0.5,M20&gt;=0.5, R20&gt;=0.5), "E2",IF(AND(C20&lt;0.5, H20 &gt;= 0.5,M20&lt;0.5, R20&lt;0.5), "E1",IF(AND(C20&lt;0.5, H20 &gt;= 0.5,M20&lt;0.5, R20&gt;=0.5), "D2",IF(AND(C20&lt;0.5, H20 &lt;0.5,M20&gt;=0.5, R20&lt;0.5), "D1",IF(AND(C20&lt;0.5, H20 &lt; 0.5,M20&gt;=0.5, R20&gt;=0.5), "C2",IF(AND(C20&lt;0.5, H20 &lt; 0.5,M20&lt;0.5, R20&lt;0.5), "C1",IF(AND(C20&lt;0.5, H20 &lt; 0.5,M20&lt;0.5, R20&gt;=0.5), "B","A"))))))))</f>
+        <v>C1</v>
+      </c>
+      <c r="AA20" s="25" t="str">
+        <f>IF(AND(D20&lt;0.5, I20 &gt;= 0.5,N20&gt;=0.5, S20&lt;0.5), "F",IF(AND(D20&lt;0.5, I20 &gt;= 0.5,N20&gt;=0.5, S20&gt;=0.5), "E2",IF(AND(D20&lt;0.5, I20 &gt;= 0.5,N20&lt;0.5, S20&lt;0.5), "E1",IF(AND(D20&lt;0.5, I20 &gt;= 0.5,N20&lt;0.5, S20&gt;=0.5), "D2",IF(AND(D20&lt;0.5, I20 &lt;0.5,N20&gt;=0.5, S20&lt;0.5), "D1",IF(AND(D20&lt;0.5, I20 &lt; 0.5,N20&gt;=0.5, S20&gt;=0.5), "C2",IF(AND(D20&lt;0.5, I20 &lt; 0.5,N20&lt;0.5, S20&lt;0.5), "C1",IF(AND(D20&lt;0.5, I20 &lt; 0.5,N20&lt;0.5, S20&gt;=0.5), "B","A"))))))))</f>
+        <v>C1</v>
+      </c>
+      <c r="AB20" s="25" t="str">
+        <f>IF(AND(E20&lt;0.5, J20 &gt;= 0.5,O20&gt;=0.5, T20&lt;0.5), "F",IF(AND(E20&lt;0.5, J20 &gt;= 0.5,O20&gt;=0.5, T20&gt;=0.5), "E2",IF(AND(E20&lt;0.5, J20 &gt;= 0.5,O20&lt;0.5, T20&lt;0.5), "E1",IF(AND(E20&lt;0.5, J20 &gt;= 0.5,O20&lt;0.5, T20&gt;=0.5), "D2",IF(AND(E20&lt;0.5, J20 &lt;0.5,O20&gt;=0.5, T20&lt;0.5), "D1",IF(AND(E20&lt;0.5, J20 &lt; 0.5,O20&gt;=0.5, T20&gt;=0.5), "C2",IF(AND(E20&lt;0.5, J20 &lt; 0.5,O20&lt;0.5, T20&lt;0.5), "C1",IF(AND(E20&lt;0.5, J20 &lt; 0.5,O20&lt;0.5, T20&gt;=0.5), "B","A"))))))))</f>
+        <v>C1</v>
+      </c>
+    </row>
+    <row r="21" spans="1:28" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A21" s="1"/>
       <c r="B21" s="1" t="s">
         <v>17</v>
@@ -1750,8 +2101,20 @@
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="22" spans="1:22" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="Z21" s="25" t="str">
+        <f>IF(AND(C21&lt;0.5, H21 &gt;= 0.5,M21&gt;=0.5, R21&lt;0.5), "F",IF(AND(C21&lt;0.5, H21 &gt;= 0.5,M21&gt;=0.5, R21&gt;=0.5), "E2",IF(AND(C21&lt;0.5, H21 &gt;= 0.5,M21&lt;0.5, R21&lt;0.5), "E1",IF(AND(C21&lt;0.5, H21 &gt;= 0.5,M21&lt;0.5, R21&gt;=0.5), "D2",IF(AND(C21&lt;0.5, H21 &lt;0.5,M21&gt;=0.5, R21&lt;0.5), "D1",IF(AND(C21&lt;0.5, H21 &lt; 0.5,M21&gt;=0.5, R21&gt;=0.5), "C2",IF(AND(C21&lt;0.5, H21 &lt; 0.5,M21&lt;0.5, R21&lt;0.5), "C1",IF(AND(C21&lt;0.5, H21 &lt; 0.5,M21&lt;0.5, R21&gt;=0.5), "B","A"))))))))</f>
+        <v>C1</v>
+      </c>
+      <c r="AA21" s="25" t="str">
+        <f>IF(AND(D21&lt;0.5, I21 &gt;= 0.5,N21&gt;=0.5, S21&lt;0.5), "F",IF(AND(D21&lt;0.5, I21 &gt;= 0.5,N21&gt;=0.5, S21&gt;=0.5), "E2",IF(AND(D21&lt;0.5, I21 &gt;= 0.5,N21&lt;0.5, S21&lt;0.5), "E1",IF(AND(D21&lt;0.5, I21 &gt;= 0.5,N21&lt;0.5, S21&gt;=0.5), "D2",IF(AND(D21&lt;0.5, I21 &lt;0.5,N21&gt;=0.5, S21&lt;0.5), "D1",IF(AND(D21&lt;0.5, I21 &lt; 0.5,N21&gt;=0.5, S21&gt;=0.5), "C2",IF(AND(D21&lt;0.5, I21 &lt; 0.5,N21&lt;0.5, S21&lt;0.5), "C1",IF(AND(D21&lt;0.5, I21 &lt; 0.5,N21&lt;0.5, S21&gt;=0.5), "B","A"))))))))</f>
+        <v>C1</v>
+      </c>
+      <c r="AB21" s="25" t="str">
+        <f>IF(AND(E21&lt;0.5, J21 &gt;= 0.5,O21&gt;=0.5, T21&lt;0.5), "F",IF(AND(E21&lt;0.5, J21 &gt;= 0.5,O21&gt;=0.5, T21&gt;=0.5), "E2",IF(AND(E21&lt;0.5, J21 &gt;= 0.5,O21&lt;0.5, T21&lt;0.5), "E1",IF(AND(E21&lt;0.5, J21 &gt;= 0.5,O21&lt;0.5, T21&gt;=0.5), "D2",IF(AND(E21&lt;0.5, J21 &lt;0.5,O21&gt;=0.5, T21&lt;0.5), "D1",IF(AND(E21&lt;0.5, J21 &lt; 0.5,O21&gt;=0.5, T21&gt;=0.5), "C2",IF(AND(E21&lt;0.5, J21 &lt; 0.5,O21&lt;0.5, T21&lt;0.5), "C1",IF(AND(E21&lt;0.5, J21 &lt; 0.5,O21&lt;0.5, T21&gt;=0.5), "B","A"))))))))</f>
+        <v>C1</v>
+      </c>
+    </row>
+    <row r="22" spans="1:28" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A22" s="4"/>
       <c r="B22" s="4" t="s">
         <v>18</v>
@@ -1800,8 +2163,20 @@
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="23" spans="1:22" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="Z22" s="25" t="str">
+        <f>IF(AND(C22&lt;0.5, H22 &gt;= 0.5,M22&gt;=0.5, R22&lt;0.5), "F",IF(AND(C22&lt;0.5, H22 &gt;= 0.5,M22&gt;=0.5, R22&gt;=0.5), "E2",IF(AND(C22&lt;0.5, H22 &gt;= 0.5,M22&lt;0.5, R22&lt;0.5), "E1",IF(AND(C22&lt;0.5, H22 &gt;= 0.5,M22&lt;0.5, R22&gt;=0.5), "D2",IF(AND(C22&lt;0.5, H22 &lt;0.5,M22&gt;=0.5, R22&lt;0.5), "D1",IF(AND(C22&lt;0.5, H22 &lt; 0.5,M22&gt;=0.5, R22&gt;=0.5), "C2",IF(AND(C22&lt;0.5, H22 &lt; 0.5,M22&lt;0.5, R22&lt;0.5), "C1",IF(AND(C22&lt;0.5, H22 &lt; 0.5,M22&lt;0.5, R22&gt;=0.5), "B","A"))))))))</f>
+        <v>C1</v>
+      </c>
+      <c r="AA22" s="25" t="str">
+        <f>IF(AND(D22&lt;0.5, I22 &gt;= 0.5,N22&gt;=0.5, S22&lt;0.5), "F",IF(AND(D22&lt;0.5, I22 &gt;= 0.5,N22&gt;=0.5, S22&gt;=0.5), "E2",IF(AND(D22&lt;0.5, I22 &gt;= 0.5,N22&lt;0.5, S22&lt;0.5), "E1",IF(AND(D22&lt;0.5, I22 &gt;= 0.5,N22&lt;0.5, S22&gt;=0.5), "D2",IF(AND(D22&lt;0.5, I22 &lt;0.5,N22&gt;=0.5, S22&lt;0.5), "D1",IF(AND(D22&lt;0.5, I22 &lt; 0.5,N22&gt;=0.5, S22&gt;=0.5), "C2",IF(AND(D22&lt;0.5, I22 &lt; 0.5,N22&lt;0.5, S22&lt;0.5), "C1",IF(AND(D22&lt;0.5, I22 &lt; 0.5,N22&lt;0.5, S22&gt;=0.5), "B","A"))))))))</f>
+        <v>C1</v>
+      </c>
+      <c r="AB22" s="25" t="str">
+        <f>IF(AND(E22&lt;0.5, J22 &gt;= 0.5,O22&gt;=0.5, T22&lt;0.5), "F",IF(AND(E22&lt;0.5, J22 &gt;= 0.5,O22&gt;=0.5, T22&gt;=0.5), "E2",IF(AND(E22&lt;0.5, J22 &gt;= 0.5,O22&lt;0.5, T22&lt;0.5), "E1",IF(AND(E22&lt;0.5, J22 &gt;= 0.5,O22&lt;0.5, T22&gt;=0.5), "D2",IF(AND(E22&lt;0.5, J22 &lt;0.5,O22&gt;=0.5, T22&lt;0.5), "D1",IF(AND(E22&lt;0.5, J22 &lt; 0.5,O22&gt;=0.5, T22&gt;=0.5), "C2",IF(AND(E22&lt;0.5, J22 &lt; 0.5,O22&lt;0.5, T22&lt;0.5), "C1",IF(AND(E22&lt;0.5, J22 &lt; 0.5,O22&lt;0.5, T22&gt;=0.5), "B","A"))))))))</f>
+        <v>C1</v>
+      </c>
+    </row>
+    <row r="23" spans="1:28" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A23" s="3">
         <v>6</v>
       </c>
@@ -1852,8 +2227,20 @@
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="24" spans="1:22" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="Z23" s="25" t="str">
+        <f>IF(AND(C23&lt;0.5, H23 &gt;= 0.5,M23&gt;=0.5, R23&lt;0.5), "F",IF(AND(C23&lt;0.5, H23 &gt;= 0.5,M23&gt;=0.5, R23&gt;=0.5), "E2",IF(AND(C23&lt;0.5, H23 &gt;= 0.5,M23&lt;0.5, R23&lt;0.5), "E1",IF(AND(C23&lt;0.5, H23 &gt;= 0.5,M23&lt;0.5, R23&gt;=0.5), "D2",IF(AND(C23&lt;0.5, H23 &lt;0.5,M23&gt;=0.5, R23&lt;0.5), "D1",IF(AND(C23&lt;0.5, H23 &lt; 0.5,M23&gt;=0.5, R23&gt;=0.5), "C2",IF(AND(C23&lt;0.5, H23 &lt; 0.5,M23&lt;0.5, R23&lt;0.5), "C1",IF(AND(C23&lt;0.5, H23 &lt; 0.5,M23&lt;0.5, R23&gt;=0.5), "B","A"))))))))</f>
+        <v>C1</v>
+      </c>
+      <c r="AA23" s="25" t="str">
+        <f>IF(AND(D23&lt;0.5, I23 &gt;= 0.5,N23&gt;=0.5, S23&lt;0.5), "F",IF(AND(D23&lt;0.5, I23 &gt;= 0.5,N23&gt;=0.5, S23&gt;=0.5), "E2",IF(AND(D23&lt;0.5, I23 &gt;= 0.5,N23&lt;0.5, S23&lt;0.5), "E1",IF(AND(D23&lt;0.5, I23 &gt;= 0.5,N23&lt;0.5, S23&gt;=0.5), "D2",IF(AND(D23&lt;0.5, I23 &lt;0.5,N23&gt;=0.5, S23&lt;0.5), "D1",IF(AND(D23&lt;0.5, I23 &lt; 0.5,N23&gt;=0.5, S23&gt;=0.5), "C2",IF(AND(D23&lt;0.5, I23 &lt; 0.5,N23&lt;0.5, S23&lt;0.5), "C1",IF(AND(D23&lt;0.5, I23 &lt; 0.5,N23&lt;0.5, S23&gt;=0.5), "B","A"))))))))</f>
+        <v>C1</v>
+      </c>
+      <c r="AB23" s="25" t="str">
+        <f>IF(AND(E23&lt;0.5, J23 &gt;= 0.5,O23&gt;=0.5, T23&lt;0.5), "F",IF(AND(E23&lt;0.5, J23 &gt;= 0.5,O23&gt;=0.5, T23&gt;=0.5), "E2",IF(AND(E23&lt;0.5, J23 &gt;= 0.5,O23&lt;0.5, T23&lt;0.5), "E1",IF(AND(E23&lt;0.5, J23 &gt;= 0.5,O23&lt;0.5, T23&gt;=0.5), "D2",IF(AND(E23&lt;0.5, J23 &lt;0.5,O23&gt;=0.5, T23&lt;0.5), "D1",IF(AND(E23&lt;0.5, J23 &lt; 0.5,O23&gt;=0.5, T23&gt;=0.5), "C2",IF(AND(E23&lt;0.5, J23 &lt; 0.5,O23&lt;0.5, T23&lt;0.5), "C1",IF(AND(E23&lt;0.5, J23 &lt; 0.5,O23&lt;0.5, T23&gt;=0.5), "B","A"))))))))</f>
+        <v>C1</v>
+      </c>
+    </row>
+    <row r="24" spans="1:28" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A24" s="1"/>
       <c r="B24" s="1" t="s">
         <v>16</v>
@@ -1899,8 +2286,20 @@
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="25" spans="1:22" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="Z24" s="25" t="str">
+        <f>IF(AND(C24&lt;0.5, H24 &gt;= 0.5,M24&gt;=0.5, R24&lt;0.5), "F",IF(AND(C24&lt;0.5, H24 &gt;= 0.5,M24&gt;=0.5, R24&gt;=0.5), "E2",IF(AND(C24&lt;0.5, H24 &gt;= 0.5,M24&lt;0.5, R24&lt;0.5), "E1",IF(AND(C24&lt;0.5, H24 &gt;= 0.5,M24&lt;0.5, R24&gt;=0.5), "D2",IF(AND(C24&lt;0.5, H24 &lt;0.5,M24&gt;=0.5, R24&lt;0.5), "D1",IF(AND(C24&lt;0.5, H24 &lt; 0.5,M24&gt;=0.5, R24&gt;=0.5), "C2",IF(AND(C24&lt;0.5, H24 &lt; 0.5,M24&lt;0.5, R24&lt;0.5), "C1",IF(AND(C24&lt;0.5, H24 &lt; 0.5,M24&lt;0.5, R24&gt;=0.5), "B","A"))))))))</f>
+        <v>C1</v>
+      </c>
+      <c r="AA24" s="25" t="str">
+        <f>IF(AND(D24&lt;0.5, I24 &gt;= 0.5,N24&gt;=0.5, S24&lt;0.5), "F",IF(AND(D24&lt;0.5, I24 &gt;= 0.5,N24&gt;=0.5, S24&gt;=0.5), "E2",IF(AND(D24&lt;0.5, I24 &gt;= 0.5,N24&lt;0.5, S24&lt;0.5), "E1",IF(AND(D24&lt;0.5, I24 &gt;= 0.5,N24&lt;0.5, S24&gt;=0.5), "D2",IF(AND(D24&lt;0.5, I24 &lt;0.5,N24&gt;=0.5, S24&lt;0.5), "D1",IF(AND(D24&lt;0.5, I24 &lt; 0.5,N24&gt;=0.5, S24&gt;=0.5), "C2",IF(AND(D24&lt;0.5, I24 &lt; 0.5,N24&lt;0.5, S24&lt;0.5), "C1",IF(AND(D24&lt;0.5, I24 &lt; 0.5,N24&lt;0.5, S24&gt;=0.5), "B","A"))))))))</f>
+        <v>C1</v>
+      </c>
+      <c r="AB24" s="25" t="str">
+        <f>IF(AND(E24&lt;0.5, J24 &gt;= 0.5,O24&gt;=0.5, T24&lt;0.5), "F",IF(AND(E24&lt;0.5, J24 &gt;= 0.5,O24&gt;=0.5, T24&gt;=0.5), "E2",IF(AND(E24&lt;0.5, J24 &gt;= 0.5,O24&lt;0.5, T24&lt;0.5), "E1",IF(AND(E24&lt;0.5, J24 &gt;= 0.5,O24&lt;0.5, T24&gt;=0.5), "D2",IF(AND(E24&lt;0.5, J24 &lt;0.5,O24&gt;=0.5, T24&lt;0.5), "D1",IF(AND(E24&lt;0.5, J24 &lt; 0.5,O24&gt;=0.5, T24&gt;=0.5), "C2",IF(AND(E24&lt;0.5, J24 &lt; 0.5,O24&lt;0.5, T24&lt;0.5), "C1",IF(AND(E24&lt;0.5, J24 &lt; 0.5,O24&lt;0.5, T24&gt;=0.5), "B","A"))))))))</f>
+        <v>C1</v>
+      </c>
+    </row>
+    <row r="25" spans="1:28" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A25" s="1"/>
       <c r="B25" s="1" t="s">
         <v>17</v>
@@ -1946,8 +2345,20 @@
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="26" spans="1:22" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="Z25" s="25" t="str">
+        <f>IF(AND(C25&lt;0.5, H25 &gt;= 0.5,M25&gt;=0.5, R25&lt;0.5), "F",IF(AND(C25&lt;0.5, H25 &gt;= 0.5,M25&gt;=0.5, R25&gt;=0.5), "E2",IF(AND(C25&lt;0.5, H25 &gt;= 0.5,M25&lt;0.5, R25&lt;0.5), "E1",IF(AND(C25&lt;0.5, H25 &gt;= 0.5,M25&lt;0.5, R25&gt;=0.5), "D2",IF(AND(C25&lt;0.5, H25 &lt;0.5,M25&gt;=0.5, R25&lt;0.5), "D1",IF(AND(C25&lt;0.5, H25 &lt; 0.5,M25&gt;=0.5, R25&gt;=0.5), "C2",IF(AND(C25&lt;0.5, H25 &lt; 0.5,M25&lt;0.5, R25&lt;0.5), "C1",IF(AND(C25&lt;0.5, H25 &lt; 0.5,M25&lt;0.5, R25&gt;=0.5), "B","A"))))))))</f>
+        <v>C1</v>
+      </c>
+      <c r="AA25" s="25" t="str">
+        <f>IF(AND(D25&lt;0.5, I25 &gt;= 0.5,N25&gt;=0.5, S25&lt;0.5), "F",IF(AND(D25&lt;0.5, I25 &gt;= 0.5,N25&gt;=0.5, S25&gt;=0.5), "E2",IF(AND(D25&lt;0.5, I25 &gt;= 0.5,N25&lt;0.5, S25&lt;0.5), "E1",IF(AND(D25&lt;0.5, I25 &gt;= 0.5,N25&lt;0.5, S25&gt;=0.5), "D2",IF(AND(D25&lt;0.5, I25 &lt;0.5,N25&gt;=0.5, S25&lt;0.5), "D1",IF(AND(D25&lt;0.5, I25 &lt; 0.5,N25&gt;=0.5, S25&gt;=0.5), "C2",IF(AND(D25&lt;0.5, I25 &lt; 0.5,N25&lt;0.5, S25&lt;0.5), "C1",IF(AND(D25&lt;0.5, I25 &lt; 0.5,N25&lt;0.5, S25&gt;=0.5), "B","A"))))))))</f>
+        <v>C1</v>
+      </c>
+      <c r="AB25" s="25" t="str">
+        <f>IF(AND(E25&lt;0.5, J25 &gt;= 0.5,O25&gt;=0.5, T25&lt;0.5), "F",IF(AND(E25&lt;0.5, J25 &gt;= 0.5,O25&gt;=0.5, T25&gt;=0.5), "E2",IF(AND(E25&lt;0.5, J25 &gt;= 0.5,O25&lt;0.5, T25&lt;0.5), "E1",IF(AND(E25&lt;0.5, J25 &gt;= 0.5,O25&lt;0.5, T25&gt;=0.5), "D2",IF(AND(E25&lt;0.5, J25 &lt;0.5,O25&gt;=0.5, T25&lt;0.5), "D1",IF(AND(E25&lt;0.5, J25 &lt; 0.5,O25&gt;=0.5, T25&gt;=0.5), "C2",IF(AND(E25&lt;0.5, J25 &lt; 0.5,O25&lt;0.5, T25&lt;0.5), "C1",IF(AND(E25&lt;0.5, J25 &lt; 0.5,O25&lt;0.5, T25&gt;=0.5), "B","A"))))))))</f>
+        <v>C1</v>
+      </c>
+    </row>
+    <row r="26" spans="1:28" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A26" s="4"/>
       <c r="B26" s="4" t="s">
         <v>18</v>
@@ -1996,8 +2407,20 @@
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="27" spans="1:22" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="Z26" s="25" t="str">
+        <f>IF(AND(C26&lt;0.5, H26 &gt;= 0.5,M26&gt;=0.5, R26&lt;0.5), "F",IF(AND(C26&lt;0.5, H26 &gt;= 0.5,M26&gt;=0.5, R26&gt;=0.5), "E2",IF(AND(C26&lt;0.5, H26 &gt;= 0.5,M26&lt;0.5, R26&lt;0.5), "E1",IF(AND(C26&lt;0.5, H26 &gt;= 0.5,M26&lt;0.5, R26&gt;=0.5), "D2",IF(AND(C26&lt;0.5, H26 &lt;0.5,M26&gt;=0.5, R26&lt;0.5), "D1",IF(AND(C26&lt;0.5, H26 &lt; 0.5,M26&gt;=0.5, R26&gt;=0.5), "C2",IF(AND(C26&lt;0.5, H26 &lt; 0.5,M26&lt;0.5, R26&lt;0.5), "C1",IF(AND(C26&lt;0.5, H26 &lt; 0.5,M26&lt;0.5, R26&gt;=0.5), "B","A"))))))))</f>
+        <v>C1</v>
+      </c>
+      <c r="AA26" s="25" t="str">
+        <f>IF(AND(D26&lt;0.5, I26 &gt;= 0.5,N26&gt;=0.5, S26&lt;0.5), "F",IF(AND(D26&lt;0.5, I26 &gt;= 0.5,N26&gt;=0.5, S26&gt;=0.5), "E2",IF(AND(D26&lt;0.5, I26 &gt;= 0.5,N26&lt;0.5, S26&lt;0.5), "E1",IF(AND(D26&lt;0.5, I26 &gt;= 0.5,N26&lt;0.5, S26&gt;=0.5), "D2",IF(AND(D26&lt;0.5, I26 &lt;0.5,N26&gt;=0.5, S26&lt;0.5), "D1",IF(AND(D26&lt;0.5, I26 &lt; 0.5,N26&gt;=0.5, S26&gt;=0.5), "C2",IF(AND(D26&lt;0.5, I26 &lt; 0.5,N26&lt;0.5, S26&lt;0.5), "C1",IF(AND(D26&lt;0.5, I26 &lt; 0.5,N26&lt;0.5, S26&gt;=0.5), "B","A"))))))))</f>
+        <v>C1</v>
+      </c>
+      <c r="AB26" s="25" t="str">
+        <f>IF(AND(E26&lt;0.5, J26 &gt;= 0.5,O26&gt;=0.5, T26&lt;0.5), "F",IF(AND(E26&lt;0.5, J26 &gt;= 0.5,O26&gt;=0.5, T26&gt;=0.5), "E2",IF(AND(E26&lt;0.5, J26 &gt;= 0.5,O26&lt;0.5, T26&lt;0.5), "E1",IF(AND(E26&lt;0.5, J26 &gt;= 0.5,O26&lt;0.5, T26&gt;=0.5), "D2",IF(AND(E26&lt;0.5, J26 &lt;0.5,O26&gt;=0.5, T26&lt;0.5), "D1",IF(AND(E26&lt;0.5, J26 &lt; 0.5,O26&gt;=0.5, T26&gt;=0.5), "C2",IF(AND(E26&lt;0.5, J26 &lt; 0.5,O26&lt;0.5, T26&lt;0.5), "C1",IF(AND(E26&lt;0.5, J26 &lt; 0.5,O26&lt;0.5, T26&gt;=0.5), "B","A"))))))))</f>
+        <v>C1</v>
+      </c>
+    </row>
+    <row r="27" spans="1:28" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A27" s="3">
         <v>7</v>
       </c>
@@ -2048,8 +2471,20 @@
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="28" spans="1:22" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="Z27" s="25" t="str">
+        <f>IF(AND(C27&lt;0.5, H27 &gt;= 0.5,M27&gt;=0.5, R27&lt;0.5), "F",IF(AND(C27&lt;0.5, H27 &gt;= 0.5,M27&gt;=0.5, R27&gt;=0.5), "E2",IF(AND(C27&lt;0.5, H27 &gt;= 0.5,M27&lt;0.5, R27&lt;0.5), "E1",IF(AND(C27&lt;0.5, H27 &gt;= 0.5,M27&lt;0.5, R27&gt;=0.5), "D2",IF(AND(C27&lt;0.5, H27 &lt;0.5,M27&gt;=0.5, R27&lt;0.5), "D1",IF(AND(C27&lt;0.5, H27 &lt; 0.5,M27&gt;=0.5, R27&gt;=0.5), "C2",IF(AND(C27&lt;0.5, H27 &lt; 0.5,M27&lt;0.5, R27&lt;0.5), "C1",IF(AND(C27&lt;0.5, H27 &lt; 0.5,M27&lt;0.5, R27&gt;=0.5), "B","A"))))))))</f>
+        <v>C1</v>
+      </c>
+      <c r="AA27" s="25" t="str">
+        <f>IF(AND(D27&lt;0.5, I27 &gt;= 0.5,N27&gt;=0.5, S27&lt;0.5), "F",IF(AND(D27&lt;0.5, I27 &gt;= 0.5,N27&gt;=0.5, S27&gt;=0.5), "E2",IF(AND(D27&lt;0.5, I27 &gt;= 0.5,N27&lt;0.5, S27&lt;0.5), "E1",IF(AND(D27&lt;0.5, I27 &gt;= 0.5,N27&lt;0.5, S27&gt;=0.5), "D2",IF(AND(D27&lt;0.5, I27 &lt;0.5,N27&gt;=0.5, S27&lt;0.5), "D1",IF(AND(D27&lt;0.5, I27 &lt; 0.5,N27&gt;=0.5, S27&gt;=0.5), "C2",IF(AND(D27&lt;0.5, I27 &lt; 0.5,N27&lt;0.5, S27&lt;0.5), "C1",IF(AND(D27&lt;0.5, I27 &lt; 0.5,N27&lt;0.5, S27&gt;=0.5), "B","A"))))))))</f>
+        <v>C1</v>
+      </c>
+      <c r="AB27" s="25" t="str">
+        <f>IF(AND(E27&lt;0.5, J27 &gt;= 0.5,O27&gt;=0.5, T27&lt;0.5), "F",IF(AND(E27&lt;0.5, J27 &gt;= 0.5,O27&gt;=0.5, T27&gt;=0.5), "E2",IF(AND(E27&lt;0.5, J27 &gt;= 0.5,O27&lt;0.5, T27&lt;0.5), "E1",IF(AND(E27&lt;0.5, J27 &gt;= 0.5,O27&lt;0.5, T27&gt;=0.5), "D2",IF(AND(E27&lt;0.5, J27 &lt;0.5,O27&gt;=0.5, T27&lt;0.5), "D1",IF(AND(E27&lt;0.5, J27 &lt; 0.5,O27&gt;=0.5, T27&gt;=0.5), "C2",IF(AND(E27&lt;0.5, J27 &lt; 0.5,O27&lt;0.5, T27&lt;0.5), "C1",IF(AND(E27&lt;0.5, J27 &lt; 0.5,O27&lt;0.5, T27&gt;=0.5), "B","A"))))))))</f>
+        <v>C1</v>
+      </c>
+    </row>
+    <row r="28" spans="1:28" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A28" s="1"/>
       <c r="B28" s="1" t="s">
         <v>16</v>
@@ -2095,8 +2530,20 @@
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="29" spans="1:22" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="Z28" s="25" t="str">
+        <f>IF(AND(C28&lt;0.5, H28 &gt;= 0.5,M28&gt;=0.5, R28&lt;0.5), "F",IF(AND(C28&lt;0.5, H28 &gt;= 0.5,M28&gt;=0.5, R28&gt;=0.5), "E2",IF(AND(C28&lt;0.5, H28 &gt;= 0.5,M28&lt;0.5, R28&lt;0.5), "E1",IF(AND(C28&lt;0.5, H28 &gt;= 0.5,M28&lt;0.5, R28&gt;=0.5), "D2",IF(AND(C28&lt;0.5, H28 &lt;0.5,M28&gt;=0.5, R28&lt;0.5), "D1",IF(AND(C28&lt;0.5, H28 &lt; 0.5,M28&gt;=0.5, R28&gt;=0.5), "C2",IF(AND(C28&lt;0.5, H28 &lt; 0.5,M28&lt;0.5, R28&lt;0.5), "C1",IF(AND(C28&lt;0.5, H28 &lt; 0.5,M28&lt;0.5, R28&gt;=0.5), "B","A"))))))))</f>
+        <v>C1</v>
+      </c>
+      <c r="AA28" s="25" t="str">
+        <f>IF(AND(D28&lt;0.5, I28 &gt;= 0.5,N28&gt;=0.5, S28&lt;0.5), "F",IF(AND(D28&lt;0.5, I28 &gt;= 0.5,N28&gt;=0.5, S28&gt;=0.5), "E2",IF(AND(D28&lt;0.5, I28 &gt;= 0.5,N28&lt;0.5, S28&lt;0.5), "E1",IF(AND(D28&lt;0.5, I28 &gt;= 0.5,N28&lt;0.5, S28&gt;=0.5), "D2",IF(AND(D28&lt;0.5, I28 &lt;0.5,N28&gt;=0.5, S28&lt;0.5), "D1",IF(AND(D28&lt;0.5, I28 &lt; 0.5,N28&gt;=0.5, S28&gt;=0.5), "C2",IF(AND(D28&lt;0.5, I28 &lt; 0.5,N28&lt;0.5, S28&lt;0.5), "C1",IF(AND(D28&lt;0.5, I28 &lt; 0.5,N28&lt;0.5, S28&gt;=0.5), "B","A"))))))))</f>
+        <v>C1</v>
+      </c>
+      <c r="AB28" s="25" t="str">
+        <f>IF(AND(E28&lt;0.5, J28 &gt;= 0.5,O28&gt;=0.5, T28&lt;0.5), "F",IF(AND(E28&lt;0.5, J28 &gt;= 0.5,O28&gt;=0.5, T28&gt;=0.5), "E2",IF(AND(E28&lt;0.5, J28 &gt;= 0.5,O28&lt;0.5, T28&lt;0.5), "E1",IF(AND(E28&lt;0.5, J28 &gt;= 0.5,O28&lt;0.5, T28&gt;=0.5), "D2",IF(AND(E28&lt;0.5, J28 &lt;0.5,O28&gt;=0.5, T28&lt;0.5), "D1",IF(AND(E28&lt;0.5, J28 &lt; 0.5,O28&gt;=0.5, T28&gt;=0.5), "C2",IF(AND(E28&lt;0.5, J28 &lt; 0.5,O28&lt;0.5, T28&lt;0.5), "C1",IF(AND(E28&lt;0.5, J28 &lt; 0.5,O28&lt;0.5, T28&gt;=0.5), "B","A"))))))))</f>
+        <v>C1</v>
+      </c>
+    </row>
+    <row r="29" spans="1:28" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A29" s="1"/>
       <c r="B29" s="1" t="s">
         <v>17</v>
@@ -2142,8 +2589,20 @@
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="30" spans="1:22" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="Z29" s="25" t="str">
+        <f>IF(AND(C29&lt;0.5, H29 &gt;= 0.5,M29&gt;=0.5, R29&lt;0.5), "F",IF(AND(C29&lt;0.5, H29 &gt;= 0.5,M29&gt;=0.5, R29&gt;=0.5), "E2",IF(AND(C29&lt;0.5, H29 &gt;= 0.5,M29&lt;0.5, R29&lt;0.5), "E1",IF(AND(C29&lt;0.5, H29 &gt;= 0.5,M29&lt;0.5, R29&gt;=0.5), "D2",IF(AND(C29&lt;0.5, H29 &lt;0.5,M29&gt;=0.5, R29&lt;0.5), "D1",IF(AND(C29&lt;0.5, H29 &lt; 0.5,M29&gt;=0.5, R29&gt;=0.5), "C2",IF(AND(C29&lt;0.5, H29 &lt; 0.5,M29&lt;0.5, R29&lt;0.5), "C1",IF(AND(C29&lt;0.5, H29 &lt; 0.5,M29&lt;0.5, R29&gt;=0.5), "B","A"))))))))</f>
+        <v>C1</v>
+      </c>
+      <c r="AA29" s="25" t="str">
+        <f>IF(AND(D29&lt;0.5, I29 &gt;= 0.5,N29&gt;=0.5, S29&lt;0.5), "F",IF(AND(D29&lt;0.5, I29 &gt;= 0.5,N29&gt;=0.5, S29&gt;=0.5), "E2",IF(AND(D29&lt;0.5, I29 &gt;= 0.5,N29&lt;0.5, S29&lt;0.5), "E1",IF(AND(D29&lt;0.5, I29 &gt;= 0.5,N29&lt;0.5, S29&gt;=0.5), "D2",IF(AND(D29&lt;0.5, I29 &lt;0.5,N29&gt;=0.5, S29&lt;0.5), "D1",IF(AND(D29&lt;0.5, I29 &lt; 0.5,N29&gt;=0.5, S29&gt;=0.5), "C2",IF(AND(D29&lt;0.5, I29 &lt; 0.5,N29&lt;0.5, S29&lt;0.5), "C1",IF(AND(D29&lt;0.5, I29 &lt; 0.5,N29&lt;0.5, S29&gt;=0.5), "B","A"))))))))</f>
+        <v>C1</v>
+      </c>
+      <c r="AB29" s="25" t="str">
+        <f>IF(AND(E29&lt;0.5, J29 &gt;= 0.5,O29&gt;=0.5, T29&lt;0.5), "F",IF(AND(E29&lt;0.5, J29 &gt;= 0.5,O29&gt;=0.5, T29&gt;=0.5), "E2",IF(AND(E29&lt;0.5, J29 &gt;= 0.5,O29&lt;0.5, T29&lt;0.5), "E1",IF(AND(E29&lt;0.5, J29 &gt;= 0.5,O29&lt;0.5, T29&gt;=0.5), "D2",IF(AND(E29&lt;0.5, J29 &lt;0.5,O29&gt;=0.5, T29&lt;0.5), "D1",IF(AND(E29&lt;0.5, J29 &lt; 0.5,O29&gt;=0.5, T29&gt;=0.5), "C2",IF(AND(E29&lt;0.5, J29 &lt; 0.5,O29&lt;0.5, T29&lt;0.5), "C1",IF(AND(E29&lt;0.5, J29 &lt; 0.5,O29&lt;0.5, T29&gt;=0.5), "B","A"))))))))</f>
+        <v>C1</v>
+      </c>
+    </row>
+    <row r="30" spans="1:28" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A30" s="4"/>
       <c r="B30" s="4" t="s">
         <v>18</v>
@@ -2192,8 +2651,20 @@
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="31" spans="1:22" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="Z30" s="25" t="str">
+        <f>IF(AND(C30&lt;0.5, H30 &gt;= 0.5,M30&gt;=0.5, R30&lt;0.5), "F",IF(AND(C30&lt;0.5, H30 &gt;= 0.5,M30&gt;=0.5, R30&gt;=0.5), "E2",IF(AND(C30&lt;0.5, H30 &gt;= 0.5,M30&lt;0.5, R30&lt;0.5), "E1",IF(AND(C30&lt;0.5, H30 &gt;= 0.5,M30&lt;0.5, R30&gt;=0.5), "D2",IF(AND(C30&lt;0.5, H30 &lt;0.5,M30&gt;=0.5, R30&lt;0.5), "D1",IF(AND(C30&lt;0.5, H30 &lt; 0.5,M30&gt;=0.5, R30&gt;=0.5), "C2",IF(AND(C30&lt;0.5, H30 &lt; 0.5,M30&lt;0.5, R30&lt;0.5), "C1",IF(AND(C30&lt;0.5, H30 &lt; 0.5,M30&lt;0.5, R30&gt;=0.5), "B","A"))))))))</f>
+        <v>C1</v>
+      </c>
+      <c r="AA30" s="25" t="str">
+        <f>IF(AND(D30&lt;0.5, I30 &gt;= 0.5,N30&gt;=0.5, S30&lt;0.5), "F",IF(AND(D30&lt;0.5, I30 &gt;= 0.5,N30&gt;=0.5, S30&gt;=0.5), "E2",IF(AND(D30&lt;0.5, I30 &gt;= 0.5,N30&lt;0.5, S30&lt;0.5), "E1",IF(AND(D30&lt;0.5, I30 &gt;= 0.5,N30&lt;0.5, S30&gt;=0.5), "D2",IF(AND(D30&lt;0.5, I30 &lt;0.5,N30&gt;=0.5, S30&lt;0.5), "D1",IF(AND(D30&lt;0.5, I30 &lt; 0.5,N30&gt;=0.5, S30&gt;=0.5), "C2",IF(AND(D30&lt;0.5, I30 &lt; 0.5,N30&lt;0.5, S30&lt;0.5), "C1",IF(AND(D30&lt;0.5, I30 &lt; 0.5,N30&lt;0.5, S30&gt;=0.5), "B","A"))))))))</f>
+        <v>C1</v>
+      </c>
+      <c r="AB30" s="25" t="str">
+        <f>IF(AND(E30&lt;0.5, J30 &gt;= 0.5,O30&gt;=0.5, T30&lt;0.5), "F",IF(AND(E30&lt;0.5, J30 &gt;= 0.5,O30&gt;=0.5, T30&gt;=0.5), "E2",IF(AND(E30&lt;0.5, J30 &gt;= 0.5,O30&lt;0.5, T30&lt;0.5), "E1",IF(AND(E30&lt;0.5, J30 &gt;= 0.5,O30&lt;0.5, T30&gt;=0.5), "D2",IF(AND(E30&lt;0.5, J30 &lt;0.5,O30&gt;=0.5, T30&lt;0.5), "D1",IF(AND(E30&lt;0.5, J30 &lt; 0.5,O30&gt;=0.5, T30&gt;=0.5), "C2",IF(AND(E30&lt;0.5, J30 &lt; 0.5,O30&lt;0.5, T30&lt;0.5), "C1",IF(AND(E30&lt;0.5, J30 &lt; 0.5,O30&lt;0.5, T30&gt;=0.5), "B","A"))))))))</f>
+        <v>C1</v>
+      </c>
+    </row>
+    <row r="31" spans="1:28" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A31" s="3">
         <v>8</v>
       </c>
@@ -2244,8 +2715,20 @@
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="32" spans="1:22" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="Z31" s="25" t="str">
+        <f>IF(AND(C31&lt;0.5, H31 &gt;= 0.5,M31&gt;=0.5, R31&lt;0.5), "F",IF(AND(C31&lt;0.5, H31 &gt;= 0.5,M31&gt;=0.5, R31&gt;=0.5), "E2",IF(AND(C31&lt;0.5, H31 &gt;= 0.5,M31&lt;0.5, R31&lt;0.5), "E1",IF(AND(C31&lt;0.5, H31 &gt;= 0.5,M31&lt;0.5, R31&gt;=0.5), "D2",IF(AND(C31&lt;0.5, H31 &lt;0.5,M31&gt;=0.5, R31&lt;0.5), "D1",IF(AND(C31&lt;0.5, H31 &lt; 0.5,M31&gt;=0.5, R31&gt;=0.5), "C2",IF(AND(C31&lt;0.5, H31 &lt; 0.5,M31&lt;0.5, R31&lt;0.5), "C1",IF(AND(C31&lt;0.5, H31 &lt; 0.5,M31&lt;0.5, R31&gt;=0.5), "B","A"))))))))</f>
+        <v>C1</v>
+      </c>
+      <c r="AA31" s="25" t="str">
+        <f>IF(AND(D31&lt;0.5, I31 &gt;= 0.5,N31&gt;=0.5, S31&lt;0.5), "F",IF(AND(D31&lt;0.5, I31 &gt;= 0.5,N31&gt;=0.5, S31&gt;=0.5), "E2",IF(AND(D31&lt;0.5, I31 &gt;= 0.5,N31&lt;0.5, S31&lt;0.5), "E1",IF(AND(D31&lt;0.5, I31 &gt;= 0.5,N31&lt;0.5, S31&gt;=0.5), "D2",IF(AND(D31&lt;0.5, I31 &lt;0.5,N31&gt;=0.5, S31&lt;0.5), "D1",IF(AND(D31&lt;0.5, I31 &lt; 0.5,N31&gt;=0.5, S31&gt;=0.5), "C2",IF(AND(D31&lt;0.5, I31 &lt; 0.5,N31&lt;0.5, S31&lt;0.5), "C1",IF(AND(D31&lt;0.5, I31 &lt; 0.5,N31&lt;0.5, S31&gt;=0.5), "B","A"))))))))</f>
+        <v>C1</v>
+      </c>
+      <c r="AB31" s="25" t="str">
+        <f>IF(AND(E31&lt;0.5, J31 &gt;= 0.5,O31&gt;=0.5, T31&lt;0.5), "F",IF(AND(E31&lt;0.5, J31 &gt;= 0.5,O31&gt;=0.5, T31&gt;=0.5), "E2",IF(AND(E31&lt;0.5, J31 &gt;= 0.5,O31&lt;0.5, T31&lt;0.5), "E1",IF(AND(E31&lt;0.5, J31 &gt;= 0.5,O31&lt;0.5, T31&gt;=0.5), "D2",IF(AND(E31&lt;0.5, J31 &lt;0.5,O31&gt;=0.5, T31&lt;0.5), "D1",IF(AND(E31&lt;0.5, J31 &lt; 0.5,O31&gt;=0.5, T31&gt;=0.5), "C2",IF(AND(E31&lt;0.5, J31 &lt; 0.5,O31&lt;0.5, T31&lt;0.5), "C1",IF(AND(E31&lt;0.5, J31 &lt; 0.5,O31&lt;0.5, T31&gt;=0.5), "B","A"))))))))</f>
+        <v>C1</v>
+      </c>
+    </row>
+    <row r="32" spans="1:28" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A32" s="1"/>
       <c r="B32" s="1" t="s">
         <v>16</v>
@@ -2291,8 +2774,20 @@
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="33" spans="1:22" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="Z32" s="25" t="str">
+        <f>IF(AND(C32&lt;0.5, H32 &gt;= 0.5,M32&gt;=0.5, R32&lt;0.5), "F",IF(AND(C32&lt;0.5, H32 &gt;= 0.5,M32&gt;=0.5, R32&gt;=0.5), "E2",IF(AND(C32&lt;0.5, H32 &gt;= 0.5,M32&lt;0.5, R32&lt;0.5), "E1",IF(AND(C32&lt;0.5, H32 &gt;= 0.5,M32&lt;0.5, R32&gt;=0.5), "D2",IF(AND(C32&lt;0.5, H32 &lt;0.5,M32&gt;=0.5, R32&lt;0.5), "D1",IF(AND(C32&lt;0.5, H32 &lt; 0.5,M32&gt;=0.5, R32&gt;=0.5), "C2",IF(AND(C32&lt;0.5, H32 &lt; 0.5,M32&lt;0.5, R32&lt;0.5), "C1",IF(AND(C32&lt;0.5, H32 &lt; 0.5,M32&lt;0.5, R32&gt;=0.5), "B","A"))))))))</f>
+        <v>C1</v>
+      </c>
+      <c r="AA32" s="25" t="str">
+        <f>IF(AND(D32&lt;0.5, I32 &gt;= 0.5,N32&gt;=0.5, S32&lt;0.5), "F",IF(AND(D32&lt;0.5, I32 &gt;= 0.5,N32&gt;=0.5, S32&gt;=0.5), "E2",IF(AND(D32&lt;0.5, I32 &gt;= 0.5,N32&lt;0.5, S32&lt;0.5), "E1",IF(AND(D32&lt;0.5, I32 &gt;= 0.5,N32&lt;0.5, S32&gt;=0.5), "D2",IF(AND(D32&lt;0.5, I32 &lt;0.5,N32&gt;=0.5, S32&lt;0.5), "D1",IF(AND(D32&lt;0.5, I32 &lt; 0.5,N32&gt;=0.5, S32&gt;=0.5), "C2",IF(AND(D32&lt;0.5, I32 &lt; 0.5,N32&lt;0.5, S32&lt;0.5), "C1",IF(AND(D32&lt;0.5, I32 &lt; 0.5,N32&lt;0.5, S32&gt;=0.5), "B","A"))))))))</f>
+        <v>C1</v>
+      </c>
+      <c r="AB32" s="25" t="str">
+        <f>IF(AND(E32&lt;0.5, J32 &gt;= 0.5,O32&gt;=0.5, T32&lt;0.5), "F",IF(AND(E32&lt;0.5, J32 &gt;= 0.5,O32&gt;=0.5, T32&gt;=0.5), "E2",IF(AND(E32&lt;0.5, J32 &gt;= 0.5,O32&lt;0.5, T32&lt;0.5), "E1",IF(AND(E32&lt;0.5, J32 &gt;= 0.5,O32&lt;0.5, T32&gt;=0.5), "D2",IF(AND(E32&lt;0.5, J32 &lt;0.5,O32&gt;=0.5, T32&lt;0.5), "D1",IF(AND(E32&lt;0.5, J32 &lt; 0.5,O32&gt;=0.5, T32&gt;=0.5), "C2",IF(AND(E32&lt;0.5, J32 &lt; 0.5,O32&lt;0.5, T32&lt;0.5), "C1",IF(AND(E32&lt;0.5, J32 &lt; 0.5,O32&lt;0.5, T32&gt;=0.5), "B","A"))))))))</f>
+        <v>C1</v>
+      </c>
+    </row>
+    <row r="33" spans="1:28" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A33" s="1"/>
       <c r="B33" s="1" t="s">
         <v>17</v>
@@ -2338,8 +2833,20 @@
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="34" spans="1:22" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="Z33" s="25" t="str">
+        <f>IF(AND(C33&lt;0.5, H33 &gt;= 0.5,M33&gt;=0.5, R33&lt;0.5), "F",IF(AND(C33&lt;0.5, H33 &gt;= 0.5,M33&gt;=0.5, R33&gt;=0.5), "E2",IF(AND(C33&lt;0.5, H33 &gt;= 0.5,M33&lt;0.5, R33&lt;0.5), "E1",IF(AND(C33&lt;0.5, H33 &gt;= 0.5,M33&lt;0.5, R33&gt;=0.5), "D2",IF(AND(C33&lt;0.5, H33 &lt;0.5,M33&gt;=0.5, R33&lt;0.5), "D1",IF(AND(C33&lt;0.5, H33 &lt; 0.5,M33&gt;=0.5, R33&gt;=0.5), "C2",IF(AND(C33&lt;0.5, H33 &lt; 0.5,M33&lt;0.5, R33&lt;0.5), "C1",IF(AND(C33&lt;0.5, H33 &lt; 0.5,M33&lt;0.5, R33&gt;=0.5), "B","A"))))))))</f>
+        <v>C1</v>
+      </c>
+      <c r="AA33" s="25" t="str">
+        <f>IF(AND(D33&lt;0.5, I33 &gt;= 0.5,N33&gt;=0.5, S33&lt;0.5), "F",IF(AND(D33&lt;0.5, I33 &gt;= 0.5,N33&gt;=0.5, S33&gt;=0.5), "E2",IF(AND(D33&lt;0.5, I33 &gt;= 0.5,N33&lt;0.5, S33&lt;0.5), "E1",IF(AND(D33&lt;0.5, I33 &gt;= 0.5,N33&lt;0.5, S33&gt;=0.5), "D2",IF(AND(D33&lt;0.5, I33 &lt;0.5,N33&gt;=0.5, S33&lt;0.5), "D1",IF(AND(D33&lt;0.5, I33 &lt; 0.5,N33&gt;=0.5, S33&gt;=0.5), "C2",IF(AND(D33&lt;0.5, I33 &lt; 0.5,N33&lt;0.5, S33&lt;0.5), "C1",IF(AND(D33&lt;0.5, I33 &lt; 0.5,N33&lt;0.5, S33&gt;=0.5), "B","A"))))))))</f>
+        <v>C1</v>
+      </c>
+      <c r="AB33" s="25" t="str">
+        <f>IF(AND(E33&lt;0.5, J33 &gt;= 0.5,O33&gt;=0.5, T33&lt;0.5), "F",IF(AND(E33&lt;0.5, J33 &gt;= 0.5,O33&gt;=0.5, T33&gt;=0.5), "E2",IF(AND(E33&lt;0.5, J33 &gt;= 0.5,O33&lt;0.5, T33&lt;0.5), "E1",IF(AND(E33&lt;0.5, J33 &gt;= 0.5,O33&lt;0.5, T33&gt;=0.5), "D2",IF(AND(E33&lt;0.5, J33 &lt;0.5,O33&gt;=0.5, T33&lt;0.5), "D1",IF(AND(E33&lt;0.5, J33 &lt; 0.5,O33&gt;=0.5, T33&gt;=0.5), "C2",IF(AND(E33&lt;0.5, J33 &lt; 0.5,O33&lt;0.5, T33&lt;0.5), "C1",IF(AND(E33&lt;0.5, J33 &lt; 0.5,O33&lt;0.5, T33&gt;=0.5), "B","A"))))))))</f>
+        <v>C1</v>
+      </c>
+    </row>
+    <row r="34" spans="1:28" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A34" s="4"/>
       <c r="B34" s="4" t="s">
         <v>18</v>
@@ -2388,8 +2895,20 @@
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="35" spans="1:22" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="Z34" s="25" t="str">
+        <f>IF(AND(C34&lt;0.5, H34 &gt;= 0.5,M34&gt;=0.5, R34&lt;0.5), "F",IF(AND(C34&lt;0.5, H34 &gt;= 0.5,M34&gt;=0.5, R34&gt;=0.5), "E2",IF(AND(C34&lt;0.5, H34 &gt;= 0.5,M34&lt;0.5, R34&lt;0.5), "E1",IF(AND(C34&lt;0.5, H34 &gt;= 0.5,M34&lt;0.5, R34&gt;=0.5), "D2",IF(AND(C34&lt;0.5, H34 &lt;0.5,M34&gt;=0.5, R34&lt;0.5), "D1",IF(AND(C34&lt;0.5, H34 &lt; 0.5,M34&gt;=0.5, R34&gt;=0.5), "C2",IF(AND(C34&lt;0.5, H34 &lt; 0.5,M34&lt;0.5, R34&lt;0.5), "C1",IF(AND(C34&lt;0.5, H34 &lt; 0.5,M34&lt;0.5, R34&gt;=0.5), "B","A"))))))))</f>
+        <v>C1</v>
+      </c>
+      <c r="AA34" s="25" t="str">
+        <f>IF(AND(D34&lt;0.5, I34 &gt;= 0.5,N34&gt;=0.5, S34&lt;0.5), "F",IF(AND(D34&lt;0.5, I34 &gt;= 0.5,N34&gt;=0.5, S34&gt;=0.5), "E2",IF(AND(D34&lt;0.5, I34 &gt;= 0.5,N34&lt;0.5, S34&lt;0.5), "E1",IF(AND(D34&lt;0.5, I34 &gt;= 0.5,N34&lt;0.5, S34&gt;=0.5), "D2",IF(AND(D34&lt;0.5, I34 &lt;0.5,N34&gt;=0.5, S34&lt;0.5), "D1",IF(AND(D34&lt;0.5, I34 &lt; 0.5,N34&gt;=0.5, S34&gt;=0.5), "C2",IF(AND(D34&lt;0.5, I34 &lt; 0.5,N34&lt;0.5, S34&lt;0.5), "C1",IF(AND(D34&lt;0.5, I34 &lt; 0.5,N34&lt;0.5, S34&gt;=0.5), "B","A"))))))))</f>
+        <v>C1</v>
+      </c>
+      <c r="AB34" s="25" t="str">
+        <f>IF(AND(E34&lt;0.5, J34 &gt;= 0.5,O34&gt;=0.5, T34&lt;0.5), "F",IF(AND(E34&lt;0.5, J34 &gt;= 0.5,O34&gt;=0.5, T34&gt;=0.5), "E2",IF(AND(E34&lt;0.5, J34 &gt;= 0.5,O34&lt;0.5, T34&lt;0.5), "E1",IF(AND(E34&lt;0.5, J34 &gt;= 0.5,O34&lt;0.5, T34&gt;=0.5), "D2",IF(AND(E34&lt;0.5, J34 &lt;0.5,O34&gt;=0.5, T34&lt;0.5), "D1",IF(AND(E34&lt;0.5, J34 &lt; 0.5,O34&gt;=0.5, T34&gt;=0.5), "C2",IF(AND(E34&lt;0.5, J34 &lt; 0.5,O34&lt;0.5, T34&lt;0.5), "C1",IF(AND(E34&lt;0.5, J34 &lt; 0.5,O34&lt;0.5, T34&gt;=0.5), "B","A"))))))))</f>
+        <v>C1</v>
+      </c>
+    </row>
+    <row r="35" spans="1:28" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A35" s="3">
         <v>9</v>
       </c>
@@ -2440,8 +2959,20 @@
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="36" spans="1:22" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="Z35" s="25" t="str">
+        <f>IF(AND(C35&lt;0.5, H35 &gt;= 0.5,M35&gt;=0.5, R35&lt;0.5), "F",IF(AND(C35&lt;0.5, H35 &gt;= 0.5,M35&gt;=0.5, R35&gt;=0.5), "E2",IF(AND(C35&lt;0.5, H35 &gt;= 0.5,M35&lt;0.5, R35&lt;0.5), "E1",IF(AND(C35&lt;0.5, H35 &gt;= 0.5,M35&lt;0.5, R35&gt;=0.5), "D2",IF(AND(C35&lt;0.5, H35 &lt;0.5,M35&gt;=0.5, R35&lt;0.5), "D1",IF(AND(C35&lt;0.5, H35 &lt; 0.5,M35&gt;=0.5, R35&gt;=0.5), "C2",IF(AND(C35&lt;0.5, H35 &lt; 0.5,M35&lt;0.5, R35&lt;0.5), "C1",IF(AND(C35&lt;0.5, H35 &lt; 0.5,M35&lt;0.5, R35&gt;=0.5), "B","A"))))))))</f>
+        <v>C1</v>
+      </c>
+      <c r="AA35" s="25" t="str">
+        <f>IF(AND(D35&lt;0.5, I35 &gt;= 0.5,N35&gt;=0.5, S35&lt;0.5), "F",IF(AND(D35&lt;0.5, I35 &gt;= 0.5,N35&gt;=0.5, S35&gt;=0.5), "E2",IF(AND(D35&lt;0.5, I35 &gt;= 0.5,N35&lt;0.5, S35&lt;0.5), "E1",IF(AND(D35&lt;0.5, I35 &gt;= 0.5,N35&lt;0.5, S35&gt;=0.5), "D2",IF(AND(D35&lt;0.5, I35 &lt;0.5,N35&gt;=0.5, S35&lt;0.5), "D1",IF(AND(D35&lt;0.5, I35 &lt; 0.5,N35&gt;=0.5, S35&gt;=0.5), "C2",IF(AND(D35&lt;0.5, I35 &lt; 0.5,N35&lt;0.5, S35&lt;0.5), "C1",IF(AND(D35&lt;0.5, I35 &lt; 0.5,N35&lt;0.5, S35&gt;=0.5), "B","A"))))))))</f>
+        <v>C1</v>
+      </c>
+      <c r="AB35" s="25" t="str">
+        <f>IF(AND(E35&lt;0.5, J35 &gt;= 0.5,O35&gt;=0.5, T35&lt;0.5), "F",IF(AND(E35&lt;0.5, J35 &gt;= 0.5,O35&gt;=0.5, T35&gt;=0.5), "E2",IF(AND(E35&lt;0.5, J35 &gt;= 0.5,O35&lt;0.5, T35&lt;0.5), "E1",IF(AND(E35&lt;0.5, J35 &gt;= 0.5,O35&lt;0.5, T35&gt;=0.5), "D2",IF(AND(E35&lt;0.5, J35 &lt;0.5,O35&gt;=0.5, T35&lt;0.5), "D1",IF(AND(E35&lt;0.5, J35 &lt; 0.5,O35&gt;=0.5, T35&gt;=0.5), "C2",IF(AND(E35&lt;0.5, J35 &lt; 0.5,O35&lt;0.5, T35&lt;0.5), "C1",IF(AND(E35&lt;0.5, J35 &lt; 0.5,O35&lt;0.5, T35&gt;=0.5), "B","A"))))))))</f>
+        <v>C1</v>
+      </c>
+    </row>
+    <row r="36" spans="1:28" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A36" s="1"/>
       <c r="B36" s="1" t="s">
         <v>16</v>
@@ -2487,8 +3018,20 @@
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="37" spans="1:22" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="Z36" s="25" t="str">
+        <f>IF(AND(C36&lt;0.5, H36 &gt;= 0.5,M36&gt;=0.5, R36&lt;0.5), "F",IF(AND(C36&lt;0.5, H36 &gt;= 0.5,M36&gt;=0.5, R36&gt;=0.5), "E2",IF(AND(C36&lt;0.5, H36 &gt;= 0.5,M36&lt;0.5, R36&lt;0.5), "E1",IF(AND(C36&lt;0.5, H36 &gt;= 0.5,M36&lt;0.5, R36&gt;=0.5), "D2",IF(AND(C36&lt;0.5, H36 &lt;0.5,M36&gt;=0.5, R36&lt;0.5), "D1",IF(AND(C36&lt;0.5, H36 &lt; 0.5,M36&gt;=0.5, R36&gt;=0.5), "C2",IF(AND(C36&lt;0.5, H36 &lt; 0.5,M36&lt;0.5, R36&lt;0.5), "C1",IF(AND(C36&lt;0.5, H36 &lt; 0.5,M36&lt;0.5, R36&gt;=0.5), "B","A"))))))))</f>
+        <v>C1</v>
+      </c>
+      <c r="AA36" s="25" t="str">
+        <f>IF(AND(D36&lt;0.5, I36 &gt;= 0.5,N36&gt;=0.5, S36&lt;0.5), "F",IF(AND(D36&lt;0.5, I36 &gt;= 0.5,N36&gt;=0.5, S36&gt;=0.5), "E2",IF(AND(D36&lt;0.5, I36 &gt;= 0.5,N36&lt;0.5, S36&lt;0.5), "E1",IF(AND(D36&lt;0.5, I36 &gt;= 0.5,N36&lt;0.5, S36&gt;=0.5), "D2",IF(AND(D36&lt;0.5, I36 &lt;0.5,N36&gt;=0.5, S36&lt;0.5), "D1",IF(AND(D36&lt;0.5, I36 &lt; 0.5,N36&gt;=0.5, S36&gt;=0.5), "C2",IF(AND(D36&lt;0.5, I36 &lt; 0.5,N36&lt;0.5, S36&lt;0.5), "C1",IF(AND(D36&lt;0.5, I36 &lt; 0.5,N36&lt;0.5, S36&gt;=0.5), "B","A"))))))))</f>
+        <v>C1</v>
+      </c>
+      <c r="AB36" s="25" t="str">
+        <f>IF(AND(E36&lt;0.5, J36 &gt;= 0.5,O36&gt;=0.5, T36&lt;0.5), "F",IF(AND(E36&lt;0.5, J36 &gt;= 0.5,O36&gt;=0.5, T36&gt;=0.5), "E2",IF(AND(E36&lt;0.5, J36 &gt;= 0.5,O36&lt;0.5, T36&lt;0.5), "E1",IF(AND(E36&lt;0.5, J36 &gt;= 0.5,O36&lt;0.5, T36&gt;=0.5), "D2",IF(AND(E36&lt;0.5, J36 &lt;0.5,O36&gt;=0.5, T36&lt;0.5), "D1",IF(AND(E36&lt;0.5, J36 &lt; 0.5,O36&gt;=0.5, T36&gt;=0.5), "C2",IF(AND(E36&lt;0.5, J36 &lt; 0.5,O36&lt;0.5, T36&lt;0.5), "C1",IF(AND(E36&lt;0.5, J36 &lt; 0.5,O36&lt;0.5, T36&gt;=0.5), "B","A"))))))))</f>
+        <v>C1</v>
+      </c>
+    </row>
+    <row r="37" spans="1:28" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A37" s="1"/>
       <c r="B37" s="1" t="s">
         <v>17</v>
@@ -2534,8 +3077,20 @@
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="38" spans="1:22" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="Z37" s="25" t="str">
+        <f>IF(AND(C37&lt;0.5, H37 &gt;= 0.5,M37&gt;=0.5, R37&lt;0.5), "F",IF(AND(C37&lt;0.5, H37 &gt;= 0.5,M37&gt;=0.5, R37&gt;=0.5), "E2",IF(AND(C37&lt;0.5, H37 &gt;= 0.5,M37&lt;0.5, R37&lt;0.5), "E1",IF(AND(C37&lt;0.5, H37 &gt;= 0.5,M37&lt;0.5, R37&gt;=0.5), "D2",IF(AND(C37&lt;0.5, H37 &lt;0.5,M37&gt;=0.5, R37&lt;0.5), "D1",IF(AND(C37&lt;0.5, H37 &lt; 0.5,M37&gt;=0.5, R37&gt;=0.5), "C2",IF(AND(C37&lt;0.5, H37 &lt; 0.5,M37&lt;0.5, R37&lt;0.5), "C1",IF(AND(C37&lt;0.5, H37 &lt; 0.5,M37&lt;0.5, R37&gt;=0.5), "B","A"))))))))</f>
+        <v>C1</v>
+      </c>
+      <c r="AA37" s="25" t="str">
+        <f>IF(AND(D37&lt;0.5, I37 &gt;= 0.5,N37&gt;=0.5, S37&lt;0.5), "F",IF(AND(D37&lt;0.5, I37 &gt;= 0.5,N37&gt;=0.5, S37&gt;=0.5), "E2",IF(AND(D37&lt;0.5, I37 &gt;= 0.5,N37&lt;0.5, S37&lt;0.5), "E1",IF(AND(D37&lt;0.5, I37 &gt;= 0.5,N37&lt;0.5, S37&gt;=0.5), "D2",IF(AND(D37&lt;0.5, I37 &lt;0.5,N37&gt;=0.5, S37&lt;0.5), "D1",IF(AND(D37&lt;0.5, I37 &lt; 0.5,N37&gt;=0.5, S37&gt;=0.5), "C2",IF(AND(D37&lt;0.5, I37 &lt; 0.5,N37&lt;0.5, S37&lt;0.5), "C1",IF(AND(D37&lt;0.5, I37 &lt; 0.5,N37&lt;0.5, S37&gt;=0.5), "B","A"))))))))</f>
+        <v>C1</v>
+      </c>
+      <c r="AB37" s="25" t="str">
+        <f>IF(AND(E37&lt;0.5, J37 &gt;= 0.5,O37&gt;=0.5, T37&lt;0.5), "F",IF(AND(E37&lt;0.5, J37 &gt;= 0.5,O37&gt;=0.5, T37&gt;=0.5), "E2",IF(AND(E37&lt;0.5, J37 &gt;= 0.5,O37&lt;0.5, T37&lt;0.5), "E1",IF(AND(E37&lt;0.5, J37 &gt;= 0.5,O37&lt;0.5, T37&gt;=0.5), "D2",IF(AND(E37&lt;0.5, J37 &lt;0.5,O37&gt;=0.5, T37&lt;0.5), "D1",IF(AND(E37&lt;0.5, J37 &lt; 0.5,O37&gt;=0.5, T37&gt;=0.5), "C2",IF(AND(E37&lt;0.5, J37 &lt; 0.5,O37&lt;0.5, T37&lt;0.5), "C1",IF(AND(E37&lt;0.5, J37 &lt; 0.5,O37&lt;0.5, T37&gt;=0.5), "B","A"))))))))</f>
+        <v>C1</v>
+      </c>
+    </row>
+    <row r="38" spans="1:28" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A38" s="4"/>
       <c r="B38" s="4" t="s">
         <v>18</v>
@@ -2584,8 +3139,20 @@
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="39" spans="1:22" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="Z38" s="25" t="str">
+        <f>IF(AND(C38&lt;0.5, H38 &gt;= 0.5,M38&gt;=0.5, R38&lt;0.5), "F",IF(AND(C38&lt;0.5, H38 &gt;= 0.5,M38&gt;=0.5, R38&gt;=0.5), "E2",IF(AND(C38&lt;0.5, H38 &gt;= 0.5,M38&lt;0.5, R38&lt;0.5), "E1",IF(AND(C38&lt;0.5, H38 &gt;= 0.5,M38&lt;0.5, R38&gt;=0.5), "D2",IF(AND(C38&lt;0.5, H38 &lt;0.5,M38&gt;=0.5, R38&lt;0.5), "D1",IF(AND(C38&lt;0.5, H38 &lt; 0.5,M38&gt;=0.5, R38&gt;=0.5), "C2",IF(AND(C38&lt;0.5, H38 &lt; 0.5,M38&lt;0.5, R38&lt;0.5), "C1",IF(AND(C38&lt;0.5, H38 &lt; 0.5,M38&lt;0.5, R38&gt;=0.5), "B","A"))))))))</f>
+        <v>C1</v>
+      </c>
+      <c r="AA38" s="25" t="str">
+        <f>IF(AND(D38&lt;0.5, I38 &gt;= 0.5,N38&gt;=0.5, S38&lt;0.5), "F",IF(AND(D38&lt;0.5, I38 &gt;= 0.5,N38&gt;=0.5, S38&gt;=0.5), "E2",IF(AND(D38&lt;0.5, I38 &gt;= 0.5,N38&lt;0.5, S38&lt;0.5), "E1",IF(AND(D38&lt;0.5, I38 &gt;= 0.5,N38&lt;0.5, S38&gt;=0.5), "D2",IF(AND(D38&lt;0.5, I38 &lt;0.5,N38&gt;=0.5, S38&lt;0.5), "D1",IF(AND(D38&lt;0.5, I38 &lt; 0.5,N38&gt;=0.5, S38&gt;=0.5), "C2",IF(AND(D38&lt;0.5, I38 &lt; 0.5,N38&lt;0.5, S38&lt;0.5), "C1",IF(AND(D38&lt;0.5, I38 &lt; 0.5,N38&lt;0.5, S38&gt;=0.5), "B","A"))))))))</f>
+        <v>C1</v>
+      </c>
+      <c r="AB38" s="25" t="str">
+        <f>IF(AND(E38&lt;0.5, J38 &gt;= 0.5,O38&gt;=0.5, T38&lt;0.5), "F",IF(AND(E38&lt;0.5, J38 &gt;= 0.5,O38&gt;=0.5, T38&gt;=0.5), "E2",IF(AND(E38&lt;0.5, J38 &gt;= 0.5,O38&lt;0.5, T38&lt;0.5), "E1",IF(AND(E38&lt;0.5, J38 &gt;= 0.5,O38&lt;0.5, T38&gt;=0.5), "D2",IF(AND(E38&lt;0.5, J38 &lt;0.5,O38&gt;=0.5, T38&lt;0.5), "D1",IF(AND(E38&lt;0.5, J38 &lt; 0.5,O38&gt;=0.5, T38&gt;=0.5), "C2",IF(AND(E38&lt;0.5, J38 &lt; 0.5,O38&lt;0.5, T38&lt;0.5), "C1",IF(AND(E38&lt;0.5, J38 &lt; 0.5,O38&lt;0.5, T38&gt;=0.5), "B","A"))))))))</f>
+        <v>C1</v>
+      </c>
+    </row>
+    <row r="39" spans="1:28" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A39" s="3">
         <v>10</v>
       </c>
@@ -2636,8 +3203,20 @@
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="40" spans="1:22" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="Z39" s="25" t="str">
+        <f>IF(AND(C39&lt;0.5, H39 &gt;= 0.5,M39&gt;=0.5, R39&lt;0.5), "F",IF(AND(C39&lt;0.5, H39 &gt;= 0.5,M39&gt;=0.5, R39&gt;=0.5), "E2",IF(AND(C39&lt;0.5, H39 &gt;= 0.5,M39&lt;0.5, R39&lt;0.5), "E1",IF(AND(C39&lt;0.5, H39 &gt;= 0.5,M39&lt;0.5, R39&gt;=0.5), "D2",IF(AND(C39&lt;0.5, H39 &lt;0.5,M39&gt;=0.5, R39&lt;0.5), "D1",IF(AND(C39&lt;0.5, H39 &lt; 0.5,M39&gt;=0.5, R39&gt;=0.5), "C2",IF(AND(C39&lt;0.5, H39 &lt; 0.5,M39&lt;0.5, R39&lt;0.5), "C1",IF(AND(C39&lt;0.5, H39 &lt; 0.5,M39&lt;0.5, R39&gt;=0.5), "B","A"))))))))</f>
+        <v>C1</v>
+      </c>
+      <c r="AA39" s="25" t="str">
+        <f>IF(AND(D39&lt;0.5, I39 &gt;= 0.5,N39&gt;=0.5, S39&lt;0.5), "F",IF(AND(D39&lt;0.5, I39 &gt;= 0.5,N39&gt;=0.5, S39&gt;=0.5), "E2",IF(AND(D39&lt;0.5, I39 &gt;= 0.5,N39&lt;0.5, S39&lt;0.5), "E1",IF(AND(D39&lt;0.5, I39 &gt;= 0.5,N39&lt;0.5, S39&gt;=0.5), "D2",IF(AND(D39&lt;0.5, I39 &lt;0.5,N39&gt;=0.5, S39&lt;0.5), "D1",IF(AND(D39&lt;0.5, I39 &lt; 0.5,N39&gt;=0.5, S39&gt;=0.5), "C2",IF(AND(D39&lt;0.5, I39 &lt; 0.5,N39&lt;0.5, S39&lt;0.5), "C1",IF(AND(D39&lt;0.5, I39 &lt; 0.5,N39&lt;0.5, S39&gt;=0.5), "B","A"))))))))</f>
+        <v>C1</v>
+      </c>
+      <c r="AB39" s="25" t="str">
+        <f>IF(AND(E39&lt;0.5, J39 &gt;= 0.5,O39&gt;=0.5, T39&lt;0.5), "F",IF(AND(E39&lt;0.5, J39 &gt;= 0.5,O39&gt;=0.5, T39&gt;=0.5), "E2",IF(AND(E39&lt;0.5, J39 &gt;= 0.5,O39&lt;0.5, T39&lt;0.5), "E1",IF(AND(E39&lt;0.5, J39 &gt;= 0.5,O39&lt;0.5, T39&gt;=0.5), "D2",IF(AND(E39&lt;0.5, J39 &lt;0.5,O39&gt;=0.5, T39&lt;0.5), "D1",IF(AND(E39&lt;0.5, J39 &lt; 0.5,O39&gt;=0.5, T39&gt;=0.5), "C2",IF(AND(E39&lt;0.5, J39 &lt; 0.5,O39&lt;0.5, T39&lt;0.5), "C1",IF(AND(E39&lt;0.5, J39 &lt; 0.5,O39&lt;0.5, T39&gt;=0.5), "B","A"))))))))</f>
+        <v>C1</v>
+      </c>
+    </row>
+    <row r="40" spans="1:28" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A40" s="1"/>
       <c r="B40" s="1" t="s">
         <v>16</v>
@@ -2683,8 +3262,20 @@
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="41" spans="1:22" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="Z40" s="25" t="str">
+        <f>IF(AND(C40&lt;0.5, H40 &gt;= 0.5,M40&gt;=0.5, R40&lt;0.5), "F",IF(AND(C40&lt;0.5, H40 &gt;= 0.5,M40&gt;=0.5, R40&gt;=0.5), "E2",IF(AND(C40&lt;0.5, H40 &gt;= 0.5,M40&lt;0.5, R40&lt;0.5), "E1",IF(AND(C40&lt;0.5, H40 &gt;= 0.5,M40&lt;0.5, R40&gt;=0.5), "D2",IF(AND(C40&lt;0.5, H40 &lt;0.5,M40&gt;=0.5, R40&lt;0.5), "D1",IF(AND(C40&lt;0.5, H40 &lt; 0.5,M40&gt;=0.5, R40&gt;=0.5), "C2",IF(AND(C40&lt;0.5, H40 &lt; 0.5,M40&lt;0.5, R40&lt;0.5), "C1",IF(AND(C40&lt;0.5, H40 &lt; 0.5,M40&lt;0.5, R40&gt;=0.5), "B","A"))))))))</f>
+        <v>C1</v>
+      </c>
+      <c r="AA40" s="25" t="str">
+        <f>IF(AND(D40&lt;0.5, I40 &gt;= 0.5,N40&gt;=0.5, S40&lt;0.5), "F",IF(AND(D40&lt;0.5, I40 &gt;= 0.5,N40&gt;=0.5, S40&gt;=0.5), "E2",IF(AND(D40&lt;0.5, I40 &gt;= 0.5,N40&lt;0.5, S40&lt;0.5), "E1",IF(AND(D40&lt;0.5, I40 &gt;= 0.5,N40&lt;0.5, S40&gt;=0.5), "D2",IF(AND(D40&lt;0.5, I40 &lt;0.5,N40&gt;=0.5, S40&lt;0.5), "D1",IF(AND(D40&lt;0.5, I40 &lt; 0.5,N40&gt;=0.5, S40&gt;=0.5), "C2",IF(AND(D40&lt;0.5, I40 &lt; 0.5,N40&lt;0.5, S40&lt;0.5), "C1",IF(AND(D40&lt;0.5, I40 &lt; 0.5,N40&lt;0.5, S40&gt;=0.5), "B","A"))))))))</f>
+        <v>C1</v>
+      </c>
+      <c r="AB40" s="25" t="str">
+        <f>IF(AND(E40&lt;0.5, J40 &gt;= 0.5,O40&gt;=0.5, T40&lt;0.5), "F",IF(AND(E40&lt;0.5, J40 &gt;= 0.5,O40&gt;=0.5, T40&gt;=0.5), "E2",IF(AND(E40&lt;0.5, J40 &gt;= 0.5,O40&lt;0.5, T40&lt;0.5), "E1",IF(AND(E40&lt;0.5, J40 &gt;= 0.5,O40&lt;0.5, T40&gt;=0.5), "D2",IF(AND(E40&lt;0.5, J40 &lt;0.5,O40&gt;=0.5, T40&lt;0.5), "D1",IF(AND(E40&lt;0.5, J40 &lt; 0.5,O40&gt;=0.5, T40&gt;=0.5), "C2",IF(AND(E40&lt;0.5, J40 &lt; 0.5,O40&lt;0.5, T40&lt;0.5), "C1",IF(AND(E40&lt;0.5, J40 &lt; 0.5,O40&lt;0.5, T40&gt;=0.5), "B","A"))))))))</f>
+        <v>C1</v>
+      </c>
+    </row>
+    <row r="41" spans="1:28" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A41" s="1"/>
       <c r="B41" s="1" t="s">
         <v>17</v>
@@ -2730,8 +3321,20 @@
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="42" spans="1:22" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="Z41" s="25" t="str">
+        <f>IF(AND(C41&lt;0.5, H41 &gt;= 0.5,M41&gt;=0.5, R41&lt;0.5), "F",IF(AND(C41&lt;0.5, H41 &gt;= 0.5,M41&gt;=0.5, R41&gt;=0.5), "E2",IF(AND(C41&lt;0.5, H41 &gt;= 0.5,M41&lt;0.5, R41&lt;0.5), "E1",IF(AND(C41&lt;0.5, H41 &gt;= 0.5,M41&lt;0.5, R41&gt;=0.5), "D2",IF(AND(C41&lt;0.5, H41 &lt;0.5,M41&gt;=0.5, R41&lt;0.5), "D1",IF(AND(C41&lt;0.5, H41 &lt; 0.5,M41&gt;=0.5, R41&gt;=0.5), "C2",IF(AND(C41&lt;0.5, H41 &lt; 0.5,M41&lt;0.5, R41&lt;0.5), "C1",IF(AND(C41&lt;0.5, H41 &lt; 0.5,M41&lt;0.5, R41&gt;=0.5), "B","A"))))))))</f>
+        <v>C1</v>
+      </c>
+      <c r="AA41" s="25" t="str">
+        <f>IF(AND(D41&lt;0.5, I41 &gt;= 0.5,N41&gt;=0.5, S41&lt;0.5), "F",IF(AND(D41&lt;0.5, I41 &gt;= 0.5,N41&gt;=0.5, S41&gt;=0.5), "E2",IF(AND(D41&lt;0.5, I41 &gt;= 0.5,N41&lt;0.5, S41&lt;0.5), "E1",IF(AND(D41&lt;0.5, I41 &gt;= 0.5,N41&lt;0.5, S41&gt;=0.5), "D2",IF(AND(D41&lt;0.5, I41 &lt;0.5,N41&gt;=0.5, S41&lt;0.5), "D1",IF(AND(D41&lt;0.5, I41 &lt; 0.5,N41&gt;=0.5, S41&gt;=0.5), "C2",IF(AND(D41&lt;0.5, I41 &lt; 0.5,N41&lt;0.5, S41&lt;0.5), "C1",IF(AND(D41&lt;0.5, I41 &lt; 0.5,N41&lt;0.5, S41&gt;=0.5), "B","A"))))))))</f>
+        <v>C1</v>
+      </c>
+      <c r="AB41" s="25" t="str">
+        <f>IF(AND(E41&lt;0.5, J41 &gt;= 0.5,O41&gt;=0.5, T41&lt;0.5), "F",IF(AND(E41&lt;0.5, J41 &gt;= 0.5,O41&gt;=0.5, T41&gt;=0.5), "E2",IF(AND(E41&lt;0.5, J41 &gt;= 0.5,O41&lt;0.5, T41&lt;0.5), "E1",IF(AND(E41&lt;0.5, J41 &gt;= 0.5,O41&lt;0.5, T41&gt;=0.5), "D2",IF(AND(E41&lt;0.5, J41 &lt;0.5,O41&gt;=0.5, T41&lt;0.5), "D1",IF(AND(E41&lt;0.5, J41 &lt; 0.5,O41&gt;=0.5, T41&gt;=0.5), "C2",IF(AND(E41&lt;0.5, J41 &lt; 0.5,O41&lt;0.5, T41&lt;0.5), "C1",IF(AND(E41&lt;0.5, J41 &lt; 0.5,O41&lt;0.5, T41&gt;=0.5), "B","A"))))))))</f>
+        <v>C1</v>
+      </c>
+    </row>
+    <row r="42" spans="1:28" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A42" s="4"/>
       <c r="B42" s="4" t="s">
         <v>18</v>
@@ -2780,8 +3383,20 @@
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="43" spans="1:22" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="Z42" s="25" t="str">
+        <f>IF(AND(C42&lt;0.5, H42 &gt;= 0.5,M42&gt;=0.5, R42&lt;0.5), "F",IF(AND(C42&lt;0.5, H42 &gt;= 0.5,M42&gt;=0.5, R42&gt;=0.5), "E2",IF(AND(C42&lt;0.5, H42 &gt;= 0.5,M42&lt;0.5, R42&lt;0.5), "E1",IF(AND(C42&lt;0.5, H42 &gt;= 0.5,M42&lt;0.5, R42&gt;=0.5), "D2",IF(AND(C42&lt;0.5, H42 &lt;0.5,M42&gt;=0.5, R42&lt;0.5), "D1",IF(AND(C42&lt;0.5, H42 &lt; 0.5,M42&gt;=0.5, R42&gt;=0.5), "C2",IF(AND(C42&lt;0.5, H42 &lt; 0.5,M42&lt;0.5, R42&lt;0.5), "C1",IF(AND(C42&lt;0.5, H42 &lt; 0.5,M42&lt;0.5, R42&gt;=0.5), "B","A"))))))))</f>
+        <v>C1</v>
+      </c>
+      <c r="AA42" s="25" t="str">
+        <f>IF(AND(D42&lt;0.5, I42 &gt;= 0.5,N42&gt;=0.5, S42&lt;0.5), "F",IF(AND(D42&lt;0.5, I42 &gt;= 0.5,N42&gt;=0.5, S42&gt;=0.5), "E2",IF(AND(D42&lt;0.5, I42 &gt;= 0.5,N42&lt;0.5, S42&lt;0.5), "E1",IF(AND(D42&lt;0.5, I42 &gt;= 0.5,N42&lt;0.5, S42&gt;=0.5), "D2",IF(AND(D42&lt;0.5, I42 &lt;0.5,N42&gt;=0.5, S42&lt;0.5), "D1",IF(AND(D42&lt;0.5, I42 &lt; 0.5,N42&gt;=0.5, S42&gt;=0.5), "C2",IF(AND(D42&lt;0.5, I42 &lt; 0.5,N42&lt;0.5, S42&lt;0.5), "C1",IF(AND(D42&lt;0.5, I42 &lt; 0.5,N42&lt;0.5, S42&gt;=0.5), "B","A"))))))))</f>
+        <v>C1</v>
+      </c>
+      <c r="AB42" s="25" t="str">
+        <f>IF(AND(E42&lt;0.5, J42 &gt;= 0.5,O42&gt;=0.5, T42&lt;0.5), "F",IF(AND(E42&lt;0.5, J42 &gt;= 0.5,O42&gt;=0.5, T42&gt;=0.5), "E2",IF(AND(E42&lt;0.5, J42 &gt;= 0.5,O42&lt;0.5, T42&lt;0.5), "E1",IF(AND(E42&lt;0.5, J42 &gt;= 0.5,O42&lt;0.5, T42&gt;=0.5), "D2",IF(AND(E42&lt;0.5, J42 &lt;0.5,O42&gt;=0.5, T42&lt;0.5), "D1",IF(AND(E42&lt;0.5, J42 &lt; 0.5,O42&gt;=0.5, T42&gt;=0.5), "C2",IF(AND(E42&lt;0.5, J42 &lt; 0.5,O42&lt;0.5, T42&lt;0.5), "C1",IF(AND(E42&lt;0.5, J42 &lt; 0.5,O42&lt;0.5, T42&gt;=0.5), "B","A"))))))))</f>
+        <v>C1</v>
+      </c>
+    </row>
+    <row r="43" spans="1:28" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A43" s="3">
         <v>11</v>
       </c>
@@ -2832,8 +3447,20 @@
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="44" spans="1:22" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="Z43" s="25" t="str">
+        <f>IF(AND(C43&lt;0.5, H43 &gt;= 0.5,M43&gt;=0.5, R43&lt;0.5), "F",IF(AND(C43&lt;0.5, H43 &gt;= 0.5,M43&gt;=0.5, R43&gt;=0.5), "E2",IF(AND(C43&lt;0.5, H43 &gt;= 0.5,M43&lt;0.5, R43&lt;0.5), "E1",IF(AND(C43&lt;0.5, H43 &gt;= 0.5,M43&lt;0.5, R43&gt;=0.5), "D2",IF(AND(C43&lt;0.5, H43 &lt;0.5,M43&gt;=0.5, R43&lt;0.5), "D1",IF(AND(C43&lt;0.5, H43 &lt; 0.5,M43&gt;=0.5, R43&gt;=0.5), "C2",IF(AND(C43&lt;0.5, H43 &lt; 0.5,M43&lt;0.5, R43&lt;0.5), "C1",IF(AND(C43&lt;0.5, H43 &lt; 0.5,M43&lt;0.5, R43&gt;=0.5), "B","A"))))))))</f>
+        <v>C1</v>
+      </c>
+      <c r="AA43" s="25" t="str">
+        <f>IF(AND(D43&lt;0.5, I43 &gt;= 0.5,N43&gt;=0.5, S43&lt;0.5), "F",IF(AND(D43&lt;0.5, I43 &gt;= 0.5,N43&gt;=0.5, S43&gt;=0.5), "E2",IF(AND(D43&lt;0.5, I43 &gt;= 0.5,N43&lt;0.5, S43&lt;0.5), "E1",IF(AND(D43&lt;0.5, I43 &gt;= 0.5,N43&lt;0.5, S43&gt;=0.5), "D2",IF(AND(D43&lt;0.5, I43 &lt;0.5,N43&gt;=0.5, S43&lt;0.5), "D1",IF(AND(D43&lt;0.5, I43 &lt; 0.5,N43&gt;=0.5, S43&gt;=0.5), "C2",IF(AND(D43&lt;0.5, I43 &lt; 0.5,N43&lt;0.5, S43&lt;0.5), "C1",IF(AND(D43&lt;0.5, I43 &lt; 0.5,N43&lt;0.5, S43&gt;=0.5), "B","A"))))))))</f>
+        <v>C1</v>
+      </c>
+      <c r="AB43" s="25" t="str">
+        <f>IF(AND(E43&lt;0.5, J43 &gt;= 0.5,O43&gt;=0.5, T43&lt;0.5), "F",IF(AND(E43&lt;0.5, J43 &gt;= 0.5,O43&gt;=0.5, T43&gt;=0.5), "E2",IF(AND(E43&lt;0.5, J43 &gt;= 0.5,O43&lt;0.5, T43&lt;0.5), "E1",IF(AND(E43&lt;0.5, J43 &gt;= 0.5,O43&lt;0.5, T43&gt;=0.5), "D2",IF(AND(E43&lt;0.5, J43 &lt;0.5,O43&gt;=0.5, T43&lt;0.5), "D1",IF(AND(E43&lt;0.5, J43 &lt; 0.5,O43&gt;=0.5, T43&gt;=0.5), "C2",IF(AND(E43&lt;0.5, J43 &lt; 0.5,O43&lt;0.5, T43&lt;0.5), "C1",IF(AND(E43&lt;0.5, J43 &lt; 0.5,O43&lt;0.5, T43&gt;=0.5), "B","A"))))))))</f>
+        <v>C1</v>
+      </c>
+    </row>
+    <row r="44" spans="1:28" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A44" s="1"/>
       <c r="B44" s="1" t="s">
         <v>16</v>
@@ -2879,8 +3506,20 @@
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="45" spans="1:22" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="Z44" s="25" t="str">
+        <f>IF(AND(C44&lt;0.5, H44 &gt;= 0.5,M44&gt;=0.5, R44&lt;0.5), "F",IF(AND(C44&lt;0.5, H44 &gt;= 0.5,M44&gt;=0.5, R44&gt;=0.5), "E2",IF(AND(C44&lt;0.5, H44 &gt;= 0.5,M44&lt;0.5, R44&lt;0.5), "E1",IF(AND(C44&lt;0.5, H44 &gt;= 0.5,M44&lt;0.5, R44&gt;=0.5), "D2",IF(AND(C44&lt;0.5, H44 &lt;0.5,M44&gt;=0.5, R44&lt;0.5), "D1",IF(AND(C44&lt;0.5, H44 &lt; 0.5,M44&gt;=0.5, R44&gt;=0.5), "C2",IF(AND(C44&lt;0.5, H44 &lt; 0.5,M44&lt;0.5, R44&lt;0.5), "C1",IF(AND(C44&lt;0.5, H44 &lt; 0.5,M44&lt;0.5, R44&gt;=0.5), "B","A"))))))))</f>
+        <v>C1</v>
+      </c>
+      <c r="AA44" s="25" t="str">
+        <f>IF(AND(D44&lt;0.5, I44 &gt;= 0.5,N44&gt;=0.5, S44&lt;0.5), "F",IF(AND(D44&lt;0.5, I44 &gt;= 0.5,N44&gt;=0.5, S44&gt;=0.5), "E2",IF(AND(D44&lt;0.5, I44 &gt;= 0.5,N44&lt;0.5, S44&lt;0.5), "E1",IF(AND(D44&lt;0.5, I44 &gt;= 0.5,N44&lt;0.5, S44&gt;=0.5), "D2",IF(AND(D44&lt;0.5, I44 &lt;0.5,N44&gt;=0.5, S44&lt;0.5), "D1",IF(AND(D44&lt;0.5, I44 &lt; 0.5,N44&gt;=0.5, S44&gt;=0.5), "C2",IF(AND(D44&lt;0.5, I44 &lt; 0.5,N44&lt;0.5, S44&lt;0.5), "C1",IF(AND(D44&lt;0.5, I44 &lt; 0.5,N44&lt;0.5, S44&gt;=0.5), "B","A"))))))))</f>
+        <v>C1</v>
+      </c>
+      <c r="AB44" s="25" t="str">
+        <f>IF(AND(E44&lt;0.5, J44 &gt;= 0.5,O44&gt;=0.5, T44&lt;0.5), "F",IF(AND(E44&lt;0.5, J44 &gt;= 0.5,O44&gt;=0.5, T44&gt;=0.5), "E2",IF(AND(E44&lt;0.5, J44 &gt;= 0.5,O44&lt;0.5, T44&lt;0.5), "E1",IF(AND(E44&lt;0.5, J44 &gt;= 0.5,O44&lt;0.5, T44&gt;=0.5), "D2",IF(AND(E44&lt;0.5, J44 &lt;0.5,O44&gt;=0.5, T44&lt;0.5), "D1",IF(AND(E44&lt;0.5, J44 &lt; 0.5,O44&gt;=0.5, T44&gt;=0.5), "C2",IF(AND(E44&lt;0.5, J44 &lt; 0.5,O44&lt;0.5, T44&lt;0.5), "C1",IF(AND(E44&lt;0.5, J44 &lt; 0.5,O44&lt;0.5, T44&gt;=0.5), "B","A"))))))))</f>
+        <v>C1</v>
+      </c>
+    </row>
+    <row r="45" spans="1:28" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A45" s="1"/>
       <c r="B45" s="1" t="s">
         <v>17</v>
@@ -2926,8 +3565,20 @@
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="46" spans="1:22" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="Z45" s="25" t="str">
+        <f>IF(AND(C45&lt;0.5, H45 &gt;= 0.5,M45&gt;=0.5, R45&lt;0.5), "F",IF(AND(C45&lt;0.5, H45 &gt;= 0.5,M45&gt;=0.5, R45&gt;=0.5), "E2",IF(AND(C45&lt;0.5, H45 &gt;= 0.5,M45&lt;0.5, R45&lt;0.5), "E1",IF(AND(C45&lt;0.5, H45 &gt;= 0.5,M45&lt;0.5, R45&gt;=0.5), "D2",IF(AND(C45&lt;0.5, H45 &lt;0.5,M45&gt;=0.5, R45&lt;0.5), "D1",IF(AND(C45&lt;0.5, H45 &lt; 0.5,M45&gt;=0.5, R45&gt;=0.5), "C2",IF(AND(C45&lt;0.5, H45 &lt; 0.5,M45&lt;0.5, R45&lt;0.5), "C1",IF(AND(C45&lt;0.5, H45 &lt; 0.5,M45&lt;0.5, R45&gt;=0.5), "B","A"))))))))</f>
+        <v>C1</v>
+      </c>
+      <c r="AA45" s="25" t="str">
+        <f>IF(AND(D45&lt;0.5, I45 &gt;= 0.5,N45&gt;=0.5, S45&lt;0.5), "F",IF(AND(D45&lt;0.5, I45 &gt;= 0.5,N45&gt;=0.5, S45&gt;=0.5), "E2",IF(AND(D45&lt;0.5, I45 &gt;= 0.5,N45&lt;0.5, S45&lt;0.5), "E1",IF(AND(D45&lt;0.5, I45 &gt;= 0.5,N45&lt;0.5, S45&gt;=0.5), "D2",IF(AND(D45&lt;0.5, I45 &lt;0.5,N45&gt;=0.5, S45&lt;0.5), "D1",IF(AND(D45&lt;0.5, I45 &lt; 0.5,N45&gt;=0.5, S45&gt;=0.5), "C2",IF(AND(D45&lt;0.5, I45 &lt; 0.5,N45&lt;0.5, S45&lt;0.5), "C1",IF(AND(D45&lt;0.5, I45 &lt; 0.5,N45&lt;0.5, S45&gt;=0.5), "B","A"))))))))</f>
+        <v>C1</v>
+      </c>
+      <c r="AB45" s="25" t="str">
+        <f>IF(AND(E45&lt;0.5, J45 &gt;= 0.5,O45&gt;=0.5, T45&lt;0.5), "F",IF(AND(E45&lt;0.5, J45 &gt;= 0.5,O45&gt;=0.5, T45&gt;=0.5), "E2",IF(AND(E45&lt;0.5, J45 &gt;= 0.5,O45&lt;0.5, T45&lt;0.5), "E1",IF(AND(E45&lt;0.5, J45 &gt;= 0.5,O45&lt;0.5, T45&gt;=0.5), "D2",IF(AND(E45&lt;0.5, J45 &lt;0.5,O45&gt;=0.5, T45&lt;0.5), "D1",IF(AND(E45&lt;0.5, J45 &lt; 0.5,O45&gt;=0.5, T45&gt;=0.5), "C2",IF(AND(E45&lt;0.5, J45 &lt; 0.5,O45&lt;0.5, T45&lt;0.5), "C1",IF(AND(E45&lt;0.5, J45 &lt; 0.5,O45&lt;0.5, T45&gt;=0.5), "B","A"))))))))</f>
+        <v>C1</v>
+      </c>
+    </row>
+    <row r="46" spans="1:28" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A46" s="4"/>
       <c r="B46" s="4" t="s">
         <v>18</v>
@@ -2976,8 +3627,20 @@
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="47" spans="1:22" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="Z46" s="25" t="str">
+        <f>IF(AND(C46&lt;0.5, H46 &gt;= 0.5,M46&gt;=0.5, R46&lt;0.5), "F",IF(AND(C46&lt;0.5, H46 &gt;= 0.5,M46&gt;=0.5, R46&gt;=0.5), "E2",IF(AND(C46&lt;0.5, H46 &gt;= 0.5,M46&lt;0.5, R46&lt;0.5), "E1",IF(AND(C46&lt;0.5, H46 &gt;= 0.5,M46&lt;0.5, R46&gt;=0.5), "D2",IF(AND(C46&lt;0.5, H46 &lt;0.5,M46&gt;=0.5, R46&lt;0.5), "D1",IF(AND(C46&lt;0.5, H46 &lt; 0.5,M46&gt;=0.5, R46&gt;=0.5), "C2",IF(AND(C46&lt;0.5, H46 &lt; 0.5,M46&lt;0.5, R46&lt;0.5), "C1",IF(AND(C46&lt;0.5, H46 &lt; 0.5,M46&lt;0.5, R46&gt;=0.5), "B","A"))))))))</f>
+        <v>C1</v>
+      </c>
+      <c r="AA46" s="25" t="str">
+        <f>IF(AND(D46&lt;0.5, I46 &gt;= 0.5,N46&gt;=0.5, S46&lt;0.5), "F",IF(AND(D46&lt;0.5, I46 &gt;= 0.5,N46&gt;=0.5, S46&gt;=0.5), "E2",IF(AND(D46&lt;0.5, I46 &gt;= 0.5,N46&lt;0.5, S46&lt;0.5), "E1",IF(AND(D46&lt;0.5, I46 &gt;= 0.5,N46&lt;0.5, S46&gt;=0.5), "D2",IF(AND(D46&lt;0.5, I46 &lt;0.5,N46&gt;=0.5, S46&lt;0.5), "D1",IF(AND(D46&lt;0.5, I46 &lt; 0.5,N46&gt;=0.5, S46&gt;=0.5), "C2",IF(AND(D46&lt;0.5, I46 &lt; 0.5,N46&lt;0.5, S46&lt;0.5), "C1",IF(AND(D46&lt;0.5, I46 &lt; 0.5,N46&lt;0.5, S46&gt;=0.5), "B","A"))))))))</f>
+        <v>C1</v>
+      </c>
+      <c r="AB46" s="25" t="str">
+        <f>IF(AND(E46&lt;0.5, J46 &gt;= 0.5,O46&gt;=0.5, T46&lt;0.5), "F",IF(AND(E46&lt;0.5, J46 &gt;= 0.5,O46&gt;=0.5, T46&gt;=0.5), "E2",IF(AND(E46&lt;0.5, J46 &gt;= 0.5,O46&lt;0.5, T46&lt;0.5), "E1",IF(AND(E46&lt;0.5, J46 &gt;= 0.5,O46&lt;0.5, T46&gt;=0.5), "D2",IF(AND(E46&lt;0.5, J46 &lt;0.5,O46&gt;=0.5, T46&lt;0.5), "D1",IF(AND(E46&lt;0.5, J46 &lt; 0.5,O46&gt;=0.5, T46&gt;=0.5), "C2",IF(AND(E46&lt;0.5, J46 &lt; 0.5,O46&lt;0.5, T46&lt;0.5), "C1",IF(AND(E46&lt;0.5, J46 &lt; 0.5,O46&lt;0.5, T46&gt;=0.5), "B","A"))))))))</f>
+        <v>C1</v>
+      </c>
+    </row>
+    <row r="47" spans="1:28" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A47" s="3">
         <v>12</v>
       </c>
@@ -3028,8 +3691,20 @@
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="48" spans="1:22" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="Z47" s="25" t="str">
+        <f>IF(AND(C47&lt;0.5, H47 &gt;= 0.5,M47&gt;=0.5, R47&lt;0.5), "F",IF(AND(C47&lt;0.5, H47 &gt;= 0.5,M47&gt;=0.5, R47&gt;=0.5), "E2",IF(AND(C47&lt;0.5, H47 &gt;= 0.5,M47&lt;0.5, R47&lt;0.5), "E1",IF(AND(C47&lt;0.5, H47 &gt;= 0.5,M47&lt;0.5, R47&gt;=0.5), "D2",IF(AND(C47&lt;0.5, H47 &lt;0.5,M47&gt;=0.5, R47&lt;0.5), "D1",IF(AND(C47&lt;0.5, H47 &lt; 0.5,M47&gt;=0.5, R47&gt;=0.5), "C2",IF(AND(C47&lt;0.5, H47 &lt; 0.5,M47&lt;0.5, R47&lt;0.5), "C1",IF(AND(C47&lt;0.5, H47 &lt; 0.5,M47&lt;0.5, R47&gt;=0.5), "B","A"))))))))</f>
+        <v>C1</v>
+      </c>
+      <c r="AA47" s="25" t="str">
+        <f>IF(AND(D47&lt;0.5, I47 &gt;= 0.5,N47&gt;=0.5, S47&lt;0.5), "F",IF(AND(D47&lt;0.5, I47 &gt;= 0.5,N47&gt;=0.5, S47&gt;=0.5), "E2",IF(AND(D47&lt;0.5, I47 &gt;= 0.5,N47&lt;0.5, S47&lt;0.5), "E1",IF(AND(D47&lt;0.5, I47 &gt;= 0.5,N47&lt;0.5, S47&gt;=0.5), "D2",IF(AND(D47&lt;0.5, I47 &lt;0.5,N47&gt;=0.5, S47&lt;0.5), "D1",IF(AND(D47&lt;0.5, I47 &lt; 0.5,N47&gt;=0.5, S47&gt;=0.5), "C2",IF(AND(D47&lt;0.5, I47 &lt; 0.5,N47&lt;0.5, S47&lt;0.5), "C1",IF(AND(D47&lt;0.5, I47 &lt; 0.5,N47&lt;0.5, S47&gt;=0.5), "B","A"))))))))</f>
+        <v>C1</v>
+      </c>
+      <c r="AB47" s="25" t="str">
+        <f>IF(AND(E47&lt;0.5, J47 &gt;= 0.5,O47&gt;=0.5, T47&lt;0.5), "F",IF(AND(E47&lt;0.5, J47 &gt;= 0.5,O47&gt;=0.5, T47&gt;=0.5), "E2",IF(AND(E47&lt;0.5, J47 &gt;= 0.5,O47&lt;0.5, T47&lt;0.5), "E1",IF(AND(E47&lt;0.5, J47 &gt;= 0.5,O47&lt;0.5, T47&gt;=0.5), "D2",IF(AND(E47&lt;0.5, J47 &lt;0.5,O47&gt;=0.5, T47&lt;0.5), "D1",IF(AND(E47&lt;0.5, J47 &lt; 0.5,O47&gt;=0.5, T47&gt;=0.5), "C2",IF(AND(E47&lt;0.5, J47 &lt; 0.5,O47&lt;0.5, T47&lt;0.5), "C1",IF(AND(E47&lt;0.5, J47 &lt; 0.5,O47&lt;0.5, T47&gt;=0.5), "B","A"))))))))</f>
+        <v>C1</v>
+      </c>
+    </row>
+    <row r="48" spans="1:28" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A48" s="1"/>
       <c r="B48" s="1" t="s">
         <v>16</v>
@@ -3075,8 +3750,20 @@
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="49" spans="1:22" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="Z48" s="25" t="str">
+        <f>IF(AND(C48&lt;0.5, H48 &gt;= 0.5,M48&gt;=0.5, R48&lt;0.5), "F",IF(AND(C48&lt;0.5, H48 &gt;= 0.5,M48&gt;=0.5, R48&gt;=0.5), "E2",IF(AND(C48&lt;0.5, H48 &gt;= 0.5,M48&lt;0.5, R48&lt;0.5), "E1",IF(AND(C48&lt;0.5, H48 &gt;= 0.5,M48&lt;0.5, R48&gt;=0.5), "D2",IF(AND(C48&lt;0.5, H48 &lt;0.5,M48&gt;=0.5, R48&lt;0.5), "D1",IF(AND(C48&lt;0.5, H48 &lt; 0.5,M48&gt;=0.5, R48&gt;=0.5), "C2",IF(AND(C48&lt;0.5, H48 &lt; 0.5,M48&lt;0.5, R48&lt;0.5), "C1",IF(AND(C48&lt;0.5, H48 &lt; 0.5,M48&lt;0.5, R48&gt;=0.5), "B","A"))))))))</f>
+        <v>C1</v>
+      </c>
+      <c r="AA48" s="25" t="str">
+        <f>IF(AND(D48&lt;0.5, I48 &gt;= 0.5,N48&gt;=0.5, S48&lt;0.5), "F",IF(AND(D48&lt;0.5, I48 &gt;= 0.5,N48&gt;=0.5, S48&gt;=0.5), "E2",IF(AND(D48&lt;0.5, I48 &gt;= 0.5,N48&lt;0.5, S48&lt;0.5), "E1",IF(AND(D48&lt;0.5, I48 &gt;= 0.5,N48&lt;0.5, S48&gt;=0.5), "D2",IF(AND(D48&lt;0.5, I48 &lt;0.5,N48&gt;=0.5, S48&lt;0.5), "D1",IF(AND(D48&lt;0.5, I48 &lt; 0.5,N48&gt;=0.5, S48&gt;=0.5), "C2",IF(AND(D48&lt;0.5, I48 &lt; 0.5,N48&lt;0.5, S48&lt;0.5), "C1",IF(AND(D48&lt;0.5, I48 &lt; 0.5,N48&lt;0.5, S48&gt;=0.5), "B","A"))))))))</f>
+        <v>C1</v>
+      </c>
+      <c r="AB48" s="25" t="str">
+        <f>IF(AND(E48&lt;0.5, J48 &gt;= 0.5,O48&gt;=0.5, T48&lt;0.5), "F",IF(AND(E48&lt;0.5, J48 &gt;= 0.5,O48&gt;=0.5, T48&gt;=0.5), "E2",IF(AND(E48&lt;0.5, J48 &gt;= 0.5,O48&lt;0.5, T48&lt;0.5), "E1",IF(AND(E48&lt;0.5, J48 &gt;= 0.5,O48&lt;0.5, T48&gt;=0.5), "D2",IF(AND(E48&lt;0.5, J48 &lt;0.5,O48&gt;=0.5, T48&lt;0.5), "D1",IF(AND(E48&lt;0.5, J48 &lt; 0.5,O48&gt;=0.5, T48&gt;=0.5), "C2",IF(AND(E48&lt;0.5, J48 &lt; 0.5,O48&lt;0.5, T48&lt;0.5), "C1",IF(AND(E48&lt;0.5, J48 &lt; 0.5,O48&lt;0.5, T48&gt;=0.5), "B","A"))))))))</f>
+        <v>C1</v>
+      </c>
+    </row>
+    <row r="49" spans="1:28" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A49" s="1"/>
       <c r="B49" s="1" t="s">
         <v>17</v>
@@ -3122,8 +3809,20 @@
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="50" spans="1:22" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="Z49" s="25" t="str">
+        <f>IF(AND(C49&lt;0.5, H49 &gt;= 0.5,M49&gt;=0.5, R49&lt;0.5), "F",IF(AND(C49&lt;0.5, H49 &gt;= 0.5,M49&gt;=0.5, R49&gt;=0.5), "E2",IF(AND(C49&lt;0.5, H49 &gt;= 0.5,M49&lt;0.5, R49&lt;0.5), "E1",IF(AND(C49&lt;0.5, H49 &gt;= 0.5,M49&lt;0.5, R49&gt;=0.5), "D2",IF(AND(C49&lt;0.5, H49 &lt;0.5,M49&gt;=0.5, R49&lt;0.5), "D1",IF(AND(C49&lt;0.5, H49 &lt; 0.5,M49&gt;=0.5, R49&gt;=0.5), "C2",IF(AND(C49&lt;0.5, H49 &lt; 0.5,M49&lt;0.5, R49&lt;0.5), "C1",IF(AND(C49&lt;0.5, H49 &lt; 0.5,M49&lt;0.5, R49&gt;=0.5), "B","A"))))))))</f>
+        <v>C1</v>
+      </c>
+      <c r="AA49" s="25" t="str">
+        <f>IF(AND(D49&lt;0.5, I49 &gt;= 0.5,N49&gt;=0.5, S49&lt;0.5), "F",IF(AND(D49&lt;0.5, I49 &gt;= 0.5,N49&gt;=0.5, S49&gt;=0.5), "E2",IF(AND(D49&lt;0.5, I49 &gt;= 0.5,N49&lt;0.5, S49&lt;0.5), "E1",IF(AND(D49&lt;0.5, I49 &gt;= 0.5,N49&lt;0.5, S49&gt;=0.5), "D2",IF(AND(D49&lt;0.5, I49 &lt;0.5,N49&gt;=0.5, S49&lt;0.5), "D1",IF(AND(D49&lt;0.5, I49 &lt; 0.5,N49&gt;=0.5, S49&gt;=0.5), "C2",IF(AND(D49&lt;0.5, I49 &lt; 0.5,N49&lt;0.5, S49&lt;0.5), "C1",IF(AND(D49&lt;0.5, I49 &lt; 0.5,N49&lt;0.5, S49&gt;=0.5), "B","A"))))))))</f>
+        <v>C1</v>
+      </c>
+      <c r="AB49" s="25" t="str">
+        <f>IF(AND(E49&lt;0.5, J49 &gt;= 0.5,O49&gt;=0.5, T49&lt;0.5), "F",IF(AND(E49&lt;0.5, J49 &gt;= 0.5,O49&gt;=0.5, T49&gt;=0.5), "E2",IF(AND(E49&lt;0.5, J49 &gt;= 0.5,O49&lt;0.5, T49&lt;0.5), "E1",IF(AND(E49&lt;0.5, J49 &gt;= 0.5,O49&lt;0.5, T49&gt;=0.5), "D2",IF(AND(E49&lt;0.5, J49 &lt;0.5,O49&gt;=0.5, T49&lt;0.5), "D1",IF(AND(E49&lt;0.5, J49 &lt; 0.5,O49&gt;=0.5, T49&gt;=0.5), "C2",IF(AND(E49&lt;0.5, J49 &lt; 0.5,O49&lt;0.5, T49&lt;0.5), "C1",IF(AND(E49&lt;0.5, J49 &lt; 0.5,O49&lt;0.5, T49&gt;=0.5), "B","A"))))))))</f>
+        <v>C1</v>
+      </c>
+    </row>
+    <row r="50" spans="1:28" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A50" s="4"/>
       <c r="B50" s="4" t="s">
         <v>18</v>
@@ -3172,8 +3871,20 @@
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="51" spans="1:22" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="Z50" s="25" t="str">
+        <f>IF(AND(C50&lt;0.5, H50 &gt;= 0.5,M50&gt;=0.5, R50&lt;0.5), "F",IF(AND(C50&lt;0.5, H50 &gt;= 0.5,M50&gt;=0.5, R50&gt;=0.5), "E2",IF(AND(C50&lt;0.5, H50 &gt;= 0.5,M50&lt;0.5, R50&lt;0.5), "E1",IF(AND(C50&lt;0.5, H50 &gt;= 0.5,M50&lt;0.5, R50&gt;=0.5), "D2",IF(AND(C50&lt;0.5, H50 &lt;0.5,M50&gt;=0.5, R50&lt;0.5), "D1",IF(AND(C50&lt;0.5, H50 &lt; 0.5,M50&gt;=0.5, R50&gt;=0.5), "C2",IF(AND(C50&lt;0.5, H50 &lt; 0.5,M50&lt;0.5, R50&lt;0.5), "C1",IF(AND(C50&lt;0.5, H50 &lt; 0.5,M50&lt;0.5, R50&gt;=0.5), "B","A"))))))))</f>
+        <v>C1</v>
+      </c>
+      <c r="AA50" s="25" t="str">
+        <f>IF(AND(D50&lt;0.5, I50 &gt;= 0.5,N50&gt;=0.5, S50&lt;0.5), "F",IF(AND(D50&lt;0.5, I50 &gt;= 0.5,N50&gt;=0.5, S50&gt;=0.5), "E2",IF(AND(D50&lt;0.5, I50 &gt;= 0.5,N50&lt;0.5, S50&lt;0.5), "E1",IF(AND(D50&lt;0.5, I50 &gt;= 0.5,N50&lt;0.5, S50&gt;=0.5), "D2",IF(AND(D50&lt;0.5, I50 &lt;0.5,N50&gt;=0.5, S50&lt;0.5), "D1",IF(AND(D50&lt;0.5, I50 &lt; 0.5,N50&gt;=0.5, S50&gt;=0.5), "C2",IF(AND(D50&lt;0.5, I50 &lt; 0.5,N50&lt;0.5, S50&lt;0.5), "C1",IF(AND(D50&lt;0.5, I50 &lt; 0.5,N50&lt;0.5, S50&gt;=0.5), "B","A"))))))))</f>
+        <v>C1</v>
+      </c>
+      <c r="AB50" s="25" t="str">
+        <f>IF(AND(E50&lt;0.5, J50 &gt;= 0.5,O50&gt;=0.5, T50&lt;0.5), "F",IF(AND(E50&lt;0.5, J50 &gt;= 0.5,O50&gt;=0.5, T50&gt;=0.5), "E2",IF(AND(E50&lt;0.5, J50 &gt;= 0.5,O50&lt;0.5, T50&lt;0.5), "E1",IF(AND(E50&lt;0.5, J50 &gt;= 0.5,O50&lt;0.5, T50&gt;=0.5), "D2",IF(AND(E50&lt;0.5, J50 &lt;0.5,O50&gt;=0.5, T50&lt;0.5), "D1",IF(AND(E50&lt;0.5, J50 &lt; 0.5,O50&gt;=0.5, T50&gt;=0.5), "C2",IF(AND(E50&lt;0.5, J50 &lt; 0.5,O50&lt;0.5, T50&lt;0.5), "C1",IF(AND(E50&lt;0.5, J50 &lt; 0.5,O50&lt;0.5, T50&gt;=0.5), "B","A"))))))))</f>
+        <v>C1</v>
+      </c>
+    </row>
+    <row r="51" spans="1:28" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A51" s="3">
         <v>13</v>
       </c>
@@ -3224,8 +3935,20 @@
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="52" spans="1:22" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="Z51" s="25" t="str">
+        <f>IF(AND(C51&lt;0.5, H51 &gt;= 0.5,M51&gt;=0.5, R51&lt;0.5), "F",IF(AND(C51&lt;0.5, H51 &gt;= 0.5,M51&gt;=0.5, R51&gt;=0.5), "E2",IF(AND(C51&lt;0.5, H51 &gt;= 0.5,M51&lt;0.5, R51&lt;0.5), "E1",IF(AND(C51&lt;0.5, H51 &gt;= 0.5,M51&lt;0.5, R51&gt;=0.5), "D2",IF(AND(C51&lt;0.5, H51 &lt;0.5,M51&gt;=0.5, R51&lt;0.5), "D1",IF(AND(C51&lt;0.5, H51 &lt; 0.5,M51&gt;=0.5, R51&gt;=0.5), "C2",IF(AND(C51&lt;0.5, H51 &lt; 0.5,M51&lt;0.5, R51&lt;0.5), "C1",IF(AND(C51&lt;0.5, H51 &lt; 0.5,M51&lt;0.5, R51&gt;=0.5), "B","A"))))))))</f>
+        <v>C1</v>
+      </c>
+      <c r="AA51" s="25" t="str">
+        <f>IF(AND(D51&lt;0.5, I51 &gt;= 0.5,N51&gt;=0.5, S51&lt;0.5), "F",IF(AND(D51&lt;0.5, I51 &gt;= 0.5,N51&gt;=0.5, S51&gt;=0.5), "E2",IF(AND(D51&lt;0.5, I51 &gt;= 0.5,N51&lt;0.5, S51&lt;0.5), "E1",IF(AND(D51&lt;0.5, I51 &gt;= 0.5,N51&lt;0.5, S51&gt;=0.5), "D2",IF(AND(D51&lt;0.5, I51 &lt;0.5,N51&gt;=0.5, S51&lt;0.5), "D1",IF(AND(D51&lt;0.5, I51 &lt; 0.5,N51&gt;=0.5, S51&gt;=0.5), "C2",IF(AND(D51&lt;0.5, I51 &lt; 0.5,N51&lt;0.5, S51&lt;0.5), "C1",IF(AND(D51&lt;0.5, I51 &lt; 0.5,N51&lt;0.5, S51&gt;=0.5), "B","A"))))))))</f>
+        <v>C1</v>
+      </c>
+      <c r="AB51" s="25" t="str">
+        <f>IF(AND(E51&lt;0.5, J51 &gt;= 0.5,O51&gt;=0.5, T51&lt;0.5), "F",IF(AND(E51&lt;0.5, J51 &gt;= 0.5,O51&gt;=0.5, T51&gt;=0.5), "E2",IF(AND(E51&lt;0.5, J51 &gt;= 0.5,O51&lt;0.5, T51&lt;0.5), "E1",IF(AND(E51&lt;0.5, J51 &gt;= 0.5,O51&lt;0.5, T51&gt;=0.5), "D2",IF(AND(E51&lt;0.5, J51 &lt;0.5,O51&gt;=0.5, T51&lt;0.5), "D1",IF(AND(E51&lt;0.5, J51 &lt; 0.5,O51&gt;=0.5, T51&gt;=0.5), "C2",IF(AND(E51&lt;0.5, J51 &lt; 0.5,O51&lt;0.5, T51&lt;0.5), "C1",IF(AND(E51&lt;0.5, J51 &lt; 0.5,O51&lt;0.5, T51&gt;=0.5), "B","A"))))))))</f>
+        <v>C1</v>
+      </c>
+    </row>
+    <row r="52" spans="1:28" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A52" s="1"/>
       <c r="B52" s="1" t="s">
         <v>16</v>
@@ -3271,8 +3994,20 @@
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="53" spans="1:22" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="Z52" s="25" t="str">
+        <f>IF(AND(C52&lt;0.5, H52 &gt;= 0.5,M52&gt;=0.5, R52&lt;0.5), "F",IF(AND(C52&lt;0.5, H52 &gt;= 0.5,M52&gt;=0.5, R52&gt;=0.5), "E2",IF(AND(C52&lt;0.5, H52 &gt;= 0.5,M52&lt;0.5, R52&lt;0.5), "E1",IF(AND(C52&lt;0.5, H52 &gt;= 0.5,M52&lt;0.5, R52&gt;=0.5), "D2",IF(AND(C52&lt;0.5, H52 &lt;0.5,M52&gt;=0.5, R52&lt;0.5), "D1",IF(AND(C52&lt;0.5, H52 &lt; 0.5,M52&gt;=0.5, R52&gt;=0.5), "C2",IF(AND(C52&lt;0.5, H52 &lt; 0.5,M52&lt;0.5, R52&lt;0.5), "C1",IF(AND(C52&lt;0.5, H52 &lt; 0.5,M52&lt;0.5, R52&gt;=0.5), "B","A"))))))))</f>
+        <v>C1</v>
+      </c>
+      <c r="AA52" s="25" t="str">
+        <f>IF(AND(D52&lt;0.5, I52 &gt;= 0.5,N52&gt;=0.5, S52&lt;0.5), "F",IF(AND(D52&lt;0.5, I52 &gt;= 0.5,N52&gt;=0.5, S52&gt;=0.5), "E2",IF(AND(D52&lt;0.5, I52 &gt;= 0.5,N52&lt;0.5, S52&lt;0.5), "E1",IF(AND(D52&lt;0.5, I52 &gt;= 0.5,N52&lt;0.5, S52&gt;=0.5), "D2",IF(AND(D52&lt;0.5, I52 &lt;0.5,N52&gt;=0.5, S52&lt;0.5), "D1",IF(AND(D52&lt;0.5, I52 &lt; 0.5,N52&gt;=0.5, S52&gt;=0.5), "C2",IF(AND(D52&lt;0.5, I52 &lt; 0.5,N52&lt;0.5, S52&lt;0.5), "C1",IF(AND(D52&lt;0.5, I52 &lt; 0.5,N52&lt;0.5, S52&gt;=0.5), "B","A"))))))))</f>
+        <v>C1</v>
+      </c>
+      <c r="AB52" s="25" t="str">
+        <f>IF(AND(E52&lt;0.5, J52 &gt;= 0.5,O52&gt;=0.5, T52&lt;0.5), "F",IF(AND(E52&lt;0.5, J52 &gt;= 0.5,O52&gt;=0.5, T52&gt;=0.5), "E2",IF(AND(E52&lt;0.5, J52 &gt;= 0.5,O52&lt;0.5, T52&lt;0.5), "E1",IF(AND(E52&lt;0.5, J52 &gt;= 0.5,O52&lt;0.5, T52&gt;=0.5), "D2",IF(AND(E52&lt;0.5, J52 &lt;0.5,O52&gt;=0.5, T52&lt;0.5), "D1",IF(AND(E52&lt;0.5, J52 &lt; 0.5,O52&gt;=0.5, T52&gt;=0.5), "C2",IF(AND(E52&lt;0.5, J52 &lt; 0.5,O52&lt;0.5, T52&lt;0.5), "C1",IF(AND(E52&lt;0.5, J52 &lt; 0.5,O52&lt;0.5, T52&gt;=0.5), "B","A"))))))))</f>
+        <v>C1</v>
+      </c>
+    </row>
+    <row r="53" spans="1:28" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A53" s="1"/>
       <c r="B53" s="1" t="s">
         <v>17</v>
@@ -3318,8 +4053,20 @@
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="54" spans="1:22" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="Z53" s="25" t="str">
+        <f>IF(AND(C53&lt;0.5, H53 &gt;= 0.5,M53&gt;=0.5, R53&lt;0.5), "F",IF(AND(C53&lt;0.5, H53 &gt;= 0.5,M53&gt;=0.5, R53&gt;=0.5), "E2",IF(AND(C53&lt;0.5, H53 &gt;= 0.5,M53&lt;0.5, R53&lt;0.5), "E1",IF(AND(C53&lt;0.5, H53 &gt;= 0.5,M53&lt;0.5, R53&gt;=0.5), "D2",IF(AND(C53&lt;0.5, H53 &lt;0.5,M53&gt;=0.5, R53&lt;0.5), "D1",IF(AND(C53&lt;0.5, H53 &lt; 0.5,M53&gt;=0.5, R53&gt;=0.5), "C2",IF(AND(C53&lt;0.5, H53 &lt; 0.5,M53&lt;0.5, R53&lt;0.5), "C1",IF(AND(C53&lt;0.5, H53 &lt; 0.5,M53&lt;0.5, R53&gt;=0.5), "B","A"))))))))</f>
+        <v>C1</v>
+      </c>
+      <c r="AA53" s="25" t="str">
+        <f>IF(AND(D53&lt;0.5, I53 &gt;= 0.5,N53&gt;=0.5, S53&lt;0.5), "F",IF(AND(D53&lt;0.5, I53 &gt;= 0.5,N53&gt;=0.5, S53&gt;=0.5), "E2",IF(AND(D53&lt;0.5, I53 &gt;= 0.5,N53&lt;0.5, S53&lt;0.5), "E1",IF(AND(D53&lt;0.5, I53 &gt;= 0.5,N53&lt;0.5, S53&gt;=0.5), "D2",IF(AND(D53&lt;0.5, I53 &lt;0.5,N53&gt;=0.5, S53&lt;0.5), "D1",IF(AND(D53&lt;0.5, I53 &lt; 0.5,N53&gt;=0.5, S53&gt;=0.5), "C2",IF(AND(D53&lt;0.5, I53 &lt; 0.5,N53&lt;0.5, S53&lt;0.5), "C1",IF(AND(D53&lt;0.5, I53 &lt; 0.5,N53&lt;0.5, S53&gt;=0.5), "B","A"))))))))</f>
+        <v>C1</v>
+      </c>
+      <c r="AB53" s="25" t="str">
+        <f>IF(AND(E53&lt;0.5, J53 &gt;= 0.5,O53&gt;=0.5, T53&lt;0.5), "F",IF(AND(E53&lt;0.5, J53 &gt;= 0.5,O53&gt;=0.5, T53&gt;=0.5), "E2",IF(AND(E53&lt;0.5, J53 &gt;= 0.5,O53&lt;0.5, T53&lt;0.5), "E1",IF(AND(E53&lt;0.5, J53 &gt;= 0.5,O53&lt;0.5, T53&gt;=0.5), "D2",IF(AND(E53&lt;0.5, J53 &lt;0.5,O53&gt;=0.5, T53&lt;0.5), "D1",IF(AND(E53&lt;0.5, J53 &lt; 0.5,O53&gt;=0.5, T53&gt;=0.5), "C2",IF(AND(E53&lt;0.5, J53 &lt; 0.5,O53&lt;0.5, T53&lt;0.5), "C1",IF(AND(E53&lt;0.5, J53 &lt; 0.5,O53&lt;0.5, T53&gt;=0.5), "B","A"))))))))</f>
+        <v>C1</v>
+      </c>
+    </row>
+    <row r="54" spans="1:28" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A54" s="4"/>
       <c r="B54" s="4" t="s">
         <v>18</v>
@@ -3368,8 +4115,20 @@
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="55" spans="1:22" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="Z54" s="25" t="str">
+        <f>IF(AND(C54&lt;0.5, H54 &gt;= 0.5,M54&gt;=0.5, R54&lt;0.5), "F",IF(AND(C54&lt;0.5, H54 &gt;= 0.5,M54&gt;=0.5, R54&gt;=0.5), "E2",IF(AND(C54&lt;0.5, H54 &gt;= 0.5,M54&lt;0.5, R54&lt;0.5), "E1",IF(AND(C54&lt;0.5, H54 &gt;= 0.5,M54&lt;0.5, R54&gt;=0.5), "D2",IF(AND(C54&lt;0.5, H54 &lt;0.5,M54&gt;=0.5, R54&lt;0.5), "D1",IF(AND(C54&lt;0.5, H54 &lt; 0.5,M54&gt;=0.5, R54&gt;=0.5), "C2",IF(AND(C54&lt;0.5, H54 &lt; 0.5,M54&lt;0.5, R54&lt;0.5), "C1",IF(AND(C54&lt;0.5, H54 &lt; 0.5,M54&lt;0.5, R54&gt;=0.5), "B","A"))))))))</f>
+        <v>C1</v>
+      </c>
+      <c r="AA54" s="25" t="str">
+        <f>IF(AND(D54&lt;0.5, I54 &gt;= 0.5,N54&gt;=0.5, S54&lt;0.5), "F",IF(AND(D54&lt;0.5, I54 &gt;= 0.5,N54&gt;=0.5, S54&gt;=0.5), "E2",IF(AND(D54&lt;0.5, I54 &gt;= 0.5,N54&lt;0.5, S54&lt;0.5), "E1",IF(AND(D54&lt;0.5, I54 &gt;= 0.5,N54&lt;0.5, S54&gt;=0.5), "D2",IF(AND(D54&lt;0.5, I54 &lt;0.5,N54&gt;=0.5, S54&lt;0.5), "D1",IF(AND(D54&lt;0.5, I54 &lt; 0.5,N54&gt;=0.5, S54&gt;=0.5), "C2",IF(AND(D54&lt;0.5, I54 &lt; 0.5,N54&lt;0.5, S54&lt;0.5), "C1",IF(AND(D54&lt;0.5, I54 &lt; 0.5,N54&lt;0.5, S54&gt;=0.5), "B","A"))))))))</f>
+        <v>C1</v>
+      </c>
+      <c r="AB54" s="25" t="str">
+        <f>IF(AND(E54&lt;0.5, J54 &gt;= 0.5,O54&gt;=0.5, T54&lt;0.5), "F",IF(AND(E54&lt;0.5, J54 &gt;= 0.5,O54&gt;=0.5, T54&gt;=0.5), "E2",IF(AND(E54&lt;0.5, J54 &gt;= 0.5,O54&lt;0.5, T54&lt;0.5), "E1",IF(AND(E54&lt;0.5, J54 &gt;= 0.5,O54&lt;0.5, T54&gt;=0.5), "D2",IF(AND(E54&lt;0.5, J54 &lt;0.5,O54&gt;=0.5, T54&lt;0.5), "D1",IF(AND(E54&lt;0.5, J54 &lt; 0.5,O54&gt;=0.5, T54&gt;=0.5), "C2",IF(AND(E54&lt;0.5, J54 &lt; 0.5,O54&lt;0.5, T54&lt;0.5), "C1",IF(AND(E54&lt;0.5, J54 &lt; 0.5,O54&lt;0.5, T54&gt;=0.5), "B","A"))))))))</f>
+        <v>C1</v>
+      </c>
+    </row>
+    <row r="55" spans="1:28" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A55" s="3">
         <v>14</v>
       </c>
@@ -3420,8 +4179,20 @@
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="56" spans="1:22" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="Z55" s="25" t="str">
+        <f>IF(AND(C55&lt;0.5, H55 &gt;= 0.5,M55&gt;=0.5, R55&lt;0.5), "F",IF(AND(C55&lt;0.5, H55 &gt;= 0.5,M55&gt;=0.5, R55&gt;=0.5), "E2",IF(AND(C55&lt;0.5, H55 &gt;= 0.5,M55&lt;0.5, R55&lt;0.5), "E1",IF(AND(C55&lt;0.5, H55 &gt;= 0.5,M55&lt;0.5, R55&gt;=0.5), "D2",IF(AND(C55&lt;0.5, H55 &lt;0.5,M55&gt;=0.5, R55&lt;0.5), "D1",IF(AND(C55&lt;0.5, H55 &lt; 0.5,M55&gt;=0.5, R55&gt;=0.5), "C2",IF(AND(C55&lt;0.5, H55 &lt; 0.5,M55&lt;0.5, R55&lt;0.5), "C1",IF(AND(C55&lt;0.5, H55 &lt; 0.5,M55&lt;0.5, R55&gt;=0.5), "B","A"))))))))</f>
+        <v>C1</v>
+      </c>
+      <c r="AA55" s="25" t="str">
+        <f>IF(AND(D55&lt;0.5, I55 &gt;= 0.5,N55&gt;=0.5, S55&lt;0.5), "F",IF(AND(D55&lt;0.5, I55 &gt;= 0.5,N55&gt;=0.5, S55&gt;=0.5), "E2",IF(AND(D55&lt;0.5, I55 &gt;= 0.5,N55&lt;0.5, S55&lt;0.5), "E1",IF(AND(D55&lt;0.5, I55 &gt;= 0.5,N55&lt;0.5, S55&gt;=0.5), "D2",IF(AND(D55&lt;0.5, I55 &lt;0.5,N55&gt;=0.5, S55&lt;0.5), "D1",IF(AND(D55&lt;0.5, I55 &lt; 0.5,N55&gt;=0.5, S55&gt;=0.5), "C2",IF(AND(D55&lt;0.5, I55 &lt; 0.5,N55&lt;0.5, S55&lt;0.5), "C1",IF(AND(D55&lt;0.5, I55 &lt; 0.5,N55&lt;0.5, S55&gt;=0.5), "B","A"))))))))</f>
+        <v>C1</v>
+      </c>
+      <c r="AB55" s="25" t="str">
+        <f>IF(AND(E55&lt;0.5, J55 &gt;= 0.5,O55&gt;=0.5, T55&lt;0.5), "F",IF(AND(E55&lt;0.5, J55 &gt;= 0.5,O55&gt;=0.5, T55&gt;=0.5), "E2",IF(AND(E55&lt;0.5, J55 &gt;= 0.5,O55&lt;0.5, T55&lt;0.5), "E1",IF(AND(E55&lt;0.5, J55 &gt;= 0.5,O55&lt;0.5, T55&gt;=0.5), "D2",IF(AND(E55&lt;0.5, J55 &lt;0.5,O55&gt;=0.5, T55&lt;0.5), "D1",IF(AND(E55&lt;0.5, J55 &lt; 0.5,O55&gt;=0.5, T55&gt;=0.5), "C2",IF(AND(E55&lt;0.5, J55 &lt; 0.5,O55&lt;0.5, T55&lt;0.5), "C1",IF(AND(E55&lt;0.5, J55 &lt; 0.5,O55&lt;0.5, T55&gt;=0.5), "B","A"))))))))</f>
+        <v>C1</v>
+      </c>
+    </row>
+    <row r="56" spans="1:28" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A56" s="1"/>
       <c r="B56" s="1" t="s">
         <v>16</v>
@@ -3467,8 +4238,20 @@
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="57" spans="1:22" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="Z56" s="25" t="str">
+        <f>IF(AND(C56&lt;0.5, H56 &gt;= 0.5,M56&gt;=0.5, R56&lt;0.5), "F",IF(AND(C56&lt;0.5, H56 &gt;= 0.5,M56&gt;=0.5, R56&gt;=0.5), "E2",IF(AND(C56&lt;0.5, H56 &gt;= 0.5,M56&lt;0.5, R56&lt;0.5), "E1",IF(AND(C56&lt;0.5, H56 &gt;= 0.5,M56&lt;0.5, R56&gt;=0.5), "D2",IF(AND(C56&lt;0.5, H56 &lt;0.5,M56&gt;=0.5, R56&lt;0.5), "D1",IF(AND(C56&lt;0.5, H56 &lt; 0.5,M56&gt;=0.5, R56&gt;=0.5), "C2",IF(AND(C56&lt;0.5, H56 &lt; 0.5,M56&lt;0.5, R56&lt;0.5), "C1",IF(AND(C56&lt;0.5, H56 &lt; 0.5,M56&lt;0.5, R56&gt;=0.5), "B","A"))))))))</f>
+        <v>C1</v>
+      </c>
+      <c r="AA56" s="25" t="str">
+        <f>IF(AND(D56&lt;0.5, I56 &gt;= 0.5,N56&gt;=0.5, S56&lt;0.5), "F",IF(AND(D56&lt;0.5, I56 &gt;= 0.5,N56&gt;=0.5, S56&gt;=0.5), "E2",IF(AND(D56&lt;0.5, I56 &gt;= 0.5,N56&lt;0.5, S56&lt;0.5), "E1",IF(AND(D56&lt;0.5, I56 &gt;= 0.5,N56&lt;0.5, S56&gt;=0.5), "D2",IF(AND(D56&lt;0.5, I56 &lt;0.5,N56&gt;=0.5, S56&lt;0.5), "D1",IF(AND(D56&lt;0.5, I56 &lt; 0.5,N56&gt;=0.5, S56&gt;=0.5), "C2",IF(AND(D56&lt;0.5, I56 &lt; 0.5,N56&lt;0.5, S56&lt;0.5), "C1",IF(AND(D56&lt;0.5, I56 &lt; 0.5,N56&lt;0.5, S56&gt;=0.5), "B","A"))))))))</f>
+        <v>C1</v>
+      </c>
+      <c r="AB56" s="25" t="str">
+        <f>IF(AND(E56&lt;0.5, J56 &gt;= 0.5,O56&gt;=0.5, T56&lt;0.5), "F",IF(AND(E56&lt;0.5, J56 &gt;= 0.5,O56&gt;=0.5, T56&gt;=0.5), "E2",IF(AND(E56&lt;0.5, J56 &gt;= 0.5,O56&lt;0.5, T56&lt;0.5), "E1",IF(AND(E56&lt;0.5, J56 &gt;= 0.5,O56&lt;0.5, T56&gt;=0.5), "D2",IF(AND(E56&lt;0.5, J56 &lt;0.5,O56&gt;=0.5, T56&lt;0.5), "D1",IF(AND(E56&lt;0.5, J56 &lt; 0.5,O56&gt;=0.5, T56&gt;=0.5), "C2",IF(AND(E56&lt;0.5, J56 &lt; 0.5,O56&lt;0.5, T56&lt;0.5), "C1",IF(AND(E56&lt;0.5, J56 &lt; 0.5,O56&lt;0.5, T56&gt;=0.5), "B","A"))))))))</f>
+        <v>C1</v>
+      </c>
+    </row>
+    <row r="57" spans="1:28" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A57" s="1"/>
       <c r="B57" s="1" t="s">
         <v>17</v>
@@ -3514,8 +4297,20 @@
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="58" spans="1:22" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="Z57" s="25" t="str">
+        <f>IF(AND(C57&lt;0.5, H57 &gt;= 0.5,M57&gt;=0.5, R57&lt;0.5), "F",IF(AND(C57&lt;0.5, H57 &gt;= 0.5,M57&gt;=0.5, R57&gt;=0.5), "E2",IF(AND(C57&lt;0.5, H57 &gt;= 0.5,M57&lt;0.5, R57&lt;0.5), "E1",IF(AND(C57&lt;0.5, H57 &gt;= 0.5,M57&lt;0.5, R57&gt;=0.5), "D2",IF(AND(C57&lt;0.5, H57 &lt;0.5,M57&gt;=0.5, R57&lt;0.5), "D1",IF(AND(C57&lt;0.5, H57 &lt; 0.5,M57&gt;=0.5, R57&gt;=0.5), "C2",IF(AND(C57&lt;0.5, H57 &lt; 0.5,M57&lt;0.5, R57&lt;0.5), "C1",IF(AND(C57&lt;0.5, H57 &lt; 0.5,M57&lt;0.5, R57&gt;=0.5), "B","A"))))))))</f>
+        <v>C1</v>
+      </c>
+      <c r="AA57" s="25" t="str">
+        <f>IF(AND(D57&lt;0.5, I57 &gt;= 0.5,N57&gt;=0.5, S57&lt;0.5), "F",IF(AND(D57&lt;0.5, I57 &gt;= 0.5,N57&gt;=0.5, S57&gt;=0.5), "E2",IF(AND(D57&lt;0.5, I57 &gt;= 0.5,N57&lt;0.5, S57&lt;0.5), "E1",IF(AND(D57&lt;0.5, I57 &gt;= 0.5,N57&lt;0.5, S57&gt;=0.5), "D2",IF(AND(D57&lt;0.5, I57 &lt;0.5,N57&gt;=0.5, S57&lt;0.5), "D1",IF(AND(D57&lt;0.5, I57 &lt; 0.5,N57&gt;=0.5, S57&gt;=0.5), "C2",IF(AND(D57&lt;0.5, I57 &lt; 0.5,N57&lt;0.5, S57&lt;0.5), "C1",IF(AND(D57&lt;0.5, I57 &lt; 0.5,N57&lt;0.5, S57&gt;=0.5), "B","A"))))))))</f>
+        <v>C1</v>
+      </c>
+      <c r="AB57" s="25" t="str">
+        <f>IF(AND(E57&lt;0.5, J57 &gt;= 0.5,O57&gt;=0.5, T57&lt;0.5), "F",IF(AND(E57&lt;0.5, J57 &gt;= 0.5,O57&gt;=0.5, T57&gt;=0.5), "E2",IF(AND(E57&lt;0.5, J57 &gt;= 0.5,O57&lt;0.5, T57&lt;0.5), "E1",IF(AND(E57&lt;0.5, J57 &gt;= 0.5,O57&lt;0.5, T57&gt;=0.5), "D2",IF(AND(E57&lt;0.5, J57 &lt;0.5,O57&gt;=0.5, T57&lt;0.5), "D1",IF(AND(E57&lt;0.5, J57 &lt; 0.5,O57&gt;=0.5, T57&gt;=0.5), "C2",IF(AND(E57&lt;0.5, J57 &lt; 0.5,O57&lt;0.5, T57&lt;0.5), "C1",IF(AND(E57&lt;0.5, J57 &lt; 0.5,O57&lt;0.5, T57&gt;=0.5), "B","A"))))))))</f>
+        <v>C1</v>
+      </c>
+    </row>
+    <row r="58" spans="1:28" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A58" s="4"/>
       <c r="B58" s="4" t="s">
         <v>18</v>
@@ -3564,8 +4359,20 @@
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="59" spans="1:22" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="Z58" s="25" t="str">
+        <f>IF(AND(C58&lt;0.5, H58 &gt;= 0.5,M58&gt;=0.5, R58&lt;0.5), "F",IF(AND(C58&lt;0.5, H58 &gt;= 0.5,M58&gt;=0.5, R58&gt;=0.5), "E2",IF(AND(C58&lt;0.5, H58 &gt;= 0.5,M58&lt;0.5, R58&lt;0.5), "E1",IF(AND(C58&lt;0.5, H58 &gt;= 0.5,M58&lt;0.5, R58&gt;=0.5), "D2",IF(AND(C58&lt;0.5, H58 &lt;0.5,M58&gt;=0.5, R58&lt;0.5), "D1",IF(AND(C58&lt;0.5, H58 &lt; 0.5,M58&gt;=0.5, R58&gt;=0.5), "C2",IF(AND(C58&lt;0.5, H58 &lt; 0.5,M58&lt;0.5, R58&lt;0.5), "C1",IF(AND(C58&lt;0.5, H58 &lt; 0.5,M58&lt;0.5, R58&gt;=0.5), "B","A"))))))))</f>
+        <v>C1</v>
+      </c>
+      <c r="AA58" s="25" t="str">
+        <f>IF(AND(D58&lt;0.5, I58 &gt;= 0.5,N58&gt;=0.5, S58&lt;0.5), "F",IF(AND(D58&lt;0.5, I58 &gt;= 0.5,N58&gt;=0.5, S58&gt;=0.5), "E2",IF(AND(D58&lt;0.5, I58 &gt;= 0.5,N58&lt;0.5, S58&lt;0.5), "E1",IF(AND(D58&lt;0.5, I58 &gt;= 0.5,N58&lt;0.5, S58&gt;=0.5), "D2",IF(AND(D58&lt;0.5, I58 &lt;0.5,N58&gt;=0.5, S58&lt;0.5), "D1",IF(AND(D58&lt;0.5, I58 &lt; 0.5,N58&gt;=0.5, S58&gt;=0.5), "C2",IF(AND(D58&lt;0.5, I58 &lt; 0.5,N58&lt;0.5, S58&lt;0.5), "C1",IF(AND(D58&lt;0.5, I58 &lt; 0.5,N58&lt;0.5, S58&gt;=0.5), "B","A"))))))))</f>
+        <v>C1</v>
+      </c>
+      <c r="AB58" s="25" t="str">
+        <f>IF(AND(E58&lt;0.5, J58 &gt;= 0.5,O58&gt;=0.5, T58&lt;0.5), "F",IF(AND(E58&lt;0.5, J58 &gt;= 0.5,O58&gt;=0.5, T58&gt;=0.5), "E2",IF(AND(E58&lt;0.5, J58 &gt;= 0.5,O58&lt;0.5, T58&lt;0.5), "E1",IF(AND(E58&lt;0.5, J58 &gt;= 0.5,O58&lt;0.5, T58&gt;=0.5), "D2",IF(AND(E58&lt;0.5, J58 &lt;0.5,O58&gt;=0.5, T58&lt;0.5), "D1",IF(AND(E58&lt;0.5, J58 &lt; 0.5,O58&gt;=0.5, T58&gt;=0.5), "C2",IF(AND(E58&lt;0.5, J58 &lt; 0.5,O58&lt;0.5, T58&lt;0.5), "C1",IF(AND(E58&lt;0.5, J58 &lt; 0.5,O58&lt;0.5, T58&gt;=0.5), "B","A"))))))))</f>
+        <v>C1</v>
+      </c>
+    </row>
+    <row r="59" spans="1:28" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A59" s="3">
         <v>15</v>
       </c>
@@ -3616,8 +4423,20 @@
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="60" spans="1:22" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="Z59" s="25" t="str">
+        <f>IF(AND(C59&lt;0.5, H59 &gt;= 0.5,M59&gt;=0.5, R59&lt;0.5), "F",IF(AND(C59&lt;0.5, H59 &gt;= 0.5,M59&gt;=0.5, R59&gt;=0.5), "E2",IF(AND(C59&lt;0.5, H59 &gt;= 0.5,M59&lt;0.5, R59&lt;0.5), "E1",IF(AND(C59&lt;0.5, H59 &gt;= 0.5,M59&lt;0.5, R59&gt;=0.5), "D2",IF(AND(C59&lt;0.5, H59 &lt;0.5,M59&gt;=0.5, R59&lt;0.5), "D1",IF(AND(C59&lt;0.5, H59 &lt; 0.5,M59&gt;=0.5, R59&gt;=0.5), "C2",IF(AND(C59&lt;0.5, H59 &lt; 0.5,M59&lt;0.5, R59&lt;0.5), "C1",IF(AND(C59&lt;0.5, H59 &lt; 0.5,M59&lt;0.5, R59&gt;=0.5), "B","A"))))))))</f>
+        <v>C1</v>
+      </c>
+      <c r="AA59" s="25" t="str">
+        <f>IF(AND(D59&lt;0.5, I59 &gt;= 0.5,N59&gt;=0.5, S59&lt;0.5), "F",IF(AND(D59&lt;0.5, I59 &gt;= 0.5,N59&gt;=0.5, S59&gt;=0.5), "E2",IF(AND(D59&lt;0.5, I59 &gt;= 0.5,N59&lt;0.5, S59&lt;0.5), "E1",IF(AND(D59&lt;0.5, I59 &gt;= 0.5,N59&lt;0.5, S59&gt;=0.5), "D2",IF(AND(D59&lt;0.5, I59 &lt;0.5,N59&gt;=0.5, S59&lt;0.5), "D1",IF(AND(D59&lt;0.5, I59 &lt; 0.5,N59&gt;=0.5, S59&gt;=0.5), "C2",IF(AND(D59&lt;0.5, I59 &lt; 0.5,N59&lt;0.5, S59&lt;0.5), "C1",IF(AND(D59&lt;0.5, I59 &lt; 0.5,N59&lt;0.5, S59&gt;=0.5), "B","A"))))))))</f>
+        <v>C1</v>
+      </c>
+      <c r="AB59" s="25" t="str">
+        <f>IF(AND(E59&lt;0.5, J59 &gt;= 0.5,O59&gt;=0.5, T59&lt;0.5), "F",IF(AND(E59&lt;0.5, J59 &gt;= 0.5,O59&gt;=0.5, T59&gt;=0.5), "E2",IF(AND(E59&lt;0.5, J59 &gt;= 0.5,O59&lt;0.5, T59&lt;0.5), "E1",IF(AND(E59&lt;0.5, J59 &gt;= 0.5,O59&lt;0.5, T59&gt;=0.5), "D2",IF(AND(E59&lt;0.5, J59 &lt;0.5,O59&gt;=0.5, T59&lt;0.5), "D1",IF(AND(E59&lt;0.5, J59 &lt; 0.5,O59&gt;=0.5, T59&gt;=0.5), "C2",IF(AND(E59&lt;0.5, J59 &lt; 0.5,O59&lt;0.5, T59&lt;0.5), "C1",IF(AND(E59&lt;0.5, J59 &lt; 0.5,O59&lt;0.5, T59&gt;=0.5), "B","A"))))))))</f>
+        <v>C1</v>
+      </c>
+    </row>
+    <row r="60" spans="1:28" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A60" s="1"/>
       <c r="B60" s="1" t="s">
         <v>16</v>
@@ -3663,8 +4482,20 @@
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="61" spans="1:22" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="Z60" s="25" t="str">
+        <f>IF(AND(C60&lt;0.5, H60 &gt;= 0.5,M60&gt;=0.5, R60&lt;0.5), "F",IF(AND(C60&lt;0.5, H60 &gt;= 0.5,M60&gt;=0.5, R60&gt;=0.5), "E2",IF(AND(C60&lt;0.5, H60 &gt;= 0.5,M60&lt;0.5, R60&lt;0.5), "E1",IF(AND(C60&lt;0.5, H60 &gt;= 0.5,M60&lt;0.5, R60&gt;=0.5), "D2",IF(AND(C60&lt;0.5, H60 &lt;0.5,M60&gt;=0.5, R60&lt;0.5), "D1",IF(AND(C60&lt;0.5, H60 &lt; 0.5,M60&gt;=0.5, R60&gt;=0.5), "C2",IF(AND(C60&lt;0.5, H60 &lt; 0.5,M60&lt;0.5, R60&lt;0.5), "C1",IF(AND(C60&lt;0.5, H60 &lt; 0.5,M60&lt;0.5, R60&gt;=0.5), "B","A"))))))))</f>
+        <v>C1</v>
+      </c>
+      <c r="AA60" s="25" t="str">
+        <f>IF(AND(D60&lt;0.5, I60 &gt;= 0.5,N60&gt;=0.5, S60&lt;0.5), "F",IF(AND(D60&lt;0.5, I60 &gt;= 0.5,N60&gt;=0.5, S60&gt;=0.5), "E2",IF(AND(D60&lt;0.5, I60 &gt;= 0.5,N60&lt;0.5, S60&lt;0.5), "E1",IF(AND(D60&lt;0.5, I60 &gt;= 0.5,N60&lt;0.5, S60&gt;=0.5), "D2",IF(AND(D60&lt;0.5, I60 &lt;0.5,N60&gt;=0.5, S60&lt;0.5), "D1",IF(AND(D60&lt;0.5, I60 &lt; 0.5,N60&gt;=0.5, S60&gt;=0.5), "C2",IF(AND(D60&lt;0.5, I60 &lt; 0.5,N60&lt;0.5, S60&lt;0.5), "C1",IF(AND(D60&lt;0.5, I60 &lt; 0.5,N60&lt;0.5, S60&gt;=0.5), "B","A"))))))))</f>
+        <v>C1</v>
+      </c>
+      <c r="AB60" s="25" t="str">
+        <f>IF(AND(E60&lt;0.5, J60 &gt;= 0.5,O60&gt;=0.5, T60&lt;0.5), "F",IF(AND(E60&lt;0.5, J60 &gt;= 0.5,O60&gt;=0.5, T60&gt;=0.5), "E2",IF(AND(E60&lt;0.5, J60 &gt;= 0.5,O60&lt;0.5, T60&lt;0.5), "E1",IF(AND(E60&lt;0.5, J60 &gt;= 0.5,O60&lt;0.5, T60&gt;=0.5), "D2",IF(AND(E60&lt;0.5, J60 &lt;0.5,O60&gt;=0.5, T60&lt;0.5), "D1",IF(AND(E60&lt;0.5, J60 &lt; 0.5,O60&gt;=0.5, T60&gt;=0.5), "C2",IF(AND(E60&lt;0.5, J60 &lt; 0.5,O60&lt;0.5, T60&lt;0.5), "C1",IF(AND(E60&lt;0.5, J60 &lt; 0.5,O60&lt;0.5, T60&gt;=0.5), "B","A"))))))))</f>
+        <v>C1</v>
+      </c>
+    </row>
+    <row r="61" spans="1:28" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A61" s="1"/>
       <c r="B61" s="1" t="s">
         <v>17</v>
@@ -3710,8 +4541,20 @@
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="62" spans="1:22" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="Z61" s="25" t="str">
+        <f>IF(AND(C61&lt;0.5, H61 &gt;= 0.5,M61&gt;=0.5, R61&lt;0.5), "F",IF(AND(C61&lt;0.5, H61 &gt;= 0.5,M61&gt;=0.5, R61&gt;=0.5), "E2",IF(AND(C61&lt;0.5, H61 &gt;= 0.5,M61&lt;0.5, R61&lt;0.5), "E1",IF(AND(C61&lt;0.5, H61 &gt;= 0.5,M61&lt;0.5, R61&gt;=0.5), "D2",IF(AND(C61&lt;0.5, H61 &lt;0.5,M61&gt;=0.5, R61&lt;0.5), "D1",IF(AND(C61&lt;0.5, H61 &lt; 0.5,M61&gt;=0.5, R61&gt;=0.5), "C2",IF(AND(C61&lt;0.5, H61 &lt; 0.5,M61&lt;0.5, R61&lt;0.5), "C1",IF(AND(C61&lt;0.5, H61 &lt; 0.5,M61&lt;0.5, R61&gt;=0.5), "B","A"))))))))</f>
+        <v>C1</v>
+      </c>
+      <c r="AA61" s="25" t="str">
+        <f>IF(AND(D61&lt;0.5, I61 &gt;= 0.5,N61&gt;=0.5, S61&lt;0.5), "F",IF(AND(D61&lt;0.5, I61 &gt;= 0.5,N61&gt;=0.5, S61&gt;=0.5), "E2",IF(AND(D61&lt;0.5, I61 &gt;= 0.5,N61&lt;0.5, S61&lt;0.5), "E1",IF(AND(D61&lt;0.5, I61 &gt;= 0.5,N61&lt;0.5, S61&gt;=0.5), "D2",IF(AND(D61&lt;0.5, I61 &lt;0.5,N61&gt;=0.5, S61&lt;0.5), "D1",IF(AND(D61&lt;0.5, I61 &lt; 0.5,N61&gt;=0.5, S61&gt;=0.5), "C2",IF(AND(D61&lt;0.5, I61 &lt; 0.5,N61&lt;0.5, S61&lt;0.5), "C1",IF(AND(D61&lt;0.5, I61 &lt; 0.5,N61&lt;0.5, S61&gt;=0.5), "B","A"))))))))</f>
+        <v>C1</v>
+      </c>
+      <c r="AB61" s="25" t="str">
+        <f>IF(AND(E61&lt;0.5, J61 &gt;= 0.5,O61&gt;=0.5, T61&lt;0.5), "F",IF(AND(E61&lt;0.5, J61 &gt;= 0.5,O61&gt;=0.5, T61&gt;=0.5), "E2",IF(AND(E61&lt;0.5, J61 &gt;= 0.5,O61&lt;0.5, T61&lt;0.5), "E1",IF(AND(E61&lt;0.5, J61 &gt;= 0.5,O61&lt;0.5, T61&gt;=0.5), "D2",IF(AND(E61&lt;0.5, J61 &lt;0.5,O61&gt;=0.5, T61&lt;0.5), "D1",IF(AND(E61&lt;0.5, J61 &lt; 0.5,O61&gt;=0.5, T61&gt;=0.5), "C2",IF(AND(E61&lt;0.5, J61 &lt; 0.5,O61&lt;0.5, T61&lt;0.5), "C1",IF(AND(E61&lt;0.5, J61 &lt; 0.5,O61&lt;0.5, T61&gt;=0.5), "B","A"))))))))</f>
+        <v>C1</v>
+      </c>
+    </row>
+    <row r="62" spans="1:28" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A62" s="4"/>
       <c r="B62" s="4" t="s">
         <v>18</v>
@@ -3760,8 +4603,20 @@
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="63" spans="1:22" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="Z62" s="25" t="str">
+        <f>IF(AND(C62&lt;0.5, H62 &gt;= 0.5,M62&gt;=0.5, R62&lt;0.5), "F",IF(AND(C62&lt;0.5, H62 &gt;= 0.5,M62&gt;=0.5, R62&gt;=0.5), "E2",IF(AND(C62&lt;0.5, H62 &gt;= 0.5,M62&lt;0.5, R62&lt;0.5), "E1",IF(AND(C62&lt;0.5, H62 &gt;= 0.5,M62&lt;0.5, R62&gt;=0.5), "D2",IF(AND(C62&lt;0.5, H62 &lt;0.5,M62&gt;=0.5, R62&lt;0.5), "D1",IF(AND(C62&lt;0.5, H62 &lt; 0.5,M62&gt;=0.5, R62&gt;=0.5), "C2",IF(AND(C62&lt;0.5, H62 &lt; 0.5,M62&lt;0.5, R62&lt;0.5), "C1",IF(AND(C62&lt;0.5, H62 &lt; 0.5,M62&lt;0.5, R62&gt;=0.5), "B","A"))))))))</f>
+        <v>C1</v>
+      </c>
+      <c r="AA62" s="25" t="str">
+        <f>IF(AND(D62&lt;0.5, I62 &gt;= 0.5,N62&gt;=0.5, S62&lt;0.5), "F",IF(AND(D62&lt;0.5, I62 &gt;= 0.5,N62&gt;=0.5, S62&gt;=0.5), "E2",IF(AND(D62&lt;0.5, I62 &gt;= 0.5,N62&lt;0.5, S62&lt;0.5), "E1",IF(AND(D62&lt;0.5, I62 &gt;= 0.5,N62&lt;0.5, S62&gt;=0.5), "D2",IF(AND(D62&lt;0.5, I62 &lt;0.5,N62&gt;=0.5, S62&lt;0.5), "D1",IF(AND(D62&lt;0.5, I62 &lt; 0.5,N62&gt;=0.5, S62&gt;=0.5), "C2",IF(AND(D62&lt;0.5, I62 &lt; 0.5,N62&lt;0.5, S62&lt;0.5), "C1",IF(AND(D62&lt;0.5, I62 &lt; 0.5,N62&lt;0.5, S62&gt;=0.5), "B","A"))))))))</f>
+        <v>C1</v>
+      </c>
+      <c r="AB62" s="25" t="str">
+        <f>IF(AND(E62&lt;0.5, J62 &gt;= 0.5,O62&gt;=0.5, T62&lt;0.5), "F",IF(AND(E62&lt;0.5, J62 &gt;= 0.5,O62&gt;=0.5, T62&gt;=0.5), "E2",IF(AND(E62&lt;0.5, J62 &gt;= 0.5,O62&lt;0.5, T62&lt;0.5), "E1",IF(AND(E62&lt;0.5, J62 &gt;= 0.5,O62&lt;0.5, T62&gt;=0.5), "D2",IF(AND(E62&lt;0.5, J62 &lt;0.5,O62&gt;=0.5, T62&lt;0.5), "D1",IF(AND(E62&lt;0.5, J62 &lt; 0.5,O62&gt;=0.5, T62&gt;=0.5), "C2",IF(AND(E62&lt;0.5, J62 &lt; 0.5,O62&lt;0.5, T62&lt;0.5), "C1",IF(AND(E62&lt;0.5, J62 &lt; 0.5,O62&lt;0.5, T62&gt;=0.5), "B","A"))))))))</f>
+        <v>C1</v>
+      </c>
+    </row>
+    <row r="63" spans="1:28" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A63" s="3">
         <v>16</v>
       </c>
@@ -3812,8 +4667,20 @@
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="64" spans="1:22" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="Z63" s="25" t="str">
+        <f>IF(AND(C63&lt;0.5, H63 &gt;= 0.5,M63&gt;=0.5, R63&lt;0.5), "F",IF(AND(C63&lt;0.5, H63 &gt;= 0.5,M63&gt;=0.5, R63&gt;=0.5), "E2",IF(AND(C63&lt;0.5, H63 &gt;= 0.5,M63&lt;0.5, R63&lt;0.5), "E1",IF(AND(C63&lt;0.5, H63 &gt;= 0.5,M63&lt;0.5, R63&gt;=0.5), "D2",IF(AND(C63&lt;0.5, H63 &lt;0.5,M63&gt;=0.5, R63&lt;0.5), "D1",IF(AND(C63&lt;0.5, H63 &lt; 0.5,M63&gt;=0.5, R63&gt;=0.5), "C2",IF(AND(C63&lt;0.5, H63 &lt; 0.5,M63&lt;0.5, R63&lt;0.5), "C1",IF(AND(C63&lt;0.5, H63 &lt; 0.5,M63&lt;0.5, R63&gt;=0.5), "B","A"))))))))</f>
+        <v>C1</v>
+      </c>
+      <c r="AA63" s="25" t="str">
+        <f>IF(AND(D63&lt;0.5, I63 &gt;= 0.5,N63&gt;=0.5, S63&lt;0.5), "F",IF(AND(D63&lt;0.5, I63 &gt;= 0.5,N63&gt;=0.5, S63&gt;=0.5), "E2",IF(AND(D63&lt;0.5, I63 &gt;= 0.5,N63&lt;0.5, S63&lt;0.5), "E1",IF(AND(D63&lt;0.5, I63 &gt;= 0.5,N63&lt;0.5, S63&gt;=0.5), "D2",IF(AND(D63&lt;0.5, I63 &lt;0.5,N63&gt;=0.5, S63&lt;0.5), "D1",IF(AND(D63&lt;0.5, I63 &lt; 0.5,N63&gt;=0.5, S63&gt;=0.5), "C2",IF(AND(D63&lt;0.5, I63 &lt; 0.5,N63&lt;0.5, S63&lt;0.5), "C1",IF(AND(D63&lt;0.5, I63 &lt; 0.5,N63&lt;0.5, S63&gt;=0.5), "B","A"))))))))</f>
+        <v>C1</v>
+      </c>
+      <c r="AB63" s="25" t="str">
+        <f>IF(AND(E63&lt;0.5, J63 &gt;= 0.5,O63&gt;=0.5, T63&lt;0.5), "F",IF(AND(E63&lt;0.5, J63 &gt;= 0.5,O63&gt;=0.5, T63&gt;=0.5), "E2",IF(AND(E63&lt;0.5, J63 &gt;= 0.5,O63&lt;0.5, T63&lt;0.5), "E1",IF(AND(E63&lt;0.5, J63 &gt;= 0.5,O63&lt;0.5, T63&gt;=0.5), "D2",IF(AND(E63&lt;0.5, J63 &lt;0.5,O63&gt;=0.5, T63&lt;0.5), "D1",IF(AND(E63&lt;0.5, J63 &lt; 0.5,O63&gt;=0.5, T63&gt;=0.5), "C2",IF(AND(E63&lt;0.5, J63 &lt; 0.5,O63&lt;0.5, T63&lt;0.5), "C1",IF(AND(E63&lt;0.5, J63 &lt; 0.5,O63&lt;0.5, T63&gt;=0.5), "B","A"))))))))</f>
+        <v>C1</v>
+      </c>
+    </row>
+    <row r="64" spans="1:28" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A64" s="1"/>
       <c r="B64" s="1" t="s">
         <v>16</v>
@@ -3859,8 +4726,20 @@
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="65" spans="1:22" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="Z64" s="25" t="str">
+        <f>IF(AND(C64&lt;0.5, H64 &gt;= 0.5,M64&gt;=0.5, R64&lt;0.5), "F",IF(AND(C64&lt;0.5, H64 &gt;= 0.5,M64&gt;=0.5, R64&gt;=0.5), "E2",IF(AND(C64&lt;0.5, H64 &gt;= 0.5,M64&lt;0.5, R64&lt;0.5), "E1",IF(AND(C64&lt;0.5, H64 &gt;= 0.5,M64&lt;0.5, R64&gt;=0.5), "D2",IF(AND(C64&lt;0.5, H64 &lt;0.5,M64&gt;=0.5, R64&lt;0.5), "D1",IF(AND(C64&lt;0.5, H64 &lt; 0.5,M64&gt;=0.5, R64&gt;=0.5), "C2",IF(AND(C64&lt;0.5, H64 &lt; 0.5,M64&lt;0.5, R64&lt;0.5), "C1",IF(AND(C64&lt;0.5, H64 &lt; 0.5,M64&lt;0.5, R64&gt;=0.5), "B","A"))))))))</f>
+        <v>C1</v>
+      </c>
+      <c r="AA64" s="25" t="str">
+        <f>IF(AND(D64&lt;0.5, I64 &gt;= 0.5,N64&gt;=0.5, S64&lt;0.5), "F",IF(AND(D64&lt;0.5, I64 &gt;= 0.5,N64&gt;=0.5, S64&gt;=0.5), "E2",IF(AND(D64&lt;0.5, I64 &gt;= 0.5,N64&lt;0.5, S64&lt;0.5), "E1",IF(AND(D64&lt;0.5, I64 &gt;= 0.5,N64&lt;0.5, S64&gt;=0.5), "D2",IF(AND(D64&lt;0.5, I64 &lt;0.5,N64&gt;=0.5, S64&lt;0.5), "D1",IF(AND(D64&lt;0.5, I64 &lt; 0.5,N64&gt;=0.5, S64&gt;=0.5), "C2",IF(AND(D64&lt;0.5, I64 &lt; 0.5,N64&lt;0.5, S64&lt;0.5), "C1",IF(AND(D64&lt;0.5, I64 &lt; 0.5,N64&lt;0.5, S64&gt;=0.5), "B","A"))))))))</f>
+        <v>C1</v>
+      </c>
+      <c r="AB64" s="25" t="str">
+        <f>IF(AND(E64&lt;0.5, J64 &gt;= 0.5,O64&gt;=0.5, T64&lt;0.5), "F",IF(AND(E64&lt;0.5, J64 &gt;= 0.5,O64&gt;=0.5, T64&gt;=0.5), "E2",IF(AND(E64&lt;0.5, J64 &gt;= 0.5,O64&lt;0.5, T64&lt;0.5), "E1",IF(AND(E64&lt;0.5, J64 &gt;= 0.5,O64&lt;0.5, T64&gt;=0.5), "D2",IF(AND(E64&lt;0.5, J64 &lt;0.5,O64&gt;=0.5, T64&lt;0.5), "D1",IF(AND(E64&lt;0.5, J64 &lt; 0.5,O64&gt;=0.5, T64&gt;=0.5), "C2",IF(AND(E64&lt;0.5, J64 &lt; 0.5,O64&lt;0.5, T64&lt;0.5), "C1",IF(AND(E64&lt;0.5, J64 &lt; 0.5,O64&lt;0.5, T64&gt;=0.5), "B","A"))))))))</f>
+        <v>C1</v>
+      </c>
+    </row>
+    <row r="65" spans="1:28" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A65" s="1"/>
       <c r="B65" s="1" t="s">
         <v>17</v>
@@ -3906,8 +4785,20 @@
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="66" spans="1:22" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="Z65" s="25" t="str">
+        <f>IF(AND(C65&lt;0.5, H65 &gt;= 0.5,M65&gt;=0.5, R65&lt;0.5), "F",IF(AND(C65&lt;0.5, H65 &gt;= 0.5,M65&gt;=0.5, R65&gt;=0.5), "E2",IF(AND(C65&lt;0.5, H65 &gt;= 0.5,M65&lt;0.5, R65&lt;0.5), "E1",IF(AND(C65&lt;0.5, H65 &gt;= 0.5,M65&lt;0.5, R65&gt;=0.5), "D2",IF(AND(C65&lt;0.5, H65 &lt;0.5,M65&gt;=0.5, R65&lt;0.5), "D1",IF(AND(C65&lt;0.5, H65 &lt; 0.5,M65&gt;=0.5, R65&gt;=0.5), "C2",IF(AND(C65&lt;0.5, H65 &lt; 0.5,M65&lt;0.5, R65&lt;0.5), "C1",IF(AND(C65&lt;0.5, H65 &lt; 0.5,M65&lt;0.5, R65&gt;=0.5), "B","A"))))))))</f>
+        <v>C1</v>
+      </c>
+      <c r="AA65" s="25" t="str">
+        <f>IF(AND(D65&lt;0.5, I65 &gt;= 0.5,N65&gt;=0.5, S65&lt;0.5), "F",IF(AND(D65&lt;0.5, I65 &gt;= 0.5,N65&gt;=0.5, S65&gt;=0.5), "E2",IF(AND(D65&lt;0.5, I65 &gt;= 0.5,N65&lt;0.5, S65&lt;0.5), "E1",IF(AND(D65&lt;0.5, I65 &gt;= 0.5,N65&lt;0.5, S65&gt;=0.5), "D2",IF(AND(D65&lt;0.5, I65 &lt;0.5,N65&gt;=0.5, S65&lt;0.5), "D1",IF(AND(D65&lt;0.5, I65 &lt; 0.5,N65&gt;=0.5, S65&gt;=0.5), "C2",IF(AND(D65&lt;0.5, I65 &lt; 0.5,N65&lt;0.5, S65&lt;0.5), "C1",IF(AND(D65&lt;0.5, I65 &lt; 0.5,N65&lt;0.5, S65&gt;=0.5), "B","A"))))))))</f>
+        <v>C1</v>
+      </c>
+      <c r="AB65" s="25" t="str">
+        <f>IF(AND(E65&lt;0.5, J65 &gt;= 0.5,O65&gt;=0.5, T65&lt;0.5), "F",IF(AND(E65&lt;0.5, J65 &gt;= 0.5,O65&gt;=0.5, T65&gt;=0.5), "E2",IF(AND(E65&lt;0.5, J65 &gt;= 0.5,O65&lt;0.5, T65&lt;0.5), "E1",IF(AND(E65&lt;0.5, J65 &gt;= 0.5,O65&lt;0.5, T65&gt;=0.5), "D2",IF(AND(E65&lt;0.5, J65 &lt;0.5,O65&gt;=0.5, T65&lt;0.5), "D1",IF(AND(E65&lt;0.5, J65 &lt; 0.5,O65&gt;=0.5, T65&gt;=0.5), "C2",IF(AND(E65&lt;0.5, J65 &lt; 0.5,O65&lt;0.5, T65&lt;0.5), "C1",IF(AND(E65&lt;0.5, J65 &lt; 0.5,O65&lt;0.5, T65&gt;=0.5), "B","A"))))))))</f>
+        <v>C1</v>
+      </c>
+    </row>
+    <row r="66" spans="1:28" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A66" s="4"/>
       <c r="B66" s="4" t="s">
         <v>18</v>
@@ -3956,8 +4847,20 @@
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="67" spans="1:22" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="Z66" s="25" t="str">
+        <f>IF(AND(C66&lt;0.5, H66 &gt;= 0.5,M66&gt;=0.5, R66&lt;0.5), "F",IF(AND(C66&lt;0.5, H66 &gt;= 0.5,M66&gt;=0.5, R66&gt;=0.5), "E2",IF(AND(C66&lt;0.5, H66 &gt;= 0.5,M66&lt;0.5, R66&lt;0.5), "E1",IF(AND(C66&lt;0.5, H66 &gt;= 0.5,M66&lt;0.5, R66&gt;=0.5), "D2",IF(AND(C66&lt;0.5, H66 &lt;0.5,M66&gt;=0.5, R66&lt;0.5), "D1",IF(AND(C66&lt;0.5, H66 &lt; 0.5,M66&gt;=0.5, R66&gt;=0.5), "C2",IF(AND(C66&lt;0.5, H66 &lt; 0.5,M66&lt;0.5, R66&lt;0.5), "C1",IF(AND(C66&lt;0.5, H66 &lt; 0.5,M66&lt;0.5, R66&gt;=0.5), "B","A"))))))))</f>
+        <v>C1</v>
+      </c>
+      <c r="AA66" s="25" t="str">
+        <f>IF(AND(D66&lt;0.5, I66 &gt;= 0.5,N66&gt;=0.5, S66&lt;0.5), "F",IF(AND(D66&lt;0.5, I66 &gt;= 0.5,N66&gt;=0.5, S66&gt;=0.5), "E2",IF(AND(D66&lt;0.5, I66 &gt;= 0.5,N66&lt;0.5, S66&lt;0.5), "E1",IF(AND(D66&lt;0.5, I66 &gt;= 0.5,N66&lt;0.5, S66&gt;=0.5), "D2",IF(AND(D66&lt;0.5, I66 &lt;0.5,N66&gt;=0.5, S66&lt;0.5), "D1",IF(AND(D66&lt;0.5, I66 &lt; 0.5,N66&gt;=0.5, S66&gt;=0.5), "C2",IF(AND(D66&lt;0.5, I66 &lt; 0.5,N66&lt;0.5, S66&lt;0.5), "C1",IF(AND(D66&lt;0.5, I66 &lt; 0.5,N66&lt;0.5, S66&gt;=0.5), "B","A"))))))))</f>
+        <v>C1</v>
+      </c>
+      <c r="AB66" s="25" t="str">
+        <f>IF(AND(E66&lt;0.5, J66 &gt;= 0.5,O66&gt;=0.5, T66&lt;0.5), "F",IF(AND(E66&lt;0.5, J66 &gt;= 0.5,O66&gt;=0.5, T66&gt;=0.5), "E2",IF(AND(E66&lt;0.5, J66 &gt;= 0.5,O66&lt;0.5, T66&lt;0.5), "E1",IF(AND(E66&lt;0.5, J66 &gt;= 0.5,O66&lt;0.5, T66&gt;=0.5), "D2",IF(AND(E66&lt;0.5, J66 &lt;0.5,O66&gt;=0.5, T66&lt;0.5), "D1",IF(AND(E66&lt;0.5, J66 &lt; 0.5,O66&gt;=0.5, T66&gt;=0.5), "C2",IF(AND(E66&lt;0.5, J66 &lt; 0.5,O66&lt;0.5, T66&lt;0.5), "C1",IF(AND(E66&lt;0.5, J66 &lt; 0.5,O66&lt;0.5, T66&gt;=0.5), "B","A"))))))))</f>
+        <v>C1</v>
+      </c>
+    </row>
+    <row r="67" spans="1:28" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A67" s="3">
         <v>17</v>
       </c>
@@ -4008,8 +4911,20 @@
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="68" spans="1:22" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="Z67" s="25" t="str">
+        <f>IF(AND(C67&lt;0.5, H67 &gt;= 0.5,M67&gt;=0.5, R67&lt;0.5), "F",IF(AND(C67&lt;0.5, H67 &gt;= 0.5,M67&gt;=0.5, R67&gt;=0.5), "E2",IF(AND(C67&lt;0.5, H67 &gt;= 0.5,M67&lt;0.5, R67&lt;0.5), "E1",IF(AND(C67&lt;0.5, H67 &gt;= 0.5,M67&lt;0.5, R67&gt;=0.5), "D2",IF(AND(C67&lt;0.5, H67 &lt;0.5,M67&gt;=0.5, R67&lt;0.5), "D1",IF(AND(C67&lt;0.5, H67 &lt; 0.5,M67&gt;=0.5, R67&gt;=0.5), "C2",IF(AND(C67&lt;0.5, H67 &lt; 0.5,M67&lt;0.5, R67&lt;0.5), "C1",IF(AND(C67&lt;0.5, H67 &lt; 0.5,M67&lt;0.5, R67&gt;=0.5), "B","A"))))))))</f>
+        <v>C1</v>
+      </c>
+      <c r="AA67" s="25" t="str">
+        <f>IF(AND(D67&lt;0.5, I67 &gt;= 0.5,N67&gt;=0.5, S67&lt;0.5), "F",IF(AND(D67&lt;0.5, I67 &gt;= 0.5,N67&gt;=0.5, S67&gt;=0.5), "E2",IF(AND(D67&lt;0.5, I67 &gt;= 0.5,N67&lt;0.5, S67&lt;0.5), "E1",IF(AND(D67&lt;0.5, I67 &gt;= 0.5,N67&lt;0.5, S67&gt;=0.5), "D2",IF(AND(D67&lt;0.5, I67 &lt;0.5,N67&gt;=0.5, S67&lt;0.5), "D1",IF(AND(D67&lt;0.5, I67 &lt; 0.5,N67&gt;=0.5, S67&gt;=0.5), "C2",IF(AND(D67&lt;0.5, I67 &lt; 0.5,N67&lt;0.5, S67&lt;0.5), "C1",IF(AND(D67&lt;0.5, I67 &lt; 0.5,N67&lt;0.5, S67&gt;=0.5), "B","A"))))))))</f>
+        <v>C1</v>
+      </c>
+      <c r="AB67" s="25" t="str">
+        <f>IF(AND(E67&lt;0.5, J67 &gt;= 0.5,O67&gt;=0.5, T67&lt;0.5), "F",IF(AND(E67&lt;0.5, J67 &gt;= 0.5,O67&gt;=0.5, T67&gt;=0.5), "E2",IF(AND(E67&lt;0.5, J67 &gt;= 0.5,O67&lt;0.5, T67&lt;0.5), "E1",IF(AND(E67&lt;0.5, J67 &gt;= 0.5,O67&lt;0.5, T67&gt;=0.5), "D2",IF(AND(E67&lt;0.5, J67 &lt;0.5,O67&gt;=0.5, T67&lt;0.5), "D1",IF(AND(E67&lt;0.5, J67 &lt; 0.5,O67&gt;=0.5, T67&gt;=0.5), "C2",IF(AND(E67&lt;0.5, J67 &lt; 0.5,O67&lt;0.5, T67&lt;0.5), "C1",IF(AND(E67&lt;0.5, J67 &lt; 0.5,O67&lt;0.5, T67&gt;=0.5), "B","A"))))))))</f>
+        <v>C1</v>
+      </c>
+    </row>
+    <row r="68" spans="1:28" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A68" s="1"/>
       <c r="B68" s="1" t="s">
         <v>16</v>
@@ -4055,8 +4970,20 @@
         <f t="shared" ref="V68:V131" si="15">IF(R68&gt;0, (T68-R68)/R68, 0)</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="69" spans="1:22" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="Z68" s="25" t="str">
+        <f>IF(AND(C68&lt;0.5, H68 &gt;= 0.5,M68&gt;=0.5, R68&lt;0.5), "F",IF(AND(C68&lt;0.5, H68 &gt;= 0.5,M68&gt;=0.5, R68&gt;=0.5), "E2",IF(AND(C68&lt;0.5, H68 &gt;= 0.5,M68&lt;0.5, R68&lt;0.5), "E1",IF(AND(C68&lt;0.5, H68 &gt;= 0.5,M68&lt;0.5, R68&gt;=0.5), "D2",IF(AND(C68&lt;0.5, H68 &lt;0.5,M68&gt;=0.5, R68&lt;0.5), "D1",IF(AND(C68&lt;0.5, H68 &lt; 0.5,M68&gt;=0.5, R68&gt;=0.5), "C2",IF(AND(C68&lt;0.5, H68 &lt; 0.5,M68&lt;0.5, R68&lt;0.5), "C1",IF(AND(C68&lt;0.5, H68 &lt; 0.5,M68&lt;0.5, R68&gt;=0.5), "B","A"))))))))</f>
+        <v>C1</v>
+      </c>
+      <c r="AA68" s="25" t="str">
+        <f>IF(AND(D68&lt;0.5, I68 &gt;= 0.5,N68&gt;=0.5, S68&lt;0.5), "F",IF(AND(D68&lt;0.5, I68 &gt;= 0.5,N68&gt;=0.5, S68&gt;=0.5), "E2",IF(AND(D68&lt;0.5, I68 &gt;= 0.5,N68&lt;0.5, S68&lt;0.5), "E1",IF(AND(D68&lt;0.5, I68 &gt;= 0.5,N68&lt;0.5, S68&gt;=0.5), "D2",IF(AND(D68&lt;0.5, I68 &lt;0.5,N68&gt;=0.5, S68&lt;0.5), "D1",IF(AND(D68&lt;0.5, I68 &lt; 0.5,N68&gt;=0.5, S68&gt;=0.5), "C2",IF(AND(D68&lt;0.5, I68 &lt; 0.5,N68&lt;0.5, S68&lt;0.5), "C1",IF(AND(D68&lt;0.5, I68 &lt; 0.5,N68&lt;0.5, S68&gt;=0.5), "B","A"))))))))</f>
+        <v>C1</v>
+      </c>
+      <c r="AB68" s="25" t="str">
+        <f>IF(AND(E68&lt;0.5, J68 &gt;= 0.5,O68&gt;=0.5, T68&lt;0.5), "F",IF(AND(E68&lt;0.5, J68 &gt;= 0.5,O68&gt;=0.5, T68&gt;=0.5), "E2",IF(AND(E68&lt;0.5, J68 &gt;= 0.5,O68&lt;0.5, T68&lt;0.5), "E1",IF(AND(E68&lt;0.5, J68 &gt;= 0.5,O68&lt;0.5, T68&gt;=0.5), "D2",IF(AND(E68&lt;0.5, J68 &lt;0.5,O68&gt;=0.5, T68&lt;0.5), "D1",IF(AND(E68&lt;0.5, J68 &lt; 0.5,O68&gt;=0.5, T68&gt;=0.5), "C2",IF(AND(E68&lt;0.5, J68 &lt; 0.5,O68&lt;0.5, T68&lt;0.5), "C1",IF(AND(E68&lt;0.5, J68 &lt; 0.5,O68&lt;0.5, T68&gt;=0.5), "B","A"))))))))</f>
+        <v>C1</v>
+      </c>
+    </row>
+    <row r="69" spans="1:28" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A69" s="1"/>
       <c r="B69" s="1" t="s">
         <v>17</v>
@@ -4102,8 +5029,20 @@
         <f t="shared" si="15"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="70" spans="1:22" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="Z69" s="25" t="str">
+        <f>IF(AND(C69&lt;0.5, H69 &gt;= 0.5,M69&gt;=0.5, R69&lt;0.5), "F",IF(AND(C69&lt;0.5, H69 &gt;= 0.5,M69&gt;=0.5, R69&gt;=0.5), "E2",IF(AND(C69&lt;0.5, H69 &gt;= 0.5,M69&lt;0.5, R69&lt;0.5), "E1",IF(AND(C69&lt;0.5, H69 &gt;= 0.5,M69&lt;0.5, R69&gt;=0.5), "D2",IF(AND(C69&lt;0.5, H69 &lt;0.5,M69&gt;=0.5, R69&lt;0.5), "D1",IF(AND(C69&lt;0.5, H69 &lt; 0.5,M69&gt;=0.5, R69&gt;=0.5), "C2",IF(AND(C69&lt;0.5, H69 &lt; 0.5,M69&lt;0.5, R69&lt;0.5), "C1",IF(AND(C69&lt;0.5, H69 &lt; 0.5,M69&lt;0.5, R69&gt;=0.5), "B","A"))))))))</f>
+        <v>C1</v>
+      </c>
+      <c r="AA69" s="25" t="str">
+        <f>IF(AND(D69&lt;0.5, I69 &gt;= 0.5,N69&gt;=0.5, S69&lt;0.5), "F",IF(AND(D69&lt;0.5, I69 &gt;= 0.5,N69&gt;=0.5, S69&gt;=0.5), "E2",IF(AND(D69&lt;0.5, I69 &gt;= 0.5,N69&lt;0.5, S69&lt;0.5), "E1",IF(AND(D69&lt;0.5, I69 &gt;= 0.5,N69&lt;0.5, S69&gt;=0.5), "D2",IF(AND(D69&lt;0.5, I69 &lt;0.5,N69&gt;=0.5, S69&lt;0.5), "D1",IF(AND(D69&lt;0.5, I69 &lt; 0.5,N69&gt;=0.5, S69&gt;=0.5), "C2",IF(AND(D69&lt;0.5, I69 &lt; 0.5,N69&lt;0.5, S69&lt;0.5), "C1",IF(AND(D69&lt;0.5, I69 &lt; 0.5,N69&lt;0.5, S69&gt;=0.5), "B","A"))))))))</f>
+        <v>C1</v>
+      </c>
+      <c r="AB69" s="25" t="str">
+        <f>IF(AND(E69&lt;0.5, J69 &gt;= 0.5,O69&gt;=0.5, T69&lt;0.5), "F",IF(AND(E69&lt;0.5, J69 &gt;= 0.5,O69&gt;=0.5, T69&gt;=0.5), "E2",IF(AND(E69&lt;0.5, J69 &gt;= 0.5,O69&lt;0.5, T69&lt;0.5), "E1",IF(AND(E69&lt;0.5, J69 &gt;= 0.5,O69&lt;0.5, T69&gt;=0.5), "D2",IF(AND(E69&lt;0.5, J69 &lt;0.5,O69&gt;=0.5, T69&lt;0.5), "D1",IF(AND(E69&lt;0.5, J69 &lt; 0.5,O69&gt;=0.5, T69&gt;=0.5), "C2",IF(AND(E69&lt;0.5, J69 &lt; 0.5,O69&lt;0.5, T69&lt;0.5), "C1",IF(AND(E69&lt;0.5, J69 &lt; 0.5,O69&lt;0.5, T69&gt;=0.5), "B","A"))))))))</f>
+        <v>C1</v>
+      </c>
+    </row>
+    <row r="70" spans="1:28" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A70" s="4"/>
       <c r="B70" s="4" t="s">
         <v>18</v>
@@ -4152,8 +5091,20 @@
         <f t="shared" si="15"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="71" spans="1:22" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="Z70" s="25" t="str">
+        <f>IF(AND(C70&lt;0.5, H70 &gt;= 0.5,M70&gt;=0.5, R70&lt;0.5), "F",IF(AND(C70&lt;0.5, H70 &gt;= 0.5,M70&gt;=0.5, R70&gt;=0.5), "E2",IF(AND(C70&lt;0.5, H70 &gt;= 0.5,M70&lt;0.5, R70&lt;0.5), "E1",IF(AND(C70&lt;0.5, H70 &gt;= 0.5,M70&lt;0.5, R70&gt;=0.5), "D2",IF(AND(C70&lt;0.5, H70 &lt;0.5,M70&gt;=0.5, R70&lt;0.5), "D1",IF(AND(C70&lt;0.5, H70 &lt; 0.5,M70&gt;=0.5, R70&gt;=0.5), "C2",IF(AND(C70&lt;0.5, H70 &lt; 0.5,M70&lt;0.5, R70&lt;0.5), "C1",IF(AND(C70&lt;0.5, H70 &lt; 0.5,M70&lt;0.5, R70&gt;=0.5), "B","A"))))))))</f>
+        <v>C1</v>
+      </c>
+      <c r="AA70" s="25" t="str">
+        <f>IF(AND(D70&lt;0.5, I70 &gt;= 0.5,N70&gt;=0.5, S70&lt;0.5), "F",IF(AND(D70&lt;0.5, I70 &gt;= 0.5,N70&gt;=0.5, S70&gt;=0.5), "E2",IF(AND(D70&lt;0.5, I70 &gt;= 0.5,N70&lt;0.5, S70&lt;0.5), "E1",IF(AND(D70&lt;0.5, I70 &gt;= 0.5,N70&lt;0.5, S70&gt;=0.5), "D2",IF(AND(D70&lt;0.5, I70 &lt;0.5,N70&gt;=0.5, S70&lt;0.5), "D1",IF(AND(D70&lt;0.5, I70 &lt; 0.5,N70&gt;=0.5, S70&gt;=0.5), "C2",IF(AND(D70&lt;0.5, I70 &lt; 0.5,N70&lt;0.5, S70&lt;0.5), "C1",IF(AND(D70&lt;0.5, I70 &lt; 0.5,N70&lt;0.5, S70&gt;=0.5), "B","A"))))))))</f>
+        <v>C1</v>
+      </c>
+      <c r="AB70" s="25" t="str">
+        <f>IF(AND(E70&lt;0.5, J70 &gt;= 0.5,O70&gt;=0.5, T70&lt;0.5), "F",IF(AND(E70&lt;0.5, J70 &gt;= 0.5,O70&gt;=0.5, T70&gt;=0.5), "E2",IF(AND(E70&lt;0.5, J70 &gt;= 0.5,O70&lt;0.5, T70&lt;0.5), "E1",IF(AND(E70&lt;0.5, J70 &gt;= 0.5,O70&lt;0.5, T70&gt;=0.5), "D2",IF(AND(E70&lt;0.5, J70 &lt;0.5,O70&gt;=0.5, T70&lt;0.5), "D1",IF(AND(E70&lt;0.5, J70 &lt; 0.5,O70&gt;=0.5, T70&gt;=0.5), "C2",IF(AND(E70&lt;0.5, J70 &lt; 0.5,O70&lt;0.5, T70&lt;0.5), "C1",IF(AND(E70&lt;0.5, J70 &lt; 0.5,O70&lt;0.5, T70&gt;=0.5), "B","A"))))))))</f>
+        <v>C1</v>
+      </c>
+    </row>
+    <row r="71" spans="1:28" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A71" s="3">
         <v>18</v>
       </c>
@@ -4204,8 +5155,20 @@
         <f t="shared" si="15"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="72" spans="1:22" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="Z71" s="25" t="str">
+        <f>IF(AND(C71&lt;0.5, H71 &gt;= 0.5,M71&gt;=0.5, R71&lt;0.5), "F",IF(AND(C71&lt;0.5, H71 &gt;= 0.5,M71&gt;=0.5, R71&gt;=0.5), "E2",IF(AND(C71&lt;0.5, H71 &gt;= 0.5,M71&lt;0.5, R71&lt;0.5), "E1",IF(AND(C71&lt;0.5, H71 &gt;= 0.5,M71&lt;0.5, R71&gt;=0.5), "D2",IF(AND(C71&lt;0.5, H71 &lt;0.5,M71&gt;=0.5, R71&lt;0.5), "D1",IF(AND(C71&lt;0.5, H71 &lt; 0.5,M71&gt;=0.5, R71&gt;=0.5), "C2",IF(AND(C71&lt;0.5, H71 &lt; 0.5,M71&lt;0.5, R71&lt;0.5), "C1",IF(AND(C71&lt;0.5, H71 &lt; 0.5,M71&lt;0.5, R71&gt;=0.5), "B","A"))))))))</f>
+        <v>C1</v>
+      </c>
+      <c r="AA71" s="25" t="str">
+        <f>IF(AND(D71&lt;0.5, I71 &gt;= 0.5,N71&gt;=0.5, S71&lt;0.5), "F",IF(AND(D71&lt;0.5, I71 &gt;= 0.5,N71&gt;=0.5, S71&gt;=0.5), "E2",IF(AND(D71&lt;0.5, I71 &gt;= 0.5,N71&lt;0.5, S71&lt;0.5), "E1",IF(AND(D71&lt;0.5, I71 &gt;= 0.5,N71&lt;0.5, S71&gt;=0.5), "D2",IF(AND(D71&lt;0.5, I71 &lt;0.5,N71&gt;=0.5, S71&lt;0.5), "D1",IF(AND(D71&lt;0.5, I71 &lt; 0.5,N71&gt;=0.5, S71&gt;=0.5), "C2",IF(AND(D71&lt;0.5, I71 &lt; 0.5,N71&lt;0.5, S71&lt;0.5), "C1",IF(AND(D71&lt;0.5, I71 &lt; 0.5,N71&lt;0.5, S71&gt;=0.5), "B","A"))))))))</f>
+        <v>C1</v>
+      </c>
+      <c r="AB71" s="25" t="str">
+        <f>IF(AND(E71&lt;0.5, J71 &gt;= 0.5,O71&gt;=0.5, T71&lt;0.5), "F",IF(AND(E71&lt;0.5, J71 &gt;= 0.5,O71&gt;=0.5, T71&gt;=0.5), "E2",IF(AND(E71&lt;0.5, J71 &gt;= 0.5,O71&lt;0.5, T71&lt;0.5), "E1",IF(AND(E71&lt;0.5, J71 &gt;= 0.5,O71&lt;0.5, T71&gt;=0.5), "D2",IF(AND(E71&lt;0.5, J71 &lt;0.5,O71&gt;=0.5, T71&lt;0.5), "D1",IF(AND(E71&lt;0.5, J71 &lt; 0.5,O71&gt;=0.5, T71&gt;=0.5), "C2",IF(AND(E71&lt;0.5, J71 &lt; 0.5,O71&lt;0.5, T71&lt;0.5), "C1",IF(AND(E71&lt;0.5, J71 &lt; 0.5,O71&lt;0.5, T71&gt;=0.5), "B","A"))))))))</f>
+        <v>C1</v>
+      </c>
+    </row>
+    <row r="72" spans="1:28" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A72" s="1"/>
       <c r="B72" s="1" t="s">
         <v>16</v>
@@ -4251,8 +5214,20 @@
         <f t="shared" si="15"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="73" spans="1:22" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="Z72" s="25" t="str">
+        <f>IF(AND(C72&lt;0.5, H72 &gt;= 0.5,M72&gt;=0.5, R72&lt;0.5), "F",IF(AND(C72&lt;0.5, H72 &gt;= 0.5,M72&gt;=0.5, R72&gt;=0.5), "E2",IF(AND(C72&lt;0.5, H72 &gt;= 0.5,M72&lt;0.5, R72&lt;0.5), "E1",IF(AND(C72&lt;0.5, H72 &gt;= 0.5,M72&lt;0.5, R72&gt;=0.5), "D2",IF(AND(C72&lt;0.5, H72 &lt;0.5,M72&gt;=0.5, R72&lt;0.5), "D1",IF(AND(C72&lt;0.5, H72 &lt; 0.5,M72&gt;=0.5, R72&gt;=0.5), "C2",IF(AND(C72&lt;0.5, H72 &lt; 0.5,M72&lt;0.5, R72&lt;0.5), "C1",IF(AND(C72&lt;0.5, H72 &lt; 0.5,M72&lt;0.5, R72&gt;=0.5), "B","A"))))))))</f>
+        <v>C1</v>
+      </c>
+      <c r="AA72" s="25" t="str">
+        <f>IF(AND(D72&lt;0.5, I72 &gt;= 0.5,N72&gt;=0.5, S72&lt;0.5), "F",IF(AND(D72&lt;0.5, I72 &gt;= 0.5,N72&gt;=0.5, S72&gt;=0.5), "E2",IF(AND(D72&lt;0.5, I72 &gt;= 0.5,N72&lt;0.5, S72&lt;0.5), "E1",IF(AND(D72&lt;0.5, I72 &gt;= 0.5,N72&lt;0.5, S72&gt;=0.5), "D2",IF(AND(D72&lt;0.5, I72 &lt;0.5,N72&gt;=0.5, S72&lt;0.5), "D1",IF(AND(D72&lt;0.5, I72 &lt; 0.5,N72&gt;=0.5, S72&gt;=0.5), "C2",IF(AND(D72&lt;0.5, I72 &lt; 0.5,N72&lt;0.5, S72&lt;0.5), "C1",IF(AND(D72&lt;0.5, I72 &lt; 0.5,N72&lt;0.5, S72&gt;=0.5), "B","A"))))))))</f>
+        <v>C1</v>
+      </c>
+      <c r="AB72" s="25" t="str">
+        <f>IF(AND(E72&lt;0.5, J72 &gt;= 0.5,O72&gt;=0.5, T72&lt;0.5), "F",IF(AND(E72&lt;0.5, J72 &gt;= 0.5,O72&gt;=0.5, T72&gt;=0.5), "E2",IF(AND(E72&lt;0.5, J72 &gt;= 0.5,O72&lt;0.5, T72&lt;0.5), "E1",IF(AND(E72&lt;0.5, J72 &gt;= 0.5,O72&lt;0.5, T72&gt;=0.5), "D2",IF(AND(E72&lt;0.5, J72 &lt;0.5,O72&gt;=0.5, T72&lt;0.5), "D1",IF(AND(E72&lt;0.5, J72 &lt; 0.5,O72&gt;=0.5, T72&gt;=0.5), "C2",IF(AND(E72&lt;0.5, J72 &lt; 0.5,O72&lt;0.5, T72&lt;0.5), "C1",IF(AND(E72&lt;0.5, J72 &lt; 0.5,O72&lt;0.5, T72&gt;=0.5), "B","A"))))))))</f>
+        <v>C1</v>
+      </c>
+    </row>
+    <row r="73" spans="1:28" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A73" s="1"/>
       <c r="B73" s="1" t="s">
         <v>17</v>
@@ -4298,8 +5273,20 @@
         <f t="shared" si="15"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="74" spans="1:22" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="Z73" s="25" t="str">
+        <f>IF(AND(C73&lt;0.5, H73 &gt;= 0.5,M73&gt;=0.5, R73&lt;0.5), "F",IF(AND(C73&lt;0.5, H73 &gt;= 0.5,M73&gt;=0.5, R73&gt;=0.5), "E2",IF(AND(C73&lt;0.5, H73 &gt;= 0.5,M73&lt;0.5, R73&lt;0.5), "E1",IF(AND(C73&lt;0.5, H73 &gt;= 0.5,M73&lt;0.5, R73&gt;=0.5), "D2",IF(AND(C73&lt;0.5, H73 &lt;0.5,M73&gt;=0.5, R73&lt;0.5), "D1",IF(AND(C73&lt;0.5, H73 &lt; 0.5,M73&gt;=0.5, R73&gt;=0.5), "C2",IF(AND(C73&lt;0.5, H73 &lt; 0.5,M73&lt;0.5, R73&lt;0.5), "C1",IF(AND(C73&lt;0.5, H73 &lt; 0.5,M73&lt;0.5, R73&gt;=0.5), "B","A"))))))))</f>
+        <v>C1</v>
+      </c>
+      <c r="AA73" s="25" t="str">
+        <f>IF(AND(D73&lt;0.5, I73 &gt;= 0.5,N73&gt;=0.5, S73&lt;0.5), "F",IF(AND(D73&lt;0.5, I73 &gt;= 0.5,N73&gt;=0.5, S73&gt;=0.5), "E2",IF(AND(D73&lt;0.5, I73 &gt;= 0.5,N73&lt;0.5, S73&lt;0.5), "E1",IF(AND(D73&lt;0.5, I73 &gt;= 0.5,N73&lt;0.5, S73&gt;=0.5), "D2",IF(AND(D73&lt;0.5, I73 &lt;0.5,N73&gt;=0.5, S73&lt;0.5), "D1",IF(AND(D73&lt;0.5, I73 &lt; 0.5,N73&gt;=0.5, S73&gt;=0.5), "C2",IF(AND(D73&lt;0.5, I73 &lt; 0.5,N73&lt;0.5, S73&lt;0.5), "C1",IF(AND(D73&lt;0.5, I73 &lt; 0.5,N73&lt;0.5, S73&gt;=0.5), "B","A"))))))))</f>
+        <v>C1</v>
+      </c>
+      <c r="AB73" s="25" t="str">
+        <f>IF(AND(E73&lt;0.5, J73 &gt;= 0.5,O73&gt;=0.5, T73&lt;0.5), "F",IF(AND(E73&lt;0.5, J73 &gt;= 0.5,O73&gt;=0.5, T73&gt;=0.5), "E2",IF(AND(E73&lt;0.5, J73 &gt;= 0.5,O73&lt;0.5, T73&lt;0.5), "E1",IF(AND(E73&lt;0.5, J73 &gt;= 0.5,O73&lt;0.5, T73&gt;=0.5), "D2",IF(AND(E73&lt;0.5, J73 &lt;0.5,O73&gt;=0.5, T73&lt;0.5), "D1",IF(AND(E73&lt;0.5, J73 &lt; 0.5,O73&gt;=0.5, T73&gt;=0.5), "C2",IF(AND(E73&lt;0.5, J73 &lt; 0.5,O73&lt;0.5, T73&lt;0.5), "C1",IF(AND(E73&lt;0.5, J73 &lt; 0.5,O73&lt;0.5, T73&gt;=0.5), "B","A"))))))))</f>
+        <v>C1</v>
+      </c>
+    </row>
+    <row r="74" spans="1:28" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A74" s="4"/>
       <c r="B74" s="4" t="s">
         <v>18</v>
@@ -4348,8 +5335,20 @@
         <f t="shared" si="15"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="75" spans="1:22" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="Z74" s="25" t="str">
+        <f>IF(AND(C74&lt;0.5, H74 &gt;= 0.5,M74&gt;=0.5, R74&lt;0.5), "F",IF(AND(C74&lt;0.5, H74 &gt;= 0.5,M74&gt;=0.5, R74&gt;=0.5), "E2",IF(AND(C74&lt;0.5, H74 &gt;= 0.5,M74&lt;0.5, R74&lt;0.5), "E1",IF(AND(C74&lt;0.5, H74 &gt;= 0.5,M74&lt;0.5, R74&gt;=0.5), "D2",IF(AND(C74&lt;0.5, H74 &lt;0.5,M74&gt;=0.5, R74&lt;0.5), "D1",IF(AND(C74&lt;0.5, H74 &lt; 0.5,M74&gt;=0.5, R74&gt;=0.5), "C2",IF(AND(C74&lt;0.5, H74 &lt; 0.5,M74&lt;0.5, R74&lt;0.5), "C1",IF(AND(C74&lt;0.5, H74 &lt; 0.5,M74&lt;0.5, R74&gt;=0.5), "B","A"))))))))</f>
+        <v>C1</v>
+      </c>
+      <c r="AA74" s="25" t="str">
+        <f>IF(AND(D74&lt;0.5, I74 &gt;= 0.5,N74&gt;=0.5, S74&lt;0.5), "F",IF(AND(D74&lt;0.5, I74 &gt;= 0.5,N74&gt;=0.5, S74&gt;=0.5), "E2",IF(AND(D74&lt;0.5, I74 &gt;= 0.5,N74&lt;0.5, S74&lt;0.5), "E1",IF(AND(D74&lt;0.5, I74 &gt;= 0.5,N74&lt;0.5, S74&gt;=0.5), "D2",IF(AND(D74&lt;0.5, I74 &lt;0.5,N74&gt;=0.5, S74&lt;0.5), "D1",IF(AND(D74&lt;0.5, I74 &lt; 0.5,N74&gt;=0.5, S74&gt;=0.5), "C2",IF(AND(D74&lt;0.5, I74 &lt; 0.5,N74&lt;0.5, S74&lt;0.5), "C1",IF(AND(D74&lt;0.5, I74 &lt; 0.5,N74&lt;0.5, S74&gt;=0.5), "B","A"))))))))</f>
+        <v>C1</v>
+      </c>
+      <c r="AB74" s="25" t="str">
+        <f>IF(AND(E74&lt;0.5, J74 &gt;= 0.5,O74&gt;=0.5, T74&lt;0.5), "F",IF(AND(E74&lt;0.5, J74 &gt;= 0.5,O74&gt;=0.5, T74&gt;=0.5), "E2",IF(AND(E74&lt;0.5, J74 &gt;= 0.5,O74&lt;0.5, T74&lt;0.5), "E1",IF(AND(E74&lt;0.5, J74 &gt;= 0.5,O74&lt;0.5, T74&gt;=0.5), "D2",IF(AND(E74&lt;0.5, J74 &lt;0.5,O74&gt;=0.5, T74&lt;0.5), "D1",IF(AND(E74&lt;0.5, J74 &lt; 0.5,O74&gt;=0.5, T74&gt;=0.5), "C2",IF(AND(E74&lt;0.5, J74 &lt; 0.5,O74&lt;0.5, T74&lt;0.5), "C1",IF(AND(E74&lt;0.5, J74 &lt; 0.5,O74&lt;0.5, T74&gt;=0.5), "B","A"))))))))</f>
+        <v>C1</v>
+      </c>
+    </row>
+    <row r="75" spans="1:28" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A75" s="3">
         <v>19</v>
       </c>
@@ -4400,8 +5399,20 @@
         <f t="shared" si="15"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="76" spans="1:22" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="Z75" s="25" t="str">
+        <f>IF(AND(C75&lt;0.5, H75 &gt;= 0.5,M75&gt;=0.5, R75&lt;0.5), "F",IF(AND(C75&lt;0.5, H75 &gt;= 0.5,M75&gt;=0.5, R75&gt;=0.5), "E2",IF(AND(C75&lt;0.5, H75 &gt;= 0.5,M75&lt;0.5, R75&lt;0.5), "E1",IF(AND(C75&lt;0.5, H75 &gt;= 0.5,M75&lt;0.5, R75&gt;=0.5), "D2",IF(AND(C75&lt;0.5, H75 &lt;0.5,M75&gt;=0.5, R75&lt;0.5), "D1",IF(AND(C75&lt;0.5, H75 &lt; 0.5,M75&gt;=0.5, R75&gt;=0.5), "C2",IF(AND(C75&lt;0.5, H75 &lt; 0.5,M75&lt;0.5, R75&lt;0.5), "C1",IF(AND(C75&lt;0.5, H75 &lt; 0.5,M75&lt;0.5, R75&gt;=0.5), "B","A"))))))))</f>
+        <v>C1</v>
+      </c>
+      <c r="AA75" s="25" t="str">
+        <f>IF(AND(D75&lt;0.5, I75 &gt;= 0.5,N75&gt;=0.5, S75&lt;0.5), "F",IF(AND(D75&lt;0.5, I75 &gt;= 0.5,N75&gt;=0.5, S75&gt;=0.5), "E2",IF(AND(D75&lt;0.5, I75 &gt;= 0.5,N75&lt;0.5, S75&lt;0.5), "E1",IF(AND(D75&lt;0.5, I75 &gt;= 0.5,N75&lt;0.5, S75&gt;=0.5), "D2",IF(AND(D75&lt;0.5, I75 &lt;0.5,N75&gt;=0.5, S75&lt;0.5), "D1",IF(AND(D75&lt;0.5, I75 &lt; 0.5,N75&gt;=0.5, S75&gt;=0.5), "C2",IF(AND(D75&lt;0.5, I75 &lt; 0.5,N75&lt;0.5, S75&lt;0.5), "C1",IF(AND(D75&lt;0.5, I75 &lt; 0.5,N75&lt;0.5, S75&gt;=0.5), "B","A"))))))))</f>
+        <v>C1</v>
+      </c>
+      <c r="AB75" s="25" t="str">
+        <f>IF(AND(E75&lt;0.5, J75 &gt;= 0.5,O75&gt;=0.5, T75&lt;0.5), "F",IF(AND(E75&lt;0.5, J75 &gt;= 0.5,O75&gt;=0.5, T75&gt;=0.5), "E2",IF(AND(E75&lt;0.5, J75 &gt;= 0.5,O75&lt;0.5, T75&lt;0.5), "E1",IF(AND(E75&lt;0.5, J75 &gt;= 0.5,O75&lt;0.5, T75&gt;=0.5), "D2",IF(AND(E75&lt;0.5, J75 &lt;0.5,O75&gt;=0.5, T75&lt;0.5), "D1",IF(AND(E75&lt;0.5, J75 &lt; 0.5,O75&gt;=0.5, T75&gt;=0.5), "C2",IF(AND(E75&lt;0.5, J75 &lt; 0.5,O75&lt;0.5, T75&lt;0.5), "C1",IF(AND(E75&lt;0.5, J75 &lt; 0.5,O75&lt;0.5, T75&gt;=0.5), "B","A"))))))))</f>
+        <v>C1</v>
+      </c>
+    </row>
+    <row r="76" spans="1:28" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A76" s="1"/>
       <c r="B76" s="1" t="s">
         <v>16</v>
@@ -4447,8 +5458,20 @@
         <f t="shared" si="15"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="77" spans="1:22" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="Z76" s="25" t="str">
+        <f>IF(AND(C76&lt;0.5, H76 &gt;= 0.5,M76&gt;=0.5, R76&lt;0.5), "F",IF(AND(C76&lt;0.5, H76 &gt;= 0.5,M76&gt;=0.5, R76&gt;=0.5), "E2",IF(AND(C76&lt;0.5, H76 &gt;= 0.5,M76&lt;0.5, R76&lt;0.5), "E1",IF(AND(C76&lt;0.5, H76 &gt;= 0.5,M76&lt;0.5, R76&gt;=0.5), "D2",IF(AND(C76&lt;0.5, H76 &lt;0.5,M76&gt;=0.5, R76&lt;0.5), "D1",IF(AND(C76&lt;0.5, H76 &lt; 0.5,M76&gt;=0.5, R76&gt;=0.5), "C2",IF(AND(C76&lt;0.5, H76 &lt; 0.5,M76&lt;0.5, R76&lt;0.5), "C1",IF(AND(C76&lt;0.5, H76 &lt; 0.5,M76&lt;0.5, R76&gt;=0.5), "B","A"))))))))</f>
+        <v>C1</v>
+      </c>
+      <c r="AA76" s="25" t="str">
+        <f>IF(AND(D76&lt;0.5, I76 &gt;= 0.5,N76&gt;=0.5, S76&lt;0.5), "F",IF(AND(D76&lt;0.5, I76 &gt;= 0.5,N76&gt;=0.5, S76&gt;=0.5), "E2",IF(AND(D76&lt;0.5, I76 &gt;= 0.5,N76&lt;0.5, S76&lt;0.5), "E1",IF(AND(D76&lt;0.5, I76 &gt;= 0.5,N76&lt;0.5, S76&gt;=0.5), "D2",IF(AND(D76&lt;0.5, I76 &lt;0.5,N76&gt;=0.5, S76&lt;0.5), "D1",IF(AND(D76&lt;0.5, I76 &lt; 0.5,N76&gt;=0.5, S76&gt;=0.5), "C2",IF(AND(D76&lt;0.5, I76 &lt; 0.5,N76&lt;0.5, S76&lt;0.5), "C1",IF(AND(D76&lt;0.5, I76 &lt; 0.5,N76&lt;0.5, S76&gt;=0.5), "B","A"))))))))</f>
+        <v>C1</v>
+      </c>
+      <c r="AB76" s="25" t="str">
+        <f>IF(AND(E76&lt;0.5, J76 &gt;= 0.5,O76&gt;=0.5, T76&lt;0.5), "F",IF(AND(E76&lt;0.5, J76 &gt;= 0.5,O76&gt;=0.5, T76&gt;=0.5), "E2",IF(AND(E76&lt;0.5, J76 &gt;= 0.5,O76&lt;0.5, T76&lt;0.5), "E1",IF(AND(E76&lt;0.5, J76 &gt;= 0.5,O76&lt;0.5, T76&gt;=0.5), "D2",IF(AND(E76&lt;0.5, J76 &lt;0.5,O76&gt;=0.5, T76&lt;0.5), "D1",IF(AND(E76&lt;0.5, J76 &lt; 0.5,O76&gt;=0.5, T76&gt;=0.5), "C2",IF(AND(E76&lt;0.5, J76 &lt; 0.5,O76&lt;0.5, T76&lt;0.5), "C1",IF(AND(E76&lt;0.5, J76 &lt; 0.5,O76&lt;0.5, T76&gt;=0.5), "B","A"))))))))</f>
+        <v>C1</v>
+      </c>
+    </row>
+    <row r="77" spans="1:28" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A77" s="1"/>
       <c r="B77" s="1" t="s">
         <v>17</v>
@@ -4494,8 +5517,20 @@
         <f t="shared" si="15"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="78" spans="1:22" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="Z77" s="25" t="str">
+        <f>IF(AND(C77&lt;0.5, H77 &gt;= 0.5,M77&gt;=0.5, R77&lt;0.5), "F",IF(AND(C77&lt;0.5, H77 &gt;= 0.5,M77&gt;=0.5, R77&gt;=0.5), "E2",IF(AND(C77&lt;0.5, H77 &gt;= 0.5,M77&lt;0.5, R77&lt;0.5), "E1",IF(AND(C77&lt;0.5, H77 &gt;= 0.5,M77&lt;0.5, R77&gt;=0.5), "D2",IF(AND(C77&lt;0.5, H77 &lt;0.5,M77&gt;=0.5, R77&lt;0.5), "D1",IF(AND(C77&lt;0.5, H77 &lt; 0.5,M77&gt;=0.5, R77&gt;=0.5), "C2",IF(AND(C77&lt;0.5, H77 &lt; 0.5,M77&lt;0.5, R77&lt;0.5), "C1",IF(AND(C77&lt;0.5, H77 &lt; 0.5,M77&lt;0.5, R77&gt;=0.5), "B","A"))))))))</f>
+        <v>C1</v>
+      </c>
+      <c r="AA77" s="25" t="str">
+        <f>IF(AND(D77&lt;0.5, I77 &gt;= 0.5,N77&gt;=0.5, S77&lt;0.5), "F",IF(AND(D77&lt;0.5, I77 &gt;= 0.5,N77&gt;=0.5, S77&gt;=0.5), "E2",IF(AND(D77&lt;0.5, I77 &gt;= 0.5,N77&lt;0.5, S77&lt;0.5), "E1",IF(AND(D77&lt;0.5, I77 &gt;= 0.5,N77&lt;0.5, S77&gt;=0.5), "D2",IF(AND(D77&lt;0.5, I77 &lt;0.5,N77&gt;=0.5, S77&lt;0.5), "D1",IF(AND(D77&lt;0.5, I77 &lt; 0.5,N77&gt;=0.5, S77&gt;=0.5), "C2",IF(AND(D77&lt;0.5, I77 &lt; 0.5,N77&lt;0.5, S77&lt;0.5), "C1",IF(AND(D77&lt;0.5, I77 &lt; 0.5,N77&lt;0.5, S77&gt;=0.5), "B","A"))))))))</f>
+        <v>C1</v>
+      </c>
+      <c r="AB77" s="25" t="str">
+        <f>IF(AND(E77&lt;0.5, J77 &gt;= 0.5,O77&gt;=0.5, T77&lt;0.5), "F",IF(AND(E77&lt;0.5, J77 &gt;= 0.5,O77&gt;=0.5, T77&gt;=0.5), "E2",IF(AND(E77&lt;0.5, J77 &gt;= 0.5,O77&lt;0.5, T77&lt;0.5), "E1",IF(AND(E77&lt;0.5, J77 &gt;= 0.5,O77&lt;0.5, T77&gt;=0.5), "D2",IF(AND(E77&lt;0.5, J77 &lt;0.5,O77&gt;=0.5, T77&lt;0.5), "D1",IF(AND(E77&lt;0.5, J77 &lt; 0.5,O77&gt;=0.5, T77&gt;=0.5), "C2",IF(AND(E77&lt;0.5, J77 &lt; 0.5,O77&lt;0.5, T77&lt;0.5), "C1",IF(AND(E77&lt;0.5, J77 &lt; 0.5,O77&lt;0.5, T77&gt;=0.5), "B","A"))))))))</f>
+        <v>C1</v>
+      </c>
+    </row>
+    <row r="78" spans="1:28" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A78" s="4"/>
       <c r="B78" s="4" t="s">
         <v>18</v>
@@ -4544,8 +5579,20 @@
         <f t="shared" si="15"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="79" spans="1:22" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="Z78" s="25" t="str">
+        <f>IF(AND(C78&lt;0.5, H78 &gt;= 0.5,M78&gt;=0.5, R78&lt;0.5), "F",IF(AND(C78&lt;0.5, H78 &gt;= 0.5,M78&gt;=0.5, R78&gt;=0.5), "E2",IF(AND(C78&lt;0.5, H78 &gt;= 0.5,M78&lt;0.5, R78&lt;0.5), "E1",IF(AND(C78&lt;0.5, H78 &gt;= 0.5,M78&lt;0.5, R78&gt;=0.5), "D2",IF(AND(C78&lt;0.5, H78 &lt;0.5,M78&gt;=0.5, R78&lt;0.5), "D1",IF(AND(C78&lt;0.5, H78 &lt; 0.5,M78&gt;=0.5, R78&gt;=0.5), "C2",IF(AND(C78&lt;0.5, H78 &lt; 0.5,M78&lt;0.5, R78&lt;0.5), "C1",IF(AND(C78&lt;0.5, H78 &lt; 0.5,M78&lt;0.5, R78&gt;=0.5), "B","A"))))))))</f>
+        <v>C1</v>
+      </c>
+      <c r="AA78" s="25" t="str">
+        <f>IF(AND(D78&lt;0.5, I78 &gt;= 0.5,N78&gt;=0.5, S78&lt;0.5), "F",IF(AND(D78&lt;0.5, I78 &gt;= 0.5,N78&gt;=0.5, S78&gt;=0.5), "E2",IF(AND(D78&lt;0.5, I78 &gt;= 0.5,N78&lt;0.5, S78&lt;0.5), "E1",IF(AND(D78&lt;0.5, I78 &gt;= 0.5,N78&lt;0.5, S78&gt;=0.5), "D2",IF(AND(D78&lt;0.5, I78 &lt;0.5,N78&gt;=0.5, S78&lt;0.5), "D1",IF(AND(D78&lt;0.5, I78 &lt; 0.5,N78&gt;=0.5, S78&gt;=0.5), "C2",IF(AND(D78&lt;0.5, I78 &lt; 0.5,N78&lt;0.5, S78&lt;0.5), "C1",IF(AND(D78&lt;0.5, I78 &lt; 0.5,N78&lt;0.5, S78&gt;=0.5), "B","A"))))))))</f>
+        <v>C1</v>
+      </c>
+      <c r="AB78" s="25" t="str">
+        <f>IF(AND(E78&lt;0.5, J78 &gt;= 0.5,O78&gt;=0.5, T78&lt;0.5), "F",IF(AND(E78&lt;0.5, J78 &gt;= 0.5,O78&gt;=0.5, T78&gt;=0.5), "E2",IF(AND(E78&lt;0.5, J78 &gt;= 0.5,O78&lt;0.5, T78&lt;0.5), "E1",IF(AND(E78&lt;0.5, J78 &gt;= 0.5,O78&lt;0.5, T78&gt;=0.5), "D2",IF(AND(E78&lt;0.5, J78 &lt;0.5,O78&gt;=0.5, T78&lt;0.5), "D1",IF(AND(E78&lt;0.5, J78 &lt; 0.5,O78&gt;=0.5, T78&gt;=0.5), "C2",IF(AND(E78&lt;0.5, J78 &lt; 0.5,O78&lt;0.5, T78&lt;0.5), "C1",IF(AND(E78&lt;0.5, J78 &lt; 0.5,O78&lt;0.5, T78&gt;=0.5), "B","A"))))))))</f>
+        <v>C1</v>
+      </c>
+    </row>
+    <row r="79" spans="1:28" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A79" s="3">
         <v>20</v>
       </c>
@@ -4596,8 +5643,20 @@
         <f t="shared" si="15"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="80" spans="1:22" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="Z79" s="25" t="str">
+        <f>IF(AND(C79&lt;0.5, H79 &gt;= 0.5,M79&gt;=0.5, R79&lt;0.5), "F",IF(AND(C79&lt;0.5, H79 &gt;= 0.5,M79&gt;=0.5, R79&gt;=0.5), "E2",IF(AND(C79&lt;0.5, H79 &gt;= 0.5,M79&lt;0.5, R79&lt;0.5), "E1",IF(AND(C79&lt;0.5, H79 &gt;= 0.5,M79&lt;0.5, R79&gt;=0.5), "D2",IF(AND(C79&lt;0.5, H79 &lt;0.5,M79&gt;=0.5, R79&lt;0.5), "D1",IF(AND(C79&lt;0.5, H79 &lt; 0.5,M79&gt;=0.5, R79&gt;=0.5), "C2",IF(AND(C79&lt;0.5, H79 &lt; 0.5,M79&lt;0.5, R79&lt;0.5), "C1",IF(AND(C79&lt;0.5, H79 &lt; 0.5,M79&lt;0.5, R79&gt;=0.5), "B","A"))))))))</f>
+        <v>C1</v>
+      </c>
+      <c r="AA79" s="25" t="str">
+        <f>IF(AND(D79&lt;0.5, I79 &gt;= 0.5,N79&gt;=0.5, S79&lt;0.5), "F",IF(AND(D79&lt;0.5, I79 &gt;= 0.5,N79&gt;=0.5, S79&gt;=0.5), "E2",IF(AND(D79&lt;0.5, I79 &gt;= 0.5,N79&lt;0.5, S79&lt;0.5), "E1",IF(AND(D79&lt;0.5, I79 &gt;= 0.5,N79&lt;0.5, S79&gt;=0.5), "D2",IF(AND(D79&lt;0.5, I79 &lt;0.5,N79&gt;=0.5, S79&lt;0.5), "D1",IF(AND(D79&lt;0.5, I79 &lt; 0.5,N79&gt;=0.5, S79&gt;=0.5), "C2",IF(AND(D79&lt;0.5, I79 &lt; 0.5,N79&lt;0.5, S79&lt;0.5), "C1",IF(AND(D79&lt;0.5, I79 &lt; 0.5,N79&lt;0.5, S79&gt;=0.5), "B","A"))))))))</f>
+        <v>C1</v>
+      </c>
+      <c r="AB79" s="25" t="str">
+        <f>IF(AND(E79&lt;0.5, J79 &gt;= 0.5,O79&gt;=0.5, T79&lt;0.5), "F",IF(AND(E79&lt;0.5, J79 &gt;= 0.5,O79&gt;=0.5, T79&gt;=0.5), "E2",IF(AND(E79&lt;0.5, J79 &gt;= 0.5,O79&lt;0.5, T79&lt;0.5), "E1",IF(AND(E79&lt;0.5, J79 &gt;= 0.5,O79&lt;0.5, T79&gt;=0.5), "D2",IF(AND(E79&lt;0.5, J79 &lt;0.5,O79&gt;=0.5, T79&lt;0.5), "D1",IF(AND(E79&lt;0.5, J79 &lt; 0.5,O79&gt;=0.5, T79&gt;=0.5), "C2",IF(AND(E79&lt;0.5, J79 &lt; 0.5,O79&lt;0.5, T79&lt;0.5), "C1",IF(AND(E79&lt;0.5, J79 &lt; 0.5,O79&lt;0.5, T79&gt;=0.5), "B","A"))))))))</f>
+        <v>C1</v>
+      </c>
+    </row>
+    <row r="80" spans="1:28" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A80" s="1"/>
       <c r="B80" s="1" t="s">
         <v>16</v>
@@ -4643,8 +5702,20 @@
         <f t="shared" si="15"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="81" spans="1:22" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="Z80" s="25" t="str">
+        <f>IF(AND(C80&lt;0.5, H80 &gt;= 0.5,M80&gt;=0.5, R80&lt;0.5), "F",IF(AND(C80&lt;0.5, H80 &gt;= 0.5,M80&gt;=0.5, R80&gt;=0.5), "E2",IF(AND(C80&lt;0.5, H80 &gt;= 0.5,M80&lt;0.5, R80&lt;0.5), "E1",IF(AND(C80&lt;0.5, H80 &gt;= 0.5,M80&lt;0.5, R80&gt;=0.5), "D2",IF(AND(C80&lt;0.5, H80 &lt;0.5,M80&gt;=0.5, R80&lt;0.5), "D1",IF(AND(C80&lt;0.5, H80 &lt; 0.5,M80&gt;=0.5, R80&gt;=0.5), "C2",IF(AND(C80&lt;0.5, H80 &lt; 0.5,M80&lt;0.5, R80&lt;0.5), "C1",IF(AND(C80&lt;0.5, H80 &lt; 0.5,M80&lt;0.5, R80&gt;=0.5), "B","A"))))))))</f>
+        <v>C1</v>
+      </c>
+      <c r="AA80" s="25" t="str">
+        <f>IF(AND(D80&lt;0.5, I80 &gt;= 0.5,N80&gt;=0.5, S80&lt;0.5), "F",IF(AND(D80&lt;0.5, I80 &gt;= 0.5,N80&gt;=0.5, S80&gt;=0.5), "E2",IF(AND(D80&lt;0.5, I80 &gt;= 0.5,N80&lt;0.5, S80&lt;0.5), "E1",IF(AND(D80&lt;0.5, I80 &gt;= 0.5,N80&lt;0.5, S80&gt;=0.5), "D2",IF(AND(D80&lt;0.5, I80 &lt;0.5,N80&gt;=0.5, S80&lt;0.5), "D1",IF(AND(D80&lt;0.5, I80 &lt; 0.5,N80&gt;=0.5, S80&gt;=0.5), "C2",IF(AND(D80&lt;0.5, I80 &lt; 0.5,N80&lt;0.5, S80&lt;0.5), "C1",IF(AND(D80&lt;0.5, I80 &lt; 0.5,N80&lt;0.5, S80&gt;=0.5), "B","A"))))))))</f>
+        <v>C1</v>
+      </c>
+      <c r="AB80" s="25" t="str">
+        <f>IF(AND(E80&lt;0.5, J80 &gt;= 0.5,O80&gt;=0.5, T80&lt;0.5), "F",IF(AND(E80&lt;0.5, J80 &gt;= 0.5,O80&gt;=0.5, T80&gt;=0.5), "E2",IF(AND(E80&lt;0.5, J80 &gt;= 0.5,O80&lt;0.5, T80&lt;0.5), "E1",IF(AND(E80&lt;0.5, J80 &gt;= 0.5,O80&lt;0.5, T80&gt;=0.5), "D2",IF(AND(E80&lt;0.5, J80 &lt;0.5,O80&gt;=0.5, T80&lt;0.5), "D1",IF(AND(E80&lt;0.5, J80 &lt; 0.5,O80&gt;=0.5, T80&gt;=0.5), "C2",IF(AND(E80&lt;0.5, J80 &lt; 0.5,O80&lt;0.5, T80&lt;0.5), "C1",IF(AND(E80&lt;0.5, J80 &lt; 0.5,O80&lt;0.5, T80&gt;=0.5), "B","A"))))))))</f>
+        <v>C1</v>
+      </c>
+    </row>
+    <row r="81" spans="1:28" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A81" s="1"/>
       <c r="B81" s="1" t="s">
         <v>17</v>
@@ -4690,8 +5761,20 @@
         <f t="shared" si="15"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="82" spans="1:22" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="Z81" s="25" t="str">
+        <f>IF(AND(C81&lt;0.5, H81 &gt;= 0.5,M81&gt;=0.5, R81&lt;0.5), "F",IF(AND(C81&lt;0.5, H81 &gt;= 0.5,M81&gt;=0.5, R81&gt;=0.5), "E2",IF(AND(C81&lt;0.5, H81 &gt;= 0.5,M81&lt;0.5, R81&lt;0.5), "E1",IF(AND(C81&lt;0.5, H81 &gt;= 0.5,M81&lt;0.5, R81&gt;=0.5), "D2",IF(AND(C81&lt;0.5, H81 &lt;0.5,M81&gt;=0.5, R81&lt;0.5), "D1",IF(AND(C81&lt;0.5, H81 &lt; 0.5,M81&gt;=0.5, R81&gt;=0.5), "C2",IF(AND(C81&lt;0.5, H81 &lt; 0.5,M81&lt;0.5, R81&lt;0.5), "C1",IF(AND(C81&lt;0.5, H81 &lt; 0.5,M81&lt;0.5, R81&gt;=0.5), "B","A"))))))))</f>
+        <v>C1</v>
+      </c>
+      <c r="AA81" s="25" t="str">
+        <f>IF(AND(D81&lt;0.5, I81 &gt;= 0.5,N81&gt;=0.5, S81&lt;0.5), "F",IF(AND(D81&lt;0.5, I81 &gt;= 0.5,N81&gt;=0.5, S81&gt;=0.5), "E2",IF(AND(D81&lt;0.5, I81 &gt;= 0.5,N81&lt;0.5, S81&lt;0.5), "E1",IF(AND(D81&lt;0.5, I81 &gt;= 0.5,N81&lt;0.5, S81&gt;=0.5), "D2",IF(AND(D81&lt;0.5, I81 &lt;0.5,N81&gt;=0.5, S81&lt;0.5), "D1",IF(AND(D81&lt;0.5, I81 &lt; 0.5,N81&gt;=0.5, S81&gt;=0.5), "C2",IF(AND(D81&lt;0.5, I81 &lt; 0.5,N81&lt;0.5, S81&lt;0.5), "C1",IF(AND(D81&lt;0.5, I81 &lt; 0.5,N81&lt;0.5, S81&gt;=0.5), "B","A"))))))))</f>
+        <v>C1</v>
+      </c>
+      <c r="AB81" s="25" t="str">
+        <f>IF(AND(E81&lt;0.5, J81 &gt;= 0.5,O81&gt;=0.5, T81&lt;0.5), "F",IF(AND(E81&lt;0.5, J81 &gt;= 0.5,O81&gt;=0.5, T81&gt;=0.5), "E2",IF(AND(E81&lt;0.5, J81 &gt;= 0.5,O81&lt;0.5, T81&lt;0.5), "E1",IF(AND(E81&lt;0.5, J81 &gt;= 0.5,O81&lt;0.5, T81&gt;=0.5), "D2",IF(AND(E81&lt;0.5, J81 &lt;0.5,O81&gt;=0.5, T81&lt;0.5), "D1",IF(AND(E81&lt;0.5, J81 &lt; 0.5,O81&gt;=0.5, T81&gt;=0.5), "C2",IF(AND(E81&lt;0.5, J81 &lt; 0.5,O81&lt;0.5, T81&lt;0.5), "C1",IF(AND(E81&lt;0.5, J81 &lt; 0.5,O81&lt;0.5, T81&gt;=0.5), "B","A"))))))))</f>
+        <v>C1</v>
+      </c>
+    </row>
+    <row r="82" spans="1:28" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A82" s="4"/>
       <c r="B82" s="4" t="s">
         <v>18</v>
@@ -4740,8 +5823,20 @@
         <f t="shared" si="15"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="83" spans="1:22" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="Z82" s="25" t="str">
+        <f>IF(AND(C82&lt;0.5, H82 &gt;= 0.5,M82&gt;=0.5, R82&lt;0.5), "F",IF(AND(C82&lt;0.5, H82 &gt;= 0.5,M82&gt;=0.5, R82&gt;=0.5), "E2",IF(AND(C82&lt;0.5, H82 &gt;= 0.5,M82&lt;0.5, R82&lt;0.5), "E1",IF(AND(C82&lt;0.5, H82 &gt;= 0.5,M82&lt;0.5, R82&gt;=0.5), "D2",IF(AND(C82&lt;0.5, H82 &lt;0.5,M82&gt;=0.5, R82&lt;0.5), "D1",IF(AND(C82&lt;0.5, H82 &lt; 0.5,M82&gt;=0.5, R82&gt;=0.5), "C2",IF(AND(C82&lt;0.5, H82 &lt; 0.5,M82&lt;0.5, R82&lt;0.5), "C1",IF(AND(C82&lt;0.5, H82 &lt; 0.5,M82&lt;0.5, R82&gt;=0.5), "B","A"))))))))</f>
+        <v>C1</v>
+      </c>
+      <c r="AA82" s="25" t="str">
+        <f>IF(AND(D82&lt;0.5, I82 &gt;= 0.5,N82&gt;=0.5, S82&lt;0.5), "F",IF(AND(D82&lt;0.5, I82 &gt;= 0.5,N82&gt;=0.5, S82&gt;=0.5), "E2",IF(AND(D82&lt;0.5, I82 &gt;= 0.5,N82&lt;0.5, S82&lt;0.5), "E1",IF(AND(D82&lt;0.5, I82 &gt;= 0.5,N82&lt;0.5, S82&gt;=0.5), "D2",IF(AND(D82&lt;0.5, I82 &lt;0.5,N82&gt;=0.5, S82&lt;0.5), "D1",IF(AND(D82&lt;0.5, I82 &lt; 0.5,N82&gt;=0.5, S82&gt;=0.5), "C2",IF(AND(D82&lt;0.5, I82 &lt; 0.5,N82&lt;0.5, S82&lt;0.5), "C1",IF(AND(D82&lt;0.5, I82 &lt; 0.5,N82&lt;0.5, S82&gt;=0.5), "B","A"))))))))</f>
+        <v>C1</v>
+      </c>
+      <c r="AB82" s="25" t="str">
+        <f>IF(AND(E82&lt;0.5, J82 &gt;= 0.5,O82&gt;=0.5, T82&lt;0.5), "F",IF(AND(E82&lt;0.5, J82 &gt;= 0.5,O82&gt;=0.5, T82&gt;=0.5), "E2",IF(AND(E82&lt;0.5, J82 &gt;= 0.5,O82&lt;0.5, T82&lt;0.5), "E1",IF(AND(E82&lt;0.5, J82 &gt;= 0.5,O82&lt;0.5, T82&gt;=0.5), "D2",IF(AND(E82&lt;0.5, J82 &lt;0.5,O82&gt;=0.5, T82&lt;0.5), "D1",IF(AND(E82&lt;0.5, J82 &lt; 0.5,O82&gt;=0.5, T82&gt;=0.5), "C2",IF(AND(E82&lt;0.5, J82 &lt; 0.5,O82&lt;0.5, T82&lt;0.5), "C1",IF(AND(E82&lt;0.5, J82 &lt; 0.5,O82&lt;0.5, T82&gt;=0.5), "B","A"))))))))</f>
+        <v>C1</v>
+      </c>
+    </row>
+    <row r="83" spans="1:28" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A83" s="3">
         <v>21</v>
       </c>
@@ -4792,8 +5887,20 @@
         <f t="shared" si="15"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="84" spans="1:22" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="Z83" s="25" t="str">
+        <f>IF(AND(C83&lt;0.5, H83 &gt;= 0.5,M83&gt;=0.5, R83&lt;0.5), "F",IF(AND(C83&lt;0.5, H83 &gt;= 0.5,M83&gt;=0.5, R83&gt;=0.5), "E2",IF(AND(C83&lt;0.5, H83 &gt;= 0.5,M83&lt;0.5, R83&lt;0.5), "E1",IF(AND(C83&lt;0.5, H83 &gt;= 0.5,M83&lt;0.5, R83&gt;=0.5), "D2",IF(AND(C83&lt;0.5, H83 &lt;0.5,M83&gt;=0.5, R83&lt;0.5), "D1",IF(AND(C83&lt;0.5, H83 &lt; 0.5,M83&gt;=0.5, R83&gt;=0.5), "C2",IF(AND(C83&lt;0.5, H83 &lt; 0.5,M83&lt;0.5, R83&lt;0.5), "C1",IF(AND(C83&lt;0.5, H83 &lt; 0.5,M83&lt;0.5, R83&gt;=0.5), "B","A"))))))))</f>
+        <v>C1</v>
+      </c>
+      <c r="AA83" s="25" t="str">
+        <f>IF(AND(D83&lt;0.5, I83 &gt;= 0.5,N83&gt;=0.5, S83&lt;0.5), "F",IF(AND(D83&lt;0.5, I83 &gt;= 0.5,N83&gt;=0.5, S83&gt;=0.5), "E2",IF(AND(D83&lt;0.5, I83 &gt;= 0.5,N83&lt;0.5, S83&lt;0.5), "E1",IF(AND(D83&lt;0.5, I83 &gt;= 0.5,N83&lt;0.5, S83&gt;=0.5), "D2",IF(AND(D83&lt;0.5, I83 &lt;0.5,N83&gt;=0.5, S83&lt;0.5), "D1",IF(AND(D83&lt;0.5, I83 &lt; 0.5,N83&gt;=0.5, S83&gt;=0.5), "C2",IF(AND(D83&lt;0.5, I83 &lt; 0.5,N83&lt;0.5, S83&lt;0.5), "C1",IF(AND(D83&lt;0.5, I83 &lt; 0.5,N83&lt;0.5, S83&gt;=0.5), "B","A"))))))))</f>
+        <v>C1</v>
+      </c>
+      <c r="AB83" s="25" t="str">
+        <f>IF(AND(E83&lt;0.5, J83 &gt;= 0.5,O83&gt;=0.5, T83&lt;0.5), "F",IF(AND(E83&lt;0.5, J83 &gt;= 0.5,O83&gt;=0.5, T83&gt;=0.5), "E2",IF(AND(E83&lt;0.5, J83 &gt;= 0.5,O83&lt;0.5, T83&lt;0.5), "E1",IF(AND(E83&lt;0.5, J83 &gt;= 0.5,O83&lt;0.5, T83&gt;=0.5), "D2",IF(AND(E83&lt;0.5, J83 &lt;0.5,O83&gt;=0.5, T83&lt;0.5), "D1",IF(AND(E83&lt;0.5, J83 &lt; 0.5,O83&gt;=0.5, T83&gt;=0.5), "C2",IF(AND(E83&lt;0.5, J83 &lt; 0.5,O83&lt;0.5, T83&lt;0.5), "C1",IF(AND(E83&lt;0.5, J83 &lt; 0.5,O83&lt;0.5, T83&gt;=0.5), "B","A"))))))))</f>
+        <v>C1</v>
+      </c>
+    </row>
+    <row r="84" spans="1:28" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A84" s="1"/>
       <c r="B84" s="1" t="s">
         <v>16</v>
@@ -4839,8 +5946,20 @@
         <f t="shared" si="15"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="85" spans="1:22" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="Z84" s="25" t="str">
+        <f>IF(AND(C84&lt;0.5, H84 &gt;= 0.5,M84&gt;=0.5, R84&lt;0.5), "F",IF(AND(C84&lt;0.5, H84 &gt;= 0.5,M84&gt;=0.5, R84&gt;=0.5), "E2",IF(AND(C84&lt;0.5, H84 &gt;= 0.5,M84&lt;0.5, R84&lt;0.5), "E1",IF(AND(C84&lt;0.5, H84 &gt;= 0.5,M84&lt;0.5, R84&gt;=0.5), "D2",IF(AND(C84&lt;0.5, H84 &lt;0.5,M84&gt;=0.5, R84&lt;0.5), "D1",IF(AND(C84&lt;0.5, H84 &lt; 0.5,M84&gt;=0.5, R84&gt;=0.5), "C2",IF(AND(C84&lt;0.5, H84 &lt; 0.5,M84&lt;0.5, R84&lt;0.5), "C1",IF(AND(C84&lt;0.5, H84 &lt; 0.5,M84&lt;0.5, R84&gt;=0.5), "B","A"))))))))</f>
+        <v>C1</v>
+      </c>
+      <c r="AA84" s="25" t="str">
+        <f>IF(AND(D84&lt;0.5, I84 &gt;= 0.5,N84&gt;=0.5, S84&lt;0.5), "F",IF(AND(D84&lt;0.5, I84 &gt;= 0.5,N84&gt;=0.5, S84&gt;=0.5), "E2",IF(AND(D84&lt;0.5, I84 &gt;= 0.5,N84&lt;0.5, S84&lt;0.5), "E1",IF(AND(D84&lt;0.5, I84 &gt;= 0.5,N84&lt;0.5, S84&gt;=0.5), "D2",IF(AND(D84&lt;0.5, I84 &lt;0.5,N84&gt;=0.5, S84&lt;0.5), "D1",IF(AND(D84&lt;0.5, I84 &lt; 0.5,N84&gt;=0.5, S84&gt;=0.5), "C2",IF(AND(D84&lt;0.5, I84 &lt; 0.5,N84&lt;0.5, S84&lt;0.5), "C1",IF(AND(D84&lt;0.5, I84 &lt; 0.5,N84&lt;0.5, S84&gt;=0.5), "B","A"))))))))</f>
+        <v>C1</v>
+      </c>
+      <c r="AB84" s="25" t="str">
+        <f>IF(AND(E84&lt;0.5, J84 &gt;= 0.5,O84&gt;=0.5, T84&lt;0.5), "F",IF(AND(E84&lt;0.5, J84 &gt;= 0.5,O84&gt;=0.5, T84&gt;=0.5), "E2",IF(AND(E84&lt;0.5, J84 &gt;= 0.5,O84&lt;0.5, T84&lt;0.5), "E1",IF(AND(E84&lt;0.5, J84 &gt;= 0.5,O84&lt;0.5, T84&gt;=0.5), "D2",IF(AND(E84&lt;0.5, J84 &lt;0.5,O84&gt;=0.5, T84&lt;0.5), "D1",IF(AND(E84&lt;0.5, J84 &lt; 0.5,O84&gt;=0.5, T84&gt;=0.5), "C2",IF(AND(E84&lt;0.5, J84 &lt; 0.5,O84&lt;0.5, T84&lt;0.5), "C1",IF(AND(E84&lt;0.5, J84 &lt; 0.5,O84&lt;0.5, T84&gt;=0.5), "B","A"))))))))</f>
+        <v>C1</v>
+      </c>
+    </row>
+    <row r="85" spans="1:28" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A85" s="1"/>
       <c r="B85" s="1" t="s">
         <v>17</v>
@@ -4886,8 +6005,20 @@
         <f t="shared" si="15"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="86" spans="1:22" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="Z85" s="25" t="str">
+        <f>IF(AND(C85&lt;0.5, H85 &gt;= 0.5,M85&gt;=0.5, R85&lt;0.5), "F",IF(AND(C85&lt;0.5, H85 &gt;= 0.5,M85&gt;=0.5, R85&gt;=0.5), "E2",IF(AND(C85&lt;0.5, H85 &gt;= 0.5,M85&lt;0.5, R85&lt;0.5), "E1",IF(AND(C85&lt;0.5, H85 &gt;= 0.5,M85&lt;0.5, R85&gt;=0.5), "D2",IF(AND(C85&lt;0.5, H85 &lt;0.5,M85&gt;=0.5, R85&lt;0.5), "D1",IF(AND(C85&lt;0.5, H85 &lt; 0.5,M85&gt;=0.5, R85&gt;=0.5), "C2",IF(AND(C85&lt;0.5, H85 &lt; 0.5,M85&lt;0.5, R85&lt;0.5), "C1",IF(AND(C85&lt;0.5, H85 &lt; 0.5,M85&lt;0.5, R85&gt;=0.5), "B","A"))))))))</f>
+        <v>C1</v>
+      </c>
+      <c r="AA85" s="25" t="str">
+        <f>IF(AND(D85&lt;0.5, I85 &gt;= 0.5,N85&gt;=0.5, S85&lt;0.5), "F",IF(AND(D85&lt;0.5, I85 &gt;= 0.5,N85&gt;=0.5, S85&gt;=0.5), "E2",IF(AND(D85&lt;0.5, I85 &gt;= 0.5,N85&lt;0.5, S85&lt;0.5), "E1",IF(AND(D85&lt;0.5, I85 &gt;= 0.5,N85&lt;0.5, S85&gt;=0.5), "D2",IF(AND(D85&lt;0.5, I85 &lt;0.5,N85&gt;=0.5, S85&lt;0.5), "D1",IF(AND(D85&lt;0.5, I85 &lt; 0.5,N85&gt;=0.5, S85&gt;=0.5), "C2",IF(AND(D85&lt;0.5, I85 &lt; 0.5,N85&lt;0.5, S85&lt;0.5), "C1",IF(AND(D85&lt;0.5, I85 &lt; 0.5,N85&lt;0.5, S85&gt;=0.5), "B","A"))))))))</f>
+        <v>C1</v>
+      </c>
+      <c r="AB85" s="25" t="str">
+        <f>IF(AND(E85&lt;0.5, J85 &gt;= 0.5,O85&gt;=0.5, T85&lt;0.5), "F",IF(AND(E85&lt;0.5, J85 &gt;= 0.5,O85&gt;=0.5, T85&gt;=0.5), "E2",IF(AND(E85&lt;0.5, J85 &gt;= 0.5,O85&lt;0.5, T85&lt;0.5), "E1",IF(AND(E85&lt;0.5, J85 &gt;= 0.5,O85&lt;0.5, T85&gt;=0.5), "D2",IF(AND(E85&lt;0.5, J85 &lt;0.5,O85&gt;=0.5, T85&lt;0.5), "D1",IF(AND(E85&lt;0.5, J85 &lt; 0.5,O85&gt;=0.5, T85&gt;=0.5), "C2",IF(AND(E85&lt;0.5, J85 &lt; 0.5,O85&lt;0.5, T85&lt;0.5), "C1",IF(AND(E85&lt;0.5, J85 &lt; 0.5,O85&lt;0.5, T85&gt;=0.5), "B","A"))))))))</f>
+        <v>C1</v>
+      </c>
+    </row>
+    <row r="86" spans="1:28" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A86" s="4"/>
       <c r="B86" s="4" t="s">
         <v>18</v>
@@ -4936,8 +6067,20 @@
         <f t="shared" si="15"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="87" spans="1:22" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="Z86" s="25" t="str">
+        <f>IF(AND(C86&lt;0.5, H86 &gt;= 0.5,M86&gt;=0.5, R86&lt;0.5), "F",IF(AND(C86&lt;0.5, H86 &gt;= 0.5,M86&gt;=0.5, R86&gt;=0.5), "E2",IF(AND(C86&lt;0.5, H86 &gt;= 0.5,M86&lt;0.5, R86&lt;0.5), "E1",IF(AND(C86&lt;0.5, H86 &gt;= 0.5,M86&lt;0.5, R86&gt;=0.5), "D2",IF(AND(C86&lt;0.5, H86 &lt;0.5,M86&gt;=0.5, R86&lt;0.5), "D1",IF(AND(C86&lt;0.5, H86 &lt; 0.5,M86&gt;=0.5, R86&gt;=0.5), "C2",IF(AND(C86&lt;0.5, H86 &lt; 0.5,M86&lt;0.5, R86&lt;0.5), "C1",IF(AND(C86&lt;0.5, H86 &lt; 0.5,M86&lt;0.5, R86&gt;=0.5), "B","A"))))))))</f>
+        <v>C1</v>
+      </c>
+      <c r="AA86" s="25" t="str">
+        <f>IF(AND(D86&lt;0.5, I86 &gt;= 0.5,N86&gt;=0.5, S86&lt;0.5), "F",IF(AND(D86&lt;0.5, I86 &gt;= 0.5,N86&gt;=0.5, S86&gt;=0.5), "E2",IF(AND(D86&lt;0.5, I86 &gt;= 0.5,N86&lt;0.5, S86&lt;0.5), "E1",IF(AND(D86&lt;0.5, I86 &gt;= 0.5,N86&lt;0.5, S86&gt;=0.5), "D2",IF(AND(D86&lt;0.5, I86 &lt;0.5,N86&gt;=0.5, S86&lt;0.5), "D1",IF(AND(D86&lt;0.5, I86 &lt; 0.5,N86&gt;=0.5, S86&gt;=0.5), "C2",IF(AND(D86&lt;0.5, I86 &lt; 0.5,N86&lt;0.5, S86&lt;0.5), "C1",IF(AND(D86&lt;0.5, I86 &lt; 0.5,N86&lt;0.5, S86&gt;=0.5), "B","A"))))))))</f>
+        <v>C1</v>
+      </c>
+      <c r="AB86" s="25" t="str">
+        <f>IF(AND(E86&lt;0.5, J86 &gt;= 0.5,O86&gt;=0.5, T86&lt;0.5), "F",IF(AND(E86&lt;0.5, J86 &gt;= 0.5,O86&gt;=0.5, T86&gt;=0.5), "E2",IF(AND(E86&lt;0.5, J86 &gt;= 0.5,O86&lt;0.5, T86&lt;0.5), "E1",IF(AND(E86&lt;0.5, J86 &gt;= 0.5,O86&lt;0.5, T86&gt;=0.5), "D2",IF(AND(E86&lt;0.5, J86 &lt;0.5,O86&gt;=0.5, T86&lt;0.5), "D1",IF(AND(E86&lt;0.5, J86 &lt; 0.5,O86&gt;=0.5, T86&gt;=0.5), "C2",IF(AND(E86&lt;0.5, J86 &lt; 0.5,O86&lt;0.5, T86&lt;0.5), "C1",IF(AND(E86&lt;0.5, J86 &lt; 0.5,O86&lt;0.5, T86&gt;=0.5), "B","A"))))))))</f>
+        <v>C1</v>
+      </c>
+    </row>
+    <row r="87" spans="1:28" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A87" s="3">
         <v>22</v>
       </c>
@@ -4988,8 +6131,20 @@
         <f t="shared" si="15"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="88" spans="1:22" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="Z87" s="25" t="str">
+        <f>IF(AND(C87&lt;0.5, H87 &gt;= 0.5,M87&gt;=0.5, R87&lt;0.5), "F",IF(AND(C87&lt;0.5, H87 &gt;= 0.5,M87&gt;=0.5, R87&gt;=0.5), "E2",IF(AND(C87&lt;0.5, H87 &gt;= 0.5,M87&lt;0.5, R87&lt;0.5), "E1",IF(AND(C87&lt;0.5, H87 &gt;= 0.5,M87&lt;0.5, R87&gt;=0.5), "D2",IF(AND(C87&lt;0.5, H87 &lt;0.5,M87&gt;=0.5, R87&lt;0.5), "D1",IF(AND(C87&lt;0.5, H87 &lt; 0.5,M87&gt;=0.5, R87&gt;=0.5), "C2",IF(AND(C87&lt;0.5, H87 &lt; 0.5,M87&lt;0.5, R87&lt;0.5), "C1",IF(AND(C87&lt;0.5, H87 &lt; 0.5,M87&lt;0.5, R87&gt;=0.5), "B","A"))))))))</f>
+        <v>C1</v>
+      </c>
+      <c r="AA87" s="25" t="str">
+        <f>IF(AND(D87&lt;0.5, I87 &gt;= 0.5,N87&gt;=0.5, S87&lt;0.5), "F",IF(AND(D87&lt;0.5, I87 &gt;= 0.5,N87&gt;=0.5, S87&gt;=0.5), "E2",IF(AND(D87&lt;0.5, I87 &gt;= 0.5,N87&lt;0.5, S87&lt;0.5), "E1",IF(AND(D87&lt;0.5, I87 &gt;= 0.5,N87&lt;0.5, S87&gt;=0.5), "D2",IF(AND(D87&lt;0.5, I87 &lt;0.5,N87&gt;=0.5, S87&lt;0.5), "D1",IF(AND(D87&lt;0.5, I87 &lt; 0.5,N87&gt;=0.5, S87&gt;=0.5), "C2",IF(AND(D87&lt;0.5, I87 &lt; 0.5,N87&lt;0.5, S87&lt;0.5), "C1",IF(AND(D87&lt;0.5, I87 &lt; 0.5,N87&lt;0.5, S87&gt;=0.5), "B","A"))))))))</f>
+        <v>C1</v>
+      </c>
+      <c r="AB87" s="25" t="str">
+        <f>IF(AND(E87&lt;0.5, J87 &gt;= 0.5,O87&gt;=0.5, T87&lt;0.5), "F",IF(AND(E87&lt;0.5, J87 &gt;= 0.5,O87&gt;=0.5, T87&gt;=0.5), "E2",IF(AND(E87&lt;0.5, J87 &gt;= 0.5,O87&lt;0.5, T87&lt;0.5), "E1",IF(AND(E87&lt;0.5, J87 &gt;= 0.5,O87&lt;0.5, T87&gt;=0.5), "D2",IF(AND(E87&lt;0.5, J87 &lt;0.5,O87&gt;=0.5, T87&lt;0.5), "D1",IF(AND(E87&lt;0.5, J87 &lt; 0.5,O87&gt;=0.5, T87&gt;=0.5), "C2",IF(AND(E87&lt;0.5, J87 &lt; 0.5,O87&lt;0.5, T87&lt;0.5), "C1",IF(AND(E87&lt;0.5, J87 &lt; 0.5,O87&lt;0.5, T87&gt;=0.5), "B","A"))))))))</f>
+        <v>C1</v>
+      </c>
+    </row>
+    <row r="88" spans="1:28" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A88" s="1"/>
       <c r="B88" s="1" t="s">
         <v>16</v>
@@ -5035,8 +6190,20 @@
         <f t="shared" si="15"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="89" spans="1:22" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="Z88" s="25" t="str">
+        <f>IF(AND(C88&lt;0.5, H88 &gt;= 0.5,M88&gt;=0.5, R88&lt;0.5), "F",IF(AND(C88&lt;0.5, H88 &gt;= 0.5,M88&gt;=0.5, R88&gt;=0.5), "E2",IF(AND(C88&lt;0.5, H88 &gt;= 0.5,M88&lt;0.5, R88&lt;0.5), "E1",IF(AND(C88&lt;0.5, H88 &gt;= 0.5,M88&lt;0.5, R88&gt;=0.5), "D2",IF(AND(C88&lt;0.5, H88 &lt;0.5,M88&gt;=0.5, R88&lt;0.5), "D1",IF(AND(C88&lt;0.5, H88 &lt; 0.5,M88&gt;=0.5, R88&gt;=0.5), "C2",IF(AND(C88&lt;0.5, H88 &lt; 0.5,M88&lt;0.5, R88&lt;0.5), "C1",IF(AND(C88&lt;0.5, H88 &lt; 0.5,M88&lt;0.5, R88&gt;=0.5), "B","A"))))))))</f>
+        <v>C1</v>
+      </c>
+      <c r="AA88" s="25" t="str">
+        <f>IF(AND(D88&lt;0.5, I88 &gt;= 0.5,N88&gt;=0.5, S88&lt;0.5), "F",IF(AND(D88&lt;0.5, I88 &gt;= 0.5,N88&gt;=0.5, S88&gt;=0.5), "E2",IF(AND(D88&lt;0.5, I88 &gt;= 0.5,N88&lt;0.5, S88&lt;0.5), "E1",IF(AND(D88&lt;0.5, I88 &gt;= 0.5,N88&lt;0.5, S88&gt;=0.5), "D2",IF(AND(D88&lt;0.5, I88 &lt;0.5,N88&gt;=0.5, S88&lt;0.5), "D1",IF(AND(D88&lt;0.5, I88 &lt; 0.5,N88&gt;=0.5, S88&gt;=0.5), "C2",IF(AND(D88&lt;0.5, I88 &lt; 0.5,N88&lt;0.5, S88&lt;0.5), "C1",IF(AND(D88&lt;0.5, I88 &lt; 0.5,N88&lt;0.5, S88&gt;=0.5), "B","A"))))))))</f>
+        <v>C1</v>
+      </c>
+      <c r="AB88" s="25" t="str">
+        <f>IF(AND(E88&lt;0.5, J88 &gt;= 0.5,O88&gt;=0.5, T88&lt;0.5), "F",IF(AND(E88&lt;0.5, J88 &gt;= 0.5,O88&gt;=0.5, T88&gt;=0.5), "E2",IF(AND(E88&lt;0.5, J88 &gt;= 0.5,O88&lt;0.5, T88&lt;0.5), "E1",IF(AND(E88&lt;0.5, J88 &gt;= 0.5,O88&lt;0.5, T88&gt;=0.5), "D2",IF(AND(E88&lt;0.5, J88 &lt;0.5,O88&gt;=0.5, T88&lt;0.5), "D1",IF(AND(E88&lt;0.5, J88 &lt; 0.5,O88&gt;=0.5, T88&gt;=0.5), "C2",IF(AND(E88&lt;0.5, J88 &lt; 0.5,O88&lt;0.5, T88&lt;0.5), "C1",IF(AND(E88&lt;0.5, J88 &lt; 0.5,O88&lt;0.5, T88&gt;=0.5), "B","A"))))))))</f>
+        <v>C1</v>
+      </c>
+    </row>
+    <row r="89" spans="1:28" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A89" s="1"/>
       <c r="B89" s="1" t="s">
         <v>17</v>
@@ -5082,8 +6249,20 @@
         <f t="shared" si="15"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="90" spans="1:22" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="Z89" s="25" t="str">
+        <f>IF(AND(C89&lt;0.5, H89 &gt;= 0.5,M89&gt;=0.5, R89&lt;0.5), "F",IF(AND(C89&lt;0.5, H89 &gt;= 0.5,M89&gt;=0.5, R89&gt;=0.5), "E2",IF(AND(C89&lt;0.5, H89 &gt;= 0.5,M89&lt;0.5, R89&lt;0.5), "E1",IF(AND(C89&lt;0.5, H89 &gt;= 0.5,M89&lt;0.5, R89&gt;=0.5), "D2",IF(AND(C89&lt;0.5, H89 &lt;0.5,M89&gt;=0.5, R89&lt;0.5), "D1",IF(AND(C89&lt;0.5, H89 &lt; 0.5,M89&gt;=0.5, R89&gt;=0.5), "C2",IF(AND(C89&lt;0.5, H89 &lt; 0.5,M89&lt;0.5, R89&lt;0.5), "C1",IF(AND(C89&lt;0.5, H89 &lt; 0.5,M89&lt;0.5, R89&gt;=0.5), "B","A"))))))))</f>
+        <v>C1</v>
+      </c>
+      <c r="AA89" s="25" t="str">
+        <f>IF(AND(D89&lt;0.5, I89 &gt;= 0.5,N89&gt;=0.5, S89&lt;0.5), "F",IF(AND(D89&lt;0.5, I89 &gt;= 0.5,N89&gt;=0.5, S89&gt;=0.5), "E2",IF(AND(D89&lt;0.5, I89 &gt;= 0.5,N89&lt;0.5, S89&lt;0.5), "E1",IF(AND(D89&lt;0.5, I89 &gt;= 0.5,N89&lt;0.5, S89&gt;=0.5), "D2",IF(AND(D89&lt;0.5, I89 &lt;0.5,N89&gt;=0.5, S89&lt;0.5), "D1",IF(AND(D89&lt;0.5, I89 &lt; 0.5,N89&gt;=0.5, S89&gt;=0.5), "C2",IF(AND(D89&lt;0.5, I89 &lt; 0.5,N89&lt;0.5, S89&lt;0.5), "C1",IF(AND(D89&lt;0.5, I89 &lt; 0.5,N89&lt;0.5, S89&gt;=0.5), "B","A"))))))))</f>
+        <v>C1</v>
+      </c>
+      <c r="AB89" s="25" t="str">
+        <f>IF(AND(E89&lt;0.5, J89 &gt;= 0.5,O89&gt;=0.5, T89&lt;0.5), "F",IF(AND(E89&lt;0.5, J89 &gt;= 0.5,O89&gt;=0.5, T89&gt;=0.5), "E2",IF(AND(E89&lt;0.5, J89 &gt;= 0.5,O89&lt;0.5, T89&lt;0.5), "E1",IF(AND(E89&lt;0.5, J89 &gt;= 0.5,O89&lt;0.5, T89&gt;=0.5), "D2",IF(AND(E89&lt;0.5, J89 &lt;0.5,O89&gt;=0.5, T89&lt;0.5), "D1",IF(AND(E89&lt;0.5, J89 &lt; 0.5,O89&gt;=0.5, T89&gt;=0.5), "C2",IF(AND(E89&lt;0.5, J89 &lt; 0.5,O89&lt;0.5, T89&lt;0.5), "C1",IF(AND(E89&lt;0.5, J89 &lt; 0.5,O89&lt;0.5, T89&gt;=0.5), "B","A"))))))))</f>
+        <v>C1</v>
+      </c>
+    </row>
+    <row r="90" spans="1:28" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A90" s="4"/>
       <c r="B90" s="4" t="s">
         <v>18</v>
@@ -5132,8 +6311,20 @@
         <f t="shared" si="15"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="91" spans="1:22" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="Z90" s="25" t="str">
+        <f>IF(AND(C90&lt;0.5, H90 &gt;= 0.5,M90&gt;=0.5, R90&lt;0.5), "F",IF(AND(C90&lt;0.5, H90 &gt;= 0.5,M90&gt;=0.5, R90&gt;=0.5), "E2",IF(AND(C90&lt;0.5, H90 &gt;= 0.5,M90&lt;0.5, R90&lt;0.5), "E1",IF(AND(C90&lt;0.5, H90 &gt;= 0.5,M90&lt;0.5, R90&gt;=0.5), "D2",IF(AND(C90&lt;0.5, H90 &lt;0.5,M90&gt;=0.5, R90&lt;0.5), "D1",IF(AND(C90&lt;0.5, H90 &lt; 0.5,M90&gt;=0.5, R90&gt;=0.5), "C2",IF(AND(C90&lt;0.5, H90 &lt; 0.5,M90&lt;0.5, R90&lt;0.5), "C1",IF(AND(C90&lt;0.5, H90 &lt; 0.5,M90&lt;0.5, R90&gt;=0.5), "B","A"))))))))</f>
+        <v>C1</v>
+      </c>
+      <c r="AA90" s="25" t="str">
+        <f>IF(AND(D90&lt;0.5, I90 &gt;= 0.5,N90&gt;=0.5, S90&lt;0.5), "F",IF(AND(D90&lt;0.5, I90 &gt;= 0.5,N90&gt;=0.5, S90&gt;=0.5), "E2",IF(AND(D90&lt;0.5, I90 &gt;= 0.5,N90&lt;0.5, S90&lt;0.5), "E1",IF(AND(D90&lt;0.5, I90 &gt;= 0.5,N90&lt;0.5, S90&gt;=0.5), "D2",IF(AND(D90&lt;0.5, I90 &lt;0.5,N90&gt;=0.5, S90&lt;0.5), "D1",IF(AND(D90&lt;0.5, I90 &lt; 0.5,N90&gt;=0.5, S90&gt;=0.5), "C2",IF(AND(D90&lt;0.5, I90 &lt; 0.5,N90&lt;0.5, S90&lt;0.5), "C1",IF(AND(D90&lt;0.5, I90 &lt; 0.5,N90&lt;0.5, S90&gt;=0.5), "B","A"))))))))</f>
+        <v>C1</v>
+      </c>
+      <c r="AB90" s="25" t="str">
+        <f>IF(AND(E90&lt;0.5, J90 &gt;= 0.5,O90&gt;=0.5, T90&lt;0.5), "F",IF(AND(E90&lt;0.5, J90 &gt;= 0.5,O90&gt;=0.5, T90&gt;=0.5), "E2",IF(AND(E90&lt;0.5, J90 &gt;= 0.5,O90&lt;0.5, T90&lt;0.5), "E1",IF(AND(E90&lt;0.5, J90 &gt;= 0.5,O90&lt;0.5, T90&gt;=0.5), "D2",IF(AND(E90&lt;0.5, J90 &lt;0.5,O90&gt;=0.5, T90&lt;0.5), "D1",IF(AND(E90&lt;0.5, J90 &lt; 0.5,O90&gt;=0.5, T90&gt;=0.5), "C2",IF(AND(E90&lt;0.5, J90 &lt; 0.5,O90&lt;0.5, T90&lt;0.5), "C1",IF(AND(E90&lt;0.5, J90 &lt; 0.5,O90&lt;0.5, T90&gt;=0.5), "B","A"))))))))</f>
+        <v>C1</v>
+      </c>
+    </row>
+    <row r="91" spans="1:28" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A91" s="3">
         <v>23</v>
       </c>
@@ -5184,8 +6375,20 @@
         <f t="shared" si="15"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="92" spans="1:22" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="Z91" s="25" t="str">
+        <f>IF(AND(C91&lt;0.5, H91 &gt;= 0.5,M91&gt;=0.5, R91&lt;0.5), "F",IF(AND(C91&lt;0.5, H91 &gt;= 0.5,M91&gt;=0.5, R91&gt;=0.5), "E2",IF(AND(C91&lt;0.5, H91 &gt;= 0.5,M91&lt;0.5, R91&lt;0.5), "E1",IF(AND(C91&lt;0.5, H91 &gt;= 0.5,M91&lt;0.5, R91&gt;=0.5), "D2",IF(AND(C91&lt;0.5, H91 &lt;0.5,M91&gt;=0.5, R91&lt;0.5), "D1",IF(AND(C91&lt;0.5, H91 &lt; 0.5,M91&gt;=0.5, R91&gt;=0.5), "C2",IF(AND(C91&lt;0.5, H91 &lt; 0.5,M91&lt;0.5, R91&lt;0.5), "C1",IF(AND(C91&lt;0.5, H91 &lt; 0.5,M91&lt;0.5, R91&gt;=0.5), "B","A"))))))))</f>
+        <v>C1</v>
+      </c>
+      <c r="AA91" s="25" t="str">
+        <f>IF(AND(D91&lt;0.5, I91 &gt;= 0.5,N91&gt;=0.5, S91&lt;0.5), "F",IF(AND(D91&lt;0.5, I91 &gt;= 0.5,N91&gt;=0.5, S91&gt;=0.5), "E2",IF(AND(D91&lt;0.5, I91 &gt;= 0.5,N91&lt;0.5, S91&lt;0.5), "E1",IF(AND(D91&lt;0.5, I91 &gt;= 0.5,N91&lt;0.5, S91&gt;=0.5), "D2",IF(AND(D91&lt;0.5, I91 &lt;0.5,N91&gt;=0.5, S91&lt;0.5), "D1",IF(AND(D91&lt;0.5, I91 &lt; 0.5,N91&gt;=0.5, S91&gt;=0.5), "C2",IF(AND(D91&lt;0.5, I91 &lt; 0.5,N91&lt;0.5, S91&lt;0.5), "C1",IF(AND(D91&lt;0.5, I91 &lt; 0.5,N91&lt;0.5, S91&gt;=0.5), "B","A"))))))))</f>
+        <v>C1</v>
+      </c>
+      <c r="AB91" s="25" t="str">
+        <f>IF(AND(E91&lt;0.5, J91 &gt;= 0.5,O91&gt;=0.5, T91&lt;0.5), "F",IF(AND(E91&lt;0.5, J91 &gt;= 0.5,O91&gt;=0.5, T91&gt;=0.5), "E2",IF(AND(E91&lt;0.5, J91 &gt;= 0.5,O91&lt;0.5, T91&lt;0.5), "E1",IF(AND(E91&lt;0.5, J91 &gt;= 0.5,O91&lt;0.5, T91&gt;=0.5), "D2",IF(AND(E91&lt;0.5, J91 &lt;0.5,O91&gt;=0.5, T91&lt;0.5), "D1",IF(AND(E91&lt;0.5, J91 &lt; 0.5,O91&gt;=0.5, T91&gt;=0.5), "C2",IF(AND(E91&lt;0.5, J91 &lt; 0.5,O91&lt;0.5, T91&lt;0.5), "C1",IF(AND(E91&lt;0.5, J91 &lt; 0.5,O91&lt;0.5, T91&gt;=0.5), "B","A"))))))))</f>
+        <v>C1</v>
+      </c>
+    </row>
+    <row r="92" spans="1:28" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A92" s="1"/>
       <c r="B92" s="1" t="s">
         <v>16</v>
@@ -5231,8 +6434,20 @@
         <f t="shared" si="15"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="93" spans="1:22" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="Z92" s="25" t="str">
+        <f>IF(AND(C92&lt;0.5, H92 &gt;= 0.5,M92&gt;=0.5, R92&lt;0.5), "F",IF(AND(C92&lt;0.5, H92 &gt;= 0.5,M92&gt;=0.5, R92&gt;=0.5), "E2",IF(AND(C92&lt;0.5, H92 &gt;= 0.5,M92&lt;0.5, R92&lt;0.5), "E1",IF(AND(C92&lt;0.5, H92 &gt;= 0.5,M92&lt;0.5, R92&gt;=0.5), "D2",IF(AND(C92&lt;0.5, H92 &lt;0.5,M92&gt;=0.5, R92&lt;0.5), "D1",IF(AND(C92&lt;0.5, H92 &lt; 0.5,M92&gt;=0.5, R92&gt;=0.5), "C2",IF(AND(C92&lt;0.5, H92 &lt; 0.5,M92&lt;0.5, R92&lt;0.5), "C1",IF(AND(C92&lt;0.5, H92 &lt; 0.5,M92&lt;0.5, R92&gt;=0.5), "B","A"))))))))</f>
+        <v>C1</v>
+      </c>
+      <c r="AA92" s="25" t="str">
+        <f>IF(AND(D92&lt;0.5, I92 &gt;= 0.5,N92&gt;=0.5, S92&lt;0.5), "F",IF(AND(D92&lt;0.5, I92 &gt;= 0.5,N92&gt;=0.5, S92&gt;=0.5), "E2",IF(AND(D92&lt;0.5, I92 &gt;= 0.5,N92&lt;0.5, S92&lt;0.5), "E1",IF(AND(D92&lt;0.5, I92 &gt;= 0.5,N92&lt;0.5, S92&gt;=0.5), "D2",IF(AND(D92&lt;0.5, I92 &lt;0.5,N92&gt;=0.5, S92&lt;0.5), "D1",IF(AND(D92&lt;0.5, I92 &lt; 0.5,N92&gt;=0.5, S92&gt;=0.5), "C2",IF(AND(D92&lt;0.5, I92 &lt; 0.5,N92&lt;0.5, S92&lt;0.5), "C1",IF(AND(D92&lt;0.5, I92 &lt; 0.5,N92&lt;0.5, S92&gt;=0.5), "B","A"))))))))</f>
+        <v>C1</v>
+      </c>
+      <c r="AB92" s="25" t="str">
+        <f>IF(AND(E92&lt;0.5, J92 &gt;= 0.5,O92&gt;=0.5, T92&lt;0.5), "F",IF(AND(E92&lt;0.5, J92 &gt;= 0.5,O92&gt;=0.5, T92&gt;=0.5), "E2",IF(AND(E92&lt;0.5, J92 &gt;= 0.5,O92&lt;0.5, T92&lt;0.5), "E1",IF(AND(E92&lt;0.5, J92 &gt;= 0.5,O92&lt;0.5, T92&gt;=0.5), "D2",IF(AND(E92&lt;0.5, J92 &lt;0.5,O92&gt;=0.5, T92&lt;0.5), "D1",IF(AND(E92&lt;0.5, J92 &lt; 0.5,O92&gt;=0.5, T92&gt;=0.5), "C2",IF(AND(E92&lt;0.5, J92 &lt; 0.5,O92&lt;0.5, T92&lt;0.5), "C1",IF(AND(E92&lt;0.5, J92 &lt; 0.5,O92&lt;0.5, T92&gt;=0.5), "B","A"))))))))</f>
+        <v>C1</v>
+      </c>
+    </row>
+    <row r="93" spans="1:28" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A93" s="1"/>
       <c r="B93" s="1" t="s">
         <v>17</v>
@@ -5278,8 +6493,20 @@
         <f t="shared" si="15"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="94" spans="1:22" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="Z93" s="25" t="str">
+        <f>IF(AND(C93&lt;0.5, H93 &gt;= 0.5,M93&gt;=0.5, R93&lt;0.5), "F",IF(AND(C93&lt;0.5, H93 &gt;= 0.5,M93&gt;=0.5, R93&gt;=0.5), "E2",IF(AND(C93&lt;0.5, H93 &gt;= 0.5,M93&lt;0.5, R93&lt;0.5), "E1",IF(AND(C93&lt;0.5, H93 &gt;= 0.5,M93&lt;0.5, R93&gt;=0.5), "D2",IF(AND(C93&lt;0.5, H93 &lt;0.5,M93&gt;=0.5, R93&lt;0.5), "D1",IF(AND(C93&lt;0.5, H93 &lt; 0.5,M93&gt;=0.5, R93&gt;=0.5), "C2",IF(AND(C93&lt;0.5, H93 &lt; 0.5,M93&lt;0.5, R93&lt;0.5), "C1",IF(AND(C93&lt;0.5, H93 &lt; 0.5,M93&lt;0.5, R93&gt;=0.5), "B","A"))))))))</f>
+        <v>C1</v>
+      </c>
+      <c r="AA93" s="25" t="str">
+        <f>IF(AND(D93&lt;0.5, I93 &gt;= 0.5,N93&gt;=0.5, S93&lt;0.5), "F",IF(AND(D93&lt;0.5, I93 &gt;= 0.5,N93&gt;=0.5, S93&gt;=0.5), "E2",IF(AND(D93&lt;0.5, I93 &gt;= 0.5,N93&lt;0.5, S93&lt;0.5), "E1",IF(AND(D93&lt;0.5, I93 &gt;= 0.5,N93&lt;0.5, S93&gt;=0.5), "D2",IF(AND(D93&lt;0.5, I93 &lt;0.5,N93&gt;=0.5, S93&lt;0.5), "D1",IF(AND(D93&lt;0.5, I93 &lt; 0.5,N93&gt;=0.5, S93&gt;=0.5), "C2",IF(AND(D93&lt;0.5, I93 &lt; 0.5,N93&lt;0.5, S93&lt;0.5), "C1",IF(AND(D93&lt;0.5, I93 &lt; 0.5,N93&lt;0.5, S93&gt;=0.5), "B","A"))))))))</f>
+        <v>C1</v>
+      </c>
+      <c r="AB93" s="25" t="str">
+        <f>IF(AND(E93&lt;0.5, J93 &gt;= 0.5,O93&gt;=0.5, T93&lt;0.5), "F",IF(AND(E93&lt;0.5, J93 &gt;= 0.5,O93&gt;=0.5, T93&gt;=0.5), "E2",IF(AND(E93&lt;0.5, J93 &gt;= 0.5,O93&lt;0.5, T93&lt;0.5), "E1",IF(AND(E93&lt;0.5, J93 &gt;= 0.5,O93&lt;0.5, T93&gt;=0.5), "D2",IF(AND(E93&lt;0.5, J93 &lt;0.5,O93&gt;=0.5, T93&lt;0.5), "D1",IF(AND(E93&lt;0.5, J93 &lt; 0.5,O93&gt;=0.5, T93&gt;=0.5), "C2",IF(AND(E93&lt;0.5, J93 &lt; 0.5,O93&lt;0.5, T93&lt;0.5), "C1",IF(AND(E93&lt;0.5, J93 &lt; 0.5,O93&lt;0.5, T93&gt;=0.5), "B","A"))))))))</f>
+        <v>C1</v>
+      </c>
+    </row>
+    <row r="94" spans="1:28" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A94" s="4"/>
       <c r="B94" s="4" t="s">
         <v>18</v>
@@ -5328,8 +6555,20 @@
         <f t="shared" si="15"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="95" spans="1:22" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="Z94" s="25" t="str">
+        <f>IF(AND(C94&lt;0.5, H94 &gt;= 0.5,M94&gt;=0.5, R94&lt;0.5), "F",IF(AND(C94&lt;0.5, H94 &gt;= 0.5,M94&gt;=0.5, R94&gt;=0.5), "E2",IF(AND(C94&lt;0.5, H94 &gt;= 0.5,M94&lt;0.5, R94&lt;0.5), "E1",IF(AND(C94&lt;0.5, H94 &gt;= 0.5,M94&lt;0.5, R94&gt;=0.5), "D2",IF(AND(C94&lt;0.5, H94 &lt;0.5,M94&gt;=0.5, R94&lt;0.5), "D1",IF(AND(C94&lt;0.5, H94 &lt; 0.5,M94&gt;=0.5, R94&gt;=0.5), "C2",IF(AND(C94&lt;0.5, H94 &lt; 0.5,M94&lt;0.5, R94&lt;0.5), "C1",IF(AND(C94&lt;0.5, H94 &lt; 0.5,M94&lt;0.5, R94&gt;=0.5), "B","A"))))))))</f>
+        <v>C1</v>
+      </c>
+      <c r="AA94" s="25" t="str">
+        <f>IF(AND(D94&lt;0.5, I94 &gt;= 0.5,N94&gt;=0.5, S94&lt;0.5), "F",IF(AND(D94&lt;0.5, I94 &gt;= 0.5,N94&gt;=0.5, S94&gt;=0.5), "E2",IF(AND(D94&lt;0.5, I94 &gt;= 0.5,N94&lt;0.5, S94&lt;0.5), "E1",IF(AND(D94&lt;0.5, I94 &gt;= 0.5,N94&lt;0.5, S94&gt;=0.5), "D2",IF(AND(D94&lt;0.5, I94 &lt;0.5,N94&gt;=0.5, S94&lt;0.5), "D1",IF(AND(D94&lt;0.5, I94 &lt; 0.5,N94&gt;=0.5, S94&gt;=0.5), "C2",IF(AND(D94&lt;0.5, I94 &lt; 0.5,N94&lt;0.5, S94&lt;0.5), "C1",IF(AND(D94&lt;0.5, I94 &lt; 0.5,N94&lt;0.5, S94&gt;=0.5), "B","A"))))))))</f>
+        <v>C1</v>
+      </c>
+      <c r="AB94" s="25" t="str">
+        <f>IF(AND(E94&lt;0.5, J94 &gt;= 0.5,O94&gt;=0.5, T94&lt;0.5), "F",IF(AND(E94&lt;0.5, J94 &gt;= 0.5,O94&gt;=0.5, T94&gt;=0.5), "E2",IF(AND(E94&lt;0.5, J94 &gt;= 0.5,O94&lt;0.5, T94&lt;0.5), "E1",IF(AND(E94&lt;0.5, J94 &gt;= 0.5,O94&lt;0.5, T94&gt;=0.5), "D2",IF(AND(E94&lt;0.5, J94 &lt;0.5,O94&gt;=0.5, T94&lt;0.5), "D1",IF(AND(E94&lt;0.5, J94 &lt; 0.5,O94&gt;=0.5, T94&gt;=0.5), "C2",IF(AND(E94&lt;0.5, J94 &lt; 0.5,O94&lt;0.5, T94&lt;0.5), "C1",IF(AND(E94&lt;0.5, J94 &lt; 0.5,O94&lt;0.5, T94&gt;=0.5), "B","A"))))))))</f>
+        <v>C1</v>
+      </c>
+    </row>
+    <row r="95" spans="1:28" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A95" s="3">
         <v>24</v>
       </c>
@@ -5380,8 +6619,20 @@
         <f t="shared" si="15"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="96" spans="1:22" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="Z95" s="25" t="str">
+        <f>IF(AND(C95&lt;0.5, H95 &gt;= 0.5,M95&gt;=0.5, R95&lt;0.5), "F",IF(AND(C95&lt;0.5, H95 &gt;= 0.5,M95&gt;=0.5, R95&gt;=0.5), "E2",IF(AND(C95&lt;0.5, H95 &gt;= 0.5,M95&lt;0.5, R95&lt;0.5), "E1",IF(AND(C95&lt;0.5, H95 &gt;= 0.5,M95&lt;0.5, R95&gt;=0.5), "D2",IF(AND(C95&lt;0.5, H95 &lt;0.5,M95&gt;=0.5, R95&lt;0.5), "D1",IF(AND(C95&lt;0.5, H95 &lt; 0.5,M95&gt;=0.5, R95&gt;=0.5), "C2",IF(AND(C95&lt;0.5, H95 &lt; 0.5,M95&lt;0.5, R95&lt;0.5), "C1",IF(AND(C95&lt;0.5, H95 &lt; 0.5,M95&lt;0.5, R95&gt;=0.5), "B","A"))))))))</f>
+        <v>C1</v>
+      </c>
+      <c r="AA95" s="25" t="str">
+        <f>IF(AND(D95&lt;0.5, I95 &gt;= 0.5,N95&gt;=0.5, S95&lt;0.5), "F",IF(AND(D95&lt;0.5, I95 &gt;= 0.5,N95&gt;=0.5, S95&gt;=0.5), "E2",IF(AND(D95&lt;0.5, I95 &gt;= 0.5,N95&lt;0.5, S95&lt;0.5), "E1",IF(AND(D95&lt;0.5, I95 &gt;= 0.5,N95&lt;0.5, S95&gt;=0.5), "D2",IF(AND(D95&lt;0.5, I95 &lt;0.5,N95&gt;=0.5, S95&lt;0.5), "D1",IF(AND(D95&lt;0.5, I95 &lt; 0.5,N95&gt;=0.5, S95&gt;=0.5), "C2",IF(AND(D95&lt;0.5, I95 &lt; 0.5,N95&lt;0.5, S95&lt;0.5), "C1",IF(AND(D95&lt;0.5, I95 &lt; 0.5,N95&lt;0.5, S95&gt;=0.5), "B","A"))))))))</f>
+        <v>C1</v>
+      </c>
+      <c r="AB95" s="25" t="str">
+        <f>IF(AND(E95&lt;0.5, J95 &gt;= 0.5,O95&gt;=0.5, T95&lt;0.5), "F",IF(AND(E95&lt;0.5, J95 &gt;= 0.5,O95&gt;=0.5, T95&gt;=0.5), "E2",IF(AND(E95&lt;0.5, J95 &gt;= 0.5,O95&lt;0.5, T95&lt;0.5), "E1",IF(AND(E95&lt;0.5, J95 &gt;= 0.5,O95&lt;0.5, T95&gt;=0.5), "D2",IF(AND(E95&lt;0.5, J95 &lt;0.5,O95&gt;=0.5, T95&lt;0.5), "D1",IF(AND(E95&lt;0.5, J95 &lt; 0.5,O95&gt;=0.5, T95&gt;=0.5), "C2",IF(AND(E95&lt;0.5, J95 &lt; 0.5,O95&lt;0.5, T95&lt;0.5), "C1",IF(AND(E95&lt;0.5, J95 &lt; 0.5,O95&lt;0.5, T95&gt;=0.5), "B","A"))))))))</f>
+        <v>C1</v>
+      </c>
+    </row>
+    <row r="96" spans="1:28" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A96" s="1"/>
       <c r="B96" s="1" t="s">
         <v>16</v>
@@ -5427,8 +6678,20 @@
         <f t="shared" si="15"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="97" spans="1:22" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="Z96" s="25" t="str">
+        <f>IF(AND(C96&lt;0.5, H96 &gt;= 0.5,M96&gt;=0.5, R96&lt;0.5), "F",IF(AND(C96&lt;0.5, H96 &gt;= 0.5,M96&gt;=0.5, R96&gt;=0.5), "E2",IF(AND(C96&lt;0.5, H96 &gt;= 0.5,M96&lt;0.5, R96&lt;0.5), "E1",IF(AND(C96&lt;0.5, H96 &gt;= 0.5,M96&lt;0.5, R96&gt;=0.5), "D2",IF(AND(C96&lt;0.5, H96 &lt;0.5,M96&gt;=0.5, R96&lt;0.5), "D1",IF(AND(C96&lt;0.5, H96 &lt; 0.5,M96&gt;=0.5, R96&gt;=0.5), "C2",IF(AND(C96&lt;0.5, H96 &lt; 0.5,M96&lt;0.5, R96&lt;0.5), "C1",IF(AND(C96&lt;0.5, H96 &lt; 0.5,M96&lt;0.5, R96&gt;=0.5), "B","A"))))))))</f>
+        <v>C1</v>
+      </c>
+      <c r="AA96" s="25" t="str">
+        <f>IF(AND(D96&lt;0.5, I96 &gt;= 0.5,N96&gt;=0.5, S96&lt;0.5), "F",IF(AND(D96&lt;0.5, I96 &gt;= 0.5,N96&gt;=0.5, S96&gt;=0.5), "E2",IF(AND(D96&lt;0.5, I96 &gt;= 0.5,N96&lt;0.5, S96&lt;0.5), "E1",IF(AND(D96&lt;0.5, I96 &gt;= 0.5,N96&lt;0.5, S96&gt;=0.5), "D2",IF(AND(D96&lt;0.5, I96 &lt;0.5,N96&gt;=0.5, S96&lt;0.5), "D1",IF(AND(D96&lt;0.5, I96 &lt; 0.5,N96&gt;=0.5, S96&gt;=0.5), "C2",IF(AND(D96&lt;0.5, I96 &lt; 0.5,N96&lt;0.5, S96&lt;0.5), "C1",IF(AND(D96&lt;0.5, I96 &lt; 0.5,N96&lt;0.5, S96&gt;=0.5), "B","A"))))))))</f>
+        <v>C1</v>
+      </c>
+      <c r="AB96" s="25" t="str">
+        <f>IF(AND(E96&lt;0.5, J96 &gt;= 0.5,O96&gt;=0.5, T96&lt;0.5), "F",IF(AND(E96&lt;0.5, J96 &gt;= 0.5,O96&gt;=0.5, T96&gt;=0.5), "E2",IF(AND(E96&lt;0.5, J96 &gt;= 0.5,O96&lt;0.5, T96&lt;0.5), "E1",IF(AND(E96&lt;0.5, J96 &gt;= 0.5,O96&lt;0.5, T96&gt;=0.5), "D2",IF(AND(E96&lt;0.5, J96 &lt;0.5,O96&gt;=0.5, T96&lt;0.5), "D1",IF(AND(E96&lt;0.5, J96 &lt; 0.5,O96&gt;=0.5, T96&gt;=0.5), "C2",IF(AND(E96&lt;0.5, J96 &lt; 0.5,O96&lt;0.5, T96&lt;0.5), "C1",IF(AND(E96&lt;0.5, J96 &lt; 0.5,O96&lt;0.5, T96&gt;=0.5), "B","A"))))))))</f>
+        <v>C1</v>
+      </c>
+    </row>
+    <row r="97" spans="1:28" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A97" s="1"/>
       <c r="B97" s="1" t="s">
         <v>17</v>
@@ -5474,8 +6737,20 @@
         <f t="shared" si="15"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="98" spans="1:22" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="Z97" s="25" t="str">
+        <f>IF(AND(C97&lt;0.5, H97 &gt;= 0.5,M97&gt;=0.5, R97&lt;0.5), "F",IF(AND(C97&lt;0.5, H97 &gt;= 0.5,M97&gt;=0.5, R97&gt;=0.5), "E2",IF(AND(C97&lt;0.5, H97 &gt;= 0.5,M97&lt;0.5, R97&lt;0.5), "E1",IF(AND(C97&lt;0.5, H97 &gt;= 0.5,M97&lt;0.5, R97&gt;=0.5), "D2",IF(AND(C97&lt;0.5, H97 &lt;0.5,M97&gt;=0.5, R97&lt;0.5), "D1",IF(AND(C97&lt;0.5, H97 &lt; 0.5,M97&gt;=0.5, R97&gt;=0.5), "C2",IF(AND(C97&lt;0.5, H97 &lt; 0.5,M97&lt;0.5, R97&lt;0.5), "C1",IF(AND(C97&lt;0.5, H97 &lt; 0.5,M97&lt;0.5, R97&gt;=0.5), "B","A"))))))))</f>
+        <v>C1</v>
+      </c>
+      <c r="AA97" s="25" t="str">
+        <f>IF(AND(D97&lt;0.5, I97 &gt;= 0.5,N97&gt;=0.5, S97&lt;0.5), "F",IF(AND(D97&lt;0.5, I97 &gt;= 0.5,N97&gt;=0.5, S97&gt;=0.5), "E2",IF(AND(D97&lt;0.5, I97 &gt;= 0.5,N97&lt;0.5, S97&lt;0.5), "E1",IF(AND(D97&lt;0.5, I97 &gt;= 0.5,N97&lt;0.5, S97&gt;=0.5), "D2",IF(AND(D97&lt;0.5, I97 &lt;0.5,N97&gt;=0.5, S97&lt;0.5), "D1",IF(AND(D97&lt;0.5, I97 &lt; 0.5,N97&gt;=0.5, S97&gt;=0.5), "C2",IF(AND(D97&lt;0.5, I97 &lt; 0.5,N97&lt;0.5, S97&lt;0.5), "C1",IF(AND(D97&lt;0.5, I97 &lt; 0.5,N97&lt;0.5, S97&gt;=0.5), "B","A"))))))))</f>
+        <v>C1</v>
+      </c>
+      <c r="AB97" s="25" t="str">
+        <f>IF(AND(E97&lt;0.5, J97 &gt;= 0.5,O97&gt;=0.5, T97&lt;0.5), "F",IF(AND(E97&lt;0.5, J97 &gt;= 0.5,O97&gt;=0.5, T97&gt;=0.5), "E2",IF(AND(E97&lt;0.5, J97 &gt;= 0.5,O97&lt;0.5, T97&lt;0.5), "E1",IF(AND(E97&lt;0.5, J97 &gt;= 0.5,O97&lt;0.5, T97&gt;=0.5), "D2",IF(AND(E97&lt;0.5, J97 &lt;0.5,O97&gt;=0.5, T97&lt;0.5), "D1",IF(AND(E97&lt;0.5, J97 &lt; 0.5,O97&gt;=0.5, T97&gt;=0.5), "C2",IF(AND(E97&lt;0.5, J97 &lt; 0.5,O97&lt;0.5, T97&lt;0.5), "C1",IF(AND(E97&lt;0.5, J97 &lt; 0.5,O97&lt;0.5, T97&gt;=0.5), "B","A"))))))))</f>
+        <v>C1</v>
+      </c>
+    </row>
+    <row r="98" spans="1:28" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A98" s="4"/>
       <c r="B98" s="4" t="s">
         <v>18</v>
@@ -5524,8 +6799,20 @@
         <f t="shared" si="15"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="99" spans="1:22" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="Z98" s="25" t="str">
+        <f>IF(AND(C98&lt;0.5, H98 &gt;= 0.5,M98&gt;=0.5, R98&lt;0.5), "F",IF(AND(C98&lt;0.5, H98 &gt;= 0.5,M98&gt;=0.5, R98&gt;=0.5), "E2",IF(AND(C98&lt;0.5, H98 &gt;= 0.5,M98&lt;0.5, R98&lt;0.5), "E1",IF(AND(C98&lt;0.5, H98 &gt;= 0.5,M98&lt;0.5, R98&gt;=0.5), "D2",IF(AND(C98&lt;0.5, H98 &lt;0.5,M98&gt;=0.5, R98&lt;0.5), "D1",IF(AND(C98&lt;0.5, H98 &lt; 0.5,M98&gt;=0.5, R98&gt;=0.5), "C2",IF(AND(C98&lt;0.5, H98 &lt; 0.5,M98&lt;0.5, R98&lt;0.5), "C1",IF(AND(C98&lt;0.5, H98 &lt; 0.5,M98&lt;0.5, R98&gt;=0.5), "B","A"))))))))</f>
+        <v>C1</v>
+      </c>
+      <c r="AA98" s="25" t="str">
+        <f>IF(AND(D98&lt;0.5, I98 &gt;= 0.5,N98&gt;=0.5, S98&lt;0.5), "F",IF(AND(D98&lt;0.5, I98 &gt;= 0.5,N98&gt;=0.5, S98&gt;=0.5), "E2",IF(AND(D98&lt;0.5, I98 &gt;= 0.5,N98&lt;0.5, S98&lt;0.5), "E1",IF(AND(D98&lt;0.5, I98 &gt;= 0.5,N98&lt;0.5, S98&gt;=0.5), "D2",IF(AND(D98&lt;0.5, I98 &lt;0.5,N98&gt;=0.5, S98&lt;0.5), "D1",IF(AND(D98&lt;0.5, I98 &lt; 0.5,N98&gt;=0.5, S98&gt;=0.5), "C2",IF(AND(D98&lt;0.5, I98 &lt; 0.5,N98&lt;0.5, S98&lt;0.5), "C1",IF(AND(D98&lt;0.5, I98 &lt; 0.5,N98&lt;0.5, S98&gt;=0.5), "B","A"))))))))</f>
+        <v>C1</v>
+      </c>
+      <c r="AB98" s="25" t="str">
+        <f>IF(AND(E98&lt;0.5, J98 &gt;= 0.5,O98&gt;=0.5, T98&lt;0.5), "F",IF(AND(E98&lt;0.5, J98 &gt;= 0.5,O98&gt;=0.5, T98&gt;=0.5), "E2",IF(AND(E98&lt;0.5, J98 &gt;= 0.5,O98&lt;0.5, T98&lt;0.5), "E1",IF(AND(E98&lt;0.5, J98 &gt;= 0.5,O98&lt;0.5, T98&gt;=0.5), "D2",IF(AND(E98&lt;0.5, J98 &lt;0.5,O98&gt;=0.5, T98&lt;0.5), "D1",IF(AND(E98&lt;0.5, J98 &lt; 0.5,O98&gt;=0.5, T98&gt;=0.5), "C2",IF(AND(E98&lt;0.5, J98 &lt; 0.5,O98&lt;0.5, T98&lt;0.5), "C1",IF(AND(E98&lt;0.5, J98 &lt; 0.5,O98&lt;0.5, T98&gt;=0.5), "B","A"))))))))</f>
+        <v>C1</v>
+      </c>
+    </row>
+    <row r="99" spans="1:28" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A99" s="3">
         <v>25</v>
       </c>
@@ -5576,8 +6863,20 @@
         <f t="shared" si="15"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="100" spans="1:22" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="Z99" s="25" t="str">
+        <f>IF(AND(C99&lt;0.5, H99 &gt;= 0.5,M99&gt;=0.5, R99&lt;0.5), "F",IF(AND(C99&lt;0.5, H99 &gt;= 0.5,M99&gt;=0.5, R99&gt;=0.5), "E2",IF(AND(C99&lt;0.5, H99 &gt;= 0.5,M99&lt;0.5, R99&lt;0.5), "E1",IF(AND(C99&lt;0.5, H99 &gt;= 0.5,M99&lt;0.5, R99&gt;=0.5), "D2",IF(AND(C99&lt;0.5, H99 &lt;0.5,M99&gt;=0.5, R99&lt;0.5), "D1",IF(AND(C99&lt;0.5, H99 &lt; 0.5,M99&gt;=0.5, R99&gt;=0.5), "C2",IF(AND(C99&lt;0.5, H99 &lt; 0.5,M99&lt;0.5, R99&lt;0.5), "C1",IF(AND(C99&lt;0.5, H99 &lt; 0.5,M99&lt;0.5, R99&gt;=0.5), "B","A"))))))))</f>
+        <v>C1</v>
+      </c>
+      <c r="AA99" s="25" t="str">
+        <f>IF(AND(D99&lt;0.5, I99 &gt;= 0.5,N99&gt;=0.5, S99&lt;0.5), "F",IF(AND(D99&lt;0.5, I99 &gt;= 0.5,N99&gt;=0.5, S99&gt;=0.5), "E2",IF(AND(D99&lt;0.5, I99 &gt;= 0.5,N99&lt;0.5, S99&lt;0.5), "E1",IF(AND(D99&lt;0.5, I99 &gt;= 0.5,N99&lt;0.5, S99&gt;=0.5), "D2",IF(AND(D99&lt;0.5, I99 &lt;0.5,N99&gt;=0.5, S99&lt;0.5), "D1",IF(AND(D99&lt;0.5, I99 &lt; 0.5,N99&gt;=0.5, S99&gt;=0.5), "C2",IF(AND(D99&lt;0.5, I99 &lt; 0.5,N99&lt;0.5, S99&lt;0.5), "C1",IF(AND(D99&lt;0.5, I99 &lt; 0.5,N99&lt;0.5, S99&gt;=0.5), "B","A"))))))))</f>
+        <v>C1</v>
+      </c>
+      <c r="AB99" s="25" t="str">
+        <f>IF(AND(E99&lt;0.5, J99 &gt;= 0.5,O99&gt;=0.5, T99&lt;0.5), "F",IF(AND(E99&lt;0.5, J99 &gt;= 0.5,O99&gt;=0.5, T99&gt;=0.5), "E2",IF(AND(E99&lt;0.5, J99 &gt;= 0.5,O99&lt;0.5, T99&lt;0.5), "E1",IF(AND(E99&lt;0.5, J99 &gt;= 0.5,O99&lt;0.5, T99&gt;=0.5), "D2",IF(AND(E99&lt;0.5, J99 &lt;0.5,O99&gt;=0.5, T99&lt;0.5), "D1",IF(AND(E99&lt;0.5, J99 &lt; 0.5,O99&gt;=0.5, T99&gt;=0.5), "C2",IF(AND(E99&lt;0.5, J99 &lt; 0.5,O99&lt;0.5, T99&lt;0.5), "C1",IF(AND(E99&lt;0.5, J99 &lt; 0.5,O99&lt;0.5, T99&gt;=0.5), "B","A"))))))))</f>
+        <v>C1</v>
+      </c>
+    </row>
+    <row r="100" spans="1:28" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A100" s="1"/>
       <c r="B100" s="1" t="s">
         <v>16</v>
@@ -5623,8 +6922,20 @@
         <f t="shared" si="15"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="101" spans="1:22" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="Z100" s="25" t="str">
+        <f>IF(AND(C100&lt;0.5, H100 &gt;= 0.5,M100&gt;=0.5, R100&lt;0.5), "F",IF(AND(C100&lt;0.5, H100 &gt;= 0.5,M100&gt;=0.5, R100&gt;=0.5), "E2",IF(AND(C100&lt;0.5, H100 &gt;= 0.5,M100&lt;0.5, R100&lt;0.5), "E1",IF(AND(C100&lt;0.5, H100 &gt;= 0.5,M100&lt;0.5, R100&gt;=0.5), "D2",IF(AND(C100&lt;0.5, H100 &lt;0.5,M100&gt;=0.5, R100&lt;0.5), "D1",IF(AND(C100&lt;0.5, H100 &lt; 0.5,M100&gt;=0.5, R100&gt;=0.5), "C2",IF(AND(C100&lt;0.5, H100 &lt; 0.5,M100&lt;0.5, R100&lt;0.5), "C1",IF(AND(C100&lt;0.5, H100 &lt; 0.5,M100&lt;0.5, R100&gt;=0.5), "B","A"))))))))</f>
+        <v>C1</v>
+      </c>
+      <c r="AA100" s="25" t="str">
+        <f>IF(AND(D100&lt;0.5, I100 &gt;= 0.5,N100&gt;=0.5, S100&lt;0.5), "F",IF(AND(D100&lt;0.5, I100 &gt;= 0.5,N100&gt;=0.5, S100&gt;=0.5), "E2",IF(AND(D100&lt;0.5, I100 &gt;= 0.5,N100&lt;0.5, S100&lt;0.5), "E1",IF(AND(D100&lt;0.5, I100 &gt;= 0.5,N100&lt;0.5, S100&gt;=0.5), "D2",IF(AND(D100&lt;0.5, I100 &lt;0.5,N100&gt;=0.5, S100&lt;0.5), "D1",IF(AND(D100&lt;0.5, I100 &lt; 0.5,N100&gt;=0.5, S100&gt;=0.5), "C2",IF(AND(D100&lt;0.5, I100 &lt; 0.5,N100&lt;0.5, S100&lt;0.5), "C1",IF(AND(D100&lt;0.5, I100 &lt; 0.5,N100&lt;0.5, S100&gt;=0.5), "B","A"))))))))</f>
+        <v>C1</v>
+      </c>
+      <c r="AB100" s="25" t="str">
+        <f>IF(AND(E100&lt;0.5, J100 &gt;= 0.5,O100&gt;=0.5, T100&lt;0.5), "F",IF(AND(E100&lt;0.5, J100 &gt;= 0.5,O100&gt;=0.5, T100&gt;=0.5), "E2",IF(AND(E100&lt;0.5, J100 &gt;= 0.5,O100&lt;0.5, T100&lt;0.5), "E1",IF(AND(E100&lt;0.5, J100 &gt;= 0.5,O100&lt;0.5, T100&gt;=0.5), "D2",IF(AND(E100&lt;0.5, J100 &lt;0.5,O100&gt;=0.5, T100&lt;0.5), "D1",IF(AND(E100&lt;0.5, J100 &lt; 0.5,O100&gt;=0.5, T100&gt;=0.5), "C2",IF(AND(E100&lt;0.5, J100 &lt; 0.5,O100&lt;0.5, T100&lt;0.5), "C1",IF(AND(E100&lt;0.5, J100 &lt; 0.5,O100&lt;0.5, T100&gt;=0.5), "B","A"))))))))</f>
+        <v>C1</v>
+      </c>
+    </row>
+    <row r="101" spans="1:28" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A101" s="1"/>
       <c r="B101" s="1" t="s">
         <v>17</v>
@@ -5670,8 +6981,20 @@
         <f t="shared" si="15"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="102" spans="1:22" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="Z101" s="25" t="str">
+        <f>IF(AND(C101&lt;0.5, H101 &gt;= 0.5,M101&gt;=0.5, R101&lt;0.5), "F",IF(AND(C101&lt;0.5, H101 &gt;= 0.5,M101&gt;=0.5, R101&gt;=0.5), "E2",IF(AND(C101&lt;0.5, H101 &gt;= 0.5,M101&lt;0.5, R101&lt;0.5), "E1",IF(AND(C101&lt;0.5, H101 &gt;= 0.5,M101&lt;0.5, R101&gt;=0.5), "D2",IF(AND(C101&lt;0.5, H101 &lt;0.5,M101&gt;=0.5, R101&lt;0.5), "D1",IF(AND(C101&lt;0.5, H101 &lt; 0.5,M101&gt;=0.5, R101&gt;=0.5), "C2",IF(AND(C101&lt;0.5, H101 &lt; 0.5,M101&lt;0.5, R101&lt;0.5), "C1",IF(AND(C101&lt;0.5, H101 &lt; 0.5,M101&lt;0.5, R101&gt;=0.5), "B","A"))))))))</f>
+        <v>C1</v>
+      </c>
+      <c r="AA101" s="25" t="str">
+        <f>IF(AND(D101&lt;0.5, I101 &gt;= 0.5,N101&gt;=0.5, S101&lt;0.5), "F",IF(AND(D101&lt;0.5, I101 &gt;= 0.5,N101&gt;=0.5, S101&gt;=0.5), "E2",IF(AND(D101&lt;0.5, I101 &gt;= 0.5,N101&lt;0.5, S101&lt;0.5), "E1",IF(AND(D101&lt;0.5, I101 &gt;= 0.5,N101&lt;0.5, S101&gt;=0.5), "D2",IF(AND(D101&lt;0.5, I101 &lt;0.5,N101&gt;=0.5, S101&lt;0.5), "D1",IF(AND(D101&lt;0.5, I101 &lt; 0.5,N101&gt;=0.5, S101&gt;=0.5), "C2",IF(AND(D101&lt;0.5, I101 &lt; 0.5,N101&lt;0.5, S101&lt;0.5), "C1",IF(AND(D101&lt;0.5, I101 &lt; 0.5,N101&lt;0.5, S101&gt;=0.5), "B","A"))))))))</f>
+        <v>C1</v>
+      </c>
+      <c r="AB101" s="25" t="str">
+        <f>IF(AND(E101&lt;0.5, J101 &gt;= 0.5,O101&gt;=0.5, T101&lt;0.5), "F",IF(AND(E101&lt;0.5, J101 &gt;= 0.5,O101&gt;=0.5, T101&gt;=0.5), "E2",IF(AND(E101&lt;0.5, J101 &gt;= 0.5,O101&lt;0.5, T101&lt;0.5), "E1",IF(AND(E101&lt;0.5, J101 &gt;= 0.5,O101&lt;0.5, T101&gt;=0.5), "D2",IF(AND(E101&lt;0.5, J101 &lt;0.5,O101&gt;=0.5, T101&lt;0.5), "D1",IF(AND(E101&lt;0.5, J101 &lt; 0.5,O101&gt;=0.5, T101&gt;=0.5), "C2",IF(AND(E101&lt;0.5, J101 &lt; 0.5,O101&lt;0.5, T101&lt;0.5), "C1",IF(AND(E101&lt;0.5, J101 &lt; 0.5,O101&lt;0.5, T101&gt;=0.5), "B","A"))))))))</f>
+        <v>C1</v>
+      </c>
+    </row>
+    <row r="102" spans="1:28" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A102" s="4"/>
       <c r="B102" s="4" t="s">
         <v>18</v>
@@ -5720,8 +7043,20 @@
         <f t="shared" si="15"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="103" spans="1:22" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="Z102" s="25" t="str">
+        <f>IF(AND(C102&lt;0.5, H102 &gt;= 0.5,M102&gt;=0.5, R102&lt;0.5), "F",IF(AND(C102&lt;0.5, H102 &gt;= 0.5,M102&gt;=0.5, R102&gt;=0.5), "E2",IF(AND(C102&lt;0.5, H102 &gt;= 0.5,M102&lt;0.5, R102&lt;0.5), "E1",IF(AND(C102&lt;0.5, H102 &gt;= 0.5,M102&lt;0.5, R102&gt;=0.5), "D2",IF(AND(C102&lt;0.5, H102 &lt;0.5,M102&gt;=0.5, R102&lt;0.5), "D1",IF(AND(C102&lt;0.5, H102 &lt; 0.5,M102&gt;=0.5, R102&gt;=0.5), "C2",IF(AND(C102&lt;0.5, H102 &lt; 0.5,M102&lt;0.5, R102&lt;0.5), "C1",IF(AND(C102&lt;0.5, H102 &lt; 0.5,M102&lt;0.5, R102&gt;=0.5), "B","A"))))))))</f>
+        <v>C1</v>
+      </c>
+      <c r="AA102" s="25" t="str">
+        <f>IF(AND(D102&lt;0.5, I102 &gt;= 0.5,N102&gt;=0.5, S102&lt;0.5), "F",IF(AND(D102&lt;0.5, I102 &gt;= 0.5,N102&gt;=0.5, S102&gt;=0.5), "E2",IF(AND(D102&lt;0.5, I102 &gt;= 0.5,N102&lt;0.5, S102&lt;0.5), "E1",IF(AND(D102&lt;0.5, I102 &gt;= 0.5,N102&lt;0.5, S102&gt;=0.5), "D2",IF(AND(D102&lt;0.5, I102 &lt;0.5,N102&gt;=0.5, S102&lt;0.5), "D1",IF(AND(D102&lt;0.5, I102 &lt; 0.5,N102&gt;=0.5, S102&gt;=0.5), "C2",IF(AND(D102&lt;0.5, I102 &lt; 0.5,N102&lt;0.5, S102&lt;0.5), "C1",IF(AND(D102&lt;0.5, I102 &lt; 0.5,N102&lt;0.5, S102&gt;=0.5), "B","A"))))))))</f>
+        <v>C1</v>
+      </c>
+      <c r="AB102" s="25" t="str">
+        <f>IF(AND(E102&lt;0.5, J102 &gt;= 0.5,O102&gt;=0.5, T102&lt;0.5), "F",IF(AND(E102&lt;0.5, J102 &gt;= 0.5,O102&gt;=0.5, T102&gt;=0.5), "E2",IF(AND(E102&lt;0.5, J102 &gt;= 0.5,O102&lt;0.5, T102&lt;0.5), "E1",IF(AND(E102&lt;0.5, J102 &gt;= 0.5,O102&lt;0.5, T102&gt;=0.5), "D2",IF(AND(E102&lt;0.5, J102 &lt;0.5,O102&gt;=0.5, T102&lt;0.5), "D1",IF(AND(E102&lt;0.5, J102 &lt; 0.5,O102&gt;=0.5, T102&gt;=0.5), "C2",IF(AND(E102&lt;0.5, J102 &lt; 0.5,O102&lt;0.5, T102&lt;0.5), "C1",IF(AND(E102&lt;0.5, J102 &lt; 0.5,O102&lt;0.5, T102&gt;=0.5), "B","A"))))))))</f>
+        <v>C1</v>
+      </c>
+    </row>
+    <row r="103" spans="1:28" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A103" s="3">
         <v>26</v>
       </c>
@@ -5772,8 +7107,20 @@
         <f t="shared" si="15"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="104" spans="1:22" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="Z103" s="25" t="str">
+        <f>IF(AND(C103&lt;0.5, H103 &gt;= 0.5,M103&gt;=0.5, R103&lt;0.5), "F",IF(AND(C103&lt;0.5, H103 &gt;= 0.5,M103&gt;=0.5, R103&gt;=0.5), "E2",IF(AND(C103&lt;0.5, H103 &gt;= 0.5,M103&lt;0.5, R103&lt;0.5), "E1",IF(AND(C103&lt;0.5, H103 &gt;= 0.5,M103&lt;0.5, R103&gt;=0.5), "D2",IF(AND(C103&lt;0.5, H103 &lt;0.5,M103&gt;=0.5, R103&lt;0.5), "D1",IF(AND(C103&lt;0.5, H103 &lt; 0.5,M103&gt;=0.5, R103&gt;=0.5), "C2",IF(AND(C103&lt;0.5, H103 &lt; 0.5,M103&lt;0.5, R103&lt;0.5), "C1",IF(AND(C103&lt;0.5, H103 &lt; 0.5,M103&lt;0.5, R103&gt;=0.5), "B","A"))))))))</f>
+        <v>C1</v>
+      </c>
+      <c r="AA103" s="25" t="str">
+        <f>IF(AND(D103&lt;0.5, I103 &gt;= 0.5,N103&gt;=0.5, S103&lt;0.5), "F",IF(AND(D103&lt;0.5, I103 &gt;= 0.5,N103&gt;=0.5, S103&gt;=0.5), "E2",IF(AND(D103&lt;0.5, I103 &gt;= 0.5,N103&lt;0.5, S103&lt;0.5), "E1",IF(AND(D103&lt;0.5, I103 &gt;= 0.5,N103&lt;0.5, S103&gt;=0.5), "D2",IF(AND(D103&lt;0.5, I103 &lt;0.5,N103&gt;=0.5, S103&lt;0.5), "D1",IF(AND(D103&lt;0.5, I103 &lt; 0.5,N103&gt;=0.5, S103&gt;=0.5), "C2",IF(AND(D103&lt;0.5, I103 &lt; 0.5,N103&lt;0.5, S103&lt;0.5), "C1",IF(AND(D103&lt;0.5, I103 &lt; 0.5,N103&lt;0.5, S103&gt;=0.5), "B","A"))))))))</f>
+        <v>C1</v>
+      </c>
+      <c r="AB103" s="25" t="str">
+        <f>IF(AND(E103&lt;0.5, J103 &gt;= 0.5,O103&gt;=0.5, T103&lt;0.5), "F",IF(AND(E103&lt;0.5, J103 &gt;= 0.5,O103&gt;=0.5, T103&gt;=0.5), "E2",IF(AND(E103&lt;0.5, J103 &gt;= 0.5,O103&lt;0.5, T103&lt;0.5), "E1",IF(AND(E103&lt;0.5, J103 &gt;= 0.5,O103&lt;0.5, T103&gt;=0.5), "D2",IF(AND(E103&lt;0.5, J103 &lt;0.5,O103&gt;=0.5, T103&lt;0.5), "D1",IF(AND(E103&lt;0.5, J103 &lt; 0.5,O103&gt;=0.5, T103&gt;=0.5), "C2",IF(AND(E103&lt;0.5, J103 &lt; 0.5,O103&lt;0.5, T103&lt;0.5), "C1",IF(AND(E103&lt;0.5, J103 &lt; 0.5,O103&lt;0.5, T103&gt;=0.5), "B","A"))))))))</f>
+        <v>C1</v>
+      </c>
+    </row>
+    <row r="104" spans="1:28" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A104" s="1"/>
       <c r="B104" s="1" t="s">
         <v>16</v>
@@ -5819,8 +7166,20 @@
         <f t="shared" si="15"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="105" spans="1:22" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="Z104" s="25" t="str">
+        <f>IF(AND(C104&lt;0.5, H104 &gt;= 0.5,M104&gt;=0.5, R104&lt;0.5), "F",IF(AND(C104&lt;0.5, H104 &gt;= 0.5,M104&gt;=0.5, R104&gt;=0.5), "E2",IF(AND(C104&lt;0.5, H104 &gt;= 0.5,M104&lt;0.5, R104&lt;0.5), "E1",IF(AND(C104&lt;0.5, H104 &gt;= 0.5,M104&lt;0.5, R104&gt;=0.5), "D2",IF(AND(C104&lt;0.5, H104 &lt;0.5,M104&gt;=0.5, R104&lt;0.5), "D1",IF(AND(C104&lt;0.5, H104 &lt; 0.5,M104&gt;=0.5, R104&gt;=0.5), "C2",IF(AND(C104&lt;0.5, H104 &lt; 0.5,M104&lt;0.5, R104&lt;0.5), "C1",IF(AND(C104&lt;0.5, H104 &lt; 0.5,M104&lt;0.5, R104&gt;=0.5), "B","A"))))))))</f>
+        <v>C1</v>
+      </c>
+      <c r="AA104" s="25" t="str">
+        <f>IF(AND(D104&lt;0.5, I104 &gt;= 0.5,N104&gt;=0.5, S104&lt;0.5), "F",IF(AND(D104&lt;0.5, I104 &gt;= 0.5,N104&gt;=0.5, S104&gt;=0.5), "E2",IF(AND(D104&lt;0.5, I104 &gt;= 0.5,N104&lt;0.5, S104&lt;0.5), "E1",IF(AND(D104&lt;0.5, I104 &gt;= 0.5,N104&lt;0.5, S104&gt;=0.5), "D2",IF(AND(D104&lt;0.5, I104 &lt;0.5,N104&gt;=0.5, S104&lt;0.5), "D1",IF(AND(D104&lt;0.5, I104 &lt; 0.5,N104&gt;=0.5, S104&gt;=0.5), "C2",IF(AND(D104&lt;0.5, I104 &lt; 0.5,N104&lt;0.5, S104&lt;0.5), "C1",IF(AND(D104&lt;0.5, I104 &lt; 0.5,N104&lt;0.5, S104&gt;=0.5), "B","A"))))))))</f>
+        <v>C1</v>
+      </c>
+      <c r="AB104" s="25" t="str">
+        <f>IF(AND(E104&lt;0.5, J104 &gt;= 0.5,O104&gt;=0.5, T104&lt;0.5), "F",IF(AND(E104&lt;0.5, J104 &gt;= 0.5,O104&gt;=0.5, T104&gt;=0.5), "E2",IF(AND(E104&lt;0.5, J104 &gt;= 0.5,O104&lt;0.5, T104&lt;0.5), "E1",IF(AND(E104&lt;0.5, J104 &gt;= 0.5,O104&lt;0.5, T104&gt;=0.5), "D2",IF(AND(E104&lt;0.5, J104 &lt;0.5,O104&gt;=0.5, T104&lt;0.5), "D1",IF(AND(E104&lt;0.5, J104 &lt; 0.5,O104&gt;=0.5, T104&gt;=0.5), "C2",IF(AND(E104&lt;0.5, J104 &lt; 0.5,O104&lt;0.5, T104&lt;0.5), "C1",IF(AND(E104&lt;0.5, J104 &lt; 0.5,O104&lt;0.5, T104&gt;=0.5), "B","A"))))))))</f>
+        <v>C1</v>
+      </c>
+    </row>
+    <row r="105" spans="1:28" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A105" s="1"/>
       <c r="B105" s="1" t="s">
         <v>17</v>
@@ -5866,8 +7225,20 @@
         <f t="shared" si="15"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="106" spans="1:22" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="Z105" s="25" t="str">
+        <f>IF(AND(C105&lt;0.5, H105 &gt;= 0.5,M105&gt;=0.5, R105&lt;0.5), "F",IF(AND(C105&lt;0.5, H105 &gt;= 0.5,M105&gt;=0.5, R105&gt;=0.5), "E2",IF(AND(C105&lt;0.5, H105 &gt;= 0.5,M105&lt;0.5, R105&lt;0.5), "E1",IF(AND(C105&lt;0.5, H105 &gt;= 0.5,M105&lt;0.5, R105&gt;=0.5), "D2",IF(AND(C105&lt;0.5, H105 &lt;0.5,M105&gt;=0.5, R105&lt;0.5), "D1",IF(AND(C105&lt;0.5, H105 &lt; 0.5,M105&gt;=0.5, R105&gt;=0.5), "C2",IF(AND(C105&lt;0.5, H105 &lt; 0.5,M105&lt;0.5, R105&lt;0.5), "C1",IF(AND(C105&lt;0.5, H105 &lt; 0.5,M105&lt;0.5, R105&gt;=0.5), "B","A"))))))))</f>
+        <v>C1</v>
+      </c>
+      <c r="AA105" s="25" t="str">
+        <f>IF(AND(D105&lt;0.5, I105 &gt;= 0.5,N105&gt;=0.5, S105&lt;0.5), "F",IF(AND(D105&lt;0.5, I105 &gt;= 0.5,N105&gt;=0.5, S105&gt;=0.5), "E2",IF(AND(D105&lt;0.5, I105 &gt;= 0.5,N105&lt;0.5, S105&lt;0.5), "E1",IF(AND(D105&lt;0.5, I105 &gt;= 0.5,N105&lt;0.5, S105&gt;=0.5), "D2",IF(AND(D105&lt;0.5, I105 &lt;0.5,N105&gt;=0.5, S105&lt;0.5), "D1",IF(AND(D105&lt;0.5, I105 &lt; 0.5,N105&gt;=0.5, S105&gt;=0.5), "C2",IF(AND(D105&lt;0.5, I105 &lt; 0.5,N105&lt;0.5, S105&lt;0.5), "C1",IF(AND(D105&lt;0.5, I105 &lt; 0.5,N105&lt;0.5, S105&gt;=0.5), "B","A"))))))))</f>
+        <v>C1</v>
+      </c>
+      <c r="AB105" s="25" t="str">
+        <f>IF(AND(E105&lt;0.5, J105 &gt;= 0.5,O105&gt;=0.5, T105&lt;0.5), "F",IF(AND(E105&lt;0.5, J105 &gt;= 0.5,O105&gt;=0.5, T105&gt;=0.5), "E2",IF(AND(E105&lt;0.5, J105 &gt;= 0.5,O105&lt;0.5, T105&lt;0.5), "E1",IF(AND(E105&lt;0.5, J105 &gt;= 0.5,O105&lt;0.5, T105&gt;=0.5), "D2",IF(AND(E105&lt;0.5, J105 &lt;0.5,O105&gt;=0.5, T105&lt;0.5), "D1",IF(AND(E105&lt;0.5, J105 &lt; 0.5,O105&gt;=0.5, T105&gt;=0.5), "C2",IF(AND(E105&lt;0.5, J105 &lt; 0.5,O105&lt;0.5, T105&lt;0.5), "C1",IF(AND(E105&lt;0.5, J105 &lt; 0.5,O105&lt;0.5, T105&gt;=0.5), "B","A"))))))))</f>
+        <v>C1</v>
+      </c>
+    </row>
+    <row r="106" spans="1:28" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A106" s="4"/>
       <c r="B106" s="4" t="s">
         <v>18</v>
@@ -5916,8 +7287,20 @@
         <f t="shared" si="15"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="107" spans="1:22" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="Z106" s="25" t="str">
+        <f>IF(AND(C106&lt;0.5, H106 &gt;= 0.5,M106&gt;=0.5, R106&lt;0.5), "F",IF(AND(C106&lt;0.5, H106 &gt;= 0.5,M106&gt;=0.5, R106&gt;=0.5), "E2",IF(AND(C106&lt;0.5, H106 &gt;= 0.5,M106&lt;0.5, R106&lt;0.5), "E1",IF(AND(C106&lt;0.5, H106 &gt;= 0.5,M106&lt;0.5, R106&gt;=0.5), "D2",IF(AND(C106&lt;0.5, H106 &lt;0.5,M106&gt;=0.5, R106&lt;0.5), "D1",IF(AND(C106&lt;0.5, H106 &lt; 0.5,M106&gt;=0.5, R106&gt;=0.5), "C2",IF(AND(C106&lt;0.5, H106 &lt; 0.5,M106&lt;0.5, R106&lt;0.5), "C1",IF(AND(C106&lt;0.5, H106 &lt; 0.5,M106&lt;0.5, R106&gt;=0.5), "B","A"))))))))</f>
+        <v>C1</v>
+      </c>
+      <c r="AA106" s="25" t="str">
+        <f>IF(AND(D106&lt;0.5, I106 &gt;= 0.5,N106&gt;=0.5, S106&lt;0.5), "F",IF(AND(D106&lt;0.5, I106 &gt;= 0.5,N106&gt;=0.5, S106&gt;=0.5), "E2",IF(AND(D106&lt;0.5, I106 &gt;= 0.5,N106&lt;0.5, S106&lt;0.5), "E1",IF(AND(D106&lt;0.5, I106 &gt;= 0.5,N106&lt;0.5, S106&gt;=0.5), "D2",IF(AND(D106&lt;0.5, I106 &lt;0.5,N106&gt;=0.5, S106&lt;0.5), "D1",IF(AND(D106&lt;0.5, I106 &lt; 0.5,N106&gt;=0.5, S106&gt;=0.5), "C2",IF(AND(D106&lt;0.5, I106 &lt; 0.5,N106&lt;0.5, S106&lt;0.5), "C1",IF(AND(D106&lt;0.5, I106 &lt; 0.5,N106&lt;0.5, S106&gt;=0.5), "B","A"))))))))</f>
+        <v>C1</v>
+      </c>
+      <c r="AB106" s="25" t="str">
+        <f>IF(AND(E106&lt;0.5, J106 &gt;= 0.5,O106&gt;=0.5, T106&lt;0.5), "F",IF(AND(E106&lt;0.5, J106 &gt;= 0.5,O106&gt;=0.5, T106&gt;=0.5), "E2",IF(AND(E106&lt;0.5, J106 &gt;= 0.5,O106&lt;0.5, T106&lt;0.5), "E1",IF(AND(E106&lt;0.5, J106 &gt;= 0.5,O106&lt;0.5, T106&gt;=0.5), "D2",IF(AND(E106&lt;0.5, J106 &lt;0.5,O106&gt;=0.5, T106&lt;0.5), "D1",IF(AND(E106&lt;0.5, J106 &lt; 0.5,O106&gt;=0.5, T106&gt;=0.5), "C2",IF(AND(E106&lt;0.5, J106 &lt; 0.5,O106&lt;0.5, T106&lt;0.5), "C1",IF(AND(E106&lt;0.5, J106 &lt; 0.5,O106&lt;0.5, T106&gt;=0.5), "B","A"))))))))</f>
+        <v>C1</v>
+      </c>
+    </row>
+    <row r="107" spans="1:28" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A107" s="3">
         <v>27</v>
       </c>
@@ -5968,8 +7351,20 @@
         <f t="shared" si="15"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="108" spans="1:22" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="Z107" s="25" t="str">
+        <f>IF(AND(C107&lt;0.5, H107 &gt;= 0.5,M107&gt;=0.5, R107&lt;0.5), "F",IF(AND(C107&lt;0.5, H107 &gt;= 0.5,M107&gt;=0.5, R107&gt;=0.5), "E2",IF(AND(C107&lt;0.5, H107 &gt;= 0.5,M107&lt;0.5, R107&lt;0.5), "E1",IF(AND(C107&lt;0.5, H107 &gt;= 0.5,M107&lt;0.5, R107&gt;=0.5), "D2",IF(AND(C107&lt;0.5, H107 &lt;0.5,M107&gt;=0.5, R107&lt;0.5), "D1",IF(AND(C107&lt;0.5, H107 &lt; 0.5,M107&gt;=0.5, R107&gt;=0.5), "C2",IF(AND(C107&lt;0.5, H107 &lt; 0.5,M107&lt;0.5, R107&lt;0.5), "C1",IF(AND(C107&lt;0.5, H107 &lt; 0.5,M107&lt;0.5, R107&gt;=0.5), "B","A"))))))))</f>
+        <v>C1</v>
+      </c>
+      <c r="AA107" s="25" t="str">
+        <f>IF(AND(D107&lt;0.5, I107 &gt;= 0.5,N107&gt;=0.5, S107&lt;0.5), "F",IF(AND(D107&lt;0.5, I107 &gt;= 0.5,N107&gt;=0.5, S107&gt;=0.5), "E2",IF(AND(D107&lt;0.5, I107 &gt;= 0.5,N107&lt;0.5, S107&lt;0.5), "E1",IF(AND(D107&lt;0.5, I107 &gt;= 0.5,N107&lt;0.5, S107&gt;=0.5), "D2",IF(AND(D107&lt;0.5, I107 &lt;0.5,N107&gt;=0.5, S107&lt;0.5), "D1",IF(AND(D107&lt;0.5, I107 &lt; 0.5,N107&gt;=0.5, S107&gt;=0.5), "C2",IF(AND(D107&lt;0.5, I107 &lt; 0.5,N107&lt;0.5, S107&lt;0.5), "C1",IF(AND(D107&lt;0.5, I107 &lt; 0.5,N107&lt;0.5, S107&gt;=0.5), "B","A"))))))))</f>
+        <v>C1</v>
+      </c>
+      <c r="AB107" s="25" t="str">
+        <f>IF(AND(E107&lt;0.5, J107 &gt;= 0.5,O107&gt;=0.5, T107&lt;0.5), "F",IF(AND(E107&lt;0.5, J107 &gt;= 0.5,O107&gt;=0.5, T107&gt;=0.5), "E2",IF(AND(E107&lt;0.5, J107 &gt;= 0.5,O107&lt;0.5, T107&lt;0.5), "E1",IF(AND(E107&lt;0.5, J107 &gt;= 0.5,O107&lt;0.5, T107&gt;=0.5), "D2",IF(AND(E107&lt;0.5, J107 &lt;0.5,O107&gt;=0.5, T107&lt;0.5), "D1",IF(AND(E107&lt;0.5, J107 &lt; 0.5,O107&gt;=0.5, T107&gt;=0.5), "C2",IF(AND(E107&lt;0.5, J107 &lt; 0.5,O107&lt;0.5, T107&lt;0.5), "C1",IF(AND(E107&lt;0.5, J107 &lt; 0.5,O107&lt;0.5, T107&gt;=0.5), "B","A"))))))))</f>
+        <v>C1</v>
+      </c>
+    </row>
+    <row r="108" spans="1:28" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A108" s="1"/>
       <c r="B108" s="1" t="s">
         <v>16</v>
@@ -6015,8 +7410,20 @@
         <f t="shared" si="15"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="109" spans="1:22" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="Z108" s="25" t="str">
+        <f>IF(AND(C108&lt;0.5, H108 &gt;= 0.5,M108&gt;=0.5, R108&lt;0.5), "F",IF(AND(C108&lt;0.5, H108 &gt;= 0.5,M108&gt;=0.5, R108&gt;=0.5), "E2",IF(AND(C108&lt;0.5, H108 &gt;= 0.5,M108&lt;0.5, R108&lt;0.5), "E1",IF(AND(C108&lt;0.5, H108 &gt;= 0.5,M108&lt;0.5, R108&gt;=0.5), "D2",IF(AND(C108&lt;0.5, H108 &lt;0.5,M108&gt;=0.5, R108&lt;0.5), "D1",IF(AND(C108&lt;0.5, H108 &lt; 0.5,M108&gt;=0.5, R108&gt;=0.5), "C2",IF(AND(C108&lt;0.5, H108 &lt; 0.5,M108&lt;0.5, R108&lt;0.5), "C1",IF(AND(C108&lt;0.5, H108 &lt; 0.5,M108&lt;0.5, R108&gt;=0.5), "B","A"))))))))</f>
+        <v>C1</v>
+      </c>
+      <c r="AA108" s="25" t="str">
+        <f>IF(AND(D108&lt;0.5, I108 &gt;= 0.5,N108&gt;=0.5, S108&lt;0.5), "F",IF(AND(D108&lt;0.5, I108 &gt;= 0.5,N108&gt;=0.5, S108&gt;=0.5), "E2",IF(AND(D108&lt;0.5, I108 &gt;= 0.5,N108&lt;0.5, S108&lt;0.5), "E1",IF(AND(D108&lt;0.5, I108 &gt;= 0.5,N108&lt;0.5, S108&gt;=0.5), "D2",IF(AND(D108&lt;0.5, I108 &lt;0.5,N108&gt;=0.5, S108&lt;0.5), "D1",IF(AND(D108&lt;0.5, I108 &lt; 0.5,N108&gt;=0.5, S108&gt;=0.5), "C2",IF(AND(D108&lt;0.5, I108 &lt; 0.5,N108&lt;0.5, S108&lt;0.5), "C1",IF(AND(D108&lt;0.5, I108 &lt; 0.5,N108&lt;0.5, S108&gt;=0.5), "B","A"))))))))</f>
+        <v>C1</v>
+      </c>
+      <c r="AB108" s="25" t="str">
+        <f>IF(AND(E108&lt;0.5, J108 &gt;= 0.5,O108&gt;=0.5, T108&lt;0.5), "F",IF(AND(E108&lt;0.5, J108 &gt;= 0.5,O108&gt;=0.5, T108&gt;=0.5), "E2",IF(AND(E108&lt;0.5, J108 &gt;= 0.5,O108&lt;0.5, T108&lt;0.5), "E1",IF(AND(E108&lt;0.5, J108 &gt;= 0.5,O108&lt;0.5, T108&gt;=0.5), "D2",IF(AND(E108&lt;0.5, J108 &lt;0.5,O108&gt;=0.5, T108&lt;0.5), "D1",IF(AND(E108&lt;0.5, J108 &lt; 0.5,O108&gt;=0.5, T108&gt;=0.5), "C2",IF(AND(E108&lt;0.5, J108 &lt; 0.5,O108&lt;0.5, T108&lt;0.5), "C1",IF(AND(E108&lt;0.5, J108 &lt; 0.5,O108&lt;0.5, T108&gt;=0.5), "B","A"))))))))</f>
+        <v>C1</v>
+      </c>
+    </row>
+    <row r="109" spans="1:28" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A109" s="1"/>
       <c r="B109" s="1" t="s">
         <v>17</v>
@@ -6062,8 +7469,20 @@
         <f t="shared" si="15"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="110" spans="1:22" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="Z109" s="25" t="str">
+        <f>IF(AND(C109&lt;0.5, H109 &gt;= 0.5,M109&gt;=0.5, R109&lt;0.5), "F",IF(AND(C109&lt;0.5, H109 &gt;= 0.5,M109&gt;=0.5, R109&gt;=0.5), "E2",IF(AND(C109&lt;0.5, H109 &gt;= 0.5,M109&lt;0.5, R109&lt;0.5), "E1",IF(AND(C109&lt;0.5, H109 &gt;= 0.5,M109&lt;0.5, R109&gt;=0.5), "D2",IF(AND(C109&lt;0.5, H109 &lt;0.5,M109&gt;=0.5, R109&lt;0.5), "D1",IF(AND(C109&lt;0.5, H109 &lt; 0.5,M109&gt;=0.5, R109&gt;=0.5), "C2",IF(AND(C109&lt;0.5, H109 &lt; 0.5,M109&lt;0.5, R109&lt;0.5), "C1",IF(AND(C109&lt;0.5, H109 &lt; 0.5,M109&lt;0.5, R109&gt;=0.5), "B","A"))))))))</f>
+        <v>C1</v>
+      </c>
+      <c r="AA109" s="25" t="str">
+        <f>IF(AND(D109&lt;0.5, I109 &gt;= 0.5,N109&gt;=0.5, S109&lt;0.5), "F",IF(AND(D109&lt;0.5, I109 &gt;= 0.5,N109&gt;=0.5, S109&gt;=0.5), "E2",IF(AND(D109&lt;0.5, I109 &gt;= 0.5,N109&lt;0.5, S109&lt;0.5), "E1",IF(AND(D109&lt;0.5, I109 &gt;= 0.5,N109&lt;0.5, S109&gt;=0.5), "D2",IF(AND(D109&lt;0.5, I109 &lt;0.5,N109&gt;=0.5, S109&lt;0.5), "D1",IF(AND(D109&lt;0.5, I109 &lt; 0.5,N109&gt;=0.5, S109&gt;=0.5), "C2",IF(AND(D109&lt;0.5, I109 &lt; 0.5,N109&lt;0.5, S109&lt;0.5), "C1",IF(AND(D109&lt;0.5, I109 &lt; 0.5,N109&lt;0.5, S109&gt;=0.5), "B","A"))))))))</f>
+        <v>C1</v>
+      </c>
+      <c r="AB109" s="25" t="str">
+        <f>IF(AND(E109&lt;0.5, J109 &gt;= 0.5,O109&gt;=0.5, T109&lt;0.5), "F",IF(AND(E109&lt;0.5, J109 &gt;= 0.5,O109&gt;=0.5, T109&gt;=0.5), "E2",IF(AND(E109&lt;0.5, J109 &gt;= 0.5,O109&lt;0.5, T109&lt;0.5), "E1",IF(AND(E109&lt;0.5, J109 &gt;= 0.5,O109&lt;0.5, T109&gt;=0.5), "D2",IF(AND(E109&lt;0.5, J109 &lt;0.5,O109&gt;=0.5, T109&lt;0.5), "D1",IF(AND(E109&lt;0.5, J109 &lt; 0.5,O109&gt;=0.5, T109&gt;=0.5), "C2",IF(AND(E109&lt;0.5, J109 &lt; 0.5,O109&lt;0.5, T109&lt;0.5), "C1",IF(AND(E109&lt;0.5, J109 &lt; 0.5,O109&lt;0.5, T109&gt;=0.5), "B","A"))))))))</f>
+        <v>C1</v>
+      </c>
+    </row>
+    <row r="110" spans="1:28" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A110" s="4"/>
       <c r="B110" s="4" t="s">
         <v>18</v>
@@ -6112,8 +7531,20 @@
         <f t="shared" si="15"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="111" spans="1:22" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="Z110" s="25" t="str">
+        <f>IF(AND(C110&lt;0.5, H110 &gt;= 0.5,M110&gt;=0.5, R110&lt;0.5), "F",IF(AND(C110&lt;0.5, H110 &gt;= 0.5,M110&gt;=0.5, R110&gt;=0.5), "E2",IF(AND(C110&lt;0.5, H110 &gt;= 0.5,M110&lt;0.5, R110&lt;0.5), "E1",IF(AND(C110&lt;0.5, H110 &gt;= 0.5,M110&lt;0.5, R110&gt;=0.5), "D2",IF(AND(C110&lt;0.5, H110 &lt;0.5,M110&gt;=0.5, R110&lt;0.5), "D1",IF(AND(C110&lt;0.5, H110 &lt; 0.5,M110&gt;=0.5, R110&gt;=0.5), "C2",IF(AND(C110&lt;0.5, H110 &lt; 0.5,M110&lt;0.5, R110&lt;0.5), "C1",IF(AND(C110&lt;0.5, H110 &lt; 0.5,M110&lt;0.5, R110&gt;=0.5), "B","A"))))))))</f>
+        <v>C1</v>
+      </c>
+      <c r="AA110" s="25" t="str">
+        <f>IF(AND(D110&lt;0.5, I110 &gt;= 0.5,N110&gt;=0.5, S110&lt;0.5), "F",IF(AND(D110&lt;0.5, I110 &gt;= 0.5,N110&gt;=0.5, S110&gt;=0.5), "E2",IF(AND(D110&lt;0.5, I110 &gt;= 0.5,N110&lt;0.5, S110&lt;0.5), "E1",IF(AND(D110&lt;0.5, I110 &gt;= 0.5,N110&lt;0.5, S110&gt;=0.5), "D2",IF(AND(D110&lt;0.5, I110 &lt;0.5,N110&gt;=0.5, S110&lt;0.5), "D1",IF(AND(D110&lt;0.5, I110 &lt; 0.5,N110&gt;=0.5, S110&gt;=0.5), "C2",IF(AND(D110&lt;0.5, I110 &lt; 0.5,N110&lt;0.5, S110&lt;0.5), "C1",IF(AND(D110&lt;0.5, I110 &lt; 0.5,N110&lt;0.5, S110&gt;=0.5), "B","A"))))))))</f>
+        <v>C1</v>
+      </c>
+      <c r="AB110" s="25" t="str">
+        <f>IF(AND(E110&lt;0.5, J110 &gt;= 0.5,O110&gt;=0.5, T110&lt;0.5), "F",IF(AND(E110&lt;0.5, J110 &gt;= 0.5,O110&gt;=0.5, T110&gt;=0.5), "E2",IF(AND(E110&lt;0.5, J110 &gt;= 0.5,O110&lt;0.5, T110&lt;0.5), "E1",IF(AND(E110&lt;0.5, J110 &gt;= 0.5,O110&lt;0.5, T110&gt;=0.5), "D2",IF(AND(E110&lt;0.5, J110 &lt;0.5,O110&gt;=0.5, T110&lt;0.5), "D1",IF(AND(E110&lt;0.5, J110 &lt; 0.5,O110&gt;=0.5, T110&gt;=0.5), "C2",IF(AND(E110&lt;0.5, J110 &lt; 0.5,O110&lt;0.5, T110&lt;0.5), "C1",IF(AND(E110&lt;0.5, J110 &lt; 0.5,O110&lt;0.5, T110&gt;=0.5), "B","A"))))))))</f>
+        <v>C1</v>
+      </c>
+    </row>
+    <row r="111" spans="1:28" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A111" s="3">
         <v>28</v>
       </c>
@@ -6164,8 +7595,20 @@
         <f t="shared" si="15"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="112" spans="1:22" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="Z111" s="25" t="str">
+        <f>IF(AND(C111&lt;0.5, H111 &gt;= 0.5,M111&gt;=0.5, R111&lt;0.5), "F",IF(AND(C111&lt;0.5, H111 &gt;= 0.5,M111&gt;=0.5, R111&gt;=0.5), "E2",IF(AND(C111&lt;0.5, H111 &gt;= 0.5,M111&lt;0.5, R111&lt;0.5), "E1",IF(AND(C111&lt;0.5, H111 &gt;= 0.5,M111&lt;0.5, R111&gt;=0.5), "D2",IF(AND(C111&lt;0.5, H111 &lt;0.5,M111&gt;=0.5, R111&lt;0.5), "D1",IF(AND(C111&lt;0.5, H111 &lt; 0.5,M111&gt;=0.5, R111&gt;=0.5), "C2",IF(AND(C111&lt;0.5, H111 &lt; 0.5,M111&lt;0.5, R111&lt;0.5), "C1",IF(AND(C111&lt;0.5, H111 &lt; 0.5,M111&lt;0.5, R111&gt;=0.5), "B","A"))))))))</f>
+        <v>C1</v>
+      </c>
+      <c r="AA111" s="25" t="str">
+        <f>IF(AND(D111&lt;0.5, I111 &gt;= 0.5,N111&gt;=0.5, S111&lt;0.5), "F",IF(AND(D111&lt;0.5, I111 &gt;= 0.5,N111&gt;=0.5, S111&gt;=0.5), "E2",IF(AND(D111&lt;0.5, I111 &gt;= 0.5,N111&lt;0.5, S111&lt;0.5), "E1",IF(AND(D111&lt;0.5, I111 &gt;= 0.5,N111&lt;0.5, S111&gt;=0.5), "D2",IF(AND(D111&lt;0.5, I111 &lt;0.5,N111&gt;=0.5, S111&lt;0.5), "D1",IF(AND(D111&lt;0.5, I111 &lt; 0.5,N111&gt;=0.5, S111&gt;=0.5), "C2",IF(AND(D111&lt;0.5, I111 &lt; 0.5,N111&lt;0.5, S111&lt;0.5), "C1",IF(AND(D111&lt;0.5, I111 &lt; 0.5,N111&lt;0.5, S111&gt;=0.5), "B","A"))))))))</f>
+        <v>C1</v>
+      </c>
+      <c r="AB111" s="25" t="str">
+        <f>IF(AND(E111&lt;0.5, J111 &gt;= 0.5,O111&gt;=0.5, T111&lt;0.5), "F",IF(AND(E111&lt;0.5, J111 &gt;= 0.5,O111&gt;=0.5, T111&gt;=0.5), "E2",IF(AND(E111&lt;0.5, J111 &gt;= 0.5,O111&lt;0.5, T111&lt;0.5), "E1",IF(AND(E111&lt;0.5, J111 &gt;= 0.5,O111&lt;0.5, T111&gt;=0.5), "D2",IF(AND(E111&lt;0.5, J111 &lt;0.5,O111&gt;=0.5, T111&lt;0.5), "D1",IF(AND(E111&lt;0.5, J111 &lt; 0.5,O111&gt;=0.5, T111&gt;=0.5), "C2",IF(AND(E111&lt;0.5, J111 &lt; 0.5,O111&lt;0.5, T111&lt;0.5), "C1",IF(AND(E111&lt;0.5, J111 &lt; 0.5,O111&lt;0.5, T111&gt;=0.5), "B","A"))))))))</f>
+        <v>C1</v>
+      </c>
+    </row>
+    <row r="112" spans="1:28" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A112" s="1"/>
       <c r="B112" s="1" t="s">
         <v>16</v>
@@ -6211,8 +7654,20 @@
         <f t="shared" si="15"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="113" spans="1:22" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="Z112" s="25" t="str">
+        <f>IF(AND(C112&lt;0.5, H112 &gt;= 0.5,M112&gt;=0.5, R112&lt;0.5), "F",IF(AND(C112&lt;0.5, H112 &gt;= 0.5,M112&gt;=0.5, R112&gt;=0.5), "E2",IF(AND(C112&lt;0.5, H112 &gt;= 0.5,M112&lt;0.5, R112&lt;0.5), "E1",IF(AND(C112&lt;0.5, H112 &gt;= 0.5,M112&lt;0.5, R112&gt;=0.5), "D2",IF(AND(C112&lt;0.5, H112 &lt;0.5,M112&gt;=0.5, R112&lt;0.5), "D1",IF(AND(C112&lt;0.5, H112 &lt; 0.5,M112&gt;=0.5, R112&gt;=0.5), "C2",IF(AND(C112&lt;0.5, H112 &lt; 0.5,M112&lt;0.5, R112&lt;0.5), "C1",IF(AND(C112&lt;0.5, H112 &lt; 0.5,M112&lt;0.5, R112&gt;=0.5), "B","A"))))))))</f>
+        <v>C1</v>
+      </c>
+      <c r="AA112" s="25" t="str">
+        <f>IF(AND(D112&lt;0.5, I112 &gt;= 0.5,N112&gt;=0.5, S112&lt;0.5), "F",IF(AND(D112&lt;0.5, I112 &gt;= 0.5,N112&gt;=0.5, S112&gt;=0.5), "E2",IF(AND(D112&lt;0.5, I112 &gt;= 0.5,N112&lt;0.5, S112&lt;0.5), "E1",IF(AND(D112&lt;0.5, I112 &gt;= 0.5,N112&lt;0.5, S112&gt;=0.5), "D2",IF(AND(D112&lt;0.5, I112 &lt;0.5,N112&gt;=0.5, S112&lt;0.5), "D1",IF(AND(D112&lt;0.5, I112 &lt; 0.5,N112&gt;=0.5, S112&gt;=0.5), "C2",IF(AND(D112&lt;0.5, I112 &lt; 0.5,N112&lt;0.5, S112&lt;0.5), "C1",IF(AND(D112&lt;0.5, I112 &lt; 0.5,N112&lt;0.5, S112&gt;=0.5), "B","A"))))))))</f>
+        <v>C1</v>
+      </c>
+      <c r="AB112" s="25" t="str">
+        <f>IF(AND(E112&lt;0.5, J112 &gt;= 0.5,O112&gt;=0.5, T112&lt;0.5), "F",IF(AND(E112&lt;0.5, J112 &gt;= 0.5,O112&gt;=0.5, T112&gt;=0.5), "E2",IF(AND(E112&lt;0.5, J112 &gt;= 0.5,O112&lt;0.5, T112&lt;0.5), "E1",IF(AND(E112&lt;0.5, J112 &gt;= 0.5,O112&lt;0.5, T112&gt;=0.5), "D2",IF(AND(E112&lt;0.5, J112 &lt;0.5,O112&gt;=0.5, T112&lt;0.5), "D1",IF(AND(E112&lt;0.5, J112 &lt; 0.5,O112&gt;=0.5, T112&gt;=0.5), "C2",IF(AND(E112&lt;0.5, J112 &lt; 0.5,O112&lt;0.5, T112&lt;0.5), "C1",IF(AND(E112&lt;0.5, J112 &lt; 0.5,O112&lt;0.5, T112&gt;=0.5), "B","A"))))))))</f>
+        <v>C1</v>
+      </c>
+    </row>
+    <row r="113" spans="1:28" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A113" s="1"/>
       <c r="B113" s="1" t="s">
         <v>17</v>
@@ -6258,8 +7713,20 @@
         <f t="shared" si="15"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="114" spans="1:22" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="Z113" s="25" t="str">
+        <f>IF(AND(C113&lt;0.5, H113 &gt;= 0.5,M113&gt;=0.5, R113&lt;0.5), "F",IF(AND(C113&lt;0.5, H113 &gt;= 0.5,M113&gt;=0.5, R113&gt;=0.5), "E2",IF(AND(C113&lt;0.5, H113 &gt;= 0.5,M113&lt;0.5, R113&lt;0.5), "E1",IF(AND(C113&lt;0.5, H113 &gt;= 0.5,M113&lt;0.5, R113&gt;=0.5), "D2",IF(AND(C113&lt;0.5, H113 &lt;0.5,M113&gt;=0.5, R113&lt;0.5), "D1",IF(AND(C113&lt;0.5, H113 &lt; 0.5,M113&gt;=0.5, R113&gt;=0.5), "C2",IF(AND(C113&lt;0.5, H113 &lt; 0.5,M113&lt;0.5, R113&lt;0.5), "C1",IF(AND(C113&lt;0.5, H113 &lt; 0.5,M113&lt;0.5, R113&gt;=0.5), "B","A"))))))))</f>
+        <v>C1</v>
+      </c>
+      <c r="AA113" s="25" t="str">
+        <f>IF(AND(D113&lt;0.5, I113 &gt;= 0.5,N113&gt;=0.5, S113&lt;0.5), "F",IF(AND(D113&lt;0.5, I113 &gt;= 0.5,N113&gt;=0.5, S113&gt;=0.5), "E2",IF(AND(D113&lt;0.5, I113 &gt;= 0.5,N113&lt;0.5, S113&lt;0.5), "E1",IF(AND(D113&lt;0.5, I113 &gt;= 0.5,N113&lt;0.5, S113&gt;=0.5), "D2",IF(AND(D113&lt;0.5, I113 &lt;0.5,N113&gt;=0.5, S113&lt;0.5), "D1",IF(AND(D113&lt;0.5, I113 &lt; 0.5,N113&gt;=0.5, S113&gt;=0.5), "C2",IF(AND(D113&lt;0.5, I113 &lt; 0.5,N113&lt;0.5, S113&lt;0.5), "C1",IF(AND(D113&lt;0.5, I113 &lt; 0.5,N113&lt;0.5, S113&gt;=0.5), "B","A"))))))))</f>
+        <v>C1</v>
+      </c>
+      <c r="AB113" s="25" t="str">
+        <f>IF(AND(E113&lt;0.5, J113 &gt;= 0.5,O113&gt;=0.5, T113&lt;0.5), "F",IF(AND(E113&lt;0.5, J113 &gt;= 0.5,O113&gt;=0.5, T113&gt;=0.5), "E2",IF(AND(E113&lt;0.5, J113 &gt;= 0.5,O113&lt;0.5, T113&lt;0.5), "E1",IF(AND(E113&lt;0.5, J113 &gt;= 0.5,O113&lt;0.5, T113&gt;=0.5), "D2",IF(AND(E113&lt;0.5, J113 &lt;0.5,O113&gt;=0.5, T113&lt;0.5), "D1",IF(AND(E113&lt;0.5, J113 &lt; 0.5,O113&gt;=0.5, T113&gt;=0.5), "C2",IF(AND(E113&lt;0.5, J113 &lt; 0.5,O113&lt;0.5, T113&lt;0.5), "C1",IF(AND(E113&lt;0.5, J113 &lt; 0.5,O113&lt;0.5, T113&gt;=0.5), "B","A"))))))))</f>
+        <v>C1</v>
+      </c>
+    </row>
+    <row r="114" spans="1:28" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A114" s="4"/>
       <c r="B114" s="4" t="s">
         <v>18</v>
@@ -6308,8 +7775,20 @@
         <f t="shared" si="15"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="115" spans="1:22" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="Z114" s="25" t="str">
+        <f>IF(AND(C114&lt;0.5, H114 &gt;= 0.5,M114&gt;=0.5, R114&lt;0.5), "F",IF(AND(C114&lt;0.5, H114 &gt;= 0.5,M114&gt;=0.5, R114&gt;=0.5), "E2",IF(AND(C114&lt;0.5, H114 &gt;= 0.5,M114&lt;0.5, R114&lt;0.5), "E1",IF(AND(C114&lt;0.5, H114 &gt;= 0.5,M114&lt;0.5, R114&gt;=0.5), "D2",IF(AND(C114&lt;0.5, H114 &lt;0.5,M114&gt;=0.5, R114&lt;0.5), "D1",IF(AND(C114&lt;0.5, H114 &lt; 0.5,M114&gt;=0.5, R114&gt;=0.5), "C2",IF(AND(C114&lt;0.5, H114 &lt; 0.5,M114&lt;0.5, R114&lt;0.5), "C1",IF(AND(C114&lt;0.5, H114 &lt; 0.5,M114&lt;0.5, R114&gt;=0.5), "B","A"))))))))</f>
+        <v>C1</v>
+      </c>
+      <c r="AA114" s="25" t="str">
+        <f>IF(AND(D114&lt;0.5, I114 &gt;= 0.5,N114&gt;=0.5, S114&lt;0.5), "F",IF(AND(D114&lt;0.5, I114 &gt;= 0.5,N114&gt;=0.5, S114&gt;=0.5), "E2",IF(AND(D114&lt;0.5, I114 &gt;= 0.5,N114&lt;0.5, S114&lt;0.5), "E1",IF(AND(D114&lt;0.5, I114 &gt;= 0.5,N114&lt;0.5, S114&gt;=0.5), "D2",IF(AND(D114&lt;0.5, I114 &lt;0.5,N114&gt;=0.5, S114&lt;0.5), "D1",IF(AND(D114&lt;0.5, I114 &lt; 0.5,N114&gt;=0.5, S114&gt;=0.5), "C2",IF(AND(D114&lt;0.5, I114 &lt; 0.5,N114&lt;0.5, S114&lt;0.5), "C1",IF(AND(D114&lt;0.5, I114 &lt; 0.5,N114&lt;0.5, S114&gt;=0.5), "B","A"))))))))</f>
+        <v>C1</v>
+      </c>
+      <c r="AB114" s="25" t="str">
+        <f>IF(AND(E114&lt;0.5, J114 &gt;= 0.5,O114&gt;=0.5, T114&lt;0.5), "F",IF(AND(E114&lt;0.5, J114 &gt;= 0.5,O114&gt;=0.5, T114&gt;=0.5), "E2",IF(AND(E114&lt;0.5, J114 &gt;= 0.5,O114&lt;0.5, T114&lt;0.5), "E1",IF(AND(E114&lt;0.5, J114 &gt;= 0.5,O114&lt;0.5, T114&gt;=0.5), "D2",IF(AND(E114&lt;0.5, J114 &lt;0.5,O114&gt;=0.5, T114&lt;0.5), "D1",IF(AND(E114&lt;0.5, J114 &lt; 0.5,O114&gt;=0.5, T114&gt;=0.5), "C2",IF(AND(E114&lt;0.5, J114 &lt; 0.5,O114&lt;0.5, T114&lt;0.5), "C1",IF(AND(E114&lt;0.5, J114 &lt; 0.5,O114&lt;0.5, T114&gt;=0.5), "B","A"))))))))</f>
+        <v>C1</v>
+      </c>
+    </row>
+    <row r="115" spans="1:28" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A115" s="3">
         <v>29</v>
       </c>
@@ -6360,8 +7839,20 @@
         <f t="shared" si="15"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="116" spans="1:22" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="Z115" s="25" t="str">
+        <f>IF(AND(C115&lt;0.5, H115 &gt;= 0.5,M115&gt;=0.5, R115&lt;0.5), "F",IF(AND(C115&lt;0.5, H115 &gt;= 0.5,M115&gt;=0.5, R115&gt;=0.5), "E2",IF(AND(C115&lt;0.5, H115 &gt;= 0.5,M115&lt;0.5, R115&lt;0.5), "E1",IF(AND(C115&lt;0.5, H115 &gt;= 0.5,M115&lt;0.5, R115&gt;=0.5), "D2",IF(AND(C115&lt;0.5, H115 &lt;0.5,M115&gt;=0.5, R115&lt;0.5), "D1",IF(AND(C115&lt;0.5, H115 &lt; 0.5,M115&gt;=0.5, R115&gt;=0.5), "C2",IF(AND(C115&lt;0.5, H115 &lt; 0.5,M115&lt;0.5, R115&lt;0.5), "C1",IF(AND(C115&lt;0.5, H115 &lt; 0.5,M115&lt;0.5, R115&gt;=0.5), "B","A"))))))))</f>
+        <v>C1</v>
+      </c>
+      <c r="AA115" s="25" t="str">
+        <f>IF(AND(D115&lt;0.5, I115 &gt;= 0.5,N115&gt;=0.5, S115&lt;0.5), "F",IF(AND(D115&lt;0.5, I115 &gt;= 0.5,N115&gt;=0.5, S115&gt;=0.5), "E2",IF(AND(D115&lt;0.5, I115 &gt;= 0.5,N115&lt;0.5, S115&lt;0.5), "E1",IF(AND(D115&lt;0.5, I115 &gt;= 0.5,N115&lt;0.5, S115&gt;=0.5), "D2",IF(AND(D115&lt;0.5, I115 &lt;0.5,N115&gt;=0.5, S115&lt;0.5), "D1",IF(AND(D115&lt;0.5, I115 &lt; 0.5,N115&gt;=0.5, S115&gt;=0.5), "C2",IF(AND(D115&lt;0.5, I115 &lt; 0.5,N115&lt;0.5, S115&lt;0.5), "C1",IF(AND(D115&lt;0.5, I115 &lt; 0.5,N115&lt;0.5, S115&gt;=0.5), "B","A"))))))))</f>
+        <v>C1</v>
+      </c>
+      <c r="AB115" s="25" t="str">
+        <f>IF(AND(E115&lt;0.5, J115 &gt;= 0.5,O115&gt;=0.5, T115&lt;0.5), "F",IF(AND(E115&lt;0.5, J115 &gt;= 0.5,O115&gt;=0.5, T115&gt;=0.5), "E2",IF(AND(E115&lt;0.5, J115 &gt;= 0.5,O115&lt;0.5, T115&lt;0.5), "E1",IF(AND(E115&lt;0.5, J115 &gt;= 0.5,O115&lt;0.5, T115&gt;=0.5), "D2",IF(AND(E115&lt;0.5, J115 &lt;0.5,O115&gt;=0.5, T115&lt;0.5), "D1",IF(AND(E115&lt;0.5, J115 &lt; 0.5,O115&gt;=0.5, T115&gt;=0.5), "C2",IF(AND(E115&lt;0.5, J115 &lt; 0.5,O115&lt;0.5, T115&lt;0.5), "C1",IF(AND(E115&lt;0.5, J115 &lt; 0.5,O115&lt;0.5, T115&gt;=0.5), "B","A"))))))))</f>
+        <v>C1</v>
+      </c>
+    </row>
+    <row r="116" spans="1:28" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A116" s="1"/>
       <c r="B116" s="1" t="s">
         <v>16</v>
@@ -6407,8 +7898,20 @@
         <f t="shared" si="15"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="117" spans="1:22" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="Z116" s="25" t="str">
+        <f>IF(AND(C116&lt;0.5, H116 &gt;= 0.5,M116&gt;=0.5, R116&lt;0.5), "F",IF(AND(C116&lt;0.5, H116 &gt;= 0.5,M116&gt;=0.5, R116&gt;=0.5), "E2",IF(AND(C116&lt;0.5, H116 &gt;= 0.5,M116&lt;0.5, R116&lt;0.5), "E1",IF(AND(C116&lt;0.5, H116 &gt;= 0.5,M116&lt;0.5, R116&gt;=0.5), "D2",IF(AND(C116&lt;0.5, H116 &lt;0.5,M116&gt;=0.5, R116&lt;0.5), "D1",IF(AND(C116&lt;0.5, H116 &lt; 0.5,M116&gt;=0.5, R116&gt;=0.5), "C2",IF(AND(C116&lt;0.5, H116 &lt; 0.5,M116&lt;0.5, R116&lt;0.5), "C1",IF(AND(C116&lt;0.5, H116 &lt; 0.5,M116&lt;0.5, R116&gt;=0.5), "B","A"))))))))</f>
+        <v>C1</v>
+      </c>
+      <c r="AA116" s="25" t="str">
+        <f>IF(AND(D116&lt;0.5, I116 &gt;= 0.5,N116&gt;=0.5, S116&lt;0.5), "F",IF(AND(D116&lt;0.5, I116 &gt;= 0.5,N116&gt;=0.5, S116&gt;=0.5), "E2",IF(AND(D116&lt;0.5, I116 &gt;= 0.5,N116&lt;0.5, S116&lt;0.5), "E1",IF(AND(D116&lt;0.5, I116 &gt;= 0.5,N116&lt;0.5, S116&gt;=0.5), "D2",IF(AND(D116&lt;0.5, I116 &lt;0.5,N116&gt;=0.5, S116&lt;0.5), "D1",IF(AND(D116&lt;0.5, I116 &lt; 0.5,N116&gt;=0.5, S116&gt;=0.5), "C2",IF(AND(D116&lt;0.5, I116 &lt; 0.5,N116&lt;0.5, S116&lt;0.5), "C1",IF(AND(D116&lt;0.5, I116 &lt; 0.5,N116&lt;0.5, S116&gt;=0.5), "B","A"))))))))</f>
+        <v>C1</v>
+      </c>
+      <c r="AB116" s="25" t="str">
+        <f>IF(AND(E116&lt;0.5, J116 &gt;= 0.5,O116&gt;=0.5, T116&lt;0.5), "F",IF(AND(E116&lt;0.5, J116 &gt;= 0.5,O116&gt;=0.5, T116&gt;=0.5), "E2",IF(AND(E116&lt;0.5, J116 &gt;= 0.5,O116&lt;0.5, T116&lt;0.5), "E1",IF(AND(E116&lt;0.5, J116 &gt;= 0.5,O116&lt;0.5, T116&gt;=0.5), "D2",IF(AND(E116&lt;0.5, J116 &lt;0.5,O116&gt;=0.5, T116&lt;0.5), "D1",IF(AND(E116&lt;0.5, J116 &lt; 0.5,O116&gt;=0.5, T116&gt;=0.5), "C2",IF(AND(E116&lt;0.5, J116 &lt; 0.5,O116&lt;0.5, T116&lt;0.5), "C1",IF(AND(E116&lt;0.5, J116 &lt; 0.5,O116&lt;0.5, T116&gt;=0.5), "B","A"))))))))</f>
+        <v>C1</v>
+      </c>
+    </row>
+    <row r="117" spans="1:28" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A117" s="1"/>
       <c r="B117" s="1" t="s">
         <v>17</v>
@@ -6454,8 +7957,20 @@
         <f t="shared" si="15"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="118" spans="1:22" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="Z117" s="25" t="str">
+        <f>IF(AND(C117&lt;0.5, H117 &gt;= 0.5,M117&gt;=0.5, R117&lt;0.5), "F",IF(AND(C117&lt;0.5, H117 &gt;= 0.5,M117&gt;=0.5, R117&gt;=0.5), "E2",IF(AND(C117&lt;0.5, H117 &gt;= 0.5,M117&lt;0.5, R117&lt;0.5), "E1",IF(AND(C117&lt;0.5, H117 &gt;= 0.5,M117&lt;0.5, R117&gt;=0.5), "D2",IF(AND(C117&lt;0.5, H117 &lt;0.5,M117&gt;=0.5, R117&lt;0.5), "D1",IF(AND(C117&lt;0.5, H117 &lt; 0.5,M117&gt;=0.5, R117&gt;=0.5), "C2",IF(AND(C117&lt;0.5, H117 &lt; 0.5,M117&lt;0.5, R117&lt;0.5), "C1",IF(AND(C117&lt;0.5, H117 &lt; 0.5,M117&lt;0.5, R117&gt;=0.5), "B","A"))))))))</f>
+        <v>C1</v>
+      </c>
+      <c r="AA117" s="25" t="str">
+        <f>IF(AND(D117&lt;0.5, I117 &gt;= 0.5,N117&gt;=0.5, S117&lt;0.5), "F",IF(AND(D117&lt;0.5, I117 &gt;= 0.5,N117&gt;=0.5, S117&gt;=0.5), "E2",IF(AND(D117&lt;0.5, I117 &gt;= 0.5,N117&lt;0.5, S117&lt;0.5), "E1",IF(AND(D117&lt;0.5, I117 &gt;= 0.5,N117&lt;0.5, S117&gt;=0.5), "D2",IF(AND(D117&lt;0.5, I117 &lt;0.5,N117&gt;=0.5, S117&lt;0.5), "D1",IF(AND(D117&lt;0.5, I117 &lt; 0.5,N117&gt;=0.5, S117&gt;=0.5), "C2",IF(AND(D117&lt;0.5, I117 &lt; 0.5,N117&lt;0.5, S117&lt;0.5), "C1",IF(AND(D117&lt;0.5, I117 &lt; 0.5,N117&lt;0.5, S117&gt;=0.5), "B","A"))))))))</f>
+        <v>C1</v>
+      </c>
+      <c r="AB117" s="25" t="str">
+        <f>IF(AND(E117&lt;0.5, J117 &gt;= 0.5,O117&gt;=0.5, T117&lt;0.5), "F",IF(AND(E117&lt;0.5, J117 &gt;= 0.5,O117&gt;=0.5, T117&gt;=0.5), "E2",IF(AND(E117&lt;0.5, J117 &gt;= 0.5,O117&lt;0.5, T117&lt;0.5), "E1",IF(AND(E117&lt;0.5, J117 &gt;= 0.5,O117&lt;0.5, T117&gt;=0.5), "D2",IF(AND(E117&lt;0.5, J117 &lt;0.5,O117&gt;=0.5, T117&lt;0.5), "D1",IF(AND(E117&lt;0.5, J117 &lt; 0.5,O117&gt;=0.5, T117&gt;=0.5), "C2",IF(AND(E117&lt;0.5, J117 &lt; 0.5,O117&lt;0.5, T117&lt;0.5), "C1",IF(AND(E117&lt;0.5, J117 &lt; 0.5,O117&lt;0.5, T117&gt;=0.5), "B","A"))))))))</f>
+        <v>C1</v>
+      </c>
+    </row>
+    <row r="118" spans="1:28" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A118" s="4"/>
       <c r="B118" s="4" t="s">
         <v>18</v>
@@ -6504,8 +8019,20 @@
         <f t="shared" si="15"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="119" spans="1:22" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="Z118" s="25" t="str">
+        <f>IF(AND(C118&lt;0.5, H118 &gt;= 0.5,M118&gt;=0.5, R118&lt;0.5), "F",IF(AND(C118&lt;0.5, H118 &gt;= 0.5,M118&gt;=0.5, R118&gt;=0.5), "E2",IF(AND(C118&lt;0.5, H118 &gt;= 0.5,M118&lt;0.5, R118&lt;0.5), "E1",IF(AND(C118&lt;0.5, H118 &gt;= 0.5,M118&lt;0.5, R118&gt;=0.5), "D2",IF(AND(C118&lt;0.5, H118 &lt;0.5,M118&gt;=0.5, R118&lt;0.5), "D1",IF(AND(C118&lt;0.5, H118 &lt; 0.5,M118&gt;=0.5, R118&gt;=0.5), "C2",IF(AND(C118&lt;0.5, H118 &lt; 0.5,M118&lt;0.5, R118&lt;0.5), "C1",IF(AND(C118&lt;0.5, H118 &lt; 0.5,M118&lt;0.5, R118&gt;=0.5), "B","A"))))))))</f>
+        <v>C1</v>
+      </c>
+      <c r="AA118" s="25" t="str">
+        <f>IF(AND(D118&lt;0.5, I118 &gt;= 0.5,N118&gt;=0.5, S118&lt;0.5), "F",IF(AND(D118&lt;0.5, I118 &gt;= 0.5,N118&gt;=0.5, S118&gt;=0.5), "E2",IF(AND(D118&lt;0.5, I118 &gt;= 0.5,N118&lt;0.5, S118&lt;0.5), "E1",IF(AND(D118&lt;0.5, I118 &gt;= 0.5,N118&lt;0.5, S118&gt;=0.5), "D2",IF(AND(D118&lt;0.5, I118 &lt;0.5,N118&gt;=0.5, S118&lt;0.5), "D1",IF(AND(D118&lt;0.5, I118 &lt; 0.5,N118&gt;=0.5, S118&gt;=0.5), "C2",IF(AND(D118&lt;0.5, I118 &lt; 0.5,N118&lt;0.5, S118&lt;0.5), "C1",IF(AND(D118&lt;0.5, I118 &lt; 0.5,N118&lt;0.5, S118&gt;=0.5), "B","A"))))))))</f>
+        <v>C1</v>
+      </c>
+      <c r="AB118" s="25" t="str">
+        <f>IF(AND(E118&lt;0.5, J118 &gt;= 0.5,O118&gt;=0.5, T118&lt;0.5), "F",IF(AND(E118&lt;0.5, J118 &gt;= 0.5,O118&gt;=0.5, T118&gt;=0.5), "E2",IF(AND(E118&lt;0.5, J118 &gt;= 0.5,O118&lt;0.5, T118&lt;0.5), "E1",IF(AND(E118&lt;0.5, J118 &gt;= 0.5,O118&lt;0.5, T118&gt;=0.5), "D2",IF(AND(E118&lt;0.5, J118 &lt;0.5,O118&gt;=0.5, T118&lt;0.5), "D1",IF(AND(E118&lt;0.5, J118 &lt; 0.5,O118&gt;=0.5, T118&gt;=0.5), "C2",IF(AND(E118&lt;0.5, J118 &lt; 0.5,O118&lt;0.5, T118&lt;0.5), "C1",IF(AND(E118&lt;0.5, J118 &lt; 0.5,O118&lt;0.5, T118&gt;=0.5), "B","A"))))))))</f>
+        <v>C1</v>
+      </c>
+    </row>
+    <row r="119" spans="1:28" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A119" s="3">
         <v>30</v>
       </c>
@@ -6556,8 +8083,20 @@
         <f t="shared" si="15"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="120" spans="1:22" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="Z119" s="25" t="str">
+        <f>IF(AND(C119&lt;0.5, H119 &gt;= 0.5,M119&gt;=0.5, R119&lt;0.5), "F",IF(AND(C119&lt;0.5, H119 &gt;= 0.5,M119&gt;=0.5, R119&gt;=0.5), "E2",IF(AND(C119&lt;0.5, H119 &gt;= 0.5,M119&lt;0.5, R119&lt;0.5), "E1",IF(AND(C119&lt;0.5, H119 &gt;= 0.5,M119&lt;0.5, R119&gt;=0.5), "D2",IF(AND(C119&lt;0.5, H119 &lt;0.5,M119&gt;=0.5, R119&lt;0.5), "D1",IF(AND(C119&lt;0.5, H119 &lt; 0.5,M119&gt;=0.5, R119&gt;=0.5), "C2",IF(AND(C119&lt;0.5, H119 &lt; 0.5,M119&lt;0.5, R119&lt;0.5), "C1",IF(AND(C119&lt;0.5, H119 &lt; 0.5,M119&lt;0.5, R119&gt;=0.5), "B","A"))))))))</f>
+        <v>C1</v>
+      </c>
+      <c r="AA119" s="25" t="str">
+        <f>IF(AND(D119&lt;0.5, I119 &gt;= 0.5,N119&gt;=0.5, S119&lt;0.5), "F",IF(AND(D119&lt;0.5, I119 &gt;= 0.5,N119&gt;=0.5, S119&gt;=0.5), "E2",IF(AND(D119&lt;0.5, I119 &gt;= 0.5,N119&lt;0.5, S119&lt;0.5), "E1",IF(AND(D119&lt;0.5, I119 &gt;= 0.5,N119&lt;0.5, S119&gt;=0.5), "D2",IF(AND(D119&lt;0.5, I119 &lt;0.5,N119&gt;=0.5, S119&lt;0.5), "D1",IF(AND(D119&lt;0.5, I119 &lt; 0.5,N119&gt;=0.5, S119&gt;=0.5), "C2",IF(AND(D119&lt;0.5, I119 &lt; 0.5,N119&lt;0.5, S119&lt;0.5), "C1",IF(AND(D119&lt;0.5, I119 &lt; 0.5,N119&lt;0.5, S119&gt;=0.5), "B","A"))))))))</f>
+        <v>C1</v>
+      </c>
+      <c r="AB119" s="25" t="str">
+        <f>IF(AND(E119&lt;0.5, J119 &gt;= 0.5,O119&gt;=0.5, T119&lt;0.5), "F",IF(AND(E119&lt;0.5, J119 &gt;= 0.5,O119&gt;=0.5, T119&gt;=0.5), "E2",IF(AND(E119&lt;0.5, J119 &gt;= 0.5,O119&lt;0.5, T119&lt;0.5), "E1",IF(AND(E119&lt;0.5, J119 &gt;= 0.5,O119&lt;0.5, T119&gt;=0.5), "D2",IF(AND(E119&lt;0.5, J119 &lt;0.5,O119&gt;=0.5, T119&lt;0.5), "D1",IF(AND(E119&lt;0.5, J119 &lt; 0.5,O119&gt;=0.5, T119&gt;=0.5), "C2",IF(AND(E119&lt;0.5, J119 &lt; 0.5,O119&lt;0.5, T119&lt;0.5), "C1",IF(AND(E119&lt;0.5, J119 &lt; 0.5,O119&lt;0.5, T119&gt;=0.5), "B","A"))))))))</f>
+        <v>C1</v>
+      </c>
+    </row>
+    <row r="120" spans="1:28" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A120" s="1"/>
       <c r="B120" s="1" t="s">
         <v>16</v>
@@ -6603,8 +8142,20 @@
         <f t="shared" si="15"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="121" spans="1:22" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="Z120" s="25" t="str">
+        <f>IF(AND(C120&lt;0.5, H120 &gt;= 0.5,M120&gt;=0.5, R120&lt;0.5), "F",IF(AND(C120&lt;0.5, H120 &gt;= 0.5,M120&gt;=0.5, R120&gt;=0.5), "E2",IF(AND(C120&lt;0.5, H120 &gt;= 0.5,M120&lt;0.5, R120&lt;0.5), "E1",IF(AND(C120&lt;0.5, H120 &gt;= 0.5,M120&lt;0.5, R120&gt;=0.5), "D2",IF(AND(C120&lt;0.5, H120 &lt;0.5,M120&gt;=0.5, R120&lt;0.5), "D1",IF(AND(C120&lt;0.5, H120 &lt; 0.5,M120&gt;=0.5, R120&gt;=0.5), "C2",IF(AND(C120&lt;0.5, H120 &lt; 0.5,M120&lt;0.5, R120&lt;0.5), "C1",IF(AND(C120&lt;0.5, H120 &lt; 0.5,M120&lt;0.5, R120&gt;=0.5), "B","A"))))))))</f>
+        <v>C1</v>
+      </c>
+      <c r="AA120" s="25" t="str">
+        <f>IF(AND(D120&lt;0.5, I120 &gt;= 0.5,N120&gt;=0.5, S120&lt;0.5), "F",IF(AND(D120&lt;0.5, I120 &gt;= 0.5,N120&gt;=0.5, S120&gt;=0.5), "E2",IF(AND(D120&lt;0.5, I120 &gt;= 0.5,N120&lt;0.5, S120&lt;0.5), "E1",IF(AND(D120&lt;0.5, I120 &gt;= 0.5,N120&lt;0.5, S120&gt;=0.5), "D2",IF(AND(D120&lt;0.5, I120 &lt;0.5,N120&gt;=0.5, S120&lt;0.5), "D1",IF(AND(D120&lt;0.5, I120 &lt; 0.5,N120&gt;=0.5, S120&gt;=0.5), "C2",IF(AND(D120&lt;0.5, I120 &lt; 0.5,N120&lt;0.5, S120&lt;0.5), "C1",IF(AND(D120&lt;0.5, I120 &lt; 0.5,N120&lt;0.5, S120&gt;=0.5), "B","A"))))))))</f>
+        <v>C1</v>
+      </c>
+      <c r="AB120" s="25" t="str">
+        <f>IF(AND(E120&lt;0.5, J120 &gt;= 0.5,O120&gt;=0.5, T120&lt;0.5), "F",IF(AND(E120&lt;0.5, J120 &gt;= 0.5,O120&gt;=0.5, T120&gt;=0.5), "E2",IF(AND(E120&lt;0.5, J120 &gt;= 0.5,O120&lt;0.5, T120&lt;0.5), "E1",IF(AND(E120&lt;0.5, J120 &gt;= 0.5,O120&lt;0.5, T120&gt;=0.5), "D2",IF(AND(E120&lt;0.5, J120 &lt;0.5,O120&gt;=0.5, T120&lt;0.5), "D1",IF(AND(E120&lt;0.5, J120 &lt; 0.5,O120&gt;=0.5, T120&gt;=0.5), "C2",IF(AND(E120&lt;0.5, J120 &lt; 0.5,O120&lt;0.5, T120&lt;0.5), "C1",IF(AND(E120&lt;0.5, J120 &lt; 0.5,O120&lt;0.5, T120&gt;=0.5), "B","A"))))))))</f>
+        <v>C1</v>
+      </c>
+    </row>
+    <row r="121" spans="1:28" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A121" s="1"/>
       <c r="B121" s="1" t="s">
         <v>17</v>
@@ -6650,8 +8201,20 @@
         <f t="shared" si="15"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="122" spans="1:22" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="Z121" s="25" t="str">
+        <f>IF(AND(C121&lt;0.5, H121 &gt;= 0.5,M121&gt;=0.5, R121&lt;0.5), "F",IF(AND(C121&lt;0.5, H121 &gt;= 0.5,M121&gt;=0.5, R121&gt;=0.5), "E2",IF(AND(C121&lt;0.5, H121 &gt;= 0.5,M121&lt;0.5, R121&lt;0.5), "E1",IF(AND(C121&lt;0.5, H121 &gt;= 0.5,M121&lt;0.5, R121&gt;=0.5), "D2",IF(AND(C121&lt;0.5, H121 &lt;0.5,M121&gt;=0.5, R121&lt;0.5), "D1",IF(AND(C121&lt;0.5, H121 &lt; 0.5,M121&gt;=0.5, R121&gt;=0.5), "C2",IF(AND(C121&lt;0.5, H121 &lt; 0.5,M121&lt;0.5, R121&lt;0.5), "C1",IF(AND(C121&lt;0.5, H121 &lt; 0.5,M121&lt;0.5, R121&gt;=0.5), "B","A"))))))))</f>
+        <v>C1</v>
+      </c>
+      <c r="AA121" s="25" t="str">
+        <f>IF(AND(D121&lt;0.5, I121 &gt;= 0.5,N121&gt;=0.5, S121&lt;0.5), "F",IF(AND(D121&lt;0.5, I121 &gt;= 0.5,N121&gt;=0.5, S121&gt;=0.5), "E2",IF(AND(D121&lt;0.5, I121 &gt;= 0.5,N121&lt;0.5, S121&lt;0.5), "E1",IF(AND(D121&lt;0.5, I121 &gt;= 0.5,N121&lt;0.5, S121&gt;=0.5), "D2",IF(AND(D121&lt;0.5, I121 &lt;0.5,N121&gt;=0.5, S121&lt;0.5), "D1",IF(AND(D121&lt;0.5, I121 &lt; 0.5,N121&gt;=0.5, S121&gt;=0.5), "C2",IF(AND(D121&lt;0.5, I121 &lt; 0.5,N121&lt;0.5, S121&lt;0.5), "C1",IF(AND(D121&lt;0.5, I121 &lt; 0.5,N121&lt;0.5, S121&gt;=0.5), "B","A"))))))))</f>
+        <v>C1</v>
+      </c>
+      <c r="AB121" s="25" t="str">
+        <f>IF(AND(E121&lt;0.5, J121 &gt;= 0.5,O121&gt;=0.5, T121&lt;0.5), "F",IF(AND(E121&lt;0.5, J121 &gt;= 0.5,O121&gt;=0.5, T121&gt;=0.5), "E2",IF(AND(E121&lt;0.5, J121 &gt;= 0.5,O121&lt;0.5, T121&lt;0.5), "E1",IF(AND(E121&lt;0.5, J121 &gt;= 0.5,O121&lt;0.5, T121&gt;=0.5), "D2",IF(AND(E121&lt;0.5, J121 &lt;0.5,O121&gt;=0.5, T121&lt;0.5), "D1",IF(AND(E121&lt;0.5, J121 &lt; 0.5,O121&gt;=0.5, T121&gt;=0.5), "C2",IF(AND(E121&lt;0.5, J121 &lt; 0.5,O121&lt;0.5, T121&lt;0.5), "C1",IF(AND(E121&lt;0.5, J121 &lt; 0.5,O121&lt;0.5, T121&gt;=0.5), "B","A"))))))))</f>
+        <v>C1</v>
+      </c>
+    </row>
+    <row r="122" spans="1:28" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A122" s="4"/>
       <c r="B122" s="4" t="s">
         <v>18</v>
@@ -6700,8 +8263,20 @@
         <f t="shared" si="15"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="123" spans="1:22" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="Z122" s="25" t="str">
+        <f>IF(AND(C122&lt;0.5, H122 &gt;= 0.5,M122&gt;=0.5, R122&lt;0.5), "F",IF(AND(C122&lt;0.5, H122 &gt;= 0.5,M122&gt;=0.5, R122&gt;=0.5), "E2",IF(AND(C122&lt;0.5, H122 &gt;= 0.5,M122&lt;0.5, R122&lt;0.5), "E1",IF(AND(C122&lt;0.5, H122 &gt;= 0.5,M122&lt;0.5, R122&gt;=0.5), "D2",IF(AND(C122&lt;0.5, H122 &lt;0.5,M122&gt;=0.5, R122&lt;0.5), "D1",IF(AND(C122&lt;0.5, H122 &lt; 0.5,M122&gt;=0.5, R122&gt;=0.5), "C2",IF(AND(C122&lt;0.5, H122 &lt; 0.5,M122&lt;0.5, R122&lt;0.5), "C1",IF(AND(C122&lt;0.5, H122 &lt; 0.5,M122&lt;0.5, R122&gt;=0.5), "B","A"))))))))</f>
+        <v>C1</v>
+      </c>
+      <c r="AA122" s="25" t="str">
+        <f>IF(AND(D122&lt;0.5, I122 &gt;= 0.5,N122&gt;=0.5, S122&lt;0.5), "F",IF(AND(D122&lt;0.5, I122 &gt;= 0.5,N122&gt;=0.5, S122&gt;=0.5), "E2",IF(AND(D122&lt;0.5, I122 &gt;= 0.5,N122&lt;0.5, S122&lt;0.5), "E1",IF(AND(D122&lt;0.5, I122 &gt;= 0.5,N122&lt;0.5, S122&gt;=0.5), "D2",IF(AND(D122&lt;0.5, I122 &lt;0.5,N122&gt;=0.5, S122&lt;0.5), "D1",IF(AND(D122&lt;0.5, I122 &lt; 0.5,N122&gt;=0.5, S122&gt;=0.5), "C2",IF(AND(D122&lt;0.5, I122 &lt; 0.5,N122&lt;0.5, S122&lt;0.5), "C1",IF(AND(D122&lt;0.5, I122 &lt; 0.5,N122&lt;0.5, S122&gt;=0.5), "B","A"))))))))</f>
+        <v>C1</v>
+      </c>
+      <c r="AB122" s="25" t="str">
+        <f>IF(AND(E122&lt;0.5, J122 &gt;= 0.5,O122&gt;=0.5, T122&lt;0.5), "F",IF(AND(E122&lt;0.5, J122 &gt;= 0.5,O122&gt;=0.5, T122&gt;=0.5), "E2",IF(AND(E122&lt;0.5, J122 &gt;= 0.5,O122&lt;0.5, T122&lt;0.5), "E1",IF(AND(E122&lt;0.5, J122 &gt;= 0.5,O122&lt;0.5, T122&gt;=0.5), "D2",IF(AND(E122&lt;0.5, J122 &lt;0.5,O122&gt;=0.5, T122&lt;0.5), "D1",IF(AND(E122&lt;0.5, J122 &lt; 0.5,O122&gt;=0.5, T122&gt;=0.5), "C2",IF(AND(E122&lt;0.5, J122 &lt; 0.5,O122&lt;0.5, T122&lt;0.5), "C1",IF(AND(E122&lt;0.5, J122 &lt; 0.5,O122&lt;0.5, T122&gt;=0.5), "B","A"))))))))</f>
+        <v>C1</v>
+      </c>
+    </row>
+    <row r="123" spans="1:28" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A123" s="3">
         <v>31</v>
       </c>
@@ -6752,8 +8327,20 @@
         <f t="shared" si="15"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="124" spans="1:22" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="Z123" s="25" t="str">
+        <f>IF(AND(C123&lt;0.5, H123 &gt;= 0.5,M123&gt;=0.5, R123&lt;0.5), "F",IF(AND(C123&lt;0.5, H123 &gt;= 0.5,M123&gt;=0.5, R123&gt;=0.5), "E2",IF(AND(C123&lt;0.5, H123 &gt;= 0.5,M123&lt;0.5, R123&lt;0.5), "E1",IF(AND(C123&lt;0.5, H123 &gt;= 0.5,M123&lt;0.5, R123&gt;=0.5), "D2",IF(AND(C123&lt;0.5, H123 &lt;0.5,M123&gt;=0.5, R123&lt;0.5), "D1",IF(AND(C123&lt;0.5, H123 &lt; 0.5,M123&gt;=0.5, R123&gt;=0.5), "C2",IF(AND(C123&lt;0.5, H123 &lt; 0.5,M123&lt;0.5, R123&lt;0.5), "C1",IF(AND(C123&lt;0.5, H123 &lt; 0.5,M123&lt;0.5, R123&gt;=0.5), "B","A"))))))))</f>
+        <v>C1</v>
+      </c>
+      <c r="AA123" s="25" t="str">
+        <f>IF(AND(D123&lt;0.5, I123 &gt;= 0.5,N123&gt;=0.5, S123&lt;0.5), "F",IF(AND(D123&lt;0.5, I123 &gt;= 0.5,N123&gt;=0.5, S123&gt;=0.5), "E2",IF(AND(D123&lt;0.5, I123 &gt;= 0.5,N123&lt;0.5, S123&lt;0.5), "E1",IF(AND(D123&lt;0.5, I123 &gt;= 0.5,N123&lt;0.5, S123&gt;=0.5), "D2",IF(AND(D123&lt;0.5, I123 &lt;0.5,N123&gt;=0.5, S123&lt;0.5), "D1",IF(AND(D123&lt;0.5, I123 &lt; 0.5,N123&gt;=0.5, S123&gt;=0.5), "C2",IF(AND(D123&lt;0.5, I123 &lt; 0.5,N123&lt;0.5, S123&lt;0.5), "C1",IF(AND(D123&lt;0.5, I123 &lt; 0.5,N123&lt;0.5, S123&gt;=0.5), "B","A"))))))))</f>
+        <v>C1</v>
+      </c>
+      <c r="AB123" s="25" t="str">
+        <f>IF(AND(E123&lt;0.5, J123 &gt;= 0.5,O123&gt;=0.5, T123&lt;0.5), "F",IF(AND(E123&lt;0.5, J123 &gt;= 0.5,O123&gt;=0.5, T123&gt;=0.5), "E2",IF(AND(E123&lt;0.5, J123 &gt;= 0.5,O123&lt;0.5, T123&lt;0.5), "E1",IF(AND(E123&lt;0.5, J123 &gt;= 0.5,O123&lt;0.5, T123&gt;=0.5), "D2",IF(AND(E123&lt;0.5, J123 &lt;0.5,O123&gt;=0.5, T123&lt;0.5), "D1",IF(AND(E123&lt;0.5, J123 &lt; 0.5,O123&gt;=0.5, T123&gt;=0.5), "C2",IF(AND(E123&lt;0.5, J123 &lt; 0.5,O123&lt;0.5, T123&lt;0.5), "C1",IF(AND(E123&lt;0.5, J123 &lt; 0.5,O123&lt;0.5, T123&gt;=0.5), "B","A"))))))))</f>
+        <v>C1</v>
+      </c>
+    </row>
+    <row r="124" spans="1:28" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A124" s="1"/>
       <c r="B124" s="1" t="s">
         <v>16</v>
@@ -6799,8 +8386,20 @@
         <f t="shared" si="15"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="125" spans="1:22" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="Z124" s="25" t="str">
+        <f>IF(AND(C124&lt;0.5, H124 &gt;= 0.5,M124&gt;=0.5, R124&lt;0.5), "F",IF(AND(C124&lt;0.5, H124 &gt;= 0.5,M124&gt;=0.5, R124&gt;=0.5), "E2",IF(AND(C124&lt;0.5, H124 &gt;= 0.5,M124&lt;0.5, R124&lt;0.5), "E1",IF(AND(C124&lt;0.5, H124 &gt;= 0.5,M124&lt;0.5, R124&gt;=0.5), "D2",IF(AND(C124&lt;0.5, H124 &lt;0.5,M124&gt;=0.5, R124&lt;0.5), "D1",IF(AND(C124&lt;0.5, H124 &lt; 0.5,M124&gt;=0.5, R124&gt;=0.5), "C2",IF(AND(C124&lt;0.5, H124 &lt; 0.5,M124&lt;0.5, R124&lt;0.5), "C1",IF(AND(C124&lt;0.5, H124 &lt; 0.5,M124&lt;0.5, R124&gt;=0.5), "B","A"))))))))</f>
+        <v>C1</v>
+      </c>
+      <c r="AA124" s="25" t="str">
+        <f>IF(AND(D124&lt;0.5, I124 &gt;= 0.5,N124&gt;=0.5, S124&lt;0.5), "F",IF(AND(D124&lt;0.5, I124 &gt;= 0.5,N124&gt;=0.5, S124&gt;=0.5), "E2",IF(AND(D124&lt;0.5, I124 &gt;= 0.5,N124&lt;0.5, S124&lt;0.5), "E1",IF(AND(D124&lt;0.5, I124 &gt;= 0.5,N124&lt;0.5, S124&gt;=0.5), "D2",IF(AND(D124&lt;0.5, I124 &lt;0.5,N124&gt;=0.5, S124&lt;0.5), "D1",IF(AND(D124&lt;0.5, I124 &lt; 0.5,N124&gt;=0.5, S124&gt;=0.5), "C2",IF(AND(D124&lt;0.5, I124 &lt; 0.5,N124&lt;0.5, S124&lt;0.5), "C1",IF(AND(D124&lt;0.5, I124 &lt; 0.5,N124&lt;0.5, S124&gt;=0.5), "B","A"))))))))</f>
+        <v>C1</v>
+      </c>
+      <c r="AB124" s="25" t="str">
+        <f>IF(AND(E124&lt;0.5, J124 &gt;= 0.5,O124&gt;=0.5, T124&lt;0.5), "F",IF(AND(E124&lt;0.5, J124 &gt;= 0.5,O124&gt;=0.5, T124&gt;=0.5), "E2",IF(AND(E124&lt;0.5, J124 &gt;= 0.5,O124&lt;0.5, T124&lt;0.5), "E1",IF(AND(E124&lt;0.5, J124 &gt;= 0.5,O124&lt;0.5, T124&gt;=0.5), "D2",IF(AND(E124&lt;0.5, J124 &lt;0.5,O124&gt;=0.5, T124&lt;0.5), "D1",IF(AND(E124&lt;0.5, J124 &lt; 0.5,O124&gt;=0.5, T124&gt;=0.5), "C2",IF(AND(E124&lt;0.5, J124 &lt; 0.5,O124&lt;0.5, T124&lt;0.5), "C1",IF(AND(E124&lt;0.5, J124 &lt; 0.5,O124&lt;0.5, T124&gt;=0.5), "B","A"))))))))</f>
+        <v>C1</v>
+      </c>
+    </row>
+    <row r="125" spans="1:28" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A125" s="1"/>
       <c r="B125" s="1" t="s">
         <v>17</v>
@@ -6846,8 +8445,20 @@
         <f t="shared" si="15"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="126" spans="1:22" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="Z125" s="25" t="str">
+        <f>IF(AND(C125&lt;0.5, H125 &gt;= 0.5,M125&gt;=0.5, R125&lt;0.5), "F",IF(AND(C125&lt;0.5, H125 &gt;= 0.5,M125&gt;=0.5, R125&gt;=0.5), "E2",IF(AND(C125&lt;0.5, H125 &gt;= 0.5,M125&lt;0.5, R125&lt;0.5), "E1",IF(AND(C125&lt;0.5, H125 &gt;= 0.5,M125&lt;0.5, R125&gt;=0.5), "D2",IF(AND(C125&lt;0.5, H125 &lt;0.5,M125&gt;=0.5, R125&lt;0.5), "D1",IF(AND(C125&lt;0.5, H125 &lt; 0.5,M125&gt;=0.5, R125&gt;=0.5), "C2",IF(AND(C125&lt;0.5, H125 &lt; 0.5,M125&lt;0.5, R125&lt;0.5), "C1",IF(AND(C125&lt;0.5, H125 &lt; 0.5,M125&lt;0.5, R125&gt;=0.5), "B","A"))))))))</f>
+        <v>C1</v>
+      </c>
+      <c r="AA125" s="25" t="str">
+        <f>IF(AND(D125&lt;0.5, I125 &gt;= 0.5,N125&gt;=0.5, S125&lt;0.5), "F",IF(AND(D125&lt;0.5, I125 &gt;= 0.5,N125&gt;=0.5, S125&gt;=0.5), "E2",IF(AND(D125&lt;0.5, I125 &gt;= 0.5,N125&lt;0.5, S125&lt;0.5), "E1",IF(AND(D125&lt;0.5, I125 &gt;= 0.5,N125&lt;0.5, S125&gt;=0.5), "D2",IF(AND(D125&lt;0.5, I125 &lt;0.5,N125&gt;=0.5, S125&lt;0.5), "D1",IF(AND(D125&lt;0.5, I125 &lt; 0.5,N125&gt;=0.5, S125&gt;=0.5), "C2",IF(AND(D125&lt;0.5, I125 &lt; 0.5,N125&lt;0.5, S125&lt;0.5), "C1",IF(AND(D125&lt;0.5, I125 &lt; 0.5,N125&lt;0.5, S125&gt;=0.5), "B","A"))))))))</f>
+        <v>C1</v>
+      </c>
+      <c r="AB125" s="25" t="str">
+        <f>IF(AND(E125&lt;0.5, J125 &gt;= 0.5,O125&gt;=0.5, T125&lt;0.5), "F",IF(AND(E125&lt;0.5, J125 &gt;= 0.5,O125&gt;=0.5, T125&gt;=0.5), "E2",IF(AND(E125&lt;0.5, J125 &gt;= 0.5,O125&lt;0.5, T125&lt;0.5), "E1",IF(AND(E125&lt;0.5, J125 &gt;= 0.5,O125&lt;0.5, T125&gt;=0.5), "D2",IF(AND(E125&lt;0.5, J125 &lt;0.5,O125&gt;=0.5, T125&lt;0.5), "D1",IF(AND(E125&lt;0.5, J125 &lt; 0.5,O125&gt;=0.5, T125&gt;=0.5), "C2",IF(AND(E125&lt;0.5, J125 &lt; 0.5,O125&lt;0.5, T125&lt;0.5), "C1",IF(AND(E125&lt;0.5, J125 &lt; 0.5,O125&lt;0.5, T125&gt;=0.5), "B","A"))))))))</f>
+        <v>C1</v>
+      </c>
+    </row>
+    <row r="126" spans="1:28" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A126" s="4"/>
       <c r="B126" s="4" t="s">
         <v>18</v>
@@ -6896,8 +8507,20 @@
         <f t="shared" si="15"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="127" spans="1:22" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="Z126" s="25" t="str">
+        <f>IF(AND(C126&lt;0.5, H126 &gt;= 0.5,M126&gt;=0.5, R126&lt;0.5), "F",IF(AND(C126&lt;0.5, H126 &gt;= 0.5,M126&gt;=0.5, R126&gt;=0.5), "E2",IF(AND(C126&lt;0.5, H126 &gt;= 0.5,M126&lt;0.5, R126&lt;0.5), "E1",IF(AND(C126&lt;0.5, H126 &gt;= 0.5,M126&lt;0.5, R126&gt;=0.5), "D2",IF(AND(C126&lt;0.5, H126 &lt;0.5,M126&gt;=0.5, R126&lt;0.5), "D1",IF(AND(C126&lt;0.5, H126 &lt; 0.5,M126&gt;=0.5, R126&gt;=0.5), "C2",IF(AND(C126&lt;0.5, H126 &lt; 0.5,M126&lt;0.5, R126&lt;0.5), "C1",IF(AND(C126&lt;0.5, H126 &lt; 0.5,M126&lt;0.5, R126&gt;=0.5), "B","A"))))))))</f>
+        <v>C1</v>
+      </c>
+      <c r="AA126" s="25" t="str">
+        <f>IF(AND(D126&lt;0.5, I126 &gt;= 0.5,N126&gt;=0.5, S126&lt;0.5), "F",IF(AND(D126&lt;0.5, I126 &gt;= 0.5,N126&gt;=0.5, S126&gt;=0.5), "E2",IF(AND(D126&lt;0.5, I126 &gt;= 0.5,N126&lt;0.5, S126&lt;0.5), "E1",IF(AND(D126&lt;0.5, I126 &gt;= 0.5,N126&lt;0.5, S126&gt;=0.5), "D2",IF(AND(D126&lt;0.5, I126 &lt;0.5,N126&gt;=0.5, S126&lt;0.5), "D1",IF(AND(D126&lt;0.5, I126 &lt; 0.5,N126&gt;=0.5, S126&gt;=0.5), "C2",IF(AND(D126&lt;0.5, I126 &lt; 0.5,N126&lt;0.5, S126&lt;0.5), "C1",IF(AND(D126&lt;0.5, I126 &lt; 0.5,N126&lt;0.5, S126&gt;=0.5), "B","A"))))))))</f>
+        <v>C1</v>
+      </c>
+      <c r="AB126" s="25" t="str">
+        <f>IF(AND(E126&lt;0.5, J126 &gt;= 0.5,O126&gt;=0.5, T126&lt;0.5), "F",IF(AND(E126&lt;0.5, J126 &gt;= 0.5,O126&gt;=0.5, T126&gt;=0.5), "E2",IF(AND(E126&lt;0.5, J126 &gt;= 0.5,O126&lt;0.5, T126&lt;0.5), "E1",IF(AND(E126&lt;0.5, J126 &gt;= 0.5,O126&lt;0.5, T126&gt;=0.5), "D2",IF(AND(E126&lt;0.5, J126 &lt;0.5,O126&gt;=0.5, T126&lt;0.5), "D1",IF(AND(E126&lt;0.5, J126 &lt; 0.5,O126&gt;=0.5, T126&gt;=0.5), "C2",IF(AND(E126&lt;0.5, J126 &lt; 0.5,O126&lt;0.5, T126&lt;0.5), "C1",IF(AND(E126&lt;0.5, J126 &lt; 0.5,O126&lt;0.5, T126&gt;=0.5), "B","A"))))))))</f>
+        <v>C1</v>
+      </c>
+    </row>
+    <row r="127" spans="1:28" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A127" s="3">
         <v>32</v>
       </c>
@@ -6948,8 +8571,20 @@
         <f t="shared" si="15"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="128" spans="1:22" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="Z127" s="25" t="str">
+        <f>IF(AND(C127&lt;0.5, H127 &gt;= 0.5,M127&gt;=0.5, R127&lt;0.5), "F",IF(AND(C127&lt;0.5, H127 &gt;= 0.5,M127&gt;=0.5, R127&gt;=0.5), "E2",IF(AND(C127&lt;0.5, H127 &gt;= 0.5,M127&lt;0.5, R127&lt;0.5), "E1",IF(AND(C127&lt;0.5, H127 &gt;= 0.5,M127&lt;0.5, R127&gt;=0.5), "D2",IF(AND(C127&lt;0.5, H127 &lt;0.5,M127&gt;=0.5, R127&lt;0.5), "D1",IF(AND(C127&lt;0.5, H127 &lt; 0.5,M127&gt;=0.5, R127&gt;=0.5), "C2",IF(AND(C127&lt;0.5, H127 &lt; 0.5,M127&lt;0.5, R127&lt;0.5), "C1",IF(AND(C127&lt;0.5, H127 &lt; 0.5,M127&lt;0.5, R127&gt;=0.5), "B","A"))))))))</f>
+        <v>C1</v>
+      </c>
+      <c r="AA127" s="25" t="str">
+        <f>IF(AND(D127&lt;0.5, I127 &gt;= 0.5,N127&gt;=0.5, S127&lt;0.5), "F",IF(AND(D127&lt;0.5, I127 &gt;= 0.5,N127&gt;=0.5, S127&gt;=0.5), "E2",IF(AND(D127&lt;0.5, I127 &gt;= 0.5,N127&lt;0.5, S127&lt;0.5), "E1",IF(AND(D127&lt;0.5, I127 &gt;= 0.5,N127&lt;0.5, S127&gt;=0.5), "D2",IF(AND(D127&lt;0.5, I127 &lt;0.5,N127&gt;=0.5, S127&lt;0.5), "D1",IF(AND(D127&lt;0.5, I127 &lt; 0.5,N127&gt;=0.5, S127&gt;=0.5), "C2",IF(AND(D127&lt;0.5, I127 &lt; 0.5,N127&lt;0.5, S127&lt;0.5), "C1",IF(AND(D127&lt;0.5, I127 &lt; 0.5,N127&lt;0.5, S127&gt;=0.5), "B","A"))))))))</f>
+        <v>C1</v>
+      </c>
+      <c r="AB127" s="25" t="str">
+        <f>IF(AND(E127&lt;0.5, J127 &gt;= 0.5,O127&gt;=0.5, T127&lt;0.5), "F",IF(AND(E127&lt;0.5, J127 &gt;= 0.5,O127&gt;=0.5, T127&gt;=0.5), "E2",IF(AND(E127&lt;0.5, J127 &gt;= 0.5,O127&lt;0.5, T127&lt;0.5), "E1",IF(AND(E127&lt;0.5, J127 &gt;= 0.5,O127&lt;0.5, T127&gt;=0.5), "D2",IF(AND(E127&lt;0.5, J127 &lt;0.5,O127&gt;=0.5, T127&lt;0.5), "D1",IF(AND(E127&lt;0.5, J127 &lt; 0.5,O127&gt;=0.5, T127&gt;=0.5), "C2",IF(AND(E127&lt;0.5, J127 &lt; 0.5,O127&lt;0.5, T127&lt;0.5), "C1",IF(AND(E127&lt;0.5, J127 &lt; 0.5,O127&lt;0.5, T127&gt;=0.5), "B","A"))))))))</f>
+        <v>C1</v>
+      </c>
+    </row>
+    <row r="128" spans="1:28" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A128" s="1"/>
       <c r="B128" s="1" t="s">
         <v>16</v>
@@ -6995,8 +8630,20 @@
         <f t="shared" si="15"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="129" spans="1:22" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="Z128" s="25" t="str">
+        <f>IF(AND(C128&lt;0.5, H128 &gt;= 0.5,M128&gt;=0.5, R128&lt;0.5), "F",IF(AND(C128&lt;0.5, H128 &gt;= 0.5,M128&gt;=0.5, R128&gt;=0.5), "E2",IF(AND(C128&lt;0.5, H128 &gt;= 0.5,M128&lt;0.5, R128&lt;0.5), "E1",IF(AND(C128&lt;0.5, H128 &gt;= 0.5,M128&lt;0.5, R128&gt;=0.5), "D2",IF(AND(C128&lt;0.5, H128 &lt;0.5,M128&gt;=0.5, R128&lt;0.5), "D1",IF(AND(C128&lt;0.5, H128 &lt; 0.5,M128&gt;=0.5, R128&gt;=0.5), "C2",IF(AND(C128&lt;0.5, H128 &lt; 0.5,M128&lt;0.5, R128&lt;0.5), "C1",IF(AND(C128&lt;0.5, H128 &lt; 0.5,M128&lt;0.5, R128&gt;=0.5), "B","A"))))))))</f>
+        <v>C1</v>
+      </c>
+      <c r="AA128" s="25" t="str">
+        <f>IF(AND(D128&lt;0.5, I128 &gt;= 0.5,N128&gt;=0.5, S128&lt;0.5), "F",IF(AND(D128&lt;0.5, I128 &gt;= 0.5,N128&gt;=0.5, S128&gt;=0.5), "E2",IF(AND(D128&lt;0.5, I128 &gt;= 0.5,N128&lt;0.5, S128&lt;0.5), "E1",IF(AND(D128&lt;0.5, I128 &gt;= 0.5,N128&lt;0.5, S128&gt;=0.5), "D2",IF(AND(D128&lt;0.5, I128 &lt;0.5,N128&gt;=0.5, S128&lt;0.5), "D1",IF(AND(D128&lt;0.5, I128 &lt; 0.5,N128&gt;=0.5, S128&gt;=0.5), "C2",IF(AND(D128&lt;0.5, I128 &lt; 0.5,N128&lt;0.5, S128&lt;0.5), "C1",IF(AND(D128&lt;0.5, I128 &lt; 0.5,N128&lt;0.5, S128&gt;=0.5), "B","A"))))))))</f>
+        <v>C1</v>
+      </c>
+      <c r="AB128" s="25" t="str">
+        <f>IF(AND(E128&lt;0.5, J128 &gt;= 0.5,O128&gt;=0.5, T128&lt;0.5), "F",IF(AND(E128&lt;0.5, J128 &gt;= 0.5,O128&gt;=0.5, T128&gt;=0.5), "E2",IF(AND(E128&lt;0.5, J128 &gt;= 0.5,O128&lt;0.5, T128&lt;0.5), "E1",IF(AND(E128&lt;0.5, J128 &gt;= 0.5,O128&lt;0.5, T128&gt;=0.5), "D2",IF(AND(E128&lt;0.5, J128 &lt;0.5,O128&gt;=0.5, T128&lt;0.5), "D1",IF(AND(E128&lt;0.5, J128 &lt; 0.5,O128&gt;=0.5, T128&gt;=0.5), "C2",IF(AND(E128&lt;0.5, J128 &lt; 0.5,O128&lt;0.5, T128&lt;0.5), "C1",IF(AND(E128&lt;0.5, J128 &lt; 0.5,O128&lt;0.5, T128&gt;=0.5), "B","A"))))))))</f>
+        <v>C1</v>
+      </c>
+    </row>
+    <row r="129" spans="1:28" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A129" s="1"/>
       <c r="B129" s="1" t="s">
         <v>17</v>
@@ -7042,8 +8689,20 @@
         <f t="shared" si="15"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="130" spans="1:22" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="Z129" s="25" t="str">
+        <f>IF(AND(C129&lt;0.5, H129 &gt;= 0.5,M129&gt;=0.5, R129&lt;0.5), "F",IF(AND(C129&lt;0.5, H129 &gt;= 0.5,M129&gt;=0.5, R129&gt;=0.5), "E2",IF(AND(C129&lt;0.5, H129 &gt;= 0.5,M129&lt;0.5, R129&lt;0.5), "E1",IF(AND(C129&lt;0.5, H129 &gt;= 0.5,M129&lt;0.5, R129&gt;=0.5), "D2",IF(AND(C129&lt;0.5, H129 &lt;0.5,M129&gt;=0.5, R129&lt;0.5), "D1",IF(AND(C129&lt;0.5, H129 &lt; 0.5,M129&gt;=0.5, R129&gt;=0.5), "C2",IF(AND(C129&lt;0.5, H129 &lt; 0.5,M129&lt;0.5, R129&lt;0.5), "C1",IF(AND(C129&lt;0.5, H129 &lt; 0.5,M129&lt;0.5, R129&gt;=0.5), "B","A"))))))))</f>
+        <v>C1</v>
+      </c>
+      <c r="AA129" s="25" t="str">
+        <f>IF(AND(D129&lt;0.5, I129 &gt;= 0.5,N129&gt;=0.5, S129&lt;0.5), "F",IF(AND(D129&lt;0.5, I129 &gt;= 0.5,N129&gt;=0.5, S129&gt;=0.5), "E2",IF(AND(D129&lt;0.5, I129 &gt;= 0.5,N129&lt;0.5, S129&lt;0.5), "E1",IF(AND(D129&lt;0.5, I129 &gt;= 0.5,N129&lt;0.5, S129&gt;=0.5), "D2",IF(AND(D129&lt;0.5, I129 &lt;0.5,N129&gt;=0.5, S129&lt;0.5), "D1",IF(AND(D129&lt;0.5, I129 &lt; 0.5,N129&gt;=0.5, S129&gt;=0.5), "C2",IF(AND(D129&lt;0.5, I129 &lt; 0.5,N129&lt;0.5, S129&lt;0.5), "C1",IF(AND(D129&lt;0.5, I129 &lt; 0.5,N129&lt;0.5, S129&gt;=0.5), "B","A"))))))))</f>
+        <v>C1</v>
+      </c>
+      <c r="AB129" s="25" t="str">
+        <f>IF(AND(E129&lt;0.5, J129 &gt;= 0.5,O129&gt;=0.5, T129&lt;0.5), "F",IF(AND(E129&lt;0.5, J129 &gt;= 0.5,O129&gt;=0.5, T129&gt;=0.5), "E2",IF(AND(E129&lt;0.5, J129 &gt;= 0.5,O129&lt;0.5, T129&lt;0.5), "E1",IF(AND(E129&lt;0.5, J129 &gt;= 0.5,O129&lt;0.5, T129&gt;=0.5), "D2",IF(AND(E129&lt;0.5, J129 &lt;0.5,O129&gt;=0.5, T129&lt;0.5), "D1",IF(AND(E129&lt;0.5, J129 &lt; 0.5,O129&gt;=0.5, T129&gt;=0.5), "C2",IF(AND(E129&lt;0.5, J129 &lt; 0.5,O129&lt;0.5, T129&lt;0.5), "C1",IF(AND(E129&lt;0.5, J129 &lt; 0.5,O129&lt;0.5, T129&gt;=0.5), "B","A"))))))))</f>
+        <v>C1</v>
+      </c>
+    </row>
+    <row r="130" spans="1:28" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A130" s="4"/>
       <c r="B130" s="4" t="s">
         <v>18</v>
@@ -7092,8 +8751,20 @@
         <f t="shared" si="15"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="131" spans="1:22" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="Z130" s="25" t="str">
+        <f>IF(AND(C130&lt;0.5, H130 &gt;= 0.5,M130&gt;=0.5, R130&lt;0.5), "F",IF(AND(C130&lt;0.5, H130 &gt;= 0.5,M130&gt;=0.5, R130&gt;=0.5), "E2",IF(AND(C130&lt;0.5, H130 &gt;= 0.5,M130&lt;0.5, R130&lt;0.5), "E1",IF(AND(C130&lt;0.5, H130 &gt;= 0.5,M130&lt;0.5, R130&gt;=0.5), "D2",IF(AND(C130&lt;0.5, H130 &lt;0.5,M130&gt;=0.5, R130&lt;0.5), "D1",IF(AND(C130&lt;0.5, H130 &lt; 0.5,M130&gt;=0.5, R130&gt;=0.5), "C2",IF(AND(C130&lt;0.5, H130 &lt; 0.5,M130&lt;0.5, R130&lt;0.5), "C1",IF(AND(C130&lt;0.5, H130 &lt; 0.5,M130&lt;0.5, R130&gt;=0.5), "B","A"))))))))</f>
+        <v>C1</v>
+      </c>
+      <c r="AA130" s="25" t="str">
+        <f>IF(AND(D130&lt;0.5, I130 &gt;= 0.5,N130&gt;=0.5, S130&lt;0.5), "F",IF(AND(D130&lt;0.5, I130 &gt;= 0.5,N130&gt;=0.5, S130&gt;=0.5), "E2",IF(AND(D130&lt;0.5, I130 &gt;= 0.5,N130&lt;0.5, S130&lt;0.5), "E1",IF(AND(D130&lt;0.5, I130 &gt;= 0.5,N130&lt;0.5, S130&gt;=0.5), "D2",IF(AND(D130&lt;0.5, I130 &lt;0.5,N130&gt;=0.5, S130&lt;0.5), "D1",IF(AND(D130&lt;0.5, I130 &lt; 0.5,N130&gt;=0.5, S130&gt;=0.5), "C2",IF(AND(D130&lt;0.5, I130 &lt; 0.5,N130&lt;0.5, S130&lt;0.5), "C1",IF(AND(D130&lt;0.5, I130 &lt; 0.5,N130&lt;0.5, S130&gt;=0.5), "B","A"))))))))</f>
+        <v>C1</v>
+      </c>
+      <c r="AB130" s="25" t="str">
+        <f>IF(AND(E130&lt;0.5, J130 &gt;= 0.5,O130&gt;=0.5, T130&lt;0.5), "F",IF(AND(E130&lt;0.5, J130 &gt;= 0.5,O130&gt;=0.5, T130&gt;=0.5), "E2",IF(AND(E130&lt;0.5, J130 &gt;= 0.5,O130&lt;0.5, T130&lt;0.5), "E1",IF(AND(E130&lt;0.5, J130 &gt;= 0.5,O130&lt;0.5, T130&gt;=0.5), "D2",IF(AND(E130&lt;0.5, J130 &lt;0.5,O130&gt;=0.5, T130&lt;0.5), "D1",IF(AND(E130&lt;0.5, J130 &lt; 0.5,O130&gt;=0.5, T130&gt;=0.5), "C2",IF(AND(E130&lt;0.5, J130 &lt; 0.5,O130&lt;0.5, T130&lt;0.5), "C1",IF(AND(E130&lt;0.5, J130 &lt; 0.5,O130&lt;0.5, T130&gt;=0.5), "B","A"))))))))</f>
+        <v>C1</v>
+      </c>
+    </row>
+    <row r="131" spans="1:28" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A131" s="3">
         <v>33</v>
       </c>
@@ -7144,8 +8815,20 @@
         <f t="shared" si="15"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="132" spans="1:22" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="Z131" s="25" t="str">
+        <f>IF(AND(C131&lt;0.5, H131 &gt;= 0.5,M131&gt;=0.5, R131&lt;0.5), "F",IF(AND(C131&lt;0.5, H131 &gt;= 0.5,M131&gt;=0.5, R131&gt;=0.5), "E2",IF(AND(C131&lt;0.5, H131 &gt;= 0.5,M131&lt;0.5, R131&lt;0.5), "E1",IF(AND(C131&lt;0.5, H131 &gt;= 0.5,M131&lt;0.5, R131&gt;=0.5), "D2",IF(AND(C131&lt;0.5, H131 &lt;0.5,M131&gt;=0.5, R131&lt;0.5), "D1",IF(AND(C131&lt;0.5, H131 &lt; 0.5,M131&gt;=0.5, R131&gt;=0.5), "C2",IF(AND(C131&lt;0.5, H131 &lt; 0.5,M131&lt;0.5, R131&lt;0.5), "C1",IF(AND(C131&lt;0.5, H131 &lt; 0.5,M131&lt;0.5, R131&gt;=0.5), "B","A"))))))))</f>
+        <v>C1</v>
+      </c>
+      <c r="AA131" s="25" t="str">
+        <f>IF(AND(D131&lt;0.5, I131 &gt;= 0.5,N131&gt;=0.5, S131&lt;0.5), "F",IF(AND(D131&lt;0.5, I131 &gt;= 0.5,N131&gt;=0.5, S131&gt;=0.5), "E2",IF(AND(D131&lt;0.5, I131 &gt;= 0.5,N131&lt;0.5, S131&lt;0.5), "E1",IF(AND(D131&lt;0.5, I131 &gt;= 0.5,N131&lt;0.5, S131&gt;=0.5), "D2",IF(AND(D131&lt;0.5, I131 &lt;0.5,N131&gt;=0.5, S131&lt;0.5), "D1",IF(AND(D131&lt;0.5, I131 &lt; 0.5,N131&gt;=0.5, S131&gt;=0.5), "C2",IF(AND(D131&lt;0.5, I131 &lt; 0.5,N131&lt;0.5, S131&lt;0.5), "C1",IF(AND(D131&lt;0.5, I131 &lt; 0.5,N131&lt;0.5, S131&gt;=0.5), "B","A"))))))))</f>
+        <v>C1</v>
+      </c>
+      <c r="AB131" s="25" t="str">
+        <f>IF(AND(E131&lt;0.5, J131 &gt;= 0.5,O131&gt;=0.5, T131&lt;0.5), "F",IF(AND(E131&lt;0.5, J131 &gt;= 0.5,O131&gt;=0.5, T131&gt;=0.5), "E2",IF(AND(E131&lt;0.5, J131 &gt;= 0.5,O131&lt;0.5, T131&lt;0.5), "E1",IF(AND(E131&lt;0.5, J131 &gt;= 0.5,O131&lt;0.5, T131&gt;=0.5), "D2",IF(AND(E131&lt;0.5, J131 &lt;0.5,O131&gt;=0.5, T131&lt;0.5), "D1",IF(AND(E131&lt;0.5, J131 &lt; 0.5,O131&gt;=0.5, T131&gt;=0.5), "C2",IF(AND(E131&lt;0.5, J131 &lt; 0.5,O131&lt;0.5, T131&lt;0.5), "C1",IF(AND(E131&lt;0.5, J131 &lt; 0.5,O131&lt;0.5, T131&gt;=0.5), "B","A"))))))))</f>
+        <v>C1</v>
+      </c>
+    </row>
+    <row r="132" spans="1:28" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A132" s="1"/>
       <c r="B132" s="1" t="s">
         <v>16</v>
@@ -7191,8 +8874,20 @@
         <f t="shared" ref="V132:V167" si="23">IF(R132&gt;0, (T132-R132)/R132, 0)</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="133" spans="1:22" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="Z132" s="25" t="str">
+        <f>IF(AND(C132&lt;0.5, H132 &gt;= 0.5,M132&gt;=0.5, R132&lt;0.5), "F",IF(AND(C132&lt;0.5, H132 &gt;= 0.5,M132&gt;=0.5, R132&gt;=0.5), "E2",IF(AND(C132&lt;0.5, H132 &gt;= 0.5,M132&lt;0.5, R132&lt;0.5), "E1",IF(AND(C132&lt;0.5, H132 &gt;= 0.5,M132&lt;0.5, R132&gt;=0.5), "D2",IF(AND(C132&lt;0.5, H132 &lt;0.5,M132&gt;=0.5, R132&lt;0.5), "D1",IF(AND(C132&lt;0.5, H132 &lt; 0.5,M132&gt;=0.5, R132&gt;=0.5), "C2",IF(AND(C132&lt;0.5, H132 &lt; 0.5,M132&lt;0.5, R132&lt;0.5), "C1",IF(AND(C132&lt;0.5, H132 &lt; 0.5,M132&lt;0.5, R132&gt;=0.5), "B","A"))))))))</f>
+        <v>C1</v>
+      </c>
+      <c r="AA132" s="25" t="str">
+        <f>IF(AND(D132&lt;0.5, I132 &gt;= 0.5,N132&gt;=0.5, S132&lt;0.5), "F",IF(AND(D132&lt;0.5, I132 &gt;= 0.5,N132&gt;=0.5, S132&gt;=0.5), "E2",IF(AND(D132&lt;0.5, I132 &gt;= 0.5,N132&lt;0.5, S132&lt;0.5), "E1",IF(AND(D132&lt;0.5, I132 &gt;= 0.5,N132&lt;0.5, S132&gt;=0.5), "D2",IF(AND(D132&lt;0.5, I132 &lt;0.5,N132&gt;=0.5, S132&lt;0.5), "D1",IF(AND(D132&lt;0.5, I132 &lt; 0.5,N132&gt;=0.5, S132&gt;=0.5), "C2",IF(AND(D132&lt;0.5, I132 &lt; 0.5,N132&lt;0.5, S132&lt;0.5), "C1",IF(AND(D132&lt;0.5, I132 &lt; 0.5,N132&lt;0.5, S132&gt;=0.5), "B","A"))))))))</f>
+        <v>C1</v>
+      </c>
+      <c r="AB132" s="25" t="str">
+        <f>IF(AND(E132&lt;0.5, J132 &gt;= 0.5,O132&gt;=0.5, T132&lt;0.5), "F",IF(AND(E132&lt;0.5, J132 &gt;= 0.5,O132&gt;=0.5, T132&gt;=0.5), "E2",IF(AND(E132&lt;0.5, J132 &gt;= 0.5,O132&lt;0.5, T132&lt;0.5), "E1",IF(AND(E132&lt;0.5, J132 &gt;= 0.5,O132&lt;0.5, T132&gt;=0.5), "D2",IF(AND(E132&lt;0.5, J132 &lt;0.5,O132&gt;=0.5, T132&lt;0.5), "D1",IF(AND(E132&lt;0.5, J132 &lt; 0.5,O132&gt;=0.5, T132&gt;=0.5), "C2",IF(AND(E132&lt;0.5, J132 &lt; 0.5,O132&lt;0.5, T132&lt;0.5), "C1",IF(AND(E132&lt;0.5, J132 &lt; 0.5,O132&lt;0.5, T132&gt;=0.5), "B","A"))))))))</f>
+        <v>C1</v>
+      </c>
+    </row>
+    <row r="133" spans="1:28" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A133" s="1"/>
       <c r="B133" s="1" t="s">
         <v>17</v>
@@ -7238,8 +8933,20 @@
         <f t="shared" si="23"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="134" spans="1:22" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="Z133" s="25" t="str">
+        <f>IF(AND(C133&lt;0.5, H133 &gt;= 0.5,M133&gt;=0.5, R133&lt;0.5), "F",IF(AND(C133&lt;0.5, H133 &gt;= 0.5,M133&gt;=0.5, R133&gt;=0.5), "E2",IF(AND(C133&lt;0.5, H133 &gt;= 0.5,M133&lt;0.5, R133&lt;0.5), "E1",IF(AND(C133&lt;0.5, H133 &gt;= 0.5,M133&lt;0.5, R133&gt;=0.5), "D2",IF(AND(C133&lt;0.5, H133 &lt;0.5,M133&gt;=0.5, R133&lt;0.5), "D1",IF(AND(C133&lt;0.5, H133 &lt; 0.5,M133&gt;=0.5, R133&gt;=0.5), "C2",IF(AND(C133&lt;0.5, H133 &lt; 0.5,M133&lt;0.5, R133&lt;0.5), "C1",IF(AND(C133&lt;0.5, H133 &lt; 0.5,M133&lt;0.5, R133&gt;=0.5), "B","A"))))))))</f>
+        <v>C1</v>
+      </c>
+      <c r="AA133" s="25" t="str">
+        <f>IF(AND(D133&lt;0.5, I133 &gt;= 0.5,N133&gt;=0.5, S133&lt;0.5), "F",IF(AND(D133&lt;0.5, I133 &gt;= 0.5,N133&gt;=0.5, S133&gt;=0.5), "E2",IF(AND(D133&lt;0.5, I133 &gt;= 0.5,N133&lt;0.5, S133&lt;0.5), "E1",IF(AND(D133&lt;0.5, I133 &gt;= 0.5,N133&lt;0.5, S133&gt;=0.5), "D2",IF(AND(D133&lt;0.5, I133 &lt;0.5,N133&gt;=0.5, S133&lt;0.5), "D1",IF(AND(D133&lt;0.5, I133 &lt; 0.5,N133&gt;=0.5, S133&gt;=0.5), "C2",IF(AND(D133&lt;0.5, I133 &lt; 0.5,N133&lt;0.5, S133&lt;0.5), "C1",IF(AND(D133&lt;0.5, I133 &lt; 0.5,N133&lt;0.5, S133&gt;=0.5), "B","A"))))))))</f>
+        <v>C1</v>
+      </c>
+      <c r="AB133" s="25" t="str">
+        <f>IF(AND(E133&lt;0.5, J133 &gt;= 0.5,O133&gt;=0.5, T133&lt;0.5), "F",IF(AND(E133&lt;0.5, J133 &gt;= 0.5,O133&gt;=0.5, T133&gt;=0.5), "E2",IF(AND(E133&lt;0.5, J133 &gt;= 0.5,O133&lt;0.5, T133&lt;0.5), "E1",IF(AND(E133&lt;0.5, J133 &gt;= 0.5,O133&lt;0.5, T133&gt;=0.5), "D2",IF(AND(E133&lt;0.5, J133 &lt;0.5,O133&gt;=0.5, T133&lt;0.5), "D1",IF(AND(E133&lt;0.5, J133 &lt; 0.5,O133&gt;=0.5, T133&gt;=0.5), "C2",IF(AND(E133&lt;0.5, J133 &lt; 0.5,O133&lt;0.5, T133&lt;0.5), "C1",IF(AND(E133&lt;0.5, J133 &lt; 0.5,O133&lt;0.5, T133&gt;=0.5), "B","A"))))))))</f>
+        <v>C1</v>
+      </c>
+    </row>
+    <row r="134" spans="1:28" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A134" s="4"/>
       <c r="B134" s="4" t="s">
         <v>18</v>
@@ -7288,8 +8995,20 @@
         <f t="shared" si="23"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="135" spans="1:22" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="Z134" s="25" t="str">
+        <f>IF(AND(C134&lt;0.5, H134 &gt;= 0.5,M134&gt;=0.5, R134&lt;0.5), "F",IF(AND(C134&lt;0.5, H134 &gt;= 0.5,M134&gt;=0.5, R134&gt;=0.5), "E2",IF(AND(C134&lt;0.5, H134 &gt;= 0.5,M134&lt;0.5, R134&lt;0.5), "E1",IF(AND(C134&lt;0.5, H134 &gt;= 0.5,M134&lt;0.5, R134&gt;=0.5), "D2",IF(AND(C134&lt;0.5, H134 &lt;0.5,M134&gt;=0.5, R134&lt;0.5), "D1",IF(AND(C134&lt;0.5, H134 &lt; 0.5,M134&gt;=0.5, R134&gt;=0.5), "C2",IF(AND(C134&lt;0.5, H134 &lt; 0.5,M134&lt;0.5, R134&lt;0.5), "C1",IF(AND(C134&lt;0.5, H134 &lt; 0.5,M134&lt;0.5, R134&gt;=0.5), "B","A"))))))))</f>
+        <v>C1</v>
+      </c>
+      <c r="AA134" s="25" t="str">
+        <f>IF(AND(D134&lt;0.5, I134 &gt;= 0.5,N134&gt;=0.5, S134&lt;0.5), "F",IF(AND(D134&lt;0.5, I134 &gt;= 0.5,N134&gt;=0.5, S134&gt;=0.5), "E2",IF(AND(D134&lt;0.5, I134 &gt;= 0.5,N134&lt;0.5, S134&lt;0.5), "E1",IF(AND(D134&lt;0.5, I134 &gt;= 0.5,N134&lt;0.5, S134&gt;=0.5), "D2",IF(AND(D134&lt;0.5, I134 &lt;0.5,N134&gt;=0.5, S134&lt;0.5), "D1",IF(AND(D134&lt;0.5, I134 &lt; 0.5,N134&gt;=0.5, S134&gt;=0.5), "C2",IF(AND(D134&lt;0.5, I134 &lt; 0.5,N134&lt;0.5, S134&lt;0.5), "C1",IF(AND(D134&lt;0.5, I134 &lt; 0.5,N134&lt;0.5, S134&gt;=0.5), "B","A"))))))))</f>
+        <v>C1</v>
+      </c>
+      <c r="AB134" s="25" t="str">
+        <f>IF(AND(E134&lt;0.5, J134 &gt;= 0.5,O134&gt;=0.5, T134&lt;0.5), "F",IF(AND(E134&lt;0.5, J134 &gt;= 0.5,O134&gt;=0.5, T134&gt;=0.5), "E2",IF(AND(E134&lt;0.5, J134 &gt;= 0.5,O134&lt;0.5, T134&lt;0.5), "E1",IF(AND(E134&lt;0.5, J134 &gt;= 0.5,O134&lt;0.5, T134&gt;=0.5), "D2",IF(AND(E134&lt;0.5, J134 &lt;0.5,O134&gt;=0.5, T134&lt;0.5), "D1",IF(AND(E134&lt;0.5, J134 &lt; 0.5,O134&gt;=0.5, T134&gt;=0.5), "C2",IF(AND(E134&lt;0.5, J134 &lt; 0.5,O134&lt;0.5, T134&lt;0.5), "C1",IF(AND(E134&lt;0.5, J134 &lt; 0.5,O134&lt;0.5, T134&gt;=0.5), "B","A"))))))))</f>
+        <v>C1</v>
+      </c>
+    </row>
+    <row r="135" spans="1:28" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A135" s="3">
         <v>34</v>
       </c>
@@ -7340,8 +9059,20 @@
         <f t="shared" si="23"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="136" spans="1:22" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="Z135" s="25" t="str">
+        <f>IF(AND(C135&lt;0.5, H135 &gt;= 0.5,M135&gt;=0.5, R135&lt;0.5), "F",IF(AND(C135&lt;0.5, H135 &gt;= 0.5,M135&gt;=0.5, R135&gt;=0.5), "E2",IF(AND(C135&lt;0.5, H135 &gt;= 0.5,M135&lt;0.5, R135&lt;0.5), "E1",IF(AND(C135&lt;0.5, H135 &gt;= 0.5,M135&lt;0.5, R135&gt;=0.5), "D2",IF(AND(C135&lt;0.5, H135 &lt;0.5,M135&gt;=0.5, R135&lt;0.5), "D1",IF(AND(C135&lt;0.5, H135 &lt; 0.5,M135&gt;=0.5, R135&gt;=0.5), "C2",IF(AND(C135&lt;0.5, H135 &lt; 0.5,M135&lt;0.5, R135&lt;0.5), "C1",IF(AND(C135&lt;0.5, H135 &lt; 0.5,M135&lt;0.5, R135&gt;=0.5), "B","A"))))))))</f>
+        <v>C1</v>
+      </c>
+      <c r="AA135" s="25" t="str">
+        <f>IF(AND(D135&lt;0.5, I135 &gt;= 0.5,N135&gt;=0.5, S135&lt;0.5), "F",IF(AND(D135&lt;0.5, I135 &gt;= 0.5,N135&gt;=0.5, S135&gt;=0.5), "E2",IF(AND(D135&lt;0.5, I135 &gt;= 0.5,N135&lt;0.5, S135&lt;0.5), "E1",IF(AND(D135&lt;0.5, I135 &gt;= 0.5,N135&lt;0.5, S135&gt;=0.5), "D2",IF(AND(D135&lt;0.5, I135 &lt;0.5,N135&gt;=0.5, S135&lt;0.5), "D1",IF(AND(D135&lt;0.5, I135 &lt; 0.5,N135&gt;=0.5, S135&gt;=0.5), "C2",IF(AND(D135&lt;0.5, I135 &lt; 0.5,N135&lt;0.5, S135&lt;0.5), "C1",IF(AND(D135&lt;0.5, I135 &lt; 0.5,N135&lt;0.5, S135&gt;=0.5), "B","A"))))))))</f>
+        <v>C1</v>
+      </c>
+      <c r="AB135" s="25" t="str">
+        <f>IF(AND(E135&lt;0.5, J135 &gt;= 0.5,O135&gt;=0.5, T135&lt;0.5), "F",IF(AND(E135&lt;0.5, J135 &gt;= 0.5,O135&gt;=0.5, T135&gt;=0.5), "E2",IF(AND(E135&lt;0.5, J135 &gt;= 0.5,O135&lt;0.5, T135&lt;0.5), "E1",IF(AND(E135&lt;0.5, J135 &gt;= 0.5,O135&lt;0.5, T135&gt;=0.5), "D2",IF(AND(E135&lt;0.5, J135 &lt;0.5,O135&gt;=0.5, T135&lt;0.5), "D1",IF(AND(E135&lt;0.5, J135 &lt; 0.5,O135&gt;=0.5, T135&gt;=0.5), "C2",IF(AND(E135&lt;0.5, J135 &lt; 0.5,O135&lt;0.5, T135&lt;0.5), "C1",IF(AND(E135&lt;0.5, J135 &lt; 0.5,O135&lt;0.5, T135&gt;=0.5), "B","A"))))))))</f>
+        <v>C1</v>
+      </c>
+    </row>
+    <row r="136" spans="1:28" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A136" s="1"/>
       <c r="B136" s="1" t="s">
         <v>16</v>
@@ -7387,8 +9118,20 @@
         <f t="shared" si="23"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="137" spans="1:22" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="Z136" s="25" t="str">
+        <f>IF(AND(C136&lt;0.5, H136 &gt;= 0.5,M136&gt;=0.5, R136&lt;0.5), "F",IF(AND(C136&lt;0.5, H136 &gt;= 0.5,M136&gt;=0.5, R136&gt;=0.5), "E2",IF(AND(C136&lt;0.5, H136 &gt;= 0.5,M136&lt;0.5, R136&lt;0.5), "E1",IF(AND(C136&lt;0.5, H136 &gt;= 0.5,M136&lt;0.5, R136&gt;=0.5), "D2",IF(AND(C136&lt;0.5, H136 &lt;0.5,M136&gt;=0.5, R136&lt;0.5), "D1",IF(AND(C136&lt;0.5, H136 &lt; 0.5,M136&gt;=0.5, R136&gt;=0.5), "C2",IF(AND(C136&lt;0.5, H136 &lt; 0.5,M136&lt;0.5, R136&lt;0.5), "C1",IF(AND(C136&lt;0.5, H136 &lt; 0.5,M136&lt;0.5, R136&gt;=0.5), "B","A"))))))))</f>
+        <v>C1</v>
+      </c>
+      <c r="AA136" s="25" t="str">
+        <f>IF(AND(D136&lt;0.5, I136 &gt;= 0.5,N136&gt;=0.5, S136&lt;0.5), "F",IF(AND(D136&lt;0.5, I136 &gt;= 0.5,N136&gt;=0.5, S136&gt;=0.5), "E2",IF(AND(D136&lt;0.5, I136 &gt;= 0.5,N136&lt;0.5, S136&lt;0.5), "E1",IF(AND(D136&lt;0.5, I136 &gt;= 0.5,N136&lt;0.5, S136&gt;=0.5), "D2",IF(AND(D136&lt;0.5, I136 &lt;0.5,N136&gt;=0.5, S136&lt;0.5), "D1",IF(AND(D136&lt;0.5, I136 &lt; 0.5,N136&gt;=0.5, S136&gt;=0.5), "C2",IF(AND(D136&lt;0.5, I136 &lt; 0.5,N136&lt;0.5, S136&lt;0.5), "C1",IF(AND(D136&lt;0.5, I136 &lt; 0.5,N136&lt;0.5, S136&gt;=0.5), "B","A"))))))))</f>
+        <v>C1</v>
+      </c>
+      <c r="AB136" s="25" t="str">
+        <f>IF(AND(E136&lt;0.5, J136 &gt;= 0.5,O136&gt;=0.5, T136&lt;0.5), "F",IF(AND(E136&lt;0.5, J136 &gt;= 0.5,O136&gt;=0.5, T136&gt;=0.5), "E2",IF(AND(E136&lt;0.5, J136 &gt;= 0.5,O136&lt;0.5, T136&lt;0.5), "E1",IF(AND(E136&lt;0.5, J136 &gt;= 0.5,O136&lt;0.5, T136&gt;=0.5), "D2",IF(AND(E136&lt;0.5, J136 &lt;0.5,O136&gt;=0.5, T136&lt;0.5), "D1",IF(AND(E136&lt;0.5, J136 &lt; 0.5,O136&gt;=0.5, T136&gt;=0.5), "C2",IF(AND(E136&lt;0.5, J136 &lt; 0.5,O136&lt;0.5, T136&lt;0.5), "C1",IF(AND(E136&lt;0.5, J136 &lt; 0.5,O136&lt;0.5, T136&gt;=0.5), "B","A"))))))))</f>
+        <v>C1</v>
+      </c>
+    </row>
+    <row r="137" spans="1:28" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A137" s="1"/>
       <c r="B137" s="1" t="s">
         <v>17</v>
@@ -7434,8 +9177,20 @@
         <f t="shared" si="23"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="138" spans="1:22" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="Z137" s="25" t="str">
+        <f>IF(AND(C137&lt;0.5, H137 &gt;= 0.5,M137&gt;=0.5, R137&lt;0.5), "F",IF(AND(C137&lt;0.5, H137 &gt;= 0.5,M137&gt;=0.5, R137&gt;=0.5), "E2",IF(AND(C137&lt;0.5, H137 &gt;= 0.5,M137&lt;0.5, R137&lt;0.5), "E1",IF(AND(C137&lt;0.5, H137 &gt;= 0.5,M137&lt;0.5, R137&gt;=0.5), "D2",IF(AND(C137&lt;0.5, H137 &lt;0.5,M137&gt;=0.5, R137&lt;0.5), "D1",IF(AND(C137&lt;0.5, H137 &lt; 0.5,M137&gt;=0.5, R137&gt;=0.5), "C2",IF(AND(C137&lt;0.5, H137 &lt; 0.5,M137&lt;0.5, R137&lt;0.5), "C1",IF(AND(C137&lt;0.5, H137 &lt; 0.5,M137&lt;0.5, R137&gt;=0.5), "B","A"))))))))</f>
+        <v>C1</v>
+      </c>
+      <c r="AA137" s="25" t="str">
+        <f>IF(AND(D137&lt;0.5, I137 &gt;= 0.5,N137&gt;=0.5, S137&lt;0.5), "F",IF(AND(D137&lt;0.5, I137 &gt;= 0.5,N137&gt;=0.5, S137&gt;=0.5), "E2",IF(AND(D137&lt;0.5, I137 &gt;= 0.5,N137&lt;0.5, S137&lt;0.5), "E1",IF(AND(D137&lt;0.5, I137 &gt;= 0.5,N137&lt;0.5, S137&gt;=0.5), "D2",IF(AND(D137&lt;0.5, I137 &lt;0.5,N137&gt;=0.5, S137&lt;0.5), "D1",IF(AND(D137&lt;0.5, I137 &lt; 0.5,N137&gt;=0.5, S137&gt;=0.5), "C2",IF(AND(D137&lt;0.5, I137 &lt; 0.5,N137&lt;0.5, S137&lt;0.5), "C1",IF(AND(D137&lt;0.5, I137 &lt; 0.5,N137&lt;0.5, S137&gt;=0.5), "B","A"))))))))</f>
+        <v>C1</v>
+      </c>
+      <c r="AB137" s="25" t="str">
+        <f>IF(AND(E137&lt;0.5, J137 &gt;= 0.5,O137&gt;=0.5, T137&lt;0.5), "F",IF(AND(E137&lt;0.5, J137 &gt;= 0.5,O137&gt;=0.5, T137&gt;=0.5), "E2",IF(AND(E137&lt;0.5, J137 &gt;= 0.5,O137&lt;0.5, T137&lt;0.5), "E1",IF(AND(E137&lt;0.5, J137 &gt;= 0.5,O137&lt;0.5, T137&gt;=0.5), "D2",IF(AND(E137&lt;0.5, J137 &lt;0.5,O137&gt;=0.5, T137&lt;0.5), "D1",IF(AND(E137&lt;0.5, J137 &lt; 0.5,O137&gt;=0.5, T137&gt;=0.5), "C2",IF(AND(E137&lt;0.5, J137 &lt; 0.5,O137&lt;0.5, T137&lt;0.5), "C1",IF(AND(E137&lt;0.5, J137 &lt; 0.5,O137&lt;0.5, T137&gt;=0.5), "B","A"))))))))</f>
+        <v>C1</v>
+      </c>
+    </row>
+    <row r="138" spans="1:28" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A138" s="4"/>
       <c r="B138" s="4" t="s">
         <v>18</v>
@@ -7484,8 +9239,20 @@
         <f t="shared" si="23"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="139" spans="1:22" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="Z138" s="25" t="str">
+        <f>IF(AND(C138&lt;0.5, H138 &gt;= 0.5,M138&gt;=0.5, R138&lt;0.5), "F",IF(AND(C138&lt;0.5, H138 &gt;= 0.5,M138&gt;=0.5, R138&gt;=0.5), "E2",IF(AND(C138&lt;0.5, H138 &gt;= 0.5,M138&lt;0.5, R138&lt;0.5), "E1",IF(AND(C138&lt;0.5, H138 &gt;= 0.5,M138&lt;0.5, R138&gt;=0.5), "D2",IF(AND(C138&lt;0.5, H138 &lt;0.5,M138&gt;=0.5, R138&lt;0.5), "D1",IF(AND(C138&lt;0.5, H138 &lt; 0.5,M138&gt;=0.5, R138&gt;=0.5), "C2",IF(AND(C138&lt;0.5, H138 &lt; 0.5,M138&lt;0.5, R138&lt;0.5), "C1",IF(AND(C138&lt;0.5, H138 &lt; 0.5,M138&lt;0.5, R138&gt;=0.5), "B","A"))))))))</f>
+        <v>C1</v>
+      </c>
+      <c r="AA138" s="25" t="str">
+        <f>IF(AND(D138&lt;0.5, I138 &gt;= 0.5,N138&gt;=0.5, S138&lt;0.5), "F",IF(AND(D138&lt;0.5, I138 &gt;= 0.5,N138&gt;=0.5, S138&gt;=0.5), "E2",IF(AND(D138&lt;0.5, I138 &gt;= 0.5,N138&lt;0.5, S138&lt;0.5), "E1",IF(AND(D138&lt;0.5, I138 &gt;= 0.5,N138&lt;0.5, S138&gt;=0.5), "D2",IF(AND(D138&lt;0.5, I138 &lt;0.5,N138&gt;=0.5, S138&lt;0.5), "D1",IF(AND(D138&lt;0.5, I138 &lt; 0.5,N138&gt;=0.5, S138&gt;=0.5), "C2",IF(AND(D138&lt;0.5, I138 &lt; 0.5,N138&lt;0.5, S138&lt;0.5), "C1",IF(AND(D138&lt;0.5, I138 &lt; 0.5,N138&lt;0.5, S138&gt;=0.5), "B","A"))))))))</f>
+        <v>C1</v>
+      </c>
+      <c r="AB138" s="25" t="str">
+        <f>IF(AND(E138&lt;0.5, J138 &gt;= 0.5,O138&gt;=0.5, T138&lt;0.5), "F",IF(AND(E138&lt;0.5, J138 &gt;= 0.5,O138&gt;=0.5, T138&gt;=0.5), "E2",IF(AND(E138&lt;0.5, J138 &gt;= 0.5,O138&lt;0.5, T138&lt;0.5), "E1",IF(AND(E138&lt;0.5, J138 &gt;= 0.5,O138&lt;0.5, T138&gt;=0.5), "D2",IF(AND(E138&lt;0.5, J138 &lt;0.5,O138&gt;=0.5, T138&lt;0.5), "D1",IF(AND(E138&lt;0.5, J138 &lt; 0.5,O138&gt;=0.5, T138&gt;=0.5), "C2",IF(AND(E138&lt;0.5, J138 &lt; 0.5,O138&lt;0.5, T138&lt;0.5), "C1",IF(AND(E138&lt;0.5, J138 &lt; 0.5,O138&lt;0.5, T138&gt;=0.5), "B","A"))))))))</f>
+        <v>C1</v>
+      </c>
+    </row>
+    <row r="139" spans="1:28" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A139" s="3">
         <v>35</v>
       </c>
@@ -7536,8 +9303,20 @@
         <f t="shared" si="23"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="140" spans="1:22" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="Z139" s="25" t="str">
+        <f>IF(AND(C139&lt;0.5, H139 &gt;= 0.5,M139&gt;=0.5, R139&lt;0.5), "F",IF(AND(C139&lt;0.5, H139 &gt;= 0.5,M139&gt;=0.5, R139&gt;=0.5), "E2",IF(AND(C139&lt;0.5, H139 &gt;= 0.5,M139&lt;0.5, R139&lt;0.5), "E1",IF(AND(C139&lt;0.5, H139 &gt;= 0.5,M139&lt;0.5, R139&gt;=0.5), "D2",IF(AND(C139&lt;0.5, H139 &lt;0.5,M139&gt;=0.5, R139&lt;0.5), "D1",IF(AND(C139&lt;0.5, H139 &lt; 0.5,M139&gt;=0.5, R139&gt;=0.5), "C2",IF(AND(C139&lt;0.5, H139 &lt; 0.5,M139&lt;0.5, R139&lt;0.5), "C1",IF(AND(C139&lt;0.5, H139 &lt; 0.5,M139&lt;0.5, R139&gt;=0.5), "B","A"))))))))</f>
+        <v>C1</v>
+      </c>
+      <c r="AA139" s="25" t="str">
+        <f>IF(AND(D139&lt;0.5, I139 &gt;= 0.5,N139&gt;=0.5, S139&lt;0.5), "F",IF(AND(D139&lt;0.5, I139 &gt;= 0.5,N139&gt;=0.5, S139&gt;=0.5), "E2",IF(AND(D139&lt;0.5, I139 &gt;= 0.5,N139&lt;0.5, S139&lt;0.5), "E1",IF(AND(D139&lt;0.5, I139 &gt;= 0.5,N139&lt;0.5, S139&gt;=0.5), "D2",IF(AND(D139&lt;0.5, I139 &lt;0.5,N139&gt;=0.5, S139&lt;0.5), "D1",IF(AND(D139&lt;0.5, I139 &lt; 0.5,N139&gt;=0.5, S139&gt;=0.5), "C2",IF(AND(D139&lt;0.5, I139 &lt; 0.5,N139&lt;0.5, S139&lt;0.5), "C1",IF(AND(D139&lt;0.5, I139 &lt; 0.5,N139&lt;0.5, S139&gt;=0.5), "B","A"))))))))</f>
+        <v>C1</v>
+      </c>
+      <c r="AB139" s="25" t="str">
+        <f>IF(AND(E139&lt;0.5, J139 &gt;= 0.5,O139&gt;=0.5, T139&lt;0.5), "F",IF(AND(E139&lt;0.5, J139 &gt;= 0.5,O139&gt;=0.5, T139&gt;=0.5), "E2",IF(AND(E139&lt;0.5, J139 &gt;= 0.5,O139&lt;0.5, T139&lt;0.5), "E1",IF(AND(E139&lt;0.5, J139 &gt;= 0.5,O139&lt;0.5, T139&gt;=0.5), "D2",IF(AND(E139&lt;0.5, J139 &lt;0.5,O139&gt;=0.5, T139&lt;0.5), "D1",IF(AND(E139&lt;0.5, J139 &lt; 0.5,O139&gt;=0.5, T139&gt;=0.5), "C2",IF(AND(E139&lt;0.5, J139 &lt; 0.5,O139&lt;0.5, T139&lt;0.5), "C1",IF(AND(E139&lt;0.5, J139 &lt; 0.5,O139&lt;0.5, T139&gt;=0.5), "B","A"))))))))</f>
+        <v>C1</v>
+      </c>
+    </row>
+    <row r="140" spans="1:28" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A140" s="1"/>
       <c r="B140" s="1" t="s">
         <v>16</v>
@@ -7583,8 +9362,20 @@
         <f t="shared" si="23"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="141" spans="1:22" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="Z140" s="25" t="str">
+        <f>IF(AND(C140&lt;0.5, H140 &gt;= 0.5,M140&gt;=0.5, R140&lt;0.5), "F",IF(AND(C140&lt;0.5, H140 &gt;= 0.5,M140&gt;=0.5, R140&gt;=0.5), "E2",IF(AND(C140&lt;0.5, H140 &gt;= 0.5,M140&lt;0.5, R140&lt;0.5), "E1",IF(AND(C140&lt;0.5, H140 &gt;= 0.5,M140&lt;0.5, R140&gt;=0.5), "D2",IF(AND(C140&lt;0.5, H140 &lt;0.5,M140&gt;=0.5, R140&lt;0.5), "D1",IF(AND(C140&lt;0.5, H140 &lt; 0.5,M140&gt;=0.5, R140&gt;=0.5), "C2",IF(AND(C140&lt;0.5, H140 &lt; 0.5,M140&lt;0.5, R140&lt;0.5), "C1",IF(AND(C140&lt;0.5, H140 &lt; 0.5,M140&lt;0.5, R140&gt;=0.5), "B","A"))))))))</f>
+        <v>C1</v>
+      </c>
+      <c r="AA140" s="25" t="str">
+        <f>IF(AND(D140&lt;0.5, I140 &gt;= 0.5,N140&gt;=0.5, S140&lt;0.5), "F",IF(AND(D140&lt;0.5, I140 &gt;= 0.5,N140&gt;=0.5, S140&gt;=0.5), "E2",IF(AND(D140&lt;0.5, I140 &gt;= 0.5,N140&lt;0.5, S140&lt;0.5), "E1",IF(AND(D140&lt;0.5, I140 &gt;= 0.5,N140&lt;0.5, S140&gt;=0.5), "D2",IF(AND(D140&lt;0.5, I140 &lt;0.5,N140&gt;=0.5, S140&lt;0.5), "D1",IF(AND(D140&lt;0.5, I140 &lt; 0.5,N140&gt;=0.5, S140&gt;=0.5), "C2",IF(AND(D140&lt;0.5, I140 &lt; 0.5,N140&lt;0.5, S140&lt;0.5), "C1",IF(AND(D140&lt;0.5, I140 &lt; 0.5,N140&lt;0.5, S140&gt;=0.5), "B","A"))))))))</f>
+        <v>C1</v>
+      </c>
+      <c r="AB140" s="25" t="str">
+        <f>IF(AND(E140&lt;0.5, J140 &gt;= 0.5,O140&gt;=0.5, T140&lt;0.5), "F",IF(AND(E140&lt;0.5, J140 &gt;= 0.5,O140&gt;=0.5, T140&gt;=0.5), "E2",IF(AND(E140&lt;0.5, J140 &gt;= 0.5,O140&lt;0.5, T140&lt;0.5), "E1",IF(AND(E140&lt;0.5, J140 &gt;= 0.5,O140&lt;0.5, T140&gt;=0.5), "D2",IF(AND(E140&lt;0.5, J140 &lt;0.5,O140&gt;=0.5, T140&lt;0.5), "D1",IF(AND(E140&lt;0.5, J140 &lt; 0.5,O140&gt;=0.5, T140&gt;=0.5), "C2",IF(AND(E140&lt;0.5, J140 &lt; 0.5,O140&lt;0.5, T140&lt;0.5), "C1",IF(AND(E140&lt;0.5, J140 &lt; 0.5,O140&lt;0.5, T140&gt;=0.5), "B","A"))))))))</f>
+        <v>C1</v>
+      </c>
+    </row>
+    <row r="141" spans="1:28" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A141" s="1"/>
       <c r="B141" s="1" t="s">
         <v>17</v>
@@ -7630,8 +9421,20 @@
         <f t="shared" si="23"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="142" spans="1:22" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="Z141" s="25" t="str">
+        <f>IF(AND(C141&lt;0.5, H141 &gt;= 0.5,M141&gt;=0.5, R141&lt;0.5), "F",IF(AND(C141&lt;0.5, H141 &gt;= 0.5,M141&gt;=0.5, R141&gt;=0.5), "E2",IF(AND(C141&lt;0.5, H141 &gt;= 0.5,M141&lt;0.5, R141&lt;0.5), "E1",IF(AND(C141&lt;0.5, H141 &gt;= 0.5,M141&lt;0.5, R141&gt;=0.5), "D2",IF(AND(C141&lt;0.5, H141 &lt;0.5,M141&gt;=0.5, R141&lt;0.5), "D1",IF(AND(C141&lt;0.5, H141 &lt; 0.5,M141&gt;=0.5, R141&gt;=0.5), "C2",IF(AND(C141&lt;0.5, H141 &lt; 0.5,M141&lt;0.5, R141&lt;0.5), "C1",IF(AND(C141&lt;0.5, H141 &lt; 0.5,M141&lt;0.5, R141&gt;=0.5), "B","A"))))))))</f>
+        <v>C1</v>
+      </c>
+      <c r="AA141" s="25" t="str">
+        <f>IF(AND(D141&lt;0.5, I141 &gt;= 0.5,N141&gt;=0.5, S141&lt;0.5), "F",IF(AND(D141&lt;0.5, I141 &gt;= 0.5,N141&gt;=0.5, S141&gt;=0.5), "E2",IF(AND(D141&lt;0.5, I141 &gt;= 0.5,N141&lt;0.5, S141&lt;0.5), "E1",IF(AND(D141&lt;0.5, I141 &gt;= 0.5,N141&lt;0.5, S141&gt;=0.5), "D2",IF(AND(D141&lt;0.5, I141 &lt;0.5,N141&gt;=0.5, S141&lt;0.5), "D1",IF(AND(D141&lt;0.5, I141 &lt; 0.5,N141&gt;=0.5, S141&gt;=0.5), "C2",IF(AND(D141&lt;0.5, I141 &lt; 0.5,N141&lt;0.5, S141&lt;0.5), "C1",IF(AND(D141&lt;0.5, I141 &lt; 0.5,N141&lt;0.5, S141&gt;=0.5), "B","A"))))))))</f>
+        <v>C1</v>
+      </c>
+      <c r="AB141" s="25" t="str">
+        <f>IF(AND(E141&lt;0.5, J141 &gt;= 0.5,O141&gt;=0.5, T141&lt;0.5), "F",IF(AND(E141&lt;0.5, J141 &gt;= 0.5,O141&gt;=0.5, T141&gt;=0.5), "E2",IF(AND(E141&lt;0.5, J141 &gt;= 0.5,O141&lt;0.5, T141&lt;0.5), "E1",IF(AND(E141&lt;0.5, J141 &gt;= 0.5,O141&lt;0.5, T141&gt;=0.5), "D2",IF(AND(E141&lt;0.5, J141 &lt;0.5,O141&gt;=0.5, T141&lt;0.5), "D1",IF(AND(E141&lt;0.5, J141 &lt; 0.5,O141&gt;=0.5, T141&gt;=0.5), "C2",IF(AND(E141&lt;0.5, J141 &lt; 0.5,O141&lt;0.5, T141&lt;0.5), "C1",IF(AND(E141&lt;0.5, J141 &lt; 0.5,O141&lt;0.5, T141&gt;=0.5), "B","A"))))))))</f>
+        <v>C1</v>
+      </c>
+    </row>
+    <row r="142" spans="1:28" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A142" s="4"/>
       <c r="B142" s="4" t="s">
         <v>18</v>
@@ -7680,8 +9483,20 @@
         <f t="shared" si="23"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="143" spans="1:22" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="Z142" s="25" t="str">
+        <f>IF(AND(C142&lt;0.5, H142 &gt;= 0.5,M142&gt;=0.5, R142&lt;0.5), "F",IF(AND(C142&lt;0.5, H142 &gt;= 0.5,M142&gt;=0.5, R142&gt;=0.5), "E2",IF(AND(C142&lt;0.5, H142 &gt;= 0.5,M142&lt;0.5, R142&lt;0.5), "E1",IF(AND(C142&lt;0.5, H142 &gt;= 0.5,M142&lt;0.5, R142&gt;=0.5), "D2",IF(AND(C142&lt;0.5, H142 &lt;0.5,M142&gt;=0.5, R142&lt;0.5), "D1",IF(AND(C142&lt;0.5, H142 &lt; 0.5,M142&gt;=0.5, R142&gt;=0.5), "C2",IF(AND(C142&lt;0.5, H142 &lt; 0.5,M142&lt;0.5, R142&lt;0.5), "C1",IF(AND(C142&lt;0.5, H142 &lt; 0.5,M142&lt;0.5, R142&gt;=0.5), "B","A"))))))))</f>
+        <v>C1</v>
+      </c>
+      <c r="AA142" s="25" t="str">
+        <f>IF(AND(D142&lt;0.5, I142 &gt;= 0.5,N142&gt;=0.5, S142&lt;0.5), "F",IF(AND(D142&lt;0.5, I142 &gt;= 0.5,N142&gt;=0.5, S142&gt;=0.5), "E2",IF(AND(D142&lt;0.5, I142 &gt;= 0.5,N142&lt;0.5, S142&lt;0.5), "E1",IF(AND(D142&lt;0.5, I142 &gt;= 0.5,N142&lt;0.5, S142&gt;=0.5), "D2",IF(AND(D142&lt;0.5, I142 &lt;0.5,N142&gt;=0.5, S142&lt;0.5), "D1",IF(AND(D142&lt;0.5, I142 &lt; 0.5,N142&gt;=0.5, S142&gt;=0.5), "C2",IF(AND(D142&lt;0.5, I142 &lt; 0.5,N142&lt;0.5, S142&lt;0.5), "C1",IF(AND(D142&lt;0.5, I142 &lt; 0.5,N142&lt;0.5, S142&gt;=0.5), "B","A"))))))))</f>
+        <v>C1</v>
+      </c>
+      <c r="AB142" s="25" t="str">
+        <f>IF(AND(E142&lt;0.5, J142 &gt;= 0.5,O142&gt;=0.5, T142&lt;0.5), "F",IF(AND(E142&lt;0.5, J142 &gt;= 0.5,O142&gt;=0.5, T142&gt;=0.5), "E2",IF(AND(E142&lt;0.5, J142 &gt;= 0.5,O142&lt;0.5, T142&lt;0.5), "E1",IF(AND(E142&lt;0.5, J142 &gt;= 0.5,O142&lt;0.5, T142&gt;=0.5), "D2",IF(AND(E142&lt;0.5, J142 &lt;0.5,O142&gt;=0.5, T142&lt;0.5), "D1",IF(AND(E142&lt;0.5, J142 &lt; 0.5,O142&gt;=0.5, T142&gt;=0.5), "C2",IF(AND(E142&lt;0.5, J142 &lt; 0.5,O142&lt;0.5, T142&lt;0.5), "C1",IF(AND(E142&lt;0.5, J142 &lt; 0.5,O142&lt;0.5, T142&gt;=0.5), "B","A"))))))))</f>
+        <v>C1</v>
+      </c>
+    </row>
+    <row r="143" spans="1:28" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A143" s="3">
         <v>36</v>
       </c>
@@ -7732,8 +9547,20 @@
         <f t="shared" si="23"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="144" spans="1:22" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="Z143" s="25" t="str">
+        <f>IF(AND(C143&lt;0.5, H143 &gt;= 0.5,M143&gt;=0.5, R143&lt;0.5), "F",IF(AND(C143&lt;0.5, H143 &gt;= 0.5,M143&gt;=0.5, R143&gt;=0.5), "E2",IF(AND(C143&lt;0.5, H143 &gt;= 0.5,M143&lt;0.5, R143&lt;0.5), "E1",IF(AND(C143&lt;0.5, H143 &gt;= 0.5,M143&lt;0.5, R143&gt;=0.5), "D2",IF(AND(C143&lt;0.5, H143 &lt;0.5,M143&gt;=0.5, R143&lt;0.5), "D1",IF(AND(C143&lt;0.5, H143 &lt; 0.5,M143&gt;=0.5, R143&gt;=0.5), "C2",IF(AND(C143&lt;0.5, H143 &lt; 0.5,M143&lt;0.5, R143&lt;0.5), "C1",IF(AND(C143&lt;0.5, H143 &lt; 0.5,M143&lt;0.5, R143&gt;=0.5), "B","A"))))))))</f>
+        <v>C1</v>
+      </c>
+      <c r="AA143" s="25" t="str">
+        <f>IF(AND(D143&lt;0.5, I143 &gt;= 0.5,N143&gt;=0.5, S143&lt;0.5), "F",IF(AND(D143&lt;0.5, I143 &gt;= 0.5,N143&gt;=0.5, S143&gt;=0.5), "E2",IF(AND(D143&lt;0.5, I143 &gt;= 0.5,N143&lt;0.5, S143&lt;0.5), "E1",IF(AND(D143&lt;0.5, I143 &gt;= 0.5,N143&lt;0.5, S143&gt;=0.5), "D2",IF(AND(D143&lt;0.5, I143 &lt;0.5,N143&gt;=0.5, S143&lt;0.5), "D1",IF(AND(D143&lt;0.5, I143 &lt; 0.5,N143&gt;=0.5, S143&gt;=0.5), "C2",IF(AND(D143&lt;0.5, I143 &lt; 0.5,N143&lt;0.5, S143&lt;0.5), "C1",IF(AND(D143&lt;0.5, I143 &lt; 0.5,N143&lt;0.5, S143&gt;=0.5), "B","A"))))))))</f>
+        <v>C1</v>
+      </c>
+      <c r="AB143" s="25" t="str">
+        <f>IF(AND(E143&lt;0.5, J143 &gt;= 0.5,O143&gt;=0.5, T143&lt;0.5), "F",IF(AND(E143&lt;0.5, J143 &gt;= 0.5,O143&gt;=0.5, T143&gt;=0.5), "E2",IF(AND(E143&lt;0.5, J143 &gt;= 0.5,O143&lt;0.5, T143&lt;0.5), "E1",IF(AND(E143&lt;0.5, J143 &gt;= 0.5,O143&lt;0.5, T143&gt;=0.5), "D2",IF(AND(E143&lt;0.5, J143 &lt;0.5,O143&gt;=0.5, T143&lt;0.5), "D1",IF(AND(E143&lt;0.5, J143 &lt; 0.5,O143&gt;=0.5, T143&gt;=0.5), "C2",IF(AND(E143&lt;0.5, J143 &lt; 0.5,O143&lt;0.5, T143&lt;0.5), "C1",IF(AND(E143&lt;0.5, J143 &lt; 0.5,O143&lt;0.5, T143&gt;=0.5), "B","A"))))))))</f>
+        <v>C1</v>
+      </c>
+    </row>
+    <row r="144" spans="1:28" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A144" s="1"/>
       <c r="B144" s="1" t="s">
         <v>16</v>
@@ -7779,8 +9606,20 @@
         <f t="shared" si="23"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="145" spans="1:22" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="Z144" s="25" t="str">
+        <f>IF(AND(C144&lt;0.5, H144 &gt;= 0.5,M144&gt;=0.5, R144&lt;0.5), "F",IF(AND(C144&lt;0.5, H144 &gt;= 0.5,M144&gt;=0.5, R144&gt;=0.5), "E2",IF(AND(C144&lt;0.5, H144 &gt;= 0.5,M144&lt;0.5, R144&lt;0.5), "E1",IF(AND(C144&lt;0.5, H144 &gt;= 0.5,M144&lt;0.5, R144&gt;=0.5), "D2",IF(AND(C144&lt;0.5, H144 &lt;0.5,M144&gt;=0.5, R144&lt;0.5), "D1",IF(AND(C144&lt;0.5, H144 &lt; 0.5,M144&gt;=0.5, R144&gt;=0.5), "C2",IF(AND(C144&lt;0.5, H144 &lt; 0.5,M144&lt;0.5, R144&lt;0.5), "C1",IF(AND(C144&lt;0.5, H144 &lt; 0.5,M144&lt;0.5, R144&gt;=0.5), "B","A"))))))))</f>
+        <v>C1</v>
+      </c>
+      <c r="AA144" s="25" t="str">
+        <f>IF(AND(D144&lt;0.5, I144 &gt;= 0.5,N144&gt;=0.5, S144&lt;0.5), "F",IF(AND(D144&lt;0.5, I144 &gt;= 0.5,N144&gt;=0.5, S144&gt;=0.5), "E2",IF(AND(D144&lt;0.5, I144 &gt;= 0.5,N144&lt;0.5, S144&lt;0.5), "E1",IF(AND(D144&lt;0.5, I144 &gt;= 0.5,N144&lt;0.5, S144&gt;=0.5), "D2",IF(AND(D144&lt;0.5, I144 &lt;0.5,N144&gt;=0.5, S144&lt;0.5), "D1",IF(AND(D144&lt;0.5, I144 &lt; 0.5,N144&gt;=0.5, S144&gt;=0.5), "C2",IF(AND(D144&lt;0.5, I144 &lt; 0.5,N144&lt;0.5, S144&lt;0.5), "C1",IF(AND(D144&lt;0.5, I144 &lt; 0.5,N144&lt;0.5, S144&gt;=0.5), "B","A"))))))))</f>
+        <v>C1</v>
+      </c>
+      <c r="AB144" s="25" t="str">
+        <f>IF(AND(E144&lt;0.5, J144 &gt;= 0.5,O144&gt;=0.5, T144&lt;0.5), "F",IF(AND(E144&lt;0.5, J144 &gt;= 0.5,O144&gt;=0.5, T144&gt;=0.5), "E2",IF(AND(E144&lt;0.5, J144 &gt;= 0.5,O144&lt;0.5, T144&lt;0.5), "E1",IF(AND(E144&lt;0.5, J144 &gt;= 0.5,O144&lt;0.5, T144&gt;=0.5), "D2",IF(AND(E144&lt;0.5, J144 &lt;0.5,O144&gt;=0.5, T144&lt;0.5), "D1",IF(AND(E144&lt;0.5, J144 &lt; 0.5,O144&gt;=0.5, T144&gt;=0.5), "C2",IF(AND(E144&lt;0.5, J144 &lt; 0.5,O144&lt;0.5, T144&lt;0.5), "C1",IF(AND(E144&lt;0.5, J144 &lt; 0.5,O144&lt;0.5, T144&gt;=0.5), "B","A"))))))))</f>
+        <v>C1</v>
+      </c>
+    </row>
+    <row r="145" spans="1:28" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A145" s="1"/>
       <c r="B145" s="1" t="s">
         <v>17</v>
@@ -7826,8 +9665,20 @@
         <f t="shared" si="23"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="146" spans="1:22" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="Z145" s="25" t="str">
+        <f>IF(AND(C145&lt;0.5, H145 &gt;= 0.5,M145&gt;=0.5, R145&lt;0.5), "F",IF(AND(C145&lt;0.5, H145 &gt;= 0.5,M145&gt;=0.5, R145&gt;=0.5), "E2",IF(AND(C145&lt;0.5, H145 &gt;= 0.5,M145&lt;0.5, R145&lt;0.5), "E1",IF(AND(C145&lt;0.5, H145 &gt;= 0.5,M145&lt;0.5, R145&gt;=0.5), "D2",IF(AND(C145&lt;0.5, H145 &lt;0.5,M145&gt;=0.5, R145&lt;0.5), "D1",IF(AND(C145&lt;0.5, H145 &lt; 0.5,M145&gt;=0.5, R145&gt;=0.5), "C2",IF(AND(C145&lt;0.5, H145 &lt; 0.5,M145&lt;0.5, R145&lt;0.5), "C1",IF(AND(C145&lt;0.5, H145 &lt; 0.5,M145&lt;0.5, R145&gt;=0.5), "B","A"))))))))</f>
+        <v>C1</v>
+      </c>
+      <c r="AA145" s="25" t="str">
+        <f>IF(AND(D145&lt;0.5, I145 &gt;= 0.5,N145&gt;=0.5, S145&lt;0.5), "F",IF(AND(D145&lt;0.5, I145 &gt;= 0.5,N145&gt;=0.5, S145&gt;=0.5), "E2",IF(AND(D145&lt;0.5, I145 &gt;= 0.5,N145&lt;0.5, S145&lt;0.5), "E1",IF(AND(D145&lt;0.5, I145 &gt;= 0.5,N145&lt;0.5, S145&gt;=0.5), "D2",IF(AND(D145&lt;0.5, I145 &lt;0.5,N145&gt;=0.5, S145&lt;0.5), "D1",IF(AND(D145&lt;0.5, I145 &lt; 0.5,N145&gt;=0.5, S145&gt;=0.5), "C2",IF(AND(D145&lt;0.5, I145 &lt; 0.5,N145&lt;0.5, S145&lt;0.5), "C1",IF(AND(D145&lt;0.5, I145 &lt; 0.5,N145&lt;0.5, S145&gt;=0.5), "B","A"))))))))</f>
+        <v>C1</v>
+      </c>
+      <c r="AB145" s="25" t="str">
+        <f>IF(AND(E145&lt;0.5, J145 &gt;= 0.5,O145&gt;=0.5, T145&lt;0.5), "F",IF(AND(E145&lt;0.5, J145 &gt;= 0.5,O145&gt;=0.5, T145&gt;=0.5), "E2",IF(AND(E145&lt;0.5, J145 &gt;= 0.5,O145&lt;0.5, T145&lt;0.5), "E1",IF(AND(E145&lt;0.5, J145 &gt;= 0.5,O145&lt;0.5, T145&gt;=0.5), "D2",IF(AND(E145&lt;0.5, J145 &lt;0.5,O145&gt;=0.5, T145&lt;0.5), "D1",IF(AND(E145&lt;0.5, J145 &lt; 0.5,O145&gt;=0.5, T145&gt;=0.5), "C2",IF(AND(E145&lt;0.5, J145 &lt; 0.5,O145&lt;0.5, T145&lt;0.5), "C1",IF(AND(E145&lt;0.5, J145 &lt; 0.5,O145&lt;0.5, T145&gt;=0.5), "B","A"))))))))</f>
+        <v>C1</v>
+      </c>
+    </row>
+    <row r="146" spans="1:28" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A146" s="4"/>
       <c r="B146" s="4" t="s">
         <v>18</v>
@@ -7876,8 +9727,20 @@
         <f t="shared" si="23"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="147" spans="1:22" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="Z146" s="25" t="str">
+        <f>IF(AND(C146&lt;0.5, H146 &gt;= 0.5,M146&gt;=0.5, R146&lt;0.5), "F",IF(AND(C146&lt;0.5, H146 &gt;= 0.5,M146&gt;=0.5, R146&gt;=0.5), "E2",IF(AND(C146&lt;0.5, H146 &gt;= 0.5,M146&lt;0.5, R146&lt;0.5), "E1",IF(AND(C146&lt;0.5, H146 &gt;= 0.5,M146&lt;0.5, R146&gt;=0.5), "D2",IF(AND(C146&lt;0.5, H146 &lt;0.5,M146&gt;=0.5, R146&lt;0.5), "D1",IF(AND(C146&lt;0.5, H146 &lt; 0.5,M146&gt;=0.5, R146&gt;=0.5), "C2",IF(AND(C146&lt;0.5, H146 &lt; 0.5,M146&lt;0.5, R146&lt;0.5), "C1",IF(AND(C146&lt;0.5, H146 &lt; 0.5,M146&lt;0.5, R146&gt;=0.5), "B","A"))))))))</f>
+        <v>C1</v>
+      </c>
+      <c r="AA146" s="25" t="str">
+        <f>IF(AND(D146&lt;0.5, I146 &gt;= 0.5,N146&gt;=0.5, S146&lt;0.5), "F",IF(AND(D146&lt;0.5, I146 &gt;= 0.5,N146&gt;=0.5, S146&gt;=0.5), "E2",IF(AND(D146&lt;0.5, I146 &gt;= 0.5,N146&lt;0.5, S146&lt;0.5), "E1",IF(AND(D146&lt;0.5, I146 &gt;= 0.5,N146&lt;0.5, S146&gt;=0.5), "D2",IF(AND(D146&lt;0.5, I146 &lt;0.5,N146&gt;=0.5, S146&lt;0.5), "D1",IF(AND(D146&lt;0.5, I146 &lt; 0.5,N146&gt;=0.5, S146&gt;=0.5), "C2",IF(AND(D146&lt;0.5, I146 &lt; 0.5,N146&lt;0.5, S146&lt;0.5), "C1",IF(AND(D146&lt;0.5, I146 &lt; 0.5,N146&lt;0.5, S146&gt;=0.5), "B","A"))))))))</f>
+        <v>C1</v>
+      </c>
+      <c r="AB146" s="25" t="str">
+        <f>IF(AND(E146&lt;0.5, J146 &gt;= 0.5,O146&gt;=0.5, T146&lt;0.5), "F",IF(AND(E146&lt;0.5, J146 &gt;= 0.5,O146&gt;=0.5, T146&gt;=0.5), "E2",IF(AND(E146&lt;0.5, J146 &gt;= 0.5,O146&lt;0.5, T146&lt;0.5), "E1",IF(AND(E146&lt;0.5, J146 &gt;= 0.5,O146&lt;0.5, T146&gt;=0.5), "D2",IF(AND(E146&lt;0.5, J146 &lt;0.5,O146&gt;=0.5, T146&lt;0.5), "D1",IF(AND(E146&lt;0.5, J146 &lt; 0.5,O146&gt;=0.5, T146&gt;=0.5), "C2",IF(AND(E146&lt;0.5, J146 &lt; 0.5,O146&lt;0.5, T146&lt;0.5), "C1",IF(AND(E146&lt;0.5, J146 &lt; 0.5,O146&lt;0.5, T146&gt;=0.5), "B","A"))))))))</f>
+        <v>C1</v>
+      </c>
+    </row>
+    <row r="147" spans="1:28" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A147" s="3">
         <v>37</v>
       </c>
@@ -7928,8 +9791,20 @@
         <f t="shared" si="23"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="148" spans="1:22" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="Z147" s="25" t="str">
+        <f>IF(AND(C147&lt;0.5, H147 &gt;= 0.5,M147&gt;=0.5, R147&lt;0.5), "F",IF(AND(C147&lt;0.5, H147 &gt;= 0.5,M147&gt;=0.5, R147&gt;=0.5), "E2",IF(AND(C147&lt;0.5, H147 &gt;= 0.5,M147&lt;0.5, R147&lt;0.5), "E1",IF(AND(C147&lt;0.5, H147 &gt;= 0.5,M147&lt;0.5, R147&gt;=0.5), "D2",IF(AND(C147&lt;0.5, H147 &lt;0.5,M147&gt;=0.5, R147&lt;0.5), "D1",IF(AND(C147&lt;0.5, H147 &lt; 0.5,M147&gt;=0.5, R147&gt;=0.5), "C2",IF(AND(C147&lt;0.5, H147 &lt; 0.5,M147&lt;0.5, R147&lt;0.5), "C1",IF(AND(C147&lt;0.5, H147 &lt; 0.5,M147&lt;0.5, R147&gt;=0.5), "B","A"))))))))</f>
+        <v>C1</v>
+      </c>
+      <c r="AA147" s="25" t="str">
+        <f>IF(AND(D147&lt;0.5, I147 &gt;= 0.5,N147&gt;=0.5, S147&lt;0.5), "F",IF(AND(D147&lt;0.5, I147 &gt;= 0.5,N147&gt;=0.5, S147&gt;=0.5), "E2",IF(AND(D147&lt;0.5, I147 &gt;= 0.5,N147&lt;0.5, S147&lt;0.5), "E1",IF(AND(D147&lt;0.5, I147 &gt;= 0.5,N147&lt;0.5, S147&gt;=0.5), "D2",IF(AND(D147&lt;0.5, I147 &lt;0.5,N147&gt;=0.5, S147&lt;0.5), "D1",IF(AND(D147&lt;0.5, I147 &lt; 0.5,N147&gt;=0.5, S147&gt;=0.5), "C2",IF(AND(D147&lt;0.5, I147 &lt; 0.5,N147&lt;0.5, S147&lt;0.5), "C1",IF(AND(D147&lt;0.5, I147 &lt; 0.5,N147&lt;0.5, S147&gt;=0.5), "B","A"))))))))</f>
+        <v>C1</v>
+      </c>
+      <c r="AB147" s="25" t="str">
+        <f>IF(AND(E147&lt;0.5, J147 &gt;= 0.5,O147&gt;=0.5, T147&lt;0.5), "F",IF(AND(E147&lt;0.5, J147 &gt;= 0.5,O147&gt;=0.5, T147&gt;=0.5), "E2",IF(AND(E147&lt;0.5, J147 &gt;= 0.5,O147&lt;0.5, T147&lt;0.5), "E1",IF(AND(E147&lt;0.5, J147 &gt;= 0.5,O147&lt;0.5, T147&gt;=0.5), "D2",IF(AND(E147&lt;0.5, J147 &lt;0.5,O147&gt;=0.5, T147&lt;0.5), "D1",IF(AND(E147&lt;0.5, J147 &lt; 0.5,O147&gt;=0.5, T147&gt;=0.5), "C2",IF(AND(E147&lt;0.5, J147 &lt; 0.5,O147&lt;0.5, T147&lt;0.5), "C1",IF(AND(E147&lt;0.5, J147 &lt; 0.5,O147&lt;0.5, T147&gt;=0.5), "B","A"))))))))</f>
+        <v>C1</v>
+      </c>
+    </row>
+    <row r="148" spans="1:28" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A148" s="1"/>
       <c r="B148" s="1" t="s">
         <v>16</v>
@@ -7975,8 +9850,20 @@
         <f t="shared" si="23"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="149" spans="1:22" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="Z148" s="25" t="str">
+        <f>IF(AND(C148&lt;0.5, H148 &gt;= 0.5,M148&gt;=0.5, R148&lt;0.5), "F",IF(AND(C148&lt;0.5, H148 &gt;= 0.5,M148&gt;=0.5, R148&gt;=0.5), "E2",IF(AND(C148&lt;0.5, H148 &gt;= 0.5,M148&lt;0.5, R148&lt;0.5), "E1",IF(AND(C148&lt;0.5, H148 &gt;= 0.5,M148&lt;0.5, R148&gt;=0.5), "D2",IF(AND(C148&lt;0.5, H148 &lt;0.5,M148&gt;=0.5, R148&lt;0.5), "D1",IF(AND(C148&lt;0.5, H148 &lt; 0.5,M148&gt;=0.5, R148&gt;=0.5), "C2",IF(AND(C148&lt;0.5, H148 &lt; 0.5,M148&lt;0.5, R148&lt;0.5), "C1",IF(AND(C148&lt;0.5, H148 &lt; 0.5,M148&lt;0.5, R148&gt;=0.5), "B","A"))))))))</f>
+        <v>C1</v>
+      </c>
+      <c r="AA148" s="25" t="str">
+        <f>IF(AND(D148&lt;0.5, I148 &gt;= 0.5,N148&gt;=0.5, S148&lt;0.5), "F",IF(AND(D148&lt;0.5, I148 &gt;= 0.5,N148&gt;=0.5, S148&gt;=0.5), "E2",IF(AND(D148&lt;0.5, I148 &gt;= 0.5,N148&lt;0.5, S148&lt;0.5), "E1",IF(AND(D148&lt;0.5, I148 &gt;= 0.5,N148&lt;0.5, S148&gt;=0.5), "D2",IF(AND(D148&lt;0.5, I148 &lt;0.5,N148&gt;=0.5, S148&lt;0.5), "D1",IF(AND(D148&lt;0.5, I148 &lt; 0.5,N148&gt;=0.5, S148&gt;=0.5), "C2",IF(AND(D148&lt;0.5, I148 &lt; 0.5,N148&lt;0.5, S148&lt;0.5), "C1",IF(AND(D148&lt;0.5, I148 &lt; 0.5,N148&lt;0.5, S148&gt;=0.5), "B","A"))))))))</f>
+        <v>C1</v>
+      </c>
+      <c r="AB148" s="25" t="str">
+        <f>IF(AND(E148&lt;0.5, J148 &gt;= 0.5,O148&gt;=0.5, T148&lt;0.5), "F",IF(AND(E148&lt;0.5, J148 &gt;= 0.5,O148&gt;=0.5, T148&gt;=0.5), "E2",IF(AND(E148&lt;0.5, J148 &gt;= 0.5,O148&lt;0.5, T148&lt;0.5), "E1",IF(AND(E148&lt;0.5, J148 &gt;= 0.5,O148&lt;0.5, T148&gt;=0.5), "D2",IF(AND(E148&lt;0.5, J148 &lt;0.5,O148&gt;=0.5, T148&lt;0.5), "D1",IF(AND(E148&lt;0.5, J148 &lt; 0.5,O148&gt;=0.5, T148&gt;=0.5), "C2",IF(AND(E148&lt;0.5, J148 &lt; 0.5,O148&lt;0.5, T148&lt;0.5), "C1",IF(AND(E148&lt;0.5, J148 &lt; 0.5,O148&lt;0.5, T148&gt;=0.5), "B","A"))))))))</f>
+        <v>C1</v>
+      </c>
+    </row>
+    <row r="149" spans="1:28" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A149" s="1"/>
       <c r="B149" s="1" t="s">
         <v>17</v>
@@ -8022,8 +9909,20 @@
         <f t="shared" si="23"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="150" spans="1:22" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="Z149" s="25" t="str">
+        <f>IF(AND(C149&lt;0.5, H149 &gt;= 0.5,M149&gt;=0.5, R149&lt;0.5), "F",IF(AND(C149&lt;0.5, H149 &gt;= 0.5,M149&gt;=0.5, R149&gt;=0.5), "E2",IF(AND(C149&lt;0.5, H149 &gt;= 0.5,M149&lt;0.5, R149&lt;0.5), "E1",IF(AND(C149&lt;0.5, H149 &gt;= 0.5,M149&lt;0.5, R149&gt;=0.5), "D2",IF(AND(C149&lt;0.5, H149 &lt;0.5,M149&gt;=0.5, R149&lt;0.5), "D1",IF(AND(C149&lt;0.5, H149 &lt; 0.5,M149&gt;=0.5, R149&gt;=0.5), "C2",IF(AND(C149&lt;0.5, H149 &lt; 0.5,M149&lt;0.5, R149&lt;0.5), "C1",IF(AND(C149&lt;0.5, H149 &lt; 0.5,M149&lt;0.5, R149&gt;=0.5), "B","A"))))))))</f>
+        <v>C1</v>
+      </c>
+      <c r="AA149" s="25" t="str">
+        <f>IF(AND(D149&lt;0.5, I149 &gt;= 0.5,N149&gt;=0.5, S149&lt;0.5), "F",IF(AND(D149&lt;0.5, I149 &gt;= 0.5,N149&gt;=0.5, S149&gt;=0.5), "E2",IF(AND(D149&lt;0.5, I149 &gt;= 0.5,N149&lt;0.5, S149&lt;0.5), "E1",IF(AND(D149&lt;0.5, I149 &gt;= 0.5,N149&lt;0.5, S149&gt;=0.5), "D2",IF(AND(D149&lt;0.5, I149 &lt;0.5,N149&gt;=0.5, S149&lt;0.5), "D1",IF(AND(D149&lt;0.5, I149 &lt; 0.5,N149&gt;=0.5, S149&gt;=0.5), "C2",IF(AND(D149&lt;0.5, I149 &lt; 0.5,N149&lt;0.5, S149&lt;0.5), "C1",IF(AND(D149&lt;0.5, I149 &lt; 0.5,N149&lt;0.5, S149&gt;=0.5), "B","A"))))))))</f>
+        <v>C1</v>
+      </c>
+      <c r="AB149" s="25" t="str">
+        <f>IF(AND(E149&lt;0.5, J149 &gt;= 0.5,O149&gt;=0.5, T149&lt;0.5), "F",IF(AND(E149&lt;0.5, J149 &gt;= 0.5,O149&gt;=0.5, T149&gt;=0.5), "E2",IF(AND(E149&lt;0.5, J149 &gt;= 0.5,O149&lt;0.5, T149&lt;0.5), "E1",IF(AND(E149&lt;0.5, J149 &gt;= 0.5,O149&lt;0.5, T149&gt;=0.5), "D2",IF(AND(E149&lt;0.5, J149 &lt;0.5,O149&gt;=0.5, T149&lt;0.5), "D1",IF(AND(E149&lt;0.5, J149 &lt; 0.5,O149&gt;=0.5, T149&gt;=0.5), "C2",IF(AND(E149&lt;0.5, J149 &lt; 0.5,O149&lt;0.5, T149&lt;0.5), "C1",IF(AND(E149&lt;0.5, J149 &lt; 0.5,O149&lt;0.5, T149&gt;=0.5), "B","A"))))))))</f>
+        <v>C1</v>
+      </c>
+    </row>
+    <row r="150" spans="1:28" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A150" s="4"/>
       <c r="B150" s="4" t="s">
         <v>18</v>
@@ -8072,8 +9971,20 @@
         <f t="shared" si="23"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="151" spans="1:22" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="Z150" s="25" t="str">
+        <f>IF(AND(C150&lt;0.5, H150 &gt;= 0.5,M150&gt;=0.5, R150&lt;0.5), "F",IF(AND(C150&lt;0.5, H150 &gt;= 0.5,M150&gt;=0.5, R150&gt;=0.5), "E2",IF(AND(C150&lt;0.5, H150 &gt;= 0.5,M150&lt;0.5, R150&lt;0.5), "E1",IF(AND(C150&lt;0.5, H150 &gt;= 0.5,M150&lt;0.5, R150&gt;=0.5), "D2",IF(AND(C150&lt;0.5, H150 &lt;0.5,M150&gt;=0.5, R150&lt;0.5), "D1",IF(AND(C150&lt;0.5, H150 &lt; 0.5,M150&gt;=0.5, R150&gt;=0.5), "C2",IF(AND(C150&lt;0.5, H150 &lt; 0.5,M150&lt;0.5, R150&lt;0.5), "C1",IF(AND(C150&lt;0.5, H150 &lt; 0.5,M150&lt;0.5, R150&gt;=0.5), "B","A"))))))))</f>
+        <v>C1</v>
+      </c>
+      <c r="AA150" s="25" t="str">
+        <f>IF(AND(D150&lt;0.5, I150 &gt;= 0.5,N150&gt;=0.5, S150&lt;0.5), "F",IF(AND(D150&lt;0.5, I150 &gt;= 0.5,N150&gt;=0.5, S150&gt;=0.5), "E2",IF(AND(D150&lt;0.5, I150 &gt;= 0.5,N150&lt;0.5, S150&lt;0.5), "E1",IF(AND(D150&lt;0.5, I150 &gt;= 0.5,N150&lt;0.5, S150&gt;=0.5), "D2",IF(AND(D150&lt;0.5, I150 &lt;0.5,N150&gt;=0.5, S150&lt;0.5), "D1",IF(AND(D150&lt;0.5, I150 &lt; 0.5,N150&gt;=0.5, S150&gt;=0.5), "C2",IF(AND(D150&lt;0.5, I150 &lt; 0.5,N150&lt;0.5, S150&lt;0.5), "C1",IF(AND(D150&lt;0.5, I150 &lt; 0.5,N150&lt;0.5, S150&gt;=0.5), "B","A"))))))))</f>
+        <v>C1</v>
+      </c>
+      <c r="AB150" s="25" t="str">
+        <f>IF(AND(E150&lt;0.5, J150 &gt;= 0.5,O150&gt;=0.5, T150&lt;0.5), "F",IF(AND(E150&lt;0.5, J150 &gt;= 0.5,O150&gt;=0.5, T150&gt;=0.5), "E2",IF(AND(E150&lt;0.5, J150 &gt;= 0.5,O150&lt;0.5, T150&lt;0.5), "E1",IF(AND(E150&lt;0.5, J150 &gt;= 0.5,O150&lt;0.5, T150&gt;=0.5), "D2",IF(AND(E150&lt;0.5, J150 &lt;0.5,O150&gt;=0.5, T150&lt;0.5), "D1",IF(AND(E150&lt;0.5, J150 &lt; 0.5,O150&gt;=0.5, T150&gt;=0.5), "C2",IF(AND(E150&lt;0.5, J150 &lt; 0.5,O150&lt;0.5, T150&lt;0.5), "C1",IF(AND(E150&lt;0.5, J150 &lt; 0.5,O150&lt;0.5, T150&gt;=0.5), "B","A"))))))))</f>
+        <v>C1</v>
+      </c>
+    </row>
+    <row r="151" spans="1:28" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A151" s="3">
         <v>38</v>
       </c>
@@ -8124,8 +10035,20 @@
         <f t="shared" si="23"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="152" spans="1:22" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="Z151" s="25" t="str">
+        <f>IF(AND(C151&lt;0.5, H151 &gt;= 0.5,M151&gt;=0.5, R151&lt;0.5), "F",IF(AND(C151&lt;0.5, H151 &gt;= 0.5,M151&gt;=0.5, R151&gt;=0.5), "E2",IF(AND(C151&lt;0.5, H151 &gt;= 0.5,M151&lt;0.5, R151&lt;0.5), "E1",IF(AND(C151&lt;0.5, H151 &gt;= 0.5,M151&lt;0.5, R151&gt;=0.5), "D2",IF(AND(C151&lt;0.5, H151 &lt;0.5,M151&gt;=0.5, R151&lt;0.5), "D1",IF(AND(C151&lt;0.5, H151 &lt; 0.5,M151&gt;=0.5, R151&gt;=0.5), "C2",IF(AND(C151&lt;0.5, H151 &lt; 0.5,M151&lt;0.5, R151&lt;0.5), "C1",IF(AND(C151&lt;0.5, H151 &lt; 0.5,M151&lt;0.5, R151&gt;=0.5), "B","A"))))))))</f>
+        <v>C1</v>
+      </c>
+      <c r="AA151" s="25" t="str">
+        <f>IF(AND(D151&lt;0.5, I151 &gt;= 0.5,N151&gt;=0.5, S151&lt;0.5), "F",IF(AND(D151&lt;0.5, I151 &gt;= 0.5,N151&gt;=0.5, S151&gt;=0.5), "E2",IF(AND(D151&lt;0.5, I151 &gt;= 0.5,N151&lt;0.5, S151&lt;0.5), "E1",IF(AND(D151&lt;0.5, I151 &gt;= 0.5,N151&lt;0.5, S151&gt;=0.5), "D2",IF(AND(D151&lt;0.5, I151 &lt;0.5,N151&gt;=0.5, S151&lt;0.5), "D1",IF(AND(D151&lt;0.5, I151 &lt; 0.5,N151&gt;=0.5, S151&gt;=0.5), "C2",IF(AND(D151&lt;0.5, I151 &lt; 0.5,N151&lt;0.5, S151&lt;0.5), "C1",IF(AND(D151&lt;0.5, I151 &lt; 0.5,N151&lt;0.5, S151&gt;=0.5), "B","A"))))))))</f>
+        <v>C1</v>
+      </c>
+      <c r="AB151" s="25" t="str">
+        <f>IF(AND(E151&lt;0.5, J151 &gt;= 0.5,O151&gt;=0.5, T151&lt;0.5), "F",IF(AND(E151&lt;0.5, J151 &gt;= 0.5,O151&gt;=0.5, T151&gt;=0.5), "E2",IF(AND(E151&lt;0.5, J151 &gt;= 0.5,O151&lt;0.5, T151&lt;0.5), "E1",IF(AND(E151&lt;0.5, J151 &gt;= 0.5,O151&lt;0.5, T151&gt;=0.5), "D2",IF(AND(E151&lt;0.5, J151 &lt;0.5,O151&gt;=0.5, T151&lt;0.5), "D1",IF(AND(E151&lt;0.5, J151 &lt; 0.5,O151&gt;=0.5, T151&gt;=0.5), "C2",IF(AND(E151&lt;0.5, J151 &lt; 0.5,O151&lt;0.5, T151&lt;0.5), "C1",IF(AND(E151&lt;0.5, J151 &lt; 0.5,O151&lt;0.5, T151&gt;=0.5), "B","A"))))))))</f>
+        <v>C1</v>
+      </c>
+    </row>
+    <row r="152" spans="1:28" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A152" s="1"/>
       <c r="B152" s="1" t="s">
         <v>16</v>
@@ -8171,8 +10094,20 @@
         <f t="shared" si="23"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="153" spans="1:22" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="Z152" s="25" t="str">
+        <f>IF(AND(C152&lt;0.5, H152 &gt;= 0.5,M152&gt;=0.5, R152&lt;0.5), "F",IF(AND(C152&lt;0.5, H152 &gt;= 0.5,M152&gt;=0.5, R152&gt;=0.5), "E2",IF(AND(C152&lt;0.5, H152 &gt;= 0.5,M152&lt;0.5, R152&lt;0.5), "E1",IF(AND(C152&lt;0.5, H152 &gt;= 0.5,M152&lt;0.5, R152&gt;=0.5), "D2",IF(AND(C152&lt;0.5, H152 &lt;0.5,M152&gt;=0.5, R152&lt;0.5), "D1",IF(AND(C152&lt;0.5, H152 &lt; 0.5,M152&gt;=0.5, R152&gt;=0.5), "C2",IF(AND(C152&lt;0.5, H152 &lt; 0.5,M152&lt;0.5, R152&lt;0.5), "C1",IF(AND(C152&lt;0.5, H152 &lt; 0.5,M152&lt;0.5, R152&gt;=0.5), "B","A"))))))))</f>
+        <v>C1</v>
+      </c>
+      <c r="AA152" s="25" t="str">
+        <f>IF(AND(D152&lt;0.5, I152 &gt;= 0.5,N152&gt;=0.5, S152&lt;0.5), "F",IF(AND(D152&lt;0.5, I152 &gt;= 0.5,N152&gt;=0.5, S152&gt;=0.5), "E2",IF(AND(D152&lt;0.5, I152 &gt;= 0.5,N152&lt;0.5, S152&lt;0.5), "E1",IF(AND(D152&lt;0.5, I152 &gt;= 0.5,N152&lt;0.5, S152&gt;=0.5), "D2",IF(AND(D152&lt;0.5, I152 &lt;0.5,N152&gt;=0.5, S152&lt;0.5), "D1",IF(AND(D152&lt;0.5, I152 &lt; 0.5,N152&gt;=0.5, S152&gt;=0.5), "C2",IF(AND(D152&lt;0.5, I152 &lt; 0.5,N152&lt;0.5, S152&lt;0.5), "C1",IF(AND(D152&lt;0.5, I152 &lt; 0.5,N152&lt;0.5, S152&gt;=0.5), "B","A"))))))))</f>
+        <v>C1</v>
+      </c>
+      <c r="AB152" s="25" t="str">
+        <f>IF(AND(E152&lt;0.5, J152 &gt;= 0.5,O152&gt;=0.5, T152&lt;0.5), "F",IF(AND(E152&lt;0.5, J152 &gt;= 0.5,O152&gt;=0.5, T152&gt;=0.5), "E2",IF(AND(E152&lt;0.5, J152 &gt;= 0.5,O152&lt;0.5, T152&lt;0.5), "E1",IF(AND(E152&lt;0.5, J152 &gt;= 0.5,O152&lt;0.5, T152&gt;=0.5), "D2",IF(AND(E152&lt;0.5, J152 &lt;0.5,O152&gt;=0.5, T152&lt;0.5), "D1",IF(AND(E152&lt;0.5, J152 &lt; 0.5,O152&gt;=0.5, T152&gt;=0.5), "C2",IF(AND(E152&lt;0.5, J152 &lt; 0.5,O152&lt;0.5, T152&lt;0.5), "C1",IF(AND(E152&lt;0.5, J152 &lt; 0.5,O152&lt;0.5, T152&gt;=0.5), "B","A"))))))))</f>
+        <v>C1</v>
+      </c>
+    </row>
+    <row r="153" spans="1:28" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A153" s="1"/>
       <c r="B153" s="1" t="s">
         <v>17</v>
@@ -8218,8 +10153,20 @@
         <f t="shared" si="23"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="154" spans="1:22" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="Z153" s="25" t="str">
+        <f>IF(AND(C153&lt;0.5, H153 &gt;= 0.5,M153&gt;=0.5, R153&lt;0.5), "F",IF(AND(C153&lt;0.5, H153 &gt;= 0.5,M153&gt;=0.5, R153&gt;=0.5), "E2",IF(AND(C153&lt;0.5, H153 &gt;= 0.5,M153&lt;0.5, R153&lt;0.5), "E1",IF(AND(C153&lt;0.5, H153 &gt;= 0.5,M153&lt;0.5, R153&gt;=0.5), "D2",IF(AND(C153&lt;0.5, H153 &lt;0.5,M153&gt;=0.5, R153&lt;0.5), "D1",IF(AND(C153&lt;0.5, H153 &lt; 0.5,M153&gt;=0.5, R153&gt;=0.5), "C2",IF(AND(C153&lt;0.5, H153 &lt; 0.5,M153&lt;0.5, R153&lt;0.5), "C1",IF(AND(C153&lt;0.5, H153 &lt; 0.5,M153&lt;0.5, R153&gt;=0.5), "B","A"))))))))</f>
+        <v>C1</v>
+      </c>
+      <c r="AA153" s="25" t="str">
+        <f>IF(AND(D153&lt;0.5, I153 &gt;= 0.5,N153&gt;=0.5, S153&lt;0.5), "F",IF(AND(D153&lt;0.5, I153 &gt;= 0.5,N153&gt;=0.5, S153&gt;=0.5), "E2",IF(AND(D153&lt;0.5, I153 &gt;= 0.5,N153&lt;0.5, S153&lt;0.5), "E1",IF(AND(D153&lt;0.5, I153 &gt;= 0.5,N153&lt;0.5, S153&gt;=0.5), "D2",IF(AND(D153&lt;0.5, I153 &lt;0.5,N153&gt;=0.5, S153&lt;0.5), "D1",IF(AND(D153&lt;0.5, I153 &lt; 0.5,N153&gt;=0.5, S153&gt;=0.5), "C2",IF(AND(D153&lt;0.5, I153 &lt; 0.5,N153&lt;0.5, S153&lt;0.5), "C1",IF(AND(D153&lt;0.5, I153 &lt; 0.5,N153&lt;0.5, S153&gt;=0.5), "B","A"))))))))</f>
+        <v>C1</v>
+      </c>
+      <c r="AB153" s="25" t="str">
+        <f>IF(AND(E153&lt;0.5, J153 &gt;= 0.5,O153&gt;=0.5, T153&lt;0.5), "F",IF(AND(E153&lt;0.5, J153 &gt;= 0.5,O153&gt;=0.5, T153&gt;=0.5), "E2",IF(AND(E153&lt;0.5, J153 &gt;= 0.5,O153&lt;0.5, T153&lt;0.5), "E1",IF(AND(E153&lt;0.5, J153 &gt;= 0.5,O153&lt;0.5, T153&gt;=0.5), "D2",IF(AND(E153&lt;0.5, J153 &lt;0.5,O153&gt;=0.5, T153&lt;0.5), "D1",IF(AND(E153&lt;0.5, J153 &lt; 0.5,O153&gt;=0.5, T153&gt;=0.5), "C2",IF(AND(E153&lt;0.5, J153 &lt; 0.5,O153&lt;0.5, T153&lt;0.5), "C1",IF(AND(E153&lt;0.5, J153 &lt; 0.5,O153&lt;0.5, T153&gt;=0.5), "B","A"))))))))</f>
+        <v>C1</v>
+      </c>
+    </row>
+    <row r="154" spans="1:28" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A154" s="4"/>
       <c r="B154" s="4" t="s">
         <v>18</v>
@@ -8268,8 +10215,20 @@
         <f t="shared" si="23"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="155" spans="1:22" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="Z154" s="25" t="str">
+        <f>IF(AND(C154&lt;0.5, H154 &gt;= 0.5,M154&gt;=0.5, R154&lt;0.5), "F",IF(AND(C154&lt;0.5, H154 &gt;= 0.5,M154&gt;=0.5, R154&gt;=0.5), "E2",IF(AND(C154&lt;0.5, H154 &gt;= 0.5,M154&lt;0.5, R154&lt;0.5), "E1",IF(AND(C154&lt;0.5, H154 &gt;= 0.5,M154&lt;0.5, R154&gt;=0.5), "D2",IF(AND(C154&lt;0.5, H154 &lt;0.5,M154&gt;=0.5, R154&lt;0.5), "D1",IF(AND(C154&lt;0.5, H154 &lt; 0.5,M154&gt;=0.5, R154&gt;=0.5), "C2",IF(AND(C154&lt;0.5, H154 &lt; 0.5,M154&lt;0.5, R154&lt;0.5), "C1",IF(AND(C154&lt;0.5, H154 &lt; 0.5,M154&lt;0.5, R154&gt;=0.5), "B","A"))))))))</f>
+        <v>C1</v>
+      </c>
+      <c r="AA154" s="25" t="str">
+        <f>IF(AND(D154&lt;0.5, I154 &gt;= 0.5,N154&gt;=0.5, S154&lt;0.5), "F",IF(AND(D154&lt;0.5, I154 &gt;= 0.5,N154&gt;=0.5, S154&gt;=0.5), "E2",IF(AND(D154&lt;0.5, I154 &gt;= 0.5,N154&lt;0.5, S154&lt;0.5), "E1",IF(AND(D154&lt;0.5, I154 &gt;= 0.5,N154&lt;0.5, S154&gt;=0.5), "D2",IF(AND(D154&lt;0.5, I154 &lt;0.5,N154&gt;=0.5, S154&lt;0.5), "D1",IF(AND(D154&lt;0.5, I154 &lt; 0.5,N154&gt;=0.5, S154&gt;=0.5), "C2",IF(AND(D154&lt;0.5, I154 &lt; 0.5,N154&lt;0.5, S154&lt;0.5), "C1",IF(AND(D154&lt;0.5, I154 &lt; 0.5,N154&lt;0.5, S154&gt;=0.5), "B","A"))))))))</f>
+        <v>C1</v>
+      </c>
+      <c r="AB154" s="25" t="str">
+        <f>IF(AND(E154&lt;0.5, J154 &gt;= 0.5,O154&gt;=0.5, T154&lt;0.5), "F",IF(AND(E154&lt;0.5, J154 &gt;= 0.5,O154&gt;=0.5, T154&gt;=0.5), "E2",IF(AND(E154&lt;0.5, J154 &gt;= 0.5,O154&lt;0.5, T154&lt;0.5), "E1",IF(AND(E154&lt;0.5, J154 &gt;= 0.5,O154&lt;0.5, T154&gt;=0.5), "D2",IF(AND(E154&lt;0.5, J154 &lt;0.5,O154&gt;=0.5, T154&lt;0.5), "D1",IF(AND(E154&lt;0.5, J154 &lt; 0.5,O154&gt;=0.5, T154&gt;=0.5), "C2",IF(AND(E154&lt;0.5, J154 &lt; 0.5,O154&lt;0.5, T154&lt;0.5), "C1",IF(AND(E154&lt;0.5, J154 &lt; 0.5,O154&lt;0.5, T154&gt;=0.5), "B","A"))))))))</f>
+        <v>C1</v>
+      </c>
+    </row>
+    <row r="155" spans="1:28" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A155" s="3">
         <v>39</v>
       </c>
@@ -8320,8 +10279,20 @@
         <f t="shared" si="23"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="156" spans="1:22" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="Z155" s="25" t="str">
+        <f>IF(AND(C155&lt;0.5, H155 &gt;= 0.5,M155&gt;=0.5, R155&lt;0.5), "F",IF(AND(C155&lt;0.5, H155 &gt;= 0.5,M155&gt;=0.5, R155&gt;=0.5), "E2",IF(AND(C155&lt;0.5, H155 &gt;= 0.5,M155&lt;0.5, R155&lt;0.5), "E1",IF(AND(C155&lt;0.5, H155 &gt;= 0.5,M155&lt;0.5, R155&gt;=0.5), "D2",IF(AND(C155&lt;0.5, H155 &lt;0.5,M155&gt;=0.5, R155&lt;0.5), "D1",IF(AND(C155&lt;0.5, H155 &lt; 0.5,M155&gt;=0.5, R155&gt;=0.5), "C2",IF(AND(C155&lt;0.5, H155 &lt; 0.5,M155&lt;0.5, R155&lt;0.5), "C1",IF(AND(C155&lt;0.5, H155 &lt; 0.5,M155&lt;0.5, R155&gt;=0.5), "B","A"))))))))</f>
+        <v>C1</v>
+      </c>
+      <c r="AA155" s="25" t="str">
+        <f>IF(AND(D155&lt;0.5, I155 &gt;= 0.5,N155&gt;=0.5, S155&lt;0.5), "F",IF(AND(D155&lt;0.5, I155 &gt;= 0.5,N155&gt;=0.5, S155&gt;=0.5), "E2",IF(AND(D155&lt;0.5, I155 &gt;= 0.5,N155&lt;0.5, S155&lt;0.5), "E1",IF(AND(D155&lt;0.5, I155 &gt;= 0.5,N155&lt;0.5, S155&gt;=0.5), "D2",IF(AND(D155&lt;0.5, I155 &lt;0.5,N155&gt;=0.5, S155&lt;0.5), "D1",IF(AND(D155&lt;0.5, I155 &lt; 0.5,N155&gt;=0.5, S155&gt;=0.5), "C2",IF(AND(D155&lt;0.5, I155 &lt; 0.5,N155&lt;0.5, S155&lt;0.5), "C1",IF(AND(D155&lt;0.5, I155 &lt; 0.5,N155&lt;0.5, S155&gt;=0.5), "B","A"))))))))</f>
+        <v>C1</v>
+      </c>
+      <c r="AB155" s="25" t="str">
+        <f>IF(AND(E155&lt;0.5, J155 &gt;= 0.5,O155&gt;=0.5, T155&lt;0.5), "F",IF(AND(E155&lt;0.5, J155 &gt;= 0.5,O155&gt;=0.5, T155&gt;=0.5), "E2",IF(AND(E155&lt;0.5, J155 &gt;= 0.5,O155&lt;0.5, T155&lt;0.5), "E1",IF(AND(E155&lt;0.5, J155 &gt;= 0.5,O155&lt;0.5, T155&gt;=0.5), "D2",IF(AND(E155&lt;0.5, J155 &lt;0.5,O155&gt;=0.5, T155&lt;0.5), "D1",IF(AND(E155&lt;0.5, J155 &lt; 0.5,O155&gt;=0.5, T155&gt;=0.5), "C2",IF(AND(E155&lt;0.5, J155 &lt; 0.5,O155&lt;0.5, T155&lt;0.5), "C1",IF(AND(E155&lt;0.5, J155 &lt; 0.5,O155&lt;0.5, T155&gt;=0.5), "B","A"))))))))</f>
+        <v>C1</v>
+      </c>
+    </row>
+    <row r="156" spans="1:28" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A156" s="1"/>
       <c r="B156" s="1" t="s">
         <v>16</v>
@@ -8367,8 +10338,20 @@
         <f t="shared" si="23"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="157" spans="1:22" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="Z156" s="25" t="str">
+        <f>IF(AND(C156&lt;0.5, H156 &gt;= 0.5,M156&gt;=0.5, R156&lt;0.5), "F",IF(AND(C156&lt;0.5, H156 &gt;= 0.5,M156&gt;=0.5, R156&gt;=0.5), "E2",IF(AND(C156&lt;0.5, H156 &gt;= 0.5,M156&lt;0.5, R156&lt;0.5), "E1",IF(AND(C156&lt;0.5, H156 &gt;= 0.5,M156&lt;0.5, R156&gt;=0.5), "D2",IF(AND(C156&lt;0.5, H156 &lt;0.5,M156&gt;=0.5, R156&lt;0.5), "D1",IF(AND(C156&lt;0.5, H156 &lt; 0.5,M156&gt;=0.5, R156&gt;=0.5), "C2",IF(AND(C156&lt;0.5, H156 &lt; 0.5,M156&lt;0.5, R156&lt;0.5), "C1",IF(AND(C156&lt;0.5, H156 &lt; 0.5,M156&lt;0.5, R156&gt;=0.5), "B","A"))))))))</f>
+        <v>C1</v>
+      </c>
+      <c r="AA156" s="25" t="str">
+        <f>IF(AND(D156&lt;0.5, I156 &gt;= 0.5,N156&gt;=0.5, S156&lt;0.5), "F",IF(AND(D156&lt;0.5, I156 &gt;= 0.5,N156&gt;=0.5, S156&gt;=0.5), "E2",IF(AND(D156&lt;0.5, I156 &gt;= 0.5,N156&lt;0.5, S156&lt;0.5), "E1",IF(AND(D156&lt;0.5, I156 &gt;= 0.5,N156&lt;0.5, S156&gt;=0.5), "D2",IF(AND(D156&lt;0.5, I156 &lt;0.5,N156&gt;=0.5, S156&lt;0.5), "D1",IF(AND(D156&lt;0.5, I156 &lt; 0.5,N156&gt;=0.5, S156&gt;=0.5), "C2",IF(AND(D156&lt;0.5, I156 &lt; 0.5,N156&lt;0.5, S156&lt;0.5), "C1",IF(AND(D156&lt;0.5, I156 &lt; 0.5,N156&lt;0.5, S156&gt;=0.5), "B","A"))))))))</f>
+        <v>C1</v>
+      </c>
+      <c r="AB156" s="25" t="str">
+        <f>IF(AND(E156&lt;0.5, J156 &gt;= 0.5,O156&gt;=0.5, T156&lt;0.5), "F",IF(AND(E156&lt;0.5, J156 &gt;= 0.5,O156&gt;=0.5, T156&gt;=0.5), "E2",IF(AND(E156&lt;0.5, J156 &gt;= 0.5,O156&lt;0.5, T156&lt;0.5), "E1",IF(AND(E156&lt;0.5, J156 &gt;= 0.5,O156&lt;0.5, T156&gt;=0.5), "D2",IF(AND(E156&lt;0.5, J156 &lt;0.5,O156&gt;=0.5, T156&lt;0.5), "D1",IF(AND(E156&lt;0.5, J156 &lt; 0.5,O156&gt;=0.5, T156&gt;=0.5), "C2",IF(AND(E156&lt;0.5, J156 &lt; 0.5,O156&lt;0.5, T156&lt;0.5), "C1",IF(AND(E156&lt;0.5, J156 &lt; 0.5,O156&lt;0.5, T156&gt;=0.5), "B","A"))))))))</f>
+        <v>C1</v>
+      </c>
+    </row>
+    <row r="157" spans="1:28" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A157" s="1"/>
       <c r="B157" s="1" t="s">
         <v>17</v>
@@ -8414,8 +10397,20 @@
         <f t="shared" si="23"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="158" spans="1:22" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="Z157" s="25" t="str">
+        <f>IF(AND(C157&lt;0.5, H157 &gt;= 0.5,M157&gt;=0.5, R157&lt;0.5), "F",IF(AND(C157&lt;0.5, H157 &gt;= 0.5,M157&gt;=0.5, R157&gt;=0.5), "E2",IF(AND(C157&lt;0.5, H157 &gt;= 0.5,M157&lt;0.5, R157&lt;0.5), "E1",IF(AND(C157&lt;0.5, H157 &gt;= 0.5,M157&lt;0.5, R157&gt;=0.5), "D2",IF(AND(C157&lt;0.5, H157 &lt;0.5,M157&gt;=0.5, R157&lt;0.5), "D1",IF(AND(C157&lt;0.5, H157 &lt; 0.5,M157&gt;=0.5, R157&gt;=0.5), "C2",IF(AND(C157&lt;0.5, H157 &lt; 0.5,M157&lt;0.5, R157&lt;0.5), "C1",IF(AND(C157&lt;0.5, H157 &lt; 0.5,M157&lt;0.5, R157&gt;=0.5), "B","A"))))))))</f>
+        <v>C1</v>
+      </c>
+      <c r="AA157" s="25" t="str">
+        <f>IF(AND(D157&lt;0.5, I157 &gt;= 0.5,N157&gt;=0.5, S157&lt;0.5), "F",IF(AND(D157&lt;0.5, I157 &gt;= 0.5,N157&gt;=0.5, S157&gt;=0.5), "E2",IF(AND(D157&lt;0.5, I157 &gt;= 0.5,N157&lt;0.5, S157&lt;0.5), "E1",IF(AND(D157&lt;0.5, I157 &gt;= 0.5,N157&lt;0.5, S157&gt;=0.5), "D2",IF(AND(D157&lt;0.5, I157 &lt;0.5,N157&gt;=0.5, S157&lt;0.5), "D1",IF(AND(D157&lt;0.5, I157 &lt; 0.5,N157&gt;=0.5, S157&gt;=0.5), "C2",IF(AND(D157&lt;0.5, I157 &lt; 0.5,N157&lt;0.5, S157&lt;0.5), "C1",IF(AND(D157&lt;0.5, I157 &lt; 0.5,N157&lt;0.5, S157&gt;=0.5), "B","A"))))))))</f>
+        <v>C1</v>
+      </c>
+      <c r="AB157" s="25" t="str">
+        <f>IF(AND(E157&lt;0.5, J157 &gt;= 0.5,O157&gt;=0.5, T157&lt;0.5), "F",IF(AND(E157&lt;0.5, J157 &gt;= 0.5,O157&gt;=0.5, T157&gt;=0.5), "E2",IF(AND(E157&lt;0.5, J157 &gt;= 0.5,O157&lt;0.5, T157&lt;0.5), "E1",IF(AND(E157&lt;0.5, J157 &gt;= 0.5,O157&lt;0.5, T157&gt;=0.5), "D2",IF(AND(E157&lt;0.5, J157 &lt;0.5,O157&gt;=0.5, T157&lt;0.5), "D1",IF(AND(E157&lt;0.5, J157 &lt; 0.5,O157&gt;=0.5, T157&gt;=0.5), "C2",IF(AND(E157&lt;0.5, J157 &lt; 0.5,O157&lt;0.5, T157&lt;0.5), "C1",IF(AND(E157&lt;0.5, J157 &lt; 0.5,O157&lt;0.5, T157&gt;=0.5), "B","A"))))))))</f>
+        <v>C1</v>
+      </c>
+    </row>
+    <row r="158" spans="1:28" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A158" s="4"/>
       <c r="B158" s="4" t="s">
         <v>18</v>
@@ -8464,8 +10459,20 @@
         <f t="shared" si="23"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="159" spans="1:22" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="Z158" s="25" t="str">
+        <f>IF(AND(C158&lt;0.5, H158 &gt;= 0.5,M158&gt;=0.5, R158&lt;0.5), "F",IF(AND(C158&lt;0.5, H158 &gt;= 0.5,M158&gt;=0.5, R158&gt;=0.5), "E2",IF(AND(C158&lt;0.5, H158 &gt;= 0.5,M158&lt;0.5, R158&lt;0.5), "E1",IF(AND(C158&lt;0.5, H158 &gt;= 0.5,M158&lt;0.5, R158&gt;=0.5), "D2",IF(AND(C158&lt;0.5, H158 &lt;0.5,M158&gt;=0.5, R158&lt;0.5), "D1",IF(AND(C158&lt;0.5, H158 &lt; 0.5,M158&gt;=0.5, R158&gt;=0.5), "C2",IF(AND(C158&lt;0.5, H158 &lt; 0.5,M158&lt;0.5, R158&lt;0.5), "C1",IF(AND(C158&lt;0.5, H158 &lt; 0.5,M158&lt;0.5, R158&gt;=0.5), "B","A"))))))))</f>
+        <v>C1</v>
+      </c>
+      <c r="AA158" s="25" t="str">
+        <f>IF(AND(D158&lt;0.5, I158 &gt;= 0.5,N158&gt;=0.5, S158&lt;0.5), "F",IF(AND(D158&lt;0.5, I158 &gt;= 0.5,N158&gt;=0.5, S158&gt;=0.5), "E2",IF(AND(D158&lt;0.5, I158 &gt;= 0.5,N158&lt;0.5, S158&lt;0.5), "E1",IF(AND(D158&lt;0.5, I158 &gt;= 0.5,N158&lt;0.5, S158&gt;=0.5), "D2",IF(AND(D158&lt;0.5, I158 &lt;0.5,N158&gt;=0.5, S158&lt;0.5), "D1",IF(AND(D158&lt;0.5, I158 &lt; 0.5,N158&gt;=0.5, S158&gt;=0.5), "C2",IF(AND(D158&lt;0.5, I158 &lt; 0.5,N158&lt;0.5, S158&lt;0.5), "C1",IF(AND(D158&lt;0.5, I158 &lt; 0.5,N158&lt;0.5, S158&gt;=0.5), "B","A"))))))))</f>
+        <v>C1</v>
+      </c>
+      <c r="AB158" s="25" t="str">
+        <f>IF(AND(E158&lt;0.5, J158 &gt;= 0.5,O158&gt;=0.5, T158&lt;0.5), "F",IF(AND(E158&lt;0.5, J158 &gt;= 0.5,O158&gt;=0.5, T158&gt;=0.5), "E2",IF(AND(E158&lt;0.5, J158 &gt;= 0.5,O158&lt;0.5, T158&lt;0.5), "E1",IF(AND(E158&lt;0.5, J158 &gt;= 0.5,O158&lt;0.5, T158&gt;=0.5), "D2",IF(AND(E158&lt;0.5, J158 &lt;0.5,O158&gt;=0.5, T158&lt;0.5), "D1",IF(AND(E158&lt;0.5, J158 &lt; 0.5,O158&gt;=0.5, T158&gt;=0.5), "C2",IF(AND(E158&lt;0.5, J158 &lt; 0.5,O158&lt;0.5, T158&lt;0.5), "C1",IF(AND(E158&lt;0.5, J158 &lt; 0.5,O158&lt;0.5, T158&gt;=0.5), "B","A"))))))))</f>
+        <v>C1</v>
+      </c>
+    </row>
+    <row r="159" spans="1:28" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A159" s="3">
         <v>40</v>
       </c>
@@ -8516,8 +10523,20 @@
         <f t="shared" si="23"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="160" spans="1:22" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="Z159" s="25" t="str">
+        <f>IF(AND(C159&lt;0.5, H159 &gt;= 0.5,M159&gt;=0.5, R159&lt;0.5), "F",IF(AND(C159&lt;0.5, H159 &gt;= 0.5,M159&gt;=0.5, R159&gt;=0.5), "E2",IF(AND(C159&lt;0.5, H159 &gt;= 0.5,M159&lt;0.5, R159&lt;0.5), "E1",IF(AND(C159&lt;0.5, H159 &gt;= 0.5,M159&lt;0.5, R159&gt;=0.5), "D2",IF(AND(C159&lt;0.5, H159 &lt;0.5,M159&gt;=0.5, R159&lt;0.5), "D1",IF(AND(C159&lt;0.5, H159 &lt; 0.5,M159&gt;=0.5, R159&gt;=0.5), "C2",IF(AND(C159&lt;0.5, H159 &lt; 0.5,M159&lt;0.5, R159&lt;0.5), "C1",IF(AND(C159&lt;0.5, H159 &lt; 0.5,M159&lt;0.5, R159&gt;=0.5), "B","A"))))))))</f>
+        <v>C1</v>
+      </c>
+      <c r="AA159" s="25" t="str">
+        <f>IF(AND(D159&lt;0.5, I159 &gt;= 0.5,N159&gt;=0.5, S159&lt;0.5), "F",IF(AND(D159&lt;0.5, I159 &gt;= 0.5,N159&gt;=0.5, S159&gt;=0.5), "E2",IF(AND(D159&lt;0.5, I159 &gt;= 0.5,N159&lt;0.5, S159&lt;0.5), "E1",IF(AND(D159&lt;0.5, I159 &gt;= 0.5,N159&lt;0.5, S159&gt;=0.5), "D2",IF(AND(D159&lt;0.5, I159 &lt;0.5,N159&gt;=0.5, S159&lt;0.5), "D1",IF(AND(D159&lt;0.5, I159 &lt; 0.5,N159&gt;=0.5, S159&gt;=0.5), "C2",IF(AND(D159&lt;0.5, I159 &lt; 0.5,N159&lt;0.5, S159&lt;0.5), "C1",IF(AND(D159&lt;0.5, I159 &lt; 0.5,N159&lt;0.5, S159&gt;=0.5), "B","A"))))))))</f>
+        <v>C1</v>
+      </c>
+      <c r="AB159" s="25" t="str">
+        <f>IF(AND(E159&lt;0.5, J159 &gt;= 0.5,O159&gt;=0.5, T159&lt;0.5), "F",IF(AND(E159&lt;0.5, J159 &gt;= 0.5,O159&gt;=0.5, T159&gt;=0.5), "E2",IF(AND(E159&lt;0.5, J159 &gt;= 0.5,O159&lt;0.5, T159&lt;0.5), "E1",IF(AND(E159&lt;0.5, J159 &gt;= 0.5,O159&lt;0.5, T159&gt;=0.5), "D2",IF(AND(E159&lt;0.5, J159 &lt;0.5,O159&gt;=0.5, T159&lt;0.5), "D1",IF(AND(E159&lt;0.5, J159 &lt; 0.5,O159&gt;=0.5, T159&gt;=0.5), "C2",IF(AND(E159&lt;0.5, J159 &lt; 0.5,O159&lt;0.5, T159&lt;0.5), "C1",IF(AND(E159&lt;0.5, J159 &lt; 0.5,O159&lt;0.5, T159&gt;=0.5), "B","A"))))))))</f>
+        <v>C1</v>
+      </c>
+    </row>
+    <row r="160" spans="1:28" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A160" s="1"/>
       <c r="B160" s="1" t="s">
         <v>16</v>
@@ -8563,8 +10582,20 @@
         <f t="shared" si="23"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="161" spans="1:22" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="Z160" s="25" t="str">
+        <f>IF(AND(C160&lt;0.5, H160 &gt;= 0.5,M160&gt;=0.5, R160&lt;0.5), "F",IF(AND(C160&lt;0.5, H160 &gt;= 0.5,M160&gt;=0.5, R160&gt;=0.5), "E2",IF(AND(C160&lt;0.5, H160 &gt;= 0.5,M160&lt;0.5, R160&lt;0.5), "E1",IF(AND(C160&lt;0.5, H160 &gt;= 0.5,M160&lt;0.5, R160&gt;=0.5), "D2",IF(AND(C160&lt;0.5, H160 &lt;0.5,M160&gt;=0.5, R160&lt;0.5), "D1",IF(AND(C160&lt;0.5, H160 &lt; 0.5,M160&gt;=0.5, R160&gt;=0.5), "C2",IF(AND(C160&lt;0.5, H160 &lt; 0.5,M160&lt;0.5, R160&lt;0.5), "C1",IF(AND(C160&lt;0.5, H160 &lt; 0.5,M160&lt;0.5, R160&gt;=0.5), "B","A"))))))))</f>
+        <v>C1</v>
+      </c>
+      <c r="AA160" s="25" t="str">
+        <f>IF(AND(D160&lt;0.5, I160 &gt;= 0.5,N160&gt;=0.5, S160&lt;0.5), "F",IF(AND(D160&lt;0.5, I160 &gt;= 0.5,N160&gt;=0.5, S160&gt;=0.5), "E2",IF(AND(D160&lt;0.5, I160 &gt;= 0.5,N160&lt;0.5, S160&lt;0.5), "E1",IF(AND(D160&lt;0.5, I160 &gt;= 0.5,N160&lt;0.5, S160&gt;=0.5), "D2",IF(AND(D160&lt;0.5, I160 &lt;0.5,N160&gt;=0.5, S160&lt;0.5), "D1",IF(AND(D160&lt;0.5, I160 &lt; 0.5,N160&gt;=0.5, S160&gt;=0.5), "C2",IF(AND(D160&lt;0.5, I160 &lt; 0.5,N160&lt;0.5, S160&lt;0.5), "C1",IF(AND(D160&lt;0.5, I160 &lt; 0.5,N160&lt;0.5, S160&gt;=0.5), "B","A"))))))))</f>
+        <v>C1</v>
+      </c>
+      <c r="AB160" s="25" t="str">
+        <f>IF(AND(E160&lt;0.5, J160 &gt;= 0.5,O160&gt;=0.5, T160&lt;0.5), "F",IF(AND(E160&lt;0.5, J160 &gt;= 0.5,O160&gt;=0.5, T160&gt;=0.5), "E2",IF(AND(E160&lt;0.5, J160 &gt;= 0.5,O160&lt;0.5, T160&lt;0.5), "E1",IF(AND(E160&lt;0.5, J160 &gt;= 0.5,O160&lt;0.5, T160&gt;=0.5), "D2",IF(AND(E160&lt;0.5, J160 &lt;0.5,O160&gt;=0.5, T160&lt;0.5), "D1",IF(AND(E160&lt;0.5, J160 &lt; 0.5,O160&gt;=0.5, T160&gt;=0.5), "C2",IF(AND(E160&lt;0.5, J160 &lt; 0.5,O160&lt;0.5, T160&lt;0.5), "C1",IF(AND(E160&lt;0.5, J160 &lt; 0.5,O160&lt;0.5, T160&gt;=0.5), "B","A"))))))))</f>
+        <v>C1</v>
+      </c>
+    </row>
+    <row r="161" spans="1:28" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A161" s="1"/>
       <c r="B161" s="1" t="s">
         <v>17</v>
@@ -8610,8 +10641,20 @@
         <f t="shared" si="23"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="162" spans="1:22" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="Z161" s="25" t="str">
+        <f>IF(AND(C161&lt;0.5, H161 &gt;= 0.5,M161&gt;=0.5, R161&lt;0.5), "F",IF(AND(C161&lt;0.5, H161 &gt;= 0.5,M161&gt;=0.5, R161&gt;=0.5), "E2",IF(AND(C161&lt;0.5, H161 &gt;= 0.5,M161&lt;0.5, R161&lt;0.5), "E1",IF(AND(C161&lt;0.5, H161 &gt;= 0.5,M161&lt;0.5, R161&gt;=0.5), "D2",IF(AND(C161&lt;0.5, H161 &lt;0.5,M161&gt;=0.5, R161&lt;0.5), "D1",IF(AND(C161&lt;0.5, H161 &lt; 0.5,M161&gt;=0.5, R161&gt;=0.5), "C2",IF(AND(C161&lt;0.5, H161 &lt; 0.5,M161&lt;0.5, R161&lt;0.5), "C1",IF(AND(C161&lt;0.5, H161 &lt; 0.5,M161&lt;0.5, R161&gt;=0.5), "B","A"))))))))</f>
+        <v>C1</v>
+      </c>
+      <c r="AA161" s="25" t="str">
+        <f>IF(AND(D161&lt;0.5, I161 &gt;= 0.5,N161&gt;=0.5, S161&lt;0.5), "F",IF(AND(D161&lt;0.5, I161 &gt;= 0.5,N161&gt;=0.5, S161&gt;=0.5), "E2",IF(AND(D161&lt;0.5, I161 &gt;= 0.5,N161&lt;0.5, S161&lt;0.5), "E1",IF(AND(D161&lt;0.5, I161 &gt;= 0.5,N161&lt;0.5, S161&gt;=0.5), "D2",IF(AND(D161&lt;0.5, I161 &lt;0.5,N161&gt;=0.5, S161&lt;0.5), "D1",IF(AND(D161&lt;0.5, I161 &lt; 0.5,N161&gt;=0.5, S161&gt;=0.5), "C2",IF(AND(D161&lt;0.5, I161 &lt; 0.5,N161&lt;0.5, S161&lt;0.5), "C1",IF(AND(D161&lt;0.5, I161 &lt; 0.5,N161&lt;0.5, S161&gt;=0.5), "B","A"))))))))</f>
+        <v>C1</v>
+      </c>
+      <c r="AB161" s="25" t="str">
+        <f>IF(AND(E161&lt;0.5, J161 &gt;= 0.5,O161&gt;=0.5, T161&lt;0.5), "F",IF(AND(E161&lt;0.5, J161 &gt;= 0.5,O161&gt;=0.5, T161&gt;=0.5), "E2",IF(AND(E161&lt;0.5, J161 &gt;= 0.5,O161&lt;0.5, T161&lt;0.5), "E1",IF(AND(E161&lt;0.5, J161 &gt;= 0.5,O161&lt;0.5, T161&gt;=0.5), "D2",IF(AND(E161&lt;0.5, J161 &lt;0.5,O161&gt;=0.5, T161&lt;0.5), "D1",IF(AND(E161&lt;0.5, J161 &lt; 0.5,O161&gt;=0.5, T161&gt;=0.5), "C2",IF(AND(E161&lt;0.5, J161 &lt; 0.5,O161&lt;0.5, T161&lt;0.5), "C1",IF(AND(E161&lt;0.5, J161 &lt; 0.5,O161&lt;0.5, T161&gt;=0.5), "B","A"))))))))</f>
+        <v>C1</v>
+      </c>
+    </row>
+    <row r="162" spans="1:28" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A162" s="4"/>
       <c r="B162" s="4" t="s">
         <v>18</v>
@@ -8660,8 +10703,20 @@
         <f t="shared" si="23"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="163" spans="1:22" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="Z162" s="25" t="str">
+        <f>IF(AND(C162&lt;0.5, H162 &gt;= 0.5,M162&gt;=0.5, R162&lt;0.5), "F",IF(AND(C162&lt;0.5, H162 &gt;= 0.5,M162&gt;=0.5, R162&gt;=0.5), "E2",IF(AND(C162&lt;0.5, H162 &gt;= 0.5,M162&lt;0.5, R162&lt;0.5), "E1",IF(AND(C162&lt;0.5, H162 &gt;= 0.5,M162&lt;0.5, R162&gt;=0.5), "D2",IF(AND(C162&lt;0.5, H162 &lt;0.5,M162&gt;=0.5, R162&lt;0.5), "D1",IF(AND(C162&lt;0.5, H162 &lt; 0.5,M162&gt;=0.5, R162&gt;=0.5), "C2",IF(AND(C162&lt;0.5, H162 &lt; 0.5,M162&lt;0.5, R162&lt;0.5), "C1",IF(AND(C162&lt;0.5, H162 &lt; 0.5,M162&lt;0.5, R162&gt;=0.5), "B","A"))))))))</f>
+        <v>C1</v>
+      </c>
+      <c r="AA162" s="25" t="str">
+        <f>IF(AND(D162&lt;0.5, I162 &gt;= 0.5,N162&gt;=0.5, S162&lt;0.5), "F",IF(AND(D162&lt;0.5, I162 &gt;= 0.5,N162&gt;=0.5, S162&gt;=0.5), "E2",IF(AND(D162&lt;0.5, I162 &gt;= 0.5,N162&lt;0.5, S162&lt;0.5), "E1",IF(AND(D162&lt;0.5, I162 &gt;= 0.5,N162&lt;0.5, S162&gt;=0.5), "D2",IF(AND(D162&lt;0.5, I162 &lt;0.5,N162&gt;=0.5, S162&lt;0.5), "D1",IF(AND(D162&lt;0.5, I162 &lt; 0.5,N162&gt;=0.5, S162&gt;=0.5), "C2",IF(AND(D162&lt;0.5, I162 &lt; 0.5,N162&lt;0.5, S162&lt;0.5), "C1",IF(AND(D162&lt;0.5, I162 &lt; 0.5,N162&lt;0.5, S162&gt;=0.5), "B","A"))))))))</f>
+        <v>C1</v>
+      </c>
+      <c r="AB162" s="25" t="str">
+        <f>IF(AND(E162&lt;0.5, J162 &gt;= 0.5,O162&gt;=0.5, T162&lt;0.5), "F",IF(AND(E162&lt;0.5, J162 &gt;= 0.5,O162&gt;=0.5, T162&gt;=0.5), "E2",IF(AND(E162&lt;0.5, J162 &gt;= 0.5,O162&lt;0.5, T162&lt;0.5), "E1",IF(AND(E162&lt;0.5, J162 &gt;= 0.5,O162&lt;0.5, T162&gt;=0.5), "D2",IF(AND(E162&lt;0.5, J162 &lt;0.5,O162&gt;=0.5, T162&lt;0.5), "D1",IF(AND(E162&lt;0.5, J162 &lt; 0.5,O162&gt;=0.5, T162&gt;=0.5), "C2",IF(AND(E162&lt;0.5, J162 &lt; 0.5,O162&lt;0.5, T162&lt;0.5), "C1",IF(AND(E162&lt;0.5, J162 &lt; 0.5,O162&lt;0.5, T162&gt;=0.5), "B","A"))))))))</f>
+        <v>C1</v>
+      </c>
+    </row>
+    <row r="163" spans="1:28" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A163" s="3">
         <v>41</v>
       </c>
@@ -8712,8 +10767,20 @@
         <f t="shared" si="23"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="164" spans="1:22" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="Z163" s="25" t="str">
+        <f>IF(AND(C163&lt;0.5, H163 &gt;= 0.5,M163&gt;=0.5, R163&lt;0.5), "F",IF(AND(C163&lt;0.5, H163 &gt;= 0.5,M163&gt;=0.5, R163&gt;=0.5), "E2",IF(AND(C163&lt;0.5, H163 &gt;= 0.5,M163&lt;0.5, R163&lt;0.5), "E1",IF(AND(C163&lt;0.5, H163 &gt;= 0.5,M163&lt;0.5, R163&gt;=0.5), "D2",IF(AND(C163&lt;0.5, H163 &lt;0.5,M163&gt;=0.5, R163&lt;0.5), "D1",IF(AND(C163&lt;0.5, H163 &lt; 0.5,M163&gt;=0.5, R163&gt;=0.5), "C2",IF(AND(C163&lt;0.5, H163 &lt; 0.5,M163&lt;0.5, R163&lt;0.5), "C1",IF(AND(C163&lt;0.5, H163 &lt; 0.5,M163&lt;0.5, R163&gt;=0.5), "B","A"))))))))</f>
+        <v>C1</v>
+      </c>
+      <c r="AA163" s="25" t="str">
+        <f>IF(AND(D163&lt;0.5, I163 &gt;= 0.5,N163&gt;=0.5, S163&lt;0.5), "F",IF(AND(D163&lt;0.5, I163 &gt;= 0.5,N163&gt;=0.5, S163&gt;=0.5), "E2",IF(AND(D163&lt;0.5, I163 &gt;= 0.5,N163&lt;0.5, S163&lt;0.5), "E1",IF(AND(D163&lt;0.5, I163 &gt;= 0.5,N163&lt;0.5, S163&gt;=0.5), "D2",IF(AND(D163&lt;0.5, I163 &lt;0.5,N163&gt;=0.5, S163&lt;0.5), "D1",IF(AND(D163&lt;0.5, I163 &lt; 0.5,N163&gt;=0.5, S163&gt;=0.5), "C2",IF(AND(D163&lt;0.5, I163 &lt; 0.5,N163&lt;0.5, S163&lt;0.5), "C1",IF(AND(D163&lt;0.5, I163 &lt; 0.5,N163&lt;0.5, S163&gt;=0.5), "B","A"))))))))</f>
+        <v>C1</v>
+      </c>
+      <c r="AB163" s="25" t="str">
+        <f>IF(AND(E163&lt;0.5, J163 &gt;= 0.5,O163&gt;=0.5, T163&lt;0.5), "F",IF(AND(E163&lt;0.5, J163 &gt;= 0.5,O163&gt;=0.5, T163&gt;=0.5), "E2",IF(AND(E163&lt;0.5, J163 &gt;= 0.5,O163&lt;0.5, T163&lt;0.5), "E1",IF(AND(E163&lt;0.5, J163 &gt;= 0.5,O163&lt;0.5, T163&gt;=0.5), "D2",IF(AND(E163&lt;0.5, J163 &lt;0.5,O163&gt;=0.5, T163&lt;0.5), "D1",IF(AND(E163&lt;0.5, J163 &lt; 0.5,O163&gt;=0.5, T163&gt;=0.5), "C2",IF(AND(E163&lt;0.5, J163 &lt; 0.5,O163&lt;0.5, T163&lt;0.5), "C1",IF(AND(E163&lt;0.5, J163 &lt; 0.5,O163&lt;0.5, T163&gt;=0.5), "B","A"))))))))</f>
+        <v>C1</v>
+      </c>
+    </row>
+    <row r="164" spans="1:28" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A164" s="1"/>
       <c r="B164" s="1" t="s">
         <v>16</v>
@@ -8759,8 +10826,20 @@
         <f t="shared" si="23"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="165" spans="1:22" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="Z164" s="25" t="str">
+        <f>IF(AND(C164&lt;0.5, H164 &gt;= 0.5,M164&gt;=0.5, R164&lt;0.5), "F",IF(AND(C164&lt;0.5, H164 &gt;= 0.5,M164&gt;=0.5, R164&gt;=0.5), "E2",IF(AND(C164&lt;0.5, H164 &gt;= 0.5,M164&lt;0.5, R164&lt;0.5), "E1",IF(AND(C164&lt;0.5, H164 &gt;= 0.5,M164&lt;0.5, R164&gt;=0.5), "D2",IF(AND(C164&lt;0.5, H164 &lt;0.5,M164&gt;=0.5, R164&lt;0.5), "D1",IF(AND(C164&lt;0.5, H164 &lt; 0.5,M164&gt;=0.5, R164&gt;=0.5), "C2",IF(AND(C164&lt;0.5, H164 &lt; 0.5,M164&lt;0.5, R164&lt;0.5), "C1",IF(AND(C164&lt;0.5, H164 &lt; 0.5,M164&lt;0.5, R164&gt;=0.5), "B","A"))))))))</f>
+        <v>C1</v>
+      </c>
+      <c r="AA164" s="25" t="str">
+        <f>IF(AND(D164&lt;0.5, I164 &gt;= 0.5,N164&gt;=0.5, S164&lt;0.5), "F",IF(AND(D164&lt;0.5, I164 &gt;= 0.5,N164&gt;=0.5, S164&gt;=0.5), "E2",IF(AND(D164&lt;0.5, I164 &gt;= 0.5,N164&lt;0.5, S164&lt;0.5), "E1",IF(AND(D164&lt;0.5, I164 &gt;= 0.5,N164&lt;0.5, S164&gt;=0.5), "D2",IF(AND(D164&lt;0.5, I164 &lt;0.5,N164&gt;=0.5, S164&lt;0.5), "D1",IF(AND(D164&lt;0.5, I164 &lt; 0.5,N164&gt;=0.5, S164&gt;=0.5), "C2",IF(AND(D164&lt;0.5, I164 &lt; 0.5,N164&lt;0.5, S164&lt;0.5), "C1",IF(AND(D164&lt;0.5, I164 &lt; 0.5,N164&lt;0.5, S164&gt;=0.5), "B","A"))))))))</f>
+        <v>C1</v>
+      </c>
+      <c r="AB164" s="25" t="str">
+        <f>IF(AND(E164&lt;0.5, J164 &gt;= 0.5,O164&gt;=0.5, T164&lt;0.5), "F",IF(AND(E164&lt;0.5, J164 &gt;= 0.5,O164&gt;=0.5, T164&gt;=0.5), "E2",IF(AND(E164&lt;0.5, J164 &gt;= 0.5,O164&lt;0.5, T164&lt;0.5), "E1",IF(AND(E164&lt;0.5, J164 &gt;= 0.5,O164&lt;0.5, T164&gt;=0.5), "D2",IF(AND(E164&lt;0.5, J164 &lt;0.5,O164&gt;=0.5, T164&lt;0.5), "D1",IF(AND(E164&lt;0.5, J164 &lt; 0.5,O164&gt;=0.5, T164&gt;=0.5), "C2",IF(AND(E164&lt;0.5, J164 &lt; 0.5,O164&lt;0.5, T164&lt;0.5), "C1",IF(AND(E164&lt;0.5, J164 &lt; 0.5,O164&lt;0.5, T164&gt;=0.5), "B","A"))))))))</f>
+        <v>C1</v>
+      </c>
+    </row>
+    <row r="165" spans="1:28" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A165" s="1"/>
       <c r="B165" s="1" t="s">
         <v>17</v>
@@ -8806,8 +10885,20 @@
         <f t="shared" si="23"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="166" spans="1:22" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="Z165" s="25" t="str">
+        <f>IF(AND(C165&lt;0.5, H165 &gt;= 0.5,M165&gt;=0.5, R165&lt;0.5), "F",IF(AND(C165&lt;0.5, H165 &gt;= 0.5,M165&gt;=0.5, R165&gt;=0.5), "E2",IF(AND(C165&lt;0.5, H165 &gt;= 0.5,M165&lt;0.5, R165&lt;0.5), "E1",IF(AND(C165&lt;0.5, H165 &gt;= 0.5,M165&lt;0.5, R165&gt;=0.5), "D2",IF(AND(C165&lt;0.5, H165 &lt;0.5,M165&gt;=0.5, R165&lt;0.5), "D1",IF(AND(C165&lt;0.5, H165 &lt; 0.5,M165&gt;=0.5, R165&gt;=0.5), "C2",IF(AND(C165&lt;0.5, H165 &lt; 0.5,M165&lt;0.5, R165&lt;0.5), "C1",IF(AND(C165&lt;0.5, H165 &lt; 0.5,M165&lt;0.5, R165&gt;=0.5), "B","A"))))))))</f>
+        <v>C1</v>
+      </c>
+      <c r="AA165" s="25" t="str">
+        <f>IF(AND(D165&lt;0.5, I165 &gt;= 0.5,N165&gt;=0.5, S165&lt;0.5), "F",IF(AND(D165&lt;0.5, I165 &gt;= 0.5,N165&gt;=0.5, S165&gt;=0.5), "E2",IF(AND(D165&lt;0.5, I165 &gt;= 0.5,N165&lt;0.5, S165&lt;0.5), "E1",IF(AND(D165&lt;0.5, I165 &gt;= 0.5,N165&lt;0.5, S165&gt;=0.5), "D2",IF(AND(D165&lt;0.5, I165 &lt;0.5,N165&gt;=0.5, S165&lt;0.5), "D1",IF(AND(D165&lt;0.5, I165 &lt; 0.5,N165&gt;=0.5, S165&gt;=0.5), "C2",IF(AND(D165&lt;0.5, I165 &lt; 0.5,N165&lt;0.5, S165&lt;0.5), "C1",IF(AND(D165&lt;0.5, I165 &lt; 0.5,N165&lt;0.5, S165&gt;=0.5), "B","A"))))))))</f>
+        <v>C1</v>
+      </c>
+      <c r="AB165" s="25" t="str">
+        <f>IF(AND(E165&lt;0.5, J165 &gt;= 0.5,O165&gt;=0.5, T165&lt;0.5), "F",IF(AND(E165&lt;0.5, J165 &gt;= 0.5,O165&gt;=0.5, T165&gt;=0.5), "E2",IF(AND(E165&lt;0.5, J165 &gt;= 0.5,O165&lt;0.5, T165&lt;0.5), "E1",IF(AND(E165&lt;0.5, J165 &gt;= 0.5,O165&lt;0.5, T165&gt;=0.5), "D2",IF(AND(E165&lt;0.5, J165 &lt;0.5,O165&gt;=0.5, T165&lt;0.5), "D1",IF(AND(E165&lt;0.5, J165 &lt; 0.5,O165&gt;=0.5, T165&gt;=0.5), "C2",IF(AND(E165&lt;0.5, J165 &lt; 0.5,O165&lt;0.5, T165&lt;0.5), "C1",IF(AND(E165&lt;0.5, J165 &lt; 0.5,O165&lt;0.5, T165&gt;=0.5), "B","A"))))))))</f>
+        <v>C1</v>
+      </c>
+    </row>
+    <row r="166" spans="1:28" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A166" s="4"/>
       <c r="B166" s="4" t="s">
         <v>18</v>
@@ -8856,8 +10947,20 @@
         <f t="shared" si="23"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="167" spans="1:22" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="Z166" s="25" t="str">
+        <f>IF(AND(C166&lt;0.5, H166 &gt;= 0.5,M166&gt;=0.5, R166&lt;0.5), "F",IF(AND(C166&lt;0.5, H166 &gt;= 0.5,M166&gt;=0.5, R166&gt;=0.5), "E2",IF(AND(C166&lt;0.5, H166 &gt;= 0.5,M166&lt;0.5, R166&lt;0.5), "E1",IF(AND(C166&lt;0.5, H166 &gt;= 0.5,M166&lt;0.5, R166&gt;=0.5), "D2",IF(AND(C166&lt;0.5, H166 &lt;0.5,M166&gt;=0.5, R166&lt;0.5), "D1",IF(AND(C166&lt;0.5, H166 &lt; 0.5,M166&gt;=0.5, R166&gt;=0.5), "C2",IF(AND(C166&lt;0.5, H166 &lt; 0.5,M166&lt;0.5, R166&lt;0.5), "C1",IF(AND(C166&lt;0.5, H166 &lt; 0.5,M166&lt;0.5, R166&gt;=0.5), "B","A"))))))))</f>
+        <v>C1</v>
+      </c>
+      <c r="AA166" s="25" t="str">
+        <f>IF(AND(D166&lt;0.5, I166 &gt;= 0.5,N166&gt;=0.5, S166&lt;0.5), "F",IF(AND(D166&lt;0.5, I166 &gt;= 0.5,N166&gt;=0.5, S166&gt;=0.5), "E2",IF(AND(D166&lt;0.5, I166 &gt;= 0.5,N166&lt;0.5, S166&lt;0.5), "E1",IF(AND(D166&lt;0.5, I166 &gt;= 0.5,N166&lt;0.5, S166&gt;=0.5), "D2",IF(AND(D166&lt;0.5, I166 &lt;0.5,N166&gt;=0.5, S166&lt;0.5), "D1",IF(AND(D166&lt;0.5, I166 &lt; 0.5,N166&gt;=0.5, S166&gt;=0.5), "C2",IF(AND(D166&lt;0.5, I166 &lt; 0.5,N166&lt;0.5, S166&lt;0.5), "C1",IF(AND(D166&lt;0.5, I166 &lt; 0.5,N166&lt;0.5, S166&gt;=0.5), "B","A"))))))))</f>
+        <v>C1</v>
+      </c>
+      <c r="AB166" s="25" t="str">
+        <f>IF(AND(E166&lt;0.5, J166 &gt;= 0.5,O166&gt;=0.5, T166&lt;0.5), "F",IF(AND(E166&lt;0.5, J166 &gt;= 0.5,O166&gt;=0.5, T166&gt;=0.5), "E2",IF(AND(E166&lt;0.5, J166 &gt;= 0.5,O166&lt;0.5, T166&lt;0.5), "E1",IF(AND(E166&lt;0.5, J166 &gt;= 0.5,O166&lt;0.5, T166&gt;=0.5), "D2",IF(AND(E166&lt;0.5, J166 &lt;0.5,O166&gt;=0.5, T166&lt;0.5), "D1",IF(AND(E166&lt;0.5, J166 &lt; 0.5,O166&gt;=0.5, T166&gt;=0.5), "C2",IF(AND(E166&lt;0.5, J166 &lt; 0.5,O166&lt;0.5, T166&lt;0.5), "C1",IF(AND(E166&lt;0.5, J166 &lt; 0.5,O166&lt;0.5, T166&gt;=0.5), "B","A"))))))))</f>
+        <v>C1</v>
+      </c>
+    </row>
+    <row r="167" spans="1:28" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C167" s="2">
         <f>SUM(C3:C166)</f>
         <v>0</v>
@@ -8938,8 +11041,11 @@
         <f t="shared" si="23"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="168" spans="1:22" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="Z167" s="25"/>
+      <c r="AA167" s="25"/>
+      <c r="AB167" s="25"/>
+    </row>
+    <row r="168" spans="1:28" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C168" s="14" t="s">
         <v>9</v>
       </c>
@@ -9000,39 +11106,41 @@
       <c r="V168" s="2" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="169" spans="1:22" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C169" s="21" t="s">
-        <v>0</v>
-      </c>
-      <c r="D169" s="22"/>
-      <c r="E169" s="22"/>
-      <c r="F169" s="22"/>
-      <c r="G169" s="23"/>
-      <c r="H169" s="21" t="s">
+      <c r="AA168" s="25"/>
+    </row>
+    <row r="169" spans="1:28" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C169" s="22" t="s">
+        <v>0</v>
+      </c>
+      <c r="D169" s="23"/>
+      <c r="E169" s="23"/>
+      <c r="F169" s="23"/>
+      <c r="G169" s="24"/>
+      <c r="H169" s="22" t="s">
         <v>1</v>
       </c>
-      <c r="I169" s="22"/>
-      <c r="J169" s="22"/>
-      <c r="K169" s="22"/>
-      <c r="L169" s="23"/>
-      <c r="M169" s="21" t="s">
+      <c r="I169" s="23"/>
+      <c r="J169" s="23"/>
+      <c r="K169" s="23"/>
+      <c r="L169" s="24"/>
+      <c r="M169" s="22" t="s">
         <v>2</v>
       </c>
-      <c r="N169" s="22"/>
-      <c r="O169" s="22"/>
-      <c r="P169" s="22"/>
-      <c r="Q169" s="23"/>
-      <c r="R169" s="21" t="s">
+      <c r="N169" s="23"/>
+      <c r="O169" s="23"/>
+      <c r="P169" s="23"/>
+      <c r="Q169" s="24"/>
+      <c r="R169" s="22" t="s">
         <v>3</v>
       </c>
-      <c r="S169" s="22"/>
-      <c r="T169" s="22"/>
-      <c r="U169" s="22"/>
-      <c r="V169" s="23"/>
+      <c r="S169" s="23"/>
+      <c r="T169" s="23"/>
+      <c r="U169" s="23"/>
+      <c r="V169" s="24"/>
+      <c r="AA169" s="25"/>
     </row>
   </sheetData>
-  <mergeCells count="9">
+  <mergeCells count="10">
     <mergeCell ref="W1:Y1"/>
     <mergeCell ref="C169:G169"/>
     <mergeCell ref="C1:G1"/>
@@ -9042,7 +11150,34 @@
     <mergeCell ref="H169:L169"/>
     <mergeCell ref="M169:Q169"/>
     <mergeCell ref="R169:V169"/>
+    <mergeCell ref="Z1:AB1"/>
   </mergeCells>
+  <conditionalFormatting sqref="Z3:AB166">
+    <cfRule type="expression" dxfId="6" priority="1">
+      <formula>Z3="D2"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="5" priority="2">
+      <formula>Z3="D1"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="4" priority="3">
+      <formula>Z3="E1"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="3" priority="4">
+      <formula>Z3="C1"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="Z3:AB166">
+    <cfRule type="expression" dxfId="2" priority="5">
+      <formula>Z3="E2"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="1" priority="6">
+      <formula>Z3="F"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="0" priority="7">
+      <formula>Z3="C2"</formula>
+    </cfRule>
+  </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>